<commit_message>
Wario - some of level 2 done, 600+ frames improved at this point.
</commit_message>
<xml_diff>
--- a/Wario/Wario.xlsx
+++ b/Wario/Wario.xlsx
@@ -621,7 +621,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -706,14 +706,14 @@
         <v>12</v>
       </c>
       <c r="B9" s="4">
-        <v>3011</v>
+        <v>2596</v>
       </c>
       <c r="C9" s="4">
         <v>3011</v>
       </c>
       <c r="D9" s="4">
         <f>IF(B9 &gt;  0,C9-B9, 0)</f>
-        <v>0</v>
+        <v>415</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75">
@@ -728,24 +728,30 @@
       <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="B11" s="4">
+        <v>2845</v>
+      </c>
       <c r="C11" s="4">
         <v>3261</v>
       </c>
       <c r="D11" s="4">
         <f>IF(B11 &gt;  0,C11-B11, 0)</f>
-        <v>0</v>
+        <v>416</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="B12" s="4">
+        <v>3359</v>
+      </c>
       <c r="C12" s="4">
         <v>3962</v>
       </c>
       <c r="D12" s="4">
         <f t="shared" ref="D12:D75" si="1">IF(B12 &gt;  0,C12-B12, 0)</f>
-        <v>0</v>
+        <v>603</v>
       </c>
     </row>
     <row r="13" spans="1:7">

</xml_diff>

<commit_message>
Wario - Level 2 done
</commit_message>
<xml_diff>
--- a/Wario/Wario.xlsx
+++ b/Wario/Wario.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="66">
   <si>
     <t>Enter pipe</t>
   </si>
@@ -617,11 +617,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J135"/>
+  <dimension ref="A1:J137"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -750,7 +750,7 @@
         <v>3962</v>
       </c>
       <c r="D12" s="4">
-        <f t="shared" ref="D12:D75" si="1">IF(B12 &gt;  0,C12-B12, 0)</f>
+        <f t="shared" ref="D12:D77" si="1">IF(B12 &gt;  0,C12-B12, 0)</f>
         <v>603</v>
       </c>
     </row>
@@ -758,100 +758,121 @@
       <c r="A13" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="B13" s="4">
+        <v>3518</v>
+      </c>
       <c r="C13" s="4">
         <v>4146</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>628</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="4" t="s">
         <v>1</v>
       </c>
+      <c r="B14" s="4">
+        <v>3675</v>
+      </c>
       <c r="C14" s="4">
         <v>4333</v>
       </c>
       <c r="D14" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>658</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="4" t="s">
-        <v>14</v>
+        <v>20</v>
+      </c>
+      <c r="B15" s="4">
+        <v>3880</v>
       </c>
       <c r="C15" s="4">
-        <v>5348</v>
+        <v>4582</v>
       </c>
       <c r="D15" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>702</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="B16" s="4">
+        <v>4470</v>
       </c>
       <c r="C16" s="4">
-        <v>5814</v>
+        <v>5348</v>
       </c>
       <c r="D16" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A17" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
+        <v>878</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="4">
+        <v>4661</v>
+      </c>
+      <c r="C17" s="4">
+        <v>5607</v>
+      </c>
+      <c r="D17" s="4">
+        <f t="shared" si="1"/>
+        <v>946</v>
+      </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="B18" s="4">
+        <v>4865</v>
       </c>
       <c r="C18" s="4">
-        <v>6063</v>
+        <v>5814</v>
       </c>
       <c r="D18" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C19" s="4">
-        <v>6632</v>
-      </c>
-      <c r="D19" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+        <v>949</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="1" customFormat="1" ht="18.75">
+      <c r="A19" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="4" t="s">
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="B20" s="4">
+        <v>5114</v>
       </c>
       <c r="C20" s="4">
-        <v>7375</v>
+        <v>6063</v>
       </c>
       <c r="D20" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>949</v>
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="4">
-        <v>7761</v>
+        <v>6632</v>
       </c>
       <c r="D21" s="4">
         <f t="shared" si="1"/>
@@ -860,10 +881,10 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="4" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="C22" s="4">
-        <v>8018</v>
+        <v>7375</v>
       </c>
       <c r="D22" s="4">
         <f t="shared" si="1"/>
@@ -872,10 +893,10 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="4" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C23" s="4">
-        <v>8307</v>
+        <v>7761</v>
       </c>
       <c r="D23" s="4">
         <f t="shared" si="1"/>
@@ -884,10 +905,10 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C24" s="4">
-        <v>8685</v>
+        <v>8018</v>
       </c>
       <c r="D24" s="4">
         <f t="shared" si="1"/>
@@ -896,10 +917,10 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="4" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C25" s="4">
-        <v>8993</v>
+        <v>8307</v>
       </c>
       <c r="D25" s="4">
         <f t="shared" si="1"/>
@@ -908,10 +929,10 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="4" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="C26" s="4">
-        <v>9350</v>
+        <v>8685</v>
       </c>
       <c r="D26" s="4">
         <f t="shared" si="1"/>
@@ -920,10 +941,10 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="4" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C27" s="4">
-        <v>9786</v>
+        <v>8993</v>
       </c>
       <c r="D27" s="4">
         <f t="shared" si="1"/>
@@ -932,54 +953,54 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="4" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="C28" s="4">
-        <v>9996</v>
+        <v>9350</v>
       </c>
       <c r="D28" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="18.75">
-      <c r="A29" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
+    <row r="29" spans="1:4">
+      <c r="A29" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="4">
+        <v>9786</v>
+      </c>
+      <c r="D29" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C30" s="4">
-        <v>10247</v>
+        <v>9996</v>
       </c>
       <c r="D30" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C31" s="4">
-        <v>11168</v>
-      </c>
-      <c r="D31" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+    <row r="31" spans="1:4" ht="18.75">
+      <c r="A31" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="4" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C32" s="4">
-        <v>16035</v>
+        <v>10247</v>
       </c>
       <c r="D32" s="4">
         <f t="shared" si="1"/>
@@ -988,10 +1009,10 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C33" s="4">
-        <v>16186</v>
+        <v>11168</v>
       </c>
       <c r="D33" s="4">
         <f t="shared" si="1"/>
@@ -1000,54 +1021,54 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="4" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C34" s="4">
-        <v>16394</v>
+        <v>16035</v>
       </c>
       <c r="D34" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="18.75">
-      <c r="A35" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
+    <row r="35" spans="1:10">
+      <c r="A35" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C35" s="4">
+        <v>16186</v>
+      </c>
+      <c r="D35" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C36" s="4">
-        <v>16644</v>
+        <v>16394</v>
       </c>
       <c r="D36" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
-      <c r="A37" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C37" s="4">
-        <v>17223</v>
-      </c>
-      <c r="D37" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+    <row r="37" spans="1:10" ht="18.75">
+      <c r="A37" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" s="4" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="C38" s="4">
-        <v>17684</v>
+        <v>16644</v>
       </c>
       <c r="D38" s="4">
         <f t="shared" si="1"/>
@@ -1059,7 +1080,7 @@
         <v>7</v>
       </c>
       <c r="C39" s="4">
-        <v>18205</v>
+        <v>17223</v>
       </c>
       <c r="D39" s="4">
         <f t="shared" si="1"/>
@@ -1068,10 +1089,10 @@
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="4" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C40" s="4">
-        <v>18401</v>
+        <v>17684</v>
       </c>
       <c r="D40" s="4">
         <f t="shared" si="1"/>
@@ -1080,54 +1101,54 @@
     </row>
     <row r="41" spans="1:10">
       <c r="A41" s="4" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="C41" s="4">
-        <v>18597</v>
+        <v>18205</v>
       </c>
       <c r="D41" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="18.75">
-      <c r="A42" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B42" s="10"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
+    <row r="42" spans="1:10">
+      <c r="A42" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C42" s="4">
+        <v>18401</v>
+      </c>
+      <c r="D42" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C43" s="4">
-        <v>19052</v>
+        <v>18597</v>
       </c>
       <c r="D43" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
-      <c r="A44" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C44" s="4">
-        <v>19925</v>
-      </c>
-      <c r="D44" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+    <row r="44" spans="1:10" ht="18.75">
+      <c r="A44" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B44" s="10"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="10"/>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="4" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="C45" s="4">
-        <v>20355</v>
+        <v>19052</v>
       </c>
       <c r="D45" s="4">
         <f t="shared" si="1"/>
@@ -1139,225 +1160,225 @@
         <v>19</v>
       </c>
       <c r="C46" s="4">
-        <v>20623</v>
+        <v>19925</v>
       </c>
       <c r="D46" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F46" s="6"/>
-      <c r="H46" s="6"/>
-      <c r="J46" s="6"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="4" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C47" s="4">
-        <v>20765</v>
+        <v>20355</v>
       </c>
       <c r="D47" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F47" s="7"/>
-      <c r="H47" s="7"/>
-      <c r="J47" s="7"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C48" s="4">
+        <v>20623</v>
+      </c>
+      <c r="D48" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F48" s="6"/>
+      <c r="H48" s="6"/>
+      <c r="J48" s="6"/>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C49" s="4">
+        <v>20765</v>
+      </c>
+      <c r="D49" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F49" s="7"/>
+      <c r="H49" s="7"/>
+      <c r="J49" s="7"/>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="A50" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C48" s="4">
+      <c r="C50" s="4">
         <v>20978</v>
       </c>
-      <c r="D48" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C49" s="4">
-        <v>21288</v>
-      </c>
-      <c r="D49" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="A50" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C50" s="4">
-        <v>21900</v>
-      </c>
       <c r="D50" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:10">
       <c r="A51" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C51" s="4">
-        <v>22268</v>
+        <v>21288</v>
       </c>
       <c r="D51" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:10">
       <c r="A52" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C52" s="4">
+        <v>21900</v>
+      </c>
+      <c r="D52" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="A53" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C53" s="4">
+        <v>22268</v>
+      </c>
+      <c r="D53" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="A54" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54" s="4">
         <v>22486</v>
       </c>
-      <c r="D52" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="4" t="s">
+      <c r="D54" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="A55" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C53" s="4">
+      <c r="C55" s="4">
         <v>22606</v>
       </c>
-      <c r="D53" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="4" t="s">
+      <c r="D55" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
+      <c r="A56" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C54" s="4">
+      <c r="C56" s="4">
         <v>22810</v>
       </c>
-      <c r="D54" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="18.75">
-      <c r="A55" s="11" t="s">
+      <c r="D56" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="18.75">
+      <c r="A57" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B55" s="11"/>
-      <c r="C55" s="11"/>
-      <c r="D55" s="11"/>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="4" t="s">
+      <c r="B57" s="11"/>
+      <c r="C57" s="11"/>
+      <c r="D57" s="11"/>
+    </row>
+    <row r="58" spans="1:10">
+      <c r="A58" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C56" s="4">
+      <c r="C58" s="4">
         <v>23060</v>
       </c>
-      <c r="D56" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="4" t="s">
+      <c r="D58" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
+      <c r="A59" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C57" s="4">
+      <c r="C59" s="4">
         <v>24356</v>
       </c>
-      <c r="D57" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="4" t="s">
+      <c r="D59" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
+      <c r="A60" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C58" s="4">
+      <c r="C60" s="4">
         <v>24520</v>
       </c>
-      <c r="D58" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="A59" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C59" s="4">
-        <v>24693</v>
-      </c>
-      <c r="D59" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
-      <c r="A60" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C60" s="4">
-        <v>25030</v>
-      </c>
       <c r="D60" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:10">
       <c r="A61" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C61" s="4">
-        <v>25625</v>
+        <v>24693</v>
       </c>
       <c r="D61" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:10">
       <c r="A62" s="4" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C62" s="4">
-        <v>26130</v>
+        <v>25030</v>
       </c>
       <c r="D62" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:10">
       <c r="A63" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C63" s="4">
-        <v>26299</v>
+        <v>25625</v>
       </c>
       <c r="D63" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:10">
       <c r="A64" s="4" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="C64" s="4">
-        <v>26404</v>
+        <v>26130</v>
       </c>
       <c r="D64" s="4">
         <f t="shared" si="1"/>
@@ -1366,119 +1387,113 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="4" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="C65" s="4">
-        <v>26607</v>
+        <v>26299</v>
       </c>
       <c r="D65" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="18.75">
-      <c r="A66" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B66" s="10"/>
-      <c r="C66" s="10"/>
-      <c r="D66" s="10"/>
+    <row r="66" spans="1:4">
+      <c r="A66" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C66" s="4">
+        <v>26404</v>
+      </c>
+      <c r="D66" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C67" s="4">
-        <v>26858</v>
+        <v>26607</v>
       </c>
       <c r="D67" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
-      <c r="A68" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C68" s="4">
-        <v>28167</v>
-      </c>
-      <c r="D68" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+    <row r="68" spans="1:4" ht="18.75">
+      <c r="A68" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B68" s="10"/>
+      <c r="C68" s="10"/>
+      <c r="D68" s="10"/>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C69" s="4">
+        <v>26858</v>
+      </c>
+      <c r="D69" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C70" s="4">
+        <v>28167</v>
+      </c>
+      <c r="D70" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C69" s="4">
+      <c r="C71" s="4">
         <v>32142</v>
       </c>
-      <c r="D69" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4">
-      <c r="A70" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C70" s="4">
-        <v>32671</v>
-      </c>
-      <c r="D70" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" ht="18.75">
-      <c r="A71" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B71" s="11"/>
-      <c r="C71" s="11"/>
-      <c r="D71" s="11"/>
+      <c r="D71" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B72" s="4">
-        <v>32921</v>
+        <v>40</v>
       </c>
       <c r="C72" s="4">
-        <v>32921</v>
+        <v>32671</v>
       </c>
       <c r="D72" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
-      <c r="A73" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B73" s="4">
-        <v>34723</v>
-      </c>
-      <c r="C73" s="4">
-        <v>34723</v>
-      </c>
-      <c r="D73" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+    <row r="73" spans="1:4" ht="18.75">
+      <c r="A73" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B73" s="11"/>
+      <c r="C73" s="11"/>
+      <c r="D73" s="11"/>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="4" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="B74" s="4">
-        <v>35373</v>
+        <v>32921</v>
       </c>
       <c r="C74" s="4">
-        <v>35373</v>
+        <v>32921</v>
       </c>
       <c r="D74" s="4">
         <f t="shared" si="1"/>
@@ -1487,69 +1502,69 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="4" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="B75" s="4">
-        <v>35577</v>
+        <v>34723</v>
       </c>
       <c r="C75" s="4">
-        <v>35577</v>
+        <v>34723</v>
       </c>
       <c r="D75" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="18.75">
-      <c r="A76" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B76" s="10"/>
-      <c r="C76" s="10"/>
-      <c r="D76" s="10"/>
+    <row r="76" spans="1:4">
+      <c r="A76" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B76" s="4">
+        <v>35373</v>
+      </c>
+      <c r="C76" s="4">
+        <v>35373</v>
+      </c>
+      <c r="D76" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="4" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B77" s="4">
-        <v>35826</v>
+        <v>35577</v>
       </c>
       <c r="C77" s="4">
-        <v>35826</v>
+        <v>35577</v>
       </c>
       <c r="D77" s="4">
-        <f t="shared" ref="D77:D186" si="2">IF(B77 &gt;  0,C77-B77, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4">
-      <c r="A78" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B78" s="4">
-        <v>36033</v>
-      </c>
-      <c r="C78" s="4">
-        <v>36033</v>
-      </c>
-      <c r="D78" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="18.75">
+      <c r="A78" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B78" s="10"/>
+      <c r="C78" s="10"/>
+      <c r="D78" s="10"/>
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B79" s="4">
-        <v>36201</v>
+        <v>35826</v>
       </c>
       <c r="C79" s="4">
-        <v>36201</v>
+        <v>35826</v>
       </c>
       <c r="D79" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="D79:D136" si="2">IF(B79 &gt;  0,C79-B79, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1558,10 +1573,10 @@
         <v>45</v>
       </c>
       <c r="B80" s="4">
-        <v>36370</v>
+        <v>36033</v>
       </c>
       <c r="C80" s="4">
-        <v>36370</v>
+        <v>36033</v>
       </c>
       <c r="D80" s="4">
         <f t="shared" si="2"/>
@@ -1573,10 +1588,10 @@
         <v>45</v>
       </c>
       <c r="B81" s="4">
-        <v>36538</v>
+        <v>36201</v>
       </c>
       <c r="C81" s="4">
-        <v>36538</v>
+        <v>36201</v>
       </c>
       <c r="D81" s="4">
         <f t="shared" si="2"/>
@@ -1585,13 +1600,13 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B82" s="4">
-        <v>36744</v>
+        <v>36370</v>
       </c>
       <c r="C82" s="4">
-        <v>36744</v>
+        <v>36370</v>
       </c>
       <c r="D82" s="4">
         <f t="shared" si="2"/>
@@ -1600,13 +1615,13 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B83" s="4">
-        <v>37194</v>
+        <v>36538</v>
       </c>
       <c r="C83" s="4">
-        <v>37194</v>
+        <v>36538</v>
       </c>
       <c r="D83" s="4">
         <f t="shared" si="2"/>
@@ -1615,13 +1630,13 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="4" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="B84" s="4">
-        <v>37481</v>
+        <v>36744</v>
       </c>
       <c r="C84" s="4">
-        <v>37481</v>
+        <v>36744</v>
       </c>
       <c r="D84" s="4">
         <f t="shared" si="2"/>
@@ -1630,13 +1645,13 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="4" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="B85" s="4">
-        <v>37662</v>
+        <v>37194</v>
       </c>
       <c r="C85" s="4">
-        <v>37662</v>
+        <v>37194</v>
       </c>
       <c r="D85" s="4">
         <f t="shared" si="2"/>
@@ -1645,13 +1660,13 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="4" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B86" s="4">
-        <v>37816</v>
+        <v>37481</v>
       </c>
       <c r="C86" s="4">
-        <v>37816</v>
+        <v>37481</v>
       </c>
       <c r="D86" s="4">
         <f t="shared" si="2"/>
@@ -1663,10 +1678,10 @@
         <v>6</v>
       </c>
       <c r="B87" s="4">
-        <v>37986</v>
+        <v>37662</v>
       </c>
       <c r="C87" s="4">
-        <v>37986</v>
+        <v>37662</v>
       </c>
       <c r="D87" s="4">
         <f t="shared" si="2"/>
@@ -1678,10 +1693,10 @@
         <v>6</v>
       </c>
       <c r="B88" s="4">
-        <v>38140</v>
+        <v>37816</v>
       </c>
       <c r="C88" s="4">
-        <v>38140</v>
+        <v>37816</v>
       </c>
       <c r="D88" s="4">
         <f t="shared" si="2"/>
@@ -1693,10 +1708,10 @@
         <v>6</v>
       </c>
       <c r="B89" s="4">
-        <v>38278</v>
+        <v>37986</v>
       </c>
       <c r="C89" s="4">
-        <v>38278</v>
+        <v>37986</v>
       </c>
       <c r="D89" s="4">
         <f t="shared" si="2"/>
@@ -1708,10 +1723,10 @@
         <v>6</v>
       </c>
       <c r="B90" s="4">
-        <v>38479</v>
+        <v>38140</v>
       </c>
       <c r="C90" s="4">
-        <v>38479</v>
+        <v>38140</v>
       </c>
       <c r="D90" s="4">
         <f t="shared" si="2"/>
@@ -1723,10 +1738,10 @@
         <v>6</v>
       </c>
       <c r="B91" s="4">
-        <v>38618</v>
+        <v>38278</v>
       </c>
       <c r="C91" s="4">
-        <v>38618</v>
+        <v>38278</v>
       </c>
       <c r="D91" s="4">
         <f t="shared" si="2"/>
@@ -1735,13 +1750,13 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="4" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="B92" s="4">
-        <v>40024</v>
+        <v>38479</v>
       </c>
       <c r="C92" s="4">
-        <v>40024</v>
+        <v>38479</v>
       </c>
       <c r="D92" s="4">
         <f t="shared" si="2"/>
@@ -1753,10 +1768,10 @@
         <v>6</v>
       </c>
       <c r="B93" s="4">
-        <v>40214</v>
+        <v>38618</v>
       </c>
       <c r="C93" s="4">
-        <v>40214</v>
+        <v>38618</v>
       </c>
       <c r="D93" s="4">
         <f t="shared" si="2"/>
@@ -1765,13 +1780,13 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B94" s="4">
-        <v>40388</v>
+        <v>40024</v>
       </c>
       <c r="C94" s="4">
-        <v>40388</v>
+        <v>40024</v>
       </c>
       <c r="D94" s="4">
         <f t="shared" si="2"/>
@@ -1780,13 +1795,13 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="4" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="B95" s="4">
-        <v>40726</v>
+        <v>40214</v>
       </c>
       <c r="C95" s="4">
-        <v>40726</v>
+        <v>40214</v>
       </c>
       <c r="D95" s="4">
         <f t="shared" si="2"/>
@@ -1795,13 +1810,13 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="4" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B96" s="4">
-        <v>40827</v>
+        <v>40388</v>
       </c>
       <c r="C96" s="4">
-        <v>40827</v>
+        <v>40388</v>
       </c>
       <c r="D96" s="4">
         <f t="shared" si="2"/>
@@ -1810,66 +1825,66 @@
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="4" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="B97" s="4">
-        <v>41030</v>
+        <v>40726</v>
       </c>
       <c r="C97" s="4">
-        <v>41030</v>
+        <v>40726</v>
       </c>
       <c r="D97" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="18.75">
-      <c r="A98" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B98" s="11"/>
-      <c r="C98" s="11"/>
-      <c r="D98" s="11"/>
+    <row r="98" spans="1:5">
+      <c r="A98" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B98" s="4">
+        <v>40827</v>
+      </c>
+      <c r="C98" s="4">
+        <v>40827</v>
+      </c>
+      <c r="D98" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="4" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B99" s="4">
-        <v>41280</v>
+        <v>41030</v>
       </c>
       <c r="C99" s="4">
-        <v>41280</v>
+        <v>41030</v>
       </c>
       <c r="D99" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:5">
-      <c r="A100" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B100" s="4">
-        <v>42038</v>
-      </c>
-      <c r="C100" s="4">
-        <v>42038</v>
-      </c>
-      <c r="D100" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
+    <row r="100" spans="1:5" ht="18.75">
+      <c r="A100" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B100" s="11"/>
+      <c r="C100" s="11"/>
+      <c r="D100" s="11"/>
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="4" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="B101" s="4">
-        <v>42649</v>
+        <v>41280</v>
       </c>
       <c r="C101" s="4">
-        <v>42649</v>
+        <v>41280</v>
       </c>
       <c r="D101" s="4">
         <f t="shared" si="2"/>
@@ -1881,10 +1896,10 @@
         <v>19</v>
       </c>
       <c r="B102" s="4">
-        <v>43208</v>
+        <v>42038</v>
       </c>
       <c r="C102" s="4">
-        <v>43208</v>
+        <v>42038</v>
       </c>
       <c r="D102" s="4">
         <f t="shared" si="2"/>
@@ -1893,20 +1908,17 @@
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B103" s="4">
-        <v>43493</v>
+        <v>42649</v>
       </c>
       <c r="C103" s="4">
-        <v>43493</v>
+        <v>42649</v>
       </c>
       <c r="D103" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
-      </c>
-      <c r="E103" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="104" spans="1:5">
@@ -1914,10 +1926,10 @@
         <v>19</v>
       </c>
       <c r="B104" s="4">
-        <v>43763</v>
+        <v>43208</v>
       </c>
       <c r="C104" s="4">
-        <v>43763</v>
+        <v>43208</v>
       </c>
       <c r="D104" s="4">
         <f t="shared" si="2"/>
@@ -1926,81 +1938,84 @@
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="4" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B105" s="4">
-        <v>44050</v>
+        <v>43493</v>
       </c>
       <c r="C105" s="4">
-        <v>44050</v>
+        <v>43493</v>
       </c>
       <c r="D105" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
+      </c>
+      <c r="E105" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="106" spans="1:5">
       <c r="A106" s="4" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="B106" s="4">
-        <v>44254</v>
+        <v>43763</v>
       </c>
       <c r="C106" s="4">
-        <v>44254</v>
+        <v>43763</v>
       </c>
       <c r="D106" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:5" ht="18.75">
-      <c r="A107" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B107" s="10"/>
-      <c r="C107" s="10"/>
-      <c r="D107" s="10"/>
+    <row r="107" spans="1:5">
+      <c r="A107" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B107" s="4">
+        <v>44050</v>
+      </c>
+      <c r="C107" s="4">
+        <v>44050</v>
+      </c>
+      <c r="D107" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="4" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="B108" s="4">
-        <v>44504</v>
+        <v>44254</v>
       </c>
       <c r="C108" s="4">
-        <v>44504</v>
+        <v>44254</v>
       </c>
       <c r="D108" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:5">
-      <c r="A109" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B109" s="4">
-        <v>46191</v>
-      </c>
-      <c r="C109" s="4">
-        <v>46191</v>
-      </c>
-      <c r="D109" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
+    <row r="109" spans="1:5" ht="18.75">
+      <c r="A109" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B109" s="10"/>
+      <c r="C109" s="10"/>
+      <c r="D109" s="10"/>
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B110" s="4">
-        <v>48585</v>
+        <v>44504</v>
       </c>
       <c r="C110" s="4">
-        <v>48585</v>
+        <v>44504</v>
       </c>
       <c r="D110" s="4">
         <f t="shared" si="2"/>
@@ -2009,13 +2024,13 @@
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B111" s="4">
-        <v>48941</v>
+        <v>46191</v>
       </c>
       <c r="C111" s="4">
-        <v>48941</v>
+        <v>46191</v>
       </c>
       <c r="D111" s="4">
         <f t="shared" si="2"/>
@@ -2024,66 +2039,66 @@
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="4" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="B112" s="4">
-        <v>49144</v>
+        <v>48585</v>
       </c>
       <c r="C112" s="4">
-        <v>49144</v>
+        <v>48585</v>
       </c>
       <c r="D112" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="18.75">
-      <c r="A113" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="B113" s="11"/>
-      <c r="C113" s="11"/>
-      <c r="D113" s="11"/>
+    <row r="113" spans="1:4">
+      <c r="A113" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B113" s="4">
+        <v>48941</v>
+      </c>
+      <c r="C113" s="4">
+        <v>48941</v>
+      </c>
+      <c r="D113" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="4" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="B114" s="4">
-        <v>49395</v>
+        <v>49144</v>
       </c>
       <c r="C114" s="4">
-        <v>49395</v>
+        <v>49144</v>
       </c>
       <c r="D114" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:4">
-      <c r="A115" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B115" s="4">
-        <v>49704</v>
-      </c>
-      <c r="C115" s="4">
-        <v>49704</v>
-      </c>
-      <c r="D115" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
+    <row r="115" spans="1:4" ht="18.75">
+      <c r="A115" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B115" s="11"/>
+      <c r="C115" s="11"/>
+      <c r="D115" s="11"/>
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="4" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="B116" s="4">
-        <v>49883</v>
+        <v>49395</v>
       </c>
       <c r="C116" s="4">
-        <v>49883</v>
+        <v>49395</v>
       </c>
       <c r="D116" s="4">
         <f t="shared" si="2"/>
@@ -2092,13 +2107,13 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="4" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="B117" s="4">
-        <v>50088</v>
+        <v>49704</v>
       </c>
       <c r="C117" s="4">
-        <v>50088</v>
+        <v>49704</v>
       </c>
       <c r="D117" s="4">
         <f t="shared" si="2"/>
@@ -2107,13 +2122,13 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="4" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B118" s="4">
-        <v>50263</v>
+        <v>49883</v>
       </c>
       <c r="C118" s="4">
-        <v>50263</v>
+        <v>49883</v>
       </c>
       <c r="D118" s="4">
         <f t="shared" si="2"/>
@@ -2122,13 +2137,13 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="4" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B119" s="4">
-        <v>50566</v>
+        <v>50088</v>
       </c>
       <c r="C119" s="4">
-        <v>50566</v>
+        <v>50088</v>
       </c>
       <c r="D119" s="4">
         <f t="shared" si="2"/>
@@ -2140,10 +2155,10 @@
         <v>7</v>
       </c>
       <c r="B120" s="4">
-        <v>50734</v>
+        <v>50263</v>
       </c>
       <c r="C120" s="4">
-        <v>50734</v>
+        <v>50263</v>
       </c>
       <c r="D120" s="4">
         <f t="shared" si="2"/>
@@ -2152,13 +2167,13 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="4" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="B121" s="4">
-        <v>50849</v>
+        <v>50566</v>
       </c>
       <c r="C121" s="4">
-        <v>50849</v>
+        <v>50566</v>
       </c>
       <c r="D121" s="4">
         <f t="shared" si="2"/>
@@ -2167,13 +2182,13 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="4" t="s">
-        <v>57</v>
+        <v>7</v>
       </c>
       <c r="B122" s="4">
-        <v>51176</v>
+        <v>50734</v>
       </c>
       <c r="C122" s="4">
-        <v>51176</v>
+        <v>50734</v>
       </c>
       <c r="D122" s="4">
         <f t="shared" si="2"/>
@@ -2182,13 +2197,13 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="4" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B123" s="4">
-        <v>51327</v>
+        <v>50849</v>
       </c>
       <c r="C123" s="4">
-        <v>51327</v>
+        <v>50849</v>
       </c>
       <c r="D123" s="4">
         <f t="shared" si="2"/>
@@ -2197,13 +2212,13 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="4" t="s">
-        <v>6</v>
+        <v>57</v>
       </c>
       <c r="B124" s="4">
-        <v>51577</v>
+        <v>51176</v>
       </c>
       <c r="C124" s="4">
-        <v>51577</v>
+        <v>51176</v>
       </c>
       <c r="D124" s="4">
         <f t="shared" si="2"/>
@@ -2212,13 +2227,13 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="4" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="B125" s="4">
-        <v>51868</v>
+        <v>51327</v>
       </c>
       <c r="C125" s="4">
-        <v>51868</v>
+        <v>51327</v>
       </c>
       <c r="D125" s="4">
         <f t="shared" si="2"/>
@@ -2227,66 +2242,66 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="4" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="B126" s="4">
-        <v>52071</v>
+        <v>51577</v>
       </c>
       <c r="C126" s="4">
-        <v>52071</v>
+        <v>51577</v>
       </c>
       <c r="D126" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="18.75">
-      <c r="A127" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="B127" s="10"/>
-      <c r="C127" s="10"/>
-      <c r="D127" s="10"/>
+    <row r="127" spans="1:4">
+      <c r="A127" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B127" s="4">
+        <v>51868</v>
+      </c>
+      <c r="C127" s="4">
+        <v>51868</v>
+      </c>
+      <c r="D127" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="4" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="B128" s="4">
-        <v>52322</v>
+        <v>52071</v>
       </c>
       <c r="C128" s="4">
-        <v>52322</v>
+        <v>52071</v>
       </c>
       <c r="D128" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:4">
-      <c r="A129" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B129" s="4">
-        <v>53245</v>
-      </c>
-      <c r="C129" s="4">
-        <v>53245</v>
-      </c>
-      <c r="D129" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
+    <row r="129" spans="1:4" ht="18.75">
+      <c r="A129" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B129" s="10"/>
+      <c r="C129" s="10"/>
+      <c r="D129" s="10"/>
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B130" s="4">
-        <v>55063</v>
+        <v>52322</v>
       </c>
       <c r="C130" s="4">
-        <v>55063</v>
+        <v>52322</v>
       </c>
       <c r="D130" s="4">
         <f t="shared" si="2"/>
@@ -2295,13 +2310,13 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="4" t="s">
-        <v>62</v>
+        <v>26</v>
       </c>
       <c r="B131" s="4">
-        <v>55385</v>
+        <v>53245</v>
       </c>
       <c r="C131" s="4">
-        <v>55385</v>
+        <v>53245</v>
       </c>
       <c r="D131" s="4">
         <f t="shared" si="2"/>
@@ -2310,13 +2325,13 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B132" s="4">
-        <v>55706</v>
+        <v>55063</v>
       </c>
       <c r="C132" s="4">
-        <v>55706</v>
+        <v>55063</v>
       </c>
       <c r="D132" s="4">
         <f t="shared" si="2"/>
@@ -2325,13 +2340,13 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B133" s="4">
-        <v>56029</v>
+        <v>55385</v>
       </c>
       <c r="C133" s="4">
-        <v>56029</v>
+        <v>55385</v>
       </c>
       <c r="D133" s="4">
         <f t="shared" si="2"/>
@@ -2340,13 +2355,13 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B134" s="4">
-        <v>58292</v>
+        <v>55706</v>
       </c>
       <c r="C134" s="4">
-        <v>58292</v>
+        <v>55706</v>
       </c>
       <c r="D134" s="4">
         <f t="shared" si="2"/>
@@ -2355,32 +2370,62 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B135" s="4">
+        <v>56029</v>
+      </c>
+      <c r="C135" s="4">
+        <v>56029</v>
+      </c>
+      <c r="D135" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
+      <c r="A136" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B136" s="4">
+        <v>58292</v>
+      </c>
+      <c r="C136" s="4">
+        <v>58292</v>
+      </c>
+      <c r="D136" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4">
+      <c r="A137" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B135" s="9">
+      <c r="B137" s="9">
         <v>0.71250000000000002</v>
       </c>
-      <c r="C135" s="9">
+      <c r="C137" s="9">
         <v>0.71250000000000002</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A107:D107"/>
-    <mergeCell ref="A113:D113"/>
-    <mergeCell ref="A127:D127"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="A55:D55"/>
-    <mergeCell ref="A66:D66"/>
-    <mergeCell ref="A71:D71"/>
-    <mergeCell ref="A76:D76"/>
-    <mergeCell ref="A98:D98"/>
+    <mergeCell ref="A37:D37"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A109:D109"/>
+    <mergeCell ref="A115:D115"/>
+    <mergeCell ref="A129:D129"/>
+    <mergeCell ref="A44:D44"/>
+    <mergeCell ref="A57:D57"/>
+    <mergeCell ref="A68:D68"/>
+    <mergeCell ref="A73:D73"/>
+    <mergeCell ref="A78:D78"/>
+    <mergeCell ref="A100:D100"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -4285,11 +4330,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A29:D29"/>
     <mergeCell ref="A127:D127"/>
     <mergeCell ref="A107:D107"/>
     <mergeCell ref="A113:D113"/>
@@ -4300,6 +4340,11 @@
     <mergeCell ref="A98:D98"/>
     <mergeCell ref="A66:D66"/>
     <mergeCell ref="A55:D55"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A29:D29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>

</xml_diff>

<commit_message>
Wario - Beginning Level 4
</commit_message>
<xml_diff>
--- a/Wario/Wario.xlsx
+++ b/Wario/Wario.xlsx
@@ -320,9 +320,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -620,8 +620,8 @@
   <dimension ref="A1:J137"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -645,12 +645,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -678,12 +678,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -717,12 +717,12 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
@@ -845,12 +845,12 @@
       </c>
     </row>
     <row r="19" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="4" t="s">
@@ -871,140 +871,173 @@
       <c r="A21" s="5" t="s">
         <v>0</v>
       </c>
+      <c r="B21" s="4">
+        <v>5680</v>
+      </c>
       <c r="C21" s="4">
         <v>6632</v>
       </c>
       <c r="D21" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>952</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="4" t="s">
         <v>0</v>
       </c>
+      <c r="B22" s="4">
+        <v>6399</v>
+      </c>
       <c r="C22" s="4">
         <v>7375</v>
       </c>
       <c r="D22" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>976</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="4" t="s">
         <v>0</v>
       </c>
+      <c r="B23" s="4">
+        <v>6767</v>
+      </c>
       <c r="C23" s="4">
         <v>7761</v>
       </c>
       <c r="D23" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>994</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="B24" s="4">
+        <v>7021</v>
+      </c>
       <c r="C24" s="4">
         <v>8018</v>
       </c>
       <c r="D24" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>997</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="B25" s="4">
+        <v>7303</v>
+      </c>
       <c r="C25" s="4">
         <v>8307</v>
       </c>
       <c r="D25" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="4" t="s">
         <v>21</v>
       </c>
+      <c r="B26" s="4">
+        <v>7679</v>
+      </c>
       <c r="C26" s="4">
         <v>8685</v>
       </c>
       <c r="D26" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="4" t="s">
         <v>0</v>
       </c>
+      <c r="B27" s="4">
+        <v>7889</v>
+      </c>
       <c r="C27" s="4">
         <v>8993</v>
       </c>
       <c r="D27" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="4" t="s">
         <v>0</v>
       </c>
+      <c r="B28" s="4">
+        <v>8242</v>
+      </c>
       <c r="C28" s="4">
         <v>9350</v>
       </c>
       <c r="D28" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="4" t="s">
         <v>22</v>
       </c>
+      <c r="B29" s="4">
+        <v>8601</v>
+      </c>
       <c r="C29" s="4">
         <v>9786</v>
       </c>
       <c r="D29" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="B30" s="4">
+        <v>8805</v>
+      </c>
       <c r="C30" s="4">
         <v>9996</v>
       </c>
       <c r="D30" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="18.75">
-      <c r="A31" s="10" t="s">
+      <c r="A31" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="B32" s="4">
+        <v>9054</v>
+      </c>
       <c r="C32" s="4">
         <v>10247</v>
       </c>
       <c r="D32" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -1056,12 +1089,12 @@
       </c>
     </row>
     <row r="37" spans="1:10" ht="18.75">
-      <c r="A37" s="11" t="s">
+      <c r="A37" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B37" s="11"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" s="4" t="s">
@@ -1136,12 +1169,12 @@
       </c>
     </row>
     <row r="44" spans="1:10" ht="18.75">
-      <c r="A44" s="10" t="s">
+      <c r="A44" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B44" s="10"/>
-      <c r="C44" s="10"/>
-      <c r="D44" s="10"/>
+      <c r="B44" s="12"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12"/>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="4" t="s">
@@ -1294,12 +1327,12 @@
       </c>
     </row>
     <row r="57" spans="1:10" ht="18.75">
-      <c r="A57" s="11" t="s">
+      <c r="A57" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B57" s="11"/>
-      <c r="C57" s="11"/>
-      <c r="D57" s="11"/>
+      <c r="B57" s="10"/>
+      <c r="C57" s="10"/>
+      <c r="D57" s="10"/>
     </row>
     <row r="58" spans="1:10">
       <c r="A58" s="4" t="s">
@@ -1422,12 +1455,12 @@
       </c>
     </row>
     <row r="68" spans="1:4" ht="18.75">
-      <c r="A68" s="10" t="s">
+      <c r="A68" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B68" s="10"/>
-      <c r="C68" s="10"/>
-      <c r="D68" s="10"/>
+      <c r="B68" s="12"/>
+      <c r="C68" s="12"/>
+      <c r="D68" s="12"/>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="4" t="s">
@@ -1478,12 +1511,12 @@
       </c>
     </row>
     <row r="73" spans="1:4" ht="18.75">
-      <c r="A73" s="11" t="s">
+      <c r="A73" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B73" s="11"/>
-      <c r="C73" s="11"/>
-      <c r="D73" s="11"/>
+      <c r="B73" s="10"/>
+      <c r="C73" s="10"/>
+      <c r="D73" s="10"/>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="4" t="s">
@@ -1546,12 +1579,12 @@
       </c>
     </row>
     <row r="78" spans="1:4" ht="18.75">
-      <c r="A78" s="10" t="s">
+      <c r="A78" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B78" s="10"/>
-      <c r="C78" s="10"/>
-      <c r="D78" s="10"/>
+      <c r="B78" s="12"/>
+      <c r="C78" s="12"/>
+      <c r="D78" s="12"/>
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="4" t="s">
@@ -1869,12 +1902,12 @@
       </c>
     </row>
     <row r="100" spans="1:5" ht="18.75">
-      <c r="A100" s="11" t="s">
+      <c r="A100" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="B100" s="11"/>
-      <c r="C100" s="11"/>
-      <c r="D100" s="11"/>
+      <c r="B100" s="10"/>
+      <c r="C100" s="10"/>
+      <c r="D100" s="10"/>
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="4" t="s">
@@ -2000,12 +2033,12 @@
       </c>
     </row>
     <row r="109" spans="1:5" ht="18.75">
-      <c r="A109" s="10" t="s">
+      <c r="A109" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B109" s="10"/>
-      <c r="C109" s="10"/>
-      <c r="D109" s="10"/>
+      <c r="B109" s="12"/>
+      <c r="C109" s="12"/>
+      <c r="D109" s="12"/>
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="4" t="s">
@@ -2083,12 +2116,12 @@
       </c>
     </row>
     <row r="115" spans="1:4" ht="18.75">
-      <c r="A115" s="11" t="s">
+      <c r="A115" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B115" s="11"/>
-      <c r="C115" s="11"/>
-      <c r="D115" s="11"/>
+      <c r="B115" s="10"/>
+      <c r="C115" s="10"/>
+      <c r="D115" s="10"/>
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="4" t="s">
@@ -2286,12 +2319,12 @@
       </c>
     </row>
     <row r="129" spans="1:4" ht="18.75">
-      <c r="A129" s="10" t="s">
+      <c r="A129" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="B129" s="10"/>
-      <c r="C129" s="10"/>
-      <c r="D129" s="10"/>
+      <c r="B129" s="12"/>
+      <c r="C129" s="12"/>
+      <c r="D129" s="12"/>
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="4" t="s">
@@ -2411,12 +2444,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A37:D37"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A31:D31"/>
     <mergeCell ref="A109:D109"/>
     <mergeCell ref="A115:D115"/>
     <mergeCell ref="A129:D129"/>
@@ -2426,6 +2453,12 @@
     <mergeCell ref="A73:D73"/>
     <mergeCell ref="A78:D78"/>
     <mergeCell ref="A100:D100"/>
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A31:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -2462,12 +2495,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -2495,12 +2528,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -2534,12 +2567,12 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
@@ -2623,12 +2656,12 @@
       </c>
     </row>
     <row r="17" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="4" t="s">
@@ -2796,12 +2829,12 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="18.75">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="4" t="s">
@@ -2879,12 +2912,12 @@
       </c>
     </row>
     <row r="35" spans="1:10" ht="18.75">
-      <c r="A35" s="11" t="s">
+      <c r="A35" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="4" t="s">
@@ -2977,12 +3010,12 @@
       </c>
     </row>
     <row r="42" spans="1:10" ht="18.75">
-      <c r="A42" s="10" t="s">
+      <c r="A42" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B42" s="10"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="4" t="s">
@@ -3171,12 +3204,12 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="18.75">
-      <c r="A55" s="11" t="s">
+      <c r="A55" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B55" s="11"/>
-      <c r="C55" s="11"/>
-      <c r="D55" s="11"/>
+      <c r="B55" s="10"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="10"/>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="4" t="s">
@@ -3329,12 +3362,12 @@
       </c>
     </row>
     <row r="66" spans="1:4" ht="18.75">
-      <c r="A66" s="10" t="s">
+      <c r="A66" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B66" s="10"/>
-      <c r="C66" s="10"/>
-      <c r="D66" s="10"/>
+      <c r="B66" s="12"/>
+      <c r="C66" s="12"/>
+      <c r="D66" s="12"/>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="4" t="s">
@@ -3397,12 +3430,12 @@
       </c>
     </row>
     <row r="71" spans="1:4" ht="18.75">
-      <c r="A71" s="11" t="s">
+      <c r="A71" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B71" s="11"/>
-      <c r="C71" s="11"/>
-      <c r="D71" s="11"/>
+      <c r="B71" s="10"/>
+      <c r="C71" s="10"/>
+      <c r="D71" s="10"/>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="4" t="s">
@@ -3465,12 +3498,12 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="18.75">
-      <c r="A76" s="10" t="s">
+      <c r="A76" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B76" s="10"/>
-      <c r="C76" s="10"/>
-      <c r="D76" s="10"/>
+      <c r="B76" s="12"/>
+      <c r="C76" s="12"/>
+      <c r="D76" s="12"/>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="4" t="s">
@@ -3788,12 +3821,12 @@
       </c>
     </row>
     <row r="98" spans="1:5" ht="18.75">
-      <c r="A98" s="11" t="s">
+      <c r="A98" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="B98" s="11"/>
-      <c r="C98" s="11"/>
-      <c r="D98" s="11"/>
+      <c r="B98" s="10"/>
+      <c r="C98" s="10"/>
+      <c r="D98" s="10"/>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="4" t="s">
@@ -3919,12 +3952,12 @@
       </c>
     </row>
     <row r="107" spans="1:5" ht="18.75">
-      <c r="A107" s="10" t="s">
+      <c r="A107" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B107" s="10"/>
-      <c r="C107" s="10"/>
-      <c r="D107" s="10"/>
+      <c r="B107" s="12"/>
+      <c r="C107" s="12"/>
+      <c r="D107" s="12"/>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="4" t="s">
@@ -4002,12 +4035,12 @@
       </c>
     </row>
     <row r="113" spans="1:4" ht="18.75">
-      <c r="A113" s="11" t="s">
+      <c r="A113" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B113" s="11"/>
-      <c r="C113" s="11"/>
-      <c r="D113" s="11"/>
+      <c r="B113" s="10"/>
+      <c r="C113" s="10"/>
+      <c r="D113" s="10"/>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="4" t="s">
@@ -4205,12 +4238,12 @@
       </c>
     </row>
     <row r="127" spans="1:4" ht="18.75">
-      <c r="A127" s="10" t="s">
+      <c r="A127" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="B127" s="10"/>
-      <c r="C127" s="10"/>
-      <c r="D127" s="10"/>
+      <c r="B127" s="12"/>
+      <c r="C127" s="12"/>
+      <c r="D127" s="12"/>
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="4" t="s">
@@ -4330,6 +4363,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A29:D29"/>
     <mergeCell ref="A127:D127"/>
     <mergeCell ref="A107:D107"/>
     <mergeCell ref="A113:D113"/>
@@ -4340,11 +4378,6 @@
     <mergeCell ref="A98:D98"/>
     <mergeCell ref="A66:D66"/>
     <mergeCell ref="A55:D55"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A29:D29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>

</xml_diff>

<commit_message>
Wario - Level 5 begin
</commit_message>
<xml_diff>
--- a/Wario/Wario.xlsx
+++ b/Wario/Wario.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="68">
   <si>
     <t>Enter pipe</t>
   </si>
@@ -213,6 +213,12 @@
   </si>
   <si>
     <t>Final In-Game Time</t>
+  </si>
+  <si>
+    <t>1st Hit</t>
+  </si>
+  <si>
+    <t>Black Screen</t>
   </si>
 </sst>
 </file>
@@ -617,11 +623,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J137"/>
+  <dimension ref="A1:J143"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -750,7 +756,7 @@
         <v>3962</v>
       </c>
       <c r="D12" s="4">
-        <f t="shared" ref="D12:D77" si="1">IF(B12 &gt;  0,C12-B12, 0)</f>
+        <f t="shared" ref="D12:D83" si="1">IF(B12 &gt;  0,C12-B12, 0)</f>
         <v>603</v>
       </c>
     </row>
@@ -1040,226 +1046,253 @@
         <v>1193</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:4">
       <c r="A33" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" s="4">
+        <v>9397</v>
+      </c>
+      <c r="C33" s="4">
+        <v>10632</v>
+      </c>
+      <c r="D33" s="4">
+        <f t="shared" si="1"/>
+        <v>1235</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" s="4">
+        <v>9633</v>
+      </c>
+      <c r="C34" s="4">
+        <v>10869</v>
+      </c>
+      <c r="D34" s="4">
+        <f t="shared" si="1"/>
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C33" s="4">
+      <c r="B35" s="4">
+        <v>9932</v>
+      </c>
+      <c r="C35" s="4">
         <v>11168</v>
       </c>
-      <c r="D33" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10">
-      <c r="A34" s="4" t="s">
+      <c r="D35" s="4">
+        <f t="shared" si="1"/>
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B36" s="4">
+        <v>11304</v>
+      </c>
+      <c r="C36" s="4">
+        <v>12540</v>
+      </c>
+      <c r="D36" s="4">
+        <f t="shared" si="1"/>
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B37" s="4">
+        <v>12308</v>
+      </c>
+      <c r="C37" s="4">
+        <v>13544</v>
+      </c>
+      <c r="D37" s="4">
+        <f t="shared" si="1"/>
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B38" s="4">
+        <v>13312</v>
+      </c>
+      <c r="C38" s="4">
+        <v>14548</v>
+      </c>
+      <c r="D38" s="4">
+        <f t="shared" si="1"/>
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B39" s="4">
+        <v>14611</v>
+      </c>
+      <c r="C39" s="4">
+        <v>15846</v>
+      </c>
+      <c r="D39" s="4">
+        <f t="shared" si="1"/>
+        <v>1235</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C34" s="4">
+      <c r="B40" s="4">
+        <v>14800</v>
+      </c>
+      <c r="C40" s="4">
         <v>16035</v>
       </c>
-      <c r="D34" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10">
-      <c r="A35" s="4" t="s">
+      <c r="D40" s="4">
+        <f t="shared" si="1"/>
+        <v>1235</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C35" s="4">
+      <c r="B41" s="4">
+        <v>14936</v>
+      </c>
+      <c r="C41" s="4">
         <v>16186</v>
       </c>
-      <c r="D35" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10">
-      <c r="A36" s="4" t="s">
+      <c r="D41" s="4">
+        <f t="shared" si="1"/>
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C36" s="4">
+      <c r="B42" s="4">
+        <v>15140</v>
+      </c>
+      <c r="C42" s="4">
         <v>16394</v>
       </c>
-      <c r="D36" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="18.75">
-      <c r="A37" s="10" t="s">
+      <c r="D42" s="4">
+        <f t="shared" si="1"/>
+        <v>1254</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="18.75">
+      <c r="A43" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B37" s="10"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
-    </row>
-    <row r="38" spans="1:10">
-      <c r="A38" s="4" t="s">
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C38" s="4">
+      <c r="B44" s="4">
+        <v>15390</v>
+      </c>
+      <c r="C44" s="4">
         <v>16644</v>
       </c>
-      <c r="D38" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10">
-      <c r="A39" s="4" t="s">
+      <c r="D44" s="4">
+        <f t="shared" si="1"/>
+        <v>1254</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C39" s="4">
+      <c r="C45" s="4">
         <v>17223</v>
       </c>
-      <c r="D39" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10">
-      <c r="A40" s="4" t="s">
+      <c r="D45" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C40" s="4">
+      <c r="C46" s="4">
         <v>17684</v>
       </c>
-      <c r="D40" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10">
-      <c r="A41" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C41" s="4">
-        <v>18205</v>
-      </c>
-      <c r="D41" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10">
-      <c r="A42" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C42" s="4">
-        <v>18401</v>
-      </c>
-      <c r="D42" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10">
-      <c r="A43" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C43" s="4">
-        <v>18597</v>
-      </c>
-      <c r="D43" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="18.75">
-      <c r="A44" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B44" s="12"/>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
-    </row>
-    <row r="45" spans="1:10">
-      <c r="A45" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C45" s="4">
-        <v>19052</v>
-      </c>
-      <c r="D45" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10">
-      <c r="A46" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C46" s="4">
-        <v>19925</v>
-      </c>
       <c r="D46" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:4">
       <c r="A47" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C47" s="4">
-        <v>20355</v>
+        <v>18205</v>
       </c>
       <c r="D47" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:4">
       <c r="A48" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C48" s="4">
-        <v>20623</v>
+        <v>18401</v>
       </c>
       <c r="D48" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F48" s="6"/>
-      <c r="H48" s="6"/>
-      <c r="J48" s="6"/>
     </row>
     <row r="49" spans="1:10">
       <c r="A49" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C49" s="4">
-        <v>20765</v>
+        <v>18597</v>
       </c>
       <c r="D49" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F49" s="7"/>
-      <c r="H49" s="7"/>
-      <c r="J49" s="7"/>
-    </row>
-    <row r="50" spans="1:10">
-      <c r="A50" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C50" s="4">
-        <v>20978</v>
-      </c>
-      <c r="D50" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+    </row>
+    <row r="50" spans="1:10" ht="18.75">
+      <c r="A50" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B50" s="12"/>
+      <c r="C50" s="12"/>
+      <c r="D50" s="12"/>
     </row>
     <row r="51" spans="1:10">
       <c r="A51" s="4" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="C51" s="4">
-        <v>21288</v>
+        <v>19052</v>
       </c>
       <c r="D51" s="4">
         <f t="shared" si="1"/>
@@ -1268,10 +1301,10 @@
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="4" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C52" s="4">
-        <v>21900</v>
+        <v>19925</v>
       </c>
       <c r="D52" s="4">
         <f t="shared" si="1"/>
@@ -1283,7 +1316,7 @@
         <v>7</v>
       </c>
       <c r="C53" s="4">
-        <v>22268</v>
+        <v>20355</v>
       </c>
       <c r="D53" s="4">
         <f t="shared" si="1"/>
@@ -1292,54 +1325,64 @@
     </row>
     <row r="54" spans="1:10">
       <c r="A54" s="4" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C54" s="4">
-        <v>22486</v>
+        <v>20623</v>
       </c>
       <c r="D54" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="F54" s="6"/>
+      <c r="H54" s="6"/>
+      <c r="J54" s="6"/>
     </row>
     <row r="55" spans="1:10">
       <c r="A55" s="4" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C55" s="4">
-        <v>22606</v>
+        <v>20765</v>
       </c>
       <c r="D55" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="F55" s="7"/>
+      <c r="H55" s="7"/>
+      <c r="J55" s="7"/>
     </row>
     <row r="56" spans="1:10">
       <c r="A56" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C56" s="4">
-        <v>22810</v>
+        <v>20978</v>
       </c>
       <c r="D56" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="18.75">
-      <c r="A57" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B57" s="10"/>
-      <c r="C57" s="10"/>
-      <c r="D57" s="10"/>
+    <row r="57" spans="1:10">
+      <c r="A57" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C57" s="4">
+        <v>21288</v>
+      </c>
+      <c r="D57" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="58" spans="1:10">
       <c r="A58" s="4" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="C58" s="4">
-        <v>23060</v>
+        <v>21900</v>
       </c>
       <c r="D58" s="4">
         <f t="shared" si="1"/>
@@ -1348,10 +1391,10 @@
     </row>
     <row r="59" spans="1:10">
       <c r="A59" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C59" s="4">
-        <v>24356</v>
+        <v>22268</v>
       </c>
       <c r="D59" s="4">
         <f t="shared" si="1"/>
@@ -1360,10 +1403,10 @@
     </row>
     <row r="60" spans="1:10">
       <c r="A60" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C60" s="4">
-        <v>24520</v>
+        <v>22486</v>
       </c>
       <c r="D60" s="4">
         <f t="shared" si="1"/>
@@ -1372,10 +1415,10 @@
     </row>
     <row r="61" spans="1:10">
       <c r="A61" s="4" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="C61" s="4">
-        <v>24693</v>
+        <v>22606</v>
       </c>
       <c r="D61" s="4">
         <f t="shared" si="1"/>
@@ -1384,34 +1427,30 @@
     </row>
     <row r="62" spans="1:10">
       <c r="A62" s="4" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="C62" s="4">
-        <v>25030</v>
+        <v>22810</v>
       </c>
       <c r="D62" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:10">
-      <c r="A63" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C63" s="4">
-        <v>25625</v>
-      </c>
-      <c r="D63" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+    <row r="63" spans="1:10" ht="18.75">
+      <c r="A63" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B63" s="10"/>
+      <c r="C63" s="10"/>
+      <c r="D63" s="10"/>
     </row>
     <row r="64" spans="1:10">
       <c r="A64" s="4" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="C64" s="4">
-        <v>26130</v>
+        <v>23060</v>
       </c>
       <c r="D64" s="4">
         <f t="shared" si="1"/>
@@ -1420,10 +1459,10 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C65" s="4">
-        <v>26299</v>
+        <v>24356</v>
       </c>
       <c r="D65" s="4">
         <f t="shared" si="1"/>
@@ -1432,10 +1471,10 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="4" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="C66" s="4">
-        <v>26404</v>
+        <v>24520</v>
       </c>
       <c r="D66" s="4">
         <f t="shared" si="1"/>
@@ -1444,30 +1483,34 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="4" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="C67" s="4">
-        <v>26607</v>
+        <v>24693</v>
       </c>
       <c r="D67" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="18.75">
-      <c r="A68" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B68" s="12"/>
-      <c r="C68" s="12"/>
-      <c r="D68" s="12"/>
+    <row r="68" spans="1:4">
+      <c r="A68" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C68" s="4">
+        <v>25030</v>
+      </c>
+      <c r="D68" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="4" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="C69" s="4">
-        <v>26858</v>
+        <v>25625</v>
       </c>
       <c r="D69" s="4">
         <f t="shared" si="1"/>
@@ -1475,11 +1518,11 @@
       </c>
     </row>
     <row r="70" spans="1:4">
-      <c r="A70" s="8" t="s">
-        <v>26</v>
+      <c r="A70" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="C70" s="4">
-        <v>28167</v>
+        <v>26130</v>
       </c>
       <c r="D70" s="4">
         <f t="shared" si="1"/>
@@ -1488,10 +1531,10 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="4" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="C71" s="4">
-        <v>32142</v>
+        <v>26299</v>
       </c>
       <c r="D71" s="4">
         <f t="shared" si="1"/>
@@ -1500,48 +1543,42 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="4" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="C72" s="4">
-        <v>32671</v>
+        <v>26404</v>
       </c>
       <c r="D72" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="18.75">
-      <c r="A73" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B73" s="10"/>
-      <c r="C73" s="10"/>
-      <c r="D73" s="10"/>
-    </row>
-    <row r="74" spans="1:4">
-      <c r="A74" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B74" s="4">
-        <v>32921</v>
-      </c>
-      <c r="C74" s="4">
-        <v>32921</v>
-      </c>
-      <c r="D74" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+    <row r="73" spans="1:4">
+      <c r="A73" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C73" s="4">
+        <v>26607</v>
+      </c>
+      <c r="D73" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="18.75">
+      <c r="A74" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B74" s="12"/>
+      <c r="C74" s="12"/>
+      <c r="D74" s="12"/>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B75" s="4">
-        <v>34723</v>
+        <v>37</v>
       </c>
       <c r="C75" s="4">
-        <v>34723</v>
+        <v>26858</v>
       </c>
       <c r="D75" s="4">
         <f t="shared" si="1"/>
@@ -1549,14 +1586,11 @@
       </c>
     </row>
     <row r="76" spans="1:4">
-      <c r="A76" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B76" s="4">
-        <v>35373</v>
+      <c r="A76" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="C76" s="4">
-        <v>35373</v>
+        <v>28167</v>
       </c>
       <c r="D76" s="4">
         <f t="shared" si="1"/>
@@ -1565,141 +1599,128 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B77" s="4">
-        <v>35577</v>
+        <v>39</v>
       </c>
       <c r="C77" s="4">
-        <v>35577</v>
+        <v>32142</v>
       </c>
       <c r="D77" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="18.75">
-      <c r="A78" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B78" s="12"/>
-      <c r="C78" s="12"/>
-      <c r="D78" s="12"/>
-    </row>
-    <row r="79" spans="1:4">
-      <c r="A79" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B79" s="4">
-        <v>35826</v>
-      </c>
-      <c r="C79" s="4">
-        <v>35826</v>
-      </c>
-      <c r="D79" s="4">
-        <f t="shared" ref="D79:D136" si="2">IF(B79 &gt;  0,C79-B79, 0)</f>
-        <v>0</v>
-      </c>
+    <row r="78" spans="1:4">
+      <c r="A78" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C78" s="4">
+        <v>32671</v>
+      </c>
+      <c r="D78" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="18.75">
+      <c r="A79" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B79" s="10"/>
+      <c r="C79" s="10"/>
+      <c r="D79" s="10"/>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B80" s="4">
-        <v>36033</v>
+        <v>32921</v>
       </c>
       <c r="C80" s="4">
-        <v>36033</v>
+        <v>32921</v>
       </c>
       <c r="D80" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="4" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="B81" s="4">
-        <v>36201</v>
+        <v>34723</v>
       </c>
       <c r="C81" s="4">
-        <v>36201</v>
+        <v>34723</v>
       </c>
       <c r="D81" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="4" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="B82" s="4">
-        <v>36370</v>
+        <v>35373</v>
       </c>
       <c r="C82" s="4">
-        <v>36370</v>
+        <v>35373</v>
       </c>
       <c r="D82" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="4" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B83" s="4">
-        <v>36538</v>
+        <v>35577</v>
       </c>
       <c r="C83" s="4">
-        <v>36538</v>
+        <v>35577</v>
       </c>
       <c r="D83" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4">
-      <c r="A84" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B84" s="4">
-        <v>36744</v>
-      </c>
-      <c r="C84" s="4">
-        <v>36744</v>
-      </c>
-      <c r="D84" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="18.75">
+      <c r="A84" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B84" s="12"/>
+      <c r="C84" s="12"/>
+      <c r="D84" s="12"/>
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B85" s="4">
-        <v>37194</v>
+        <v>35826</v>
       </c>
       <c r="C85" s="4">
-        <v>37194</v>
+        <v>35826</v>
       </c>
       <c r="D85" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="D85:D142" si="2">IF(B85 &gt;  0,C85-B85, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="4" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="B86" s="4">
-        <v>37481</v>
+        <v>36033</v>
       </c>
       <c r="C86" s="4">
-        <v>37481</v>
+        <v>36033</v>
       </c>
       <c r="D86" s="4">
         <f t="shared" si="2"/>
@@ -1708,13 +1729,13 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="4" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="B87" s="4">
-        <v>37662</v>
+        <v>36201</v>
       </c>
       <c r="C87" s="4">
-        <v>37662</v>
+        <v>36201</v>
       </c>
       <c r="D87" s="4">
         <f t="shared" si="2"/>
@@ -1723,13 +1744,13 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="4" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="B88" s="4">
-        <v>37816</v>
+        <v>36370</v>
       </c>
       <c r="C88" s="4">
-        <v>37816</v>
+        <v>36370</v>
       </c>
       <c r="D88" s="4">
         <f t="shared" si="2"/>
@@ -1738,13 +1759,13 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="4" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="B89" s="4">
-        <v>37986</v>
+        <v>36538</v>
       </c>
       <c r="C89" s="4">
-        <v>37986</v>
+        <v>36538</v>
       </c>
       <c r="D89" s="4">
         <f t="shared" si="2"/>
@@ -1753,13 +1774,13 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="4" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="B90" s="4">
-        <v>38140</v>
+        <v>36744</v>
       </c>
       <c r="C90" s="4">
-        <v>38140</v>
+        <v>36744</v>
       </c>
       <c r="D90" s="4">
         <f t="shared" si="2"/>
@@ -1768,13 +1789,13 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="4" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="B91" s="4">
-        <v>38278</v>
+        <v>37194</v>
       </c>
       <c r="C91" s="4">
-        <v>38278</v>
+        <v>37194</v>
       </c>
       <c r="D91" s="4">
         <f t="shared" si="2"/>
@@ -1783,13 +1804,13 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="4" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B92" s="4">
-        <v>38479</v>
+        <v>37481</v>
       </c>
       <c r="C92" s="4">
-        <v>38479</v>
+        <v>37481</v>
       </c>
       <c r="D92" s="4">
         <f t="shared" si="2"/>
@@ -1801,10 +1822,10 @@
         <v>6</v>
       </c>
       <c r="B93" s="4">
-        <v>38618</v>
+        <v>37662</v>
       </c>
       <c r="C93" s="4">
-        <v>38618</v>
+        <v>37662</v>
       </c>
       <c r="D93" s="4">
         <f t="shared" si="2"/>
@@ -1813,13 +1834,13 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="4" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="B94" s="4">
-        <v>40024</v>
+        <v>37816</v>
       </c>
       <c r="C94" s="4">
-        <v>40024</v>
+        <v>37816</v>
       </c>
       <c r="D94" s="4">
         <f t="shared" si="2"/>
@@ -1831,10 +1852,10 @@
         <v>6</v>
       </c>
       <c r="B95" s="4">
-        <v>40214</v>
+        <v>37986</v>
       </c>
       <c r="C95" s="4">
-        <v>40214</v>
+        <v>37986</v>
       </c>
       <c r="D95" s="4">
         <f t="shared" si="2"/>
@@ -1843,13 +1864,13 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="4" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="B96" s="4">
-        <v>40388</v>
+        <v>38140</v>
       </c>
       <c r="C96" s="4">
-        <v>40388</v>
+        <v>38140</v>
       </c>
       <c r="D96" s="4">
         <f t="shared" si="2"/>
@@ -1858,13 +1879,13 @@
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="4" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="B97" s="4">
-        <v>40726</v>
+        <v>38278</v>
       </c>
       <c r="C97" s="4">
-        <v>40726</v>
+        <v>38278</v>
       </c>
       <c r="D97" s="4">
         <f t="shared" si="2"/>
@@ -1873,13 +1894,13 @@
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="4" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="B98" s="4">
-        <v>40827</v>
+        <v>38479</v>
       </c>
       <c r="C98" s="4">
-        <v>40827</v>
+        <v>38479</v>
       </c>
       <c r="D98" s="4">
         <f t="shared" si="2"/>
@@ -1888,36 +1909,43 @@
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="4" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="B99" s="4">
-        <v>41030</v>
+        <v>38618</v>
       </c>
       <c r="C99" s="4">
-        <v>41030</v>
+        <v>38618</v>
       </c>
       <c r="D99" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="18.75">
-      <c r="A100" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="B100" s="10"/>
-      <c r="C100" s="10"/>
-      <c r="D100" s="10"/>
+    <row r="100" spans="1:5">
+      <c r="A100" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B100" s="4">
+        <v>40024</v>
+      </c>
+      <c r="C100" s="4">
+        <v>40024</v>
+      </c>
+      <c r="D100" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="4" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="B101" s="4">
-        <v>41280</v>
+        <v>40214</v>
       </c>
       <c r="C101" s="4">
-        <v>41280</v>
+        <v>40214</v>
       </c>
       <c r="D101" s="4">
         <f t="shared" si="2"/>
@@ -1929,10 +1957,10 @@
         <v>19</v>
       </c>
       <c r="B102" s="4">
-        <v>42038</v>
+        <v>40388</v>
       </c>
       <c r="C102" s="4">
-        <v>42038</v>
+        <v>40388</v>
       </c>
       <c r="D102" s="4">
         <f t="shared" si="2"/>
@@ -1944,10 +1972,10 @@
         <v>19</v>
       </c>
       <c r="B103" s="4">
-        <v>42649</v>
+        <v>40726</v>
       </c>
       <c r="C103" s="4">
-        <v>42649</v>
+        <v>40726</v>
       </c>
       <c r="D103" s="4">
         <f t="shared" si="2"/>
@@ -1956,13 +1984,13 @@
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="4" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B104" s="4">
-        <v>43208</v>
+        <v>40827</v>
       </c>
       <c r="C104" s="4">
-        <v>43208</v>
+        <v>40827</v>
       </c>
       <c r="D104" s="4">
         <f t="shared" si="2"/>
@@ -1971,46 +1999,36 @@
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="4" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="B105" s="4">
-        <v>43493</v>
+        <v>41030</v>
       </c>
       <c r="C105" s="4">
-        <v>43493</v>
+        <v>41030</v>
       </c>
       <c r="D105" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E105" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5">
-      <c r="A106" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B106" s="4">
-        <v>43763</v>
-      </c>
-      <c r="C106" s="4">
-        <v>43763</v>
-      </c>
-      <c r="D106" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
+    </row>
+    <row r="106" spans="1:5" ht="18.75">
+      <c r="A106" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B106" s="10"/>
+      <c r="C106" s="10"/>
+      <c r="D106" s="10"/>
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="4" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="B107" s="4">
-        <v>44050</v>
+        <v>41280</v>
       </c>
       <c r="C107" s="4">
-        <v>44050</v>
+        <v>41280</v>
       </c>
       <c r="D107" s="4">
         <f t="shared" si="2"/>
@@ -2019,36 +2037,43 @@
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="4" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="B108" s="4">
-        <v>44254</v>
+        <v>42038</v>
       </c>
       <c r="C108" s="4">
-        <v>44254</v>
+        <v>42038</v>
       </c>
       <c r="D108" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:5" ht="18.75">
-      <c r="A109" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="B109" s="12"/>
-      <c r="C109" s="12"/>
-      <c r="D109" s="12"/>
+    <row r="109" spans="1:5">
+      <c r="A109" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B109" s="4">
+        <v>42649</v>
+      </c>
+      <c r="C109" s="4">
+        <v>42649</v>
+      </c>
+      <c r="D109" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="4" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="B110" s="4">
-        <v>44504</v>
+        <v>43208</v>
       </c>
       <c r="C110" s="4">
-        <v>44504</v>
+        <v>43208</v>
       </c>
       <c r="D110" s="4">
         <f t="shared" si="2"/>
@@ -2057,28 +2082,31 @@
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="4" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B111" s="4">
-        <v>46191</v>
+        <v>43493</v>
       </c>
       <c r="C111" s="4">
-        <v>46191</v>
+        <v>43493</v>
       </c>
       <c r="D111" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
+      </c>
+      <c r="E111" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="4" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="B112" s="4">
-        <v>48585</v>
+        <v>43763</v>
       </c>
       <c r="C112" s="4">
-        <v>48585</v>
+        <v>43763</v>
       </c>
       <c r="D112" s="4">
         <f t="shared" si="2"/>
@@ -2090,10 +2118,10 @@
         <v>27</v>
       </c>
       <c r="B113" s="4">
-        <v>48941</v>
+        <v>44050</v>
       </c>
       <c r="C113" s="4">
-        <v>48941</v>
+        <v>44050</v>
       </c>
       <c r="D113" s="4">
         <f t="shared" si="2"/>
@@ -2105,10 +2133,10 @@
         <v>34</v>
       </c>
       <c r="B114" s="4">
-        <v>49144</v>
+        <v>44254</v>
       </c>
       <c r="C114" s="4">
-        <v>49144</v>
+        <v>44254</v>
       </c>
       <c r="D114" s="4">
         <f t="shared" si="2"/>
@@ -2116,22 +2144,22 @@
       </c>
     </row>
     <row r="115" spans="1:4" ht="18.75">
-      <c r="A115" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="B115" s="10"/>
-      <c r="C115" s="10"/>
-      <c r="D115" s="10"/>
+      <c r="A115" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B115" s="12"/>
+      <c r="C115" s="12"/>
+      <c r="D115" s="12"/>
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B116" s="4">
-        <v>49395</v>
+        <v>44504</v>
       </c>
       <c r="C116" s="4">
-        <v>49395</v>
+        <v>44504</v>
       </c>
       <c r="D116" s="4">
         <f t="shared" si="2"/>
@@ -2140,13 +2168,13 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="4" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="B117" s="4">
-        <v>49704</v>
+        <v>46191</v>
       </c>
       <c r="C117" s="4">
-        <v>49704</v>
+        <v>46191</v>
       </c>
       <c r="D117" s="4">
         <f t="shared" si="2"/>
@@ -2155,13 +2183,13 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="4" t="s">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="B118" s="4">
-        <v>49883</v>
+        <v>48585</v>
       </c>
       <c r="C118" s="4">
-        <v>49883</v>
+        <v>48585</v>
       </c>
       <c r="D118" s="4">
         <f t="shared" si="2"/>
@@ -2170,13 +2198,13 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="4" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B119" s="4">
-        <v>50088</v>
+        <v>48941</v>
       </c>
       <c r="C119" s="4">
-        <v>50088</v>
+        <v>48941</v>
       </c>
       <c r="D119" s="4">
         <f t="shared" si="2"/>
@@ -2185,43 +2213,36 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="4" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="B120" s="4">
-        <v>50263</v>
+        <v>49144</v>
       </c>
       <c r="C120" s="4">
-        <v>50263</v>
+        <v>49144</v>
       </c>
       <c r="D120" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:4">
-      <c r="A121" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B121" s="4">
-        <v>50566</v>
-      </c>
-      <c r="C121" s="4">
-        <v>50566</v>
-      </c>
-      <c r="D121" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
+    <row r="121" spans="1:4" ht="18.75">
+      <c r="A121" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B121" s="10"/>
+      <c r="C121" s="10"/>
+      <c r="D121" s="10"/>
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="4" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="B122" s="4">
-        <v>50734</v>
+        <v>49395</v>
       </c>
       <c r="C122" s="4">
-        <v>50734</v>
+        <v>49395</v>
       </c>
       <c r="D122" s="4">
         <f t="shared" si="2"/>
@@ -2230,13 +2251,13 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="4" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="B123" s="4">
-        <v>50849</v>
+        <v>49704</v>
       </c>
       <c r="C123" s="4">
-        <v>50849</v>
+        <v>49704</v>
       </c>
       <c r="D123" s="4">
         <f t="shared" si="2"/>
@@ -2245,13 +2266,13 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="4" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="B124" s="4">
-        <v>51176</v>
+        <v>49883</v>
       </c>
       <c r="C124" s="4">
-        <v>51176</v>
+        <v>49883</v>
       </c>
       <c r="D124" s="4">
         <f t="shared" si="2"/>
@@ -2260,13 +2281,13 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="4" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B125" s="4">
-        <v>51327</v>
+        <v>50088</v>
       </c>
       <c r="C125" s="4">
-        <v>51327</v>
+        <v>50088</v>
       </c>
       <c r="D125" s="4">
         <f t="shared" si="2"/>
@@ -2275,13 +2296,13 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B126" s="4">
-        <v>51577</v>
+        <v>50263</v>
       </c>
       <c r="C126" s="4">
-        <v>51577</v>
+        <v>50263</v>
       </c>
       <c r="D126" s="4">
         <f t="shared" si="2"/>
@@ -2290,13 +2311,13 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="4" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="B127" s="4">
-        <v>51868</v>
+        <v>50566</v>
       </c>
       <c r="C127" s="4">
-        <v>51868</v>
+        <v>50566</v>
       </c>
       <c r="D127" s="4">
         <f t="shared" si="2"/>
@@ -2305,36 +2326,43 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="4" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="B128" s="4">
-        <v>52071</v>
+        <v>50734</v>
       </c>
       <c r="C128" s="4">
-        <v>52071</v>
+        <v>50734</v>
       </c>
       <c r="D128" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="18.75">
-      <c r="A129" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="B129" s="12"/>
-      <c r="C129" s="12"/>
-      <c r="D129" s="12"/>
+    <row r="129" spans="1:4">
+      <c r="A129" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B129" s="4">
+        <v>50849</v>
+      </c>
+      <c r="C129" s="4">
+        <v>50849</v>
+      </c>
+      <c r="D129" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B130" s="4">
-        <v>52322</v>
+        <v>51176</v>
       </c>
       <c r="C130" s="4">
-        <v>52322</v>
+        <v>51176</v>
       </c>
       <c r="D130" s="4">
         <f t="shared" si="2"/>
@@ -2343,13 +2371,13 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="4" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="B131" s="4">
-        <v>53245</v>
+        <v>51327</v>
       </c>
       <c r="C131" s="4">
-        <v>53245</v>
+        <v>51327</v>
       </c>
       <c r="D131" s="4">
         <f t="shared" si="2"/>
@@ -2358,13 +2386,13 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="4" t="s">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="B132" s="4">
-        <v>55063</v>
+        <v>51577</v>
       </c>
       <c r="C132" s="4">
-        <v>55063</v>
+        <v>51577</v>
       </c>
       <c r="D132" s="4">
         <f t="shared" si="2"/>
@@ -2373,13 +2401,13 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="4" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="B133" s="4">
-        <v>55385</v>
+        <v>51868</v>
       </c>
       <c r="C133" s="4">
-        <v>55385</v>
+        <v>51868</v>
       </c>
       <c r="D133" s="4">
         <f t="shared" si="2"/>
@@ -2388,43 +2416,36 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="4" t="s">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="B134" s="4">
-        <v>55706</v>
+        <v>52071</v>
       </c>
       <c r="C134" s="4">
-        <v>55706</v>
+        <v>52071</v>
       </c>
       <c r="D134" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:4">
-      <c r="A135" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B135" s="4">
-        <v>56029</v>
-      </c>
-      <c r="C135" s="4">
-        <v>56029</v>
-      </c>
-      <c r="D135" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
+    <row r="135" spans="1:4" ht="18.75">
+      <c r="A135" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B135" s="12"/>
+      <c r="C135" s="12"/>
+      <c r="D135" s="12"/>
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="4" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B136" s="4">
-        <v>58292</v>
+        <v>52322</v>
       </c>
       <c r="C136" s="4">
-        <v>58292</v>
+        <v>52322</v>
       </c>
       <c r="D136" s="4">
         <f t="shared" si="2"/>
@@ -2433,27 +2454,117 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B137" s="4">
+        <v>53245</v>
+      </c>
+      <c r="C137" s="4">
+        <v>53245</v>
+      </c>
+      <c r="D137" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4">
+      <c r="A138" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B138" s="4">
+        <v>55063</v>
+      </c>
+      <c r="C138" s="4">
+        <v>55063</v>
+      </c>
+      <c r="D138" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4">
+      <c r="A139" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B139" s="4">
+        <v>55385</v>
+      </c>
+      <c r="C139" s="4">
+        <v>55385</v>
+      </c>
+      <c r="D139" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4">
+      <c r="A140" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B140" s="4">
+        <v>55706</v>
+      </c>
+      <c r="C140" s="4">
+        <v>55706</v>
+      </c>
+      <c r="D140" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4">
+      <c r="A141" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B141" s="4">
+        <v>56029</v>
+      </c>
+      <c r="C141" s="4">
+        <v>56029</v>
+      </c>
+      <c r="D141" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4">
+      <c r="A142" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B142" s="4">
+        <v>58292</v>
+      </c>
+      <c r="C142" s="4">
+        <v>58292</v>
+      </c>
+      <c r="D142" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4">
+      <c r="A143" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B137" s="9">
+      <c r="B143" s="9">
         <v>0.71250000000000002</v>
       </c>
-      <c r="C137" s="9">
+      <c r="C143" s="9">
         <v>0.71250000000000002</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A109:D109"/>
     <mergeCell ref="A115:D115"/>
-    <mergeCell ref="A129:D129"/>
-    <mergeCell ref="A44:D44"/>
-    <mergeCell ref="A57:D57"/>
-    <mergeCell ref="A68:D68"/>
-    <mergeCell ref="A73:D73"/>
-    <mergeCell ref="A78:D78"/>
-    <mergeCell ref="A100:D100"/>
-    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="A121:D121"/>
+    <mergeCell ref="A135:D135"/>
+    <mergeCell ref="A50:D50"/>
+    <mergeCell ref="A63:D63"/>
+    <mergeCell ref="A74:D74"/>
+    <mergeCell ref="A79:D79"/>
+    <mergeCell ref="A84:D84"/>
+    <mergeCell ref="A106:D106"/>
+    <mergeCell ref="A43:D43"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="A10:D10"/>

</xml_diff>

<commit_message>
Wario - Level 6 begin
</commit_message>
<xml_diff>
--- a/Wario/Wario.xlsx
+++ b/Wario/Wario.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="69">
   <si>
     <t>Enter pipe</t>
   </si>
@@ -219,6 +219,9 @@
   </si>
   <si>
     <t>Black Screen</t>
+  </si>
+  <si>
+    <t>Leave Level 5</t>
   </si>
 </sst>
 </file>
@@ -623,11 +626,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J143"/>
+  <dimension ref="A1:J144"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B45" sqref="B45"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -756,7 +759,7 @@
         <v>3962</v>
       </c>
       <c r="D12" s="4">
-        <f t="shared" ref="D12:D83" si="1">IF(B12 &gt;  0,C12-B12, 0)</f>
+        <f t="shared" ref="D12:D84" si="1">IF(B12 &gt;  0,C12-B12, 0)</f>
         <v>603</v>
       </c>
     </row>
@@ -1223,100 +1226,121 @@
       <c r="A45" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="B45" s="4">
+        <v>15841</v>
+      </c>
       <c r="C45" s="4">
         <v>17223</v>
       </c>
       <c r="D45" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="B46" s="4">
+        <v>16245</v>
+      </c>
       <c r="C46" s="4">
         <v>17684</v>
       </c>
       <c r="D46" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1439</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="B47" s="4">
+        <v>16760</v>
+      </c>
       <c r="C47" s="4">
         <v>18205</v>
       </c>
       <c r="D47" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="B48" s="4">
+        <v>16939</v>
+      </c>
       <c r="C48" s="4">
         <v>18401</v>
       </c>
       <c r="D48" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="49" spans="1:10">
       <c r="A49" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="B49" s="4">
+        <v>17105</v>
+      </c>
       <c r="C49" s="4">
         <v>18597</v>
       </c>
       <c r="D49" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" ht="18.75">
-      <c r="A50" s="12" t="s">
+        <f t="shared" ref="D49" si="2">IF(B49 &gt;  0,C49-B49, 0)</f>
+        <v>1492</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="A50" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B50" s="4">
+        <v>17309</v>
+      </c>
+      <c r="C50" s="4">
+        <v>18801</v>
+      </c>
+      <c r="D50" s="4">
+        <f t="shared" si="1"/>
+        <v>1492</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="18.75">
+      <c r="A51" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B50" s="12"/>
-      <c r="C50" s="12"/>
-      <c r="D50" s="12"/>
-    </row>
-    <row r="51" spans="1:10">
-      <c r="A51" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C51" s="4">
-        <v>19052</v>
-      </c>
-      <c r="D51" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="B51" s="12"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="12"/>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="4" t="s">
-        <v>19</v>
+        <v>31</v>
+      </c>
+      <c r="B52" s="4">
+        <v>17558</v>
       </c>
       <c r="C52" s="4">
-        <v>19925</v>
+        <v>19052</v>
       </c>
       <c r="D52" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="53" spans="1:10">
       <c r="A53" s="4" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C53" s="4">
-        <v>20355</v>
+        <v>19925</v>
       </c>
       <c r="D53" s="4">
         <f t="shared" si="1"/>
@@ -1325,52 +1349,52 @@
     </row>
     <row r="54" spans="1:10">
       <c r="A54" s="4" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C54" s="4">
-        <v>20623</v>
+        <v>20355</v>
       </c>
       <c r="D54" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F54" s="6"/>
-      <c r="H54" s="6"/>
-      <c r="J54" s="6"/>
     </row>
     <row r="55" spans="1:10">
       <c r="A55" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C55" s="4">
-        <v>20765</v>
+        <v>20623</v>
       </c>
       <c r="D55" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F55" s="7"/>
-      <c r="H55" s="7"/>
-      <c r="J55" s="7"/>
+      <c r="F55" s="6"/>
+      <c r="H55" s="6"/>
+      <c r="J55" s="6"/>
     </row>
     <row r="56" spans="1:10">
       <c r="A56" s="4" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="C56" s="4">
-        <v>20978</v>
+        <v>20765</v>
       </c>
       <c r="D56" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="F56" s="7"/>
+      <c r="H56" s="7"/>
+      <c r="J56" s="7"/>
     </row>
     <row r="57" spans="1:10">
       <c r="A57" s="4" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="C57" s="4">
-        <v>21288</v>
+        <v>20978</v>
       </c>
       <c r="D57" s="4">
         <f t="shared" si="1"/>
@@ -1382,7 +1406,7 @@
         <v>7</v>
       </c>
       <c r="C58" s="4">
-        <v>21900</v>
+        <v>21288</v>
       </c>
       <c r="D58" s="4">
         <f t="shared" si="1"/>
@@ -1394,7 +1418,7 @@
         <v>7</v>
       </c>
       <c r="C59" s="4">
-        <v>22268</v>
+        <v>21900</v>
       </c>
       <c r="D59" s="4">
         <f t="shared" si="1"/>
@@ -1406,7 +1430,7 @@
         <v>7</v>
       </c>
       <c r="C60" s="4">
-        <v>22486</v>
+        <v>22268</v>
       </c>
       <c r="D60" s="4">
         <f t="shared" si="1"/>
@@ -1415,10 +1439,10 @@
     </row>
     <row r="61" spans="1:10">
       <c r="A61" s="4" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="C61" s="4">
-        <v>22606</v>
+        <v>22486</v>
       </c>
       <c r="D61" s="4">
         <f t="shared" si="1"/>
@@ -1427,42 +1451,42 @@
     </row>
     <row r="62" spans="1:10">
       <c r="A62" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C62" s="4">
+        <v>22606</v>
+      </c>
+      <c r="D62" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
+      <c r="A63" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C62" s="4">
+      <c r="C63" s="4">
         <v>22810</v>
       </c>
-      <c r="D62" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" ht="18.75">
-      <c r="A63" s="10" t="s">
+      <c r="D63" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="18.75">
+      <c r="A64" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B63" s="10"/>
-      <c r="C63" s="10"/>
-      <c r="D63" s="10"/>
-    </row>
-    <row r="64" spans="1:10">
-      <c r="A64" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C64" s="4">
-        <v>23060</v>
-      </c>
-      <c r="D64" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="B64" s="10"/>
+      <c r="C64" s="10"/>
+      <c r="D64" s="10"/>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="4" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="C65" s="4">
-        <v>24356</v>
+        <v>23060</v>
       </c>
       <c r="D65" s="4">
         <f t="shared" si="1"/>
@@ -1474,7 +1498,7 @@
         <v>6</v>
       </c>
       <c r="C66" s="4">
-        <v>24520</v>
+        <v>24356</v>
       </c>
       <c r="D66" s="4">
         <f t="shared" si="1"/>
@@ -1483,10 +1507,10 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C67" s="4">
-        <v>24693</v>
+        <v>24520</v>
       </c>
       <c r="D67" s="4">
         <f t="shared" si="1"/>
@@ -1495,10 +1519,10 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="4" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C68" s="4">
-        <v>25030</v>
+        <v>24693</v>
       </c>
       <c r="D68" s="4">
         <f t="shared" si="1"/>
@@ -1507,10 +1531,10 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="4" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C69" s="4">
-        <v>25625</v>
+        <v>25030</v>
       </c>
       <c r="D69" s="4">
         <f t="shared" si="1"/>
@@ -1522,7 +1546,7 @@
         <v>7</v>
       </c>
       <c r="C70" s="4">
-        <v>26130</v>
+        <v>25625</v>
       </c>
       <c r="D70" s="4">
         <f t="shared" si="1"/>
@@ -1534,7 +1558,7 @@
         <v>7</v>
       </c>
       <c r="C71" s="4">
-        <v>26299</v>
+        <v>26130</v>
       </c>
       <c r="D71" s="4">
         <f t="shared" si="1"/>
@@ -1543,10 +1567,10 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="4" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="C72" s="4">
-        <v>26404</v>
+        <v>26299</v>
       </c>
       <c r="D72" s="4">
         <f t="shared" si="1"/>
@@ -1555,54 +1579,54 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C73" s="4">
+        <v>26404</v>
+      </c>
+      <c r="D73" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C73" s="4">
+      <c r="C74" s="4">
         <v>26607</v>
       </c>
-      <c r="D73" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" ht="18.75">
-      <c r="A74" s="12" t="s">
+      <c r="D74" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="18.75">
+      <c r="A75" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B74" s="12"/>
-      <c r="C74" s="12"/>
-      <c r="D74" s="12"/>
-    </row>
-    <row r="75" spans="1:4">
-      <c r="A75" s="4" t="s">
+      <c r="B75" s="12"/>
+      <c r="C75" s="12"/>
+      <c r="D75" s="12"/>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C75" s="4">
+      <c r="C76" s="4">
         <v>26858</v>
       </c>
-      <c r="D75" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4">
-      <c r="A76" s="8" t="s">
+      <c r="D76" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C76" s="4">
+      <c r="C77" s="4">
         <v>28167</v>
-      </c>
-      <c r="D76" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4">
-      <c r="A77" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C77" s="4">
-        <v>32142</v>
       </c>
       <c r="D77" s="4">
         <f t="shared" si="1"/>
@@ -1611,48 +1635,45 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C78" s="4">
+        <v>32142</v>
+      </c>
+      <c r="D78" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C78" s="4">
+      <c r="C79" s="4">
         <v>32671</v>
       </c>
-      <c r="D78" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" ht="18.75">
-      <c r="A79" s="10" t="s">
+      <c r="D79" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="18.75">
+      <c r="A80" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B79" s="10"/>
-      <c r="C79" s="10"/>
-      <c r="D79" s="10"/>
-    </row>
-    <row r="80" spans="1:4">
-      <c r="A80" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B80" s="4">
-        <v>32921</v>
-      </c>
-      <c r="C80" s="4">
-        <v>32921</v>
-      </c>
-      <c r="D80" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="B80" s="10"/>
+      <c r="C80" s="10"/>
+      <c r="D80" s="10"/>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="4" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="B81" s="4">
-        <v>34723</v>
+        <v>32921</v>
       </c>
       <c r="C81" s="4">
-        <v>34723</v>
+        <v>32921</v>
       </c>
       <c r="D81" s="4">
         <f t="shared" si="1"/>
@@ -1661,13 +1682,13 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="4" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B82" s="4">
-        <v>35373</v>
+        <v>34723</v>
       </c>
       <c r="C82" s="4">
-        <v>35373</v>
+        <v>34723</v>
       </c>
       <c r="D82" s="4">
         <f t="shared" si="1"/>
@@ -1676,54 +1697,54 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B83" s="4">
+        <v>35373</v>
+      </c>
+      <c r="C83" s="4">
+        <v>35373</v>
+      </c>
+      <c r="D83" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B83" s="4">
+      <c r="B84" s="4">
         <v>35577</v>
       </c>
-      <c r="C83" s="4">
+      <c r="C84" s="4">
         <v>35577</v>
       </c>
-      <c r="D83" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" ht="18.75">
-      <c r="A84" s="12" t="s">
+      <c r="D84" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="18.75">
+      <c r="A85" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B84" s="12"/>
-      <c r="C84" s="12"/>
-      <c r="D84" s="12"/>
-    </row>
-    <row r="85" spans="1:4">
-      <c r="A85" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B85" s="4">
-        <v>35826</v>
-      </c>
-      <c r="C85" s="4">
-        <v>35826</v>
-      </c>
-      <c r="D85" s="4">
-        <f t="shared" ref="D85:D142" si="2">IF(B85 &gt;  0,C85-B85, 0)</f>
-        <v>0</v>
-      </c>
+      <c r="B85" s="12"/>
+      <c r="C85" s="12"/>
+      <c r="D85" s="12"/>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B86" s="4">
-        <v>36033</v>
+        <v>35826</v>
       </c>
       <c r="C86" s="4">
-        <v>36033</v>
+        <v>35826</v>
       </c>
       <c r="D86" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="D86:D143" si="3">IF(B86 &gt;  0,C86-B86, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1732,13 +1753,13 @@
         <v>45</v>
       </c>
       <c r="B87" s="4">
-        <v>36201</v>
+        <v>36033</v>
       </c>
       <c r="C87" s="4">
-        <v>36201</v>
+        <v>36033</v>
       </c>
       <c r="D87" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -1747,13 +1768,13 @@
         <v>45</v>
       </c>
       <c r="B88" s="4">
-        <v>36370</v>
+        <v>36201</v>
       </c>
       <c r="C88" s="4">
-        <v>36370</v>
+        <v>36201</v>
       </c>
       <c r="D88" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -1762,73 +1783,73 @@
         <v>45</v>
       </c>
       <c r="B89" s="4">
-        <v>36538</v>
+        <v>36370</v>
       </c>
       <c r="C89" s="4">
-        <v>36538</v>
+        <v>36370</v>
       </c>
       <c r="D89" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B90" s="4">
-        <v>36744</v>
+        <v>36538</v>
       </c>
       <c r="C90" s="4">
-        <v>36744</v>
+        <v>36538</v>
       </c>
       <c r="D90" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B91" s="4">
-        <v>37194</v>
+        <v>36744</v>
       </c>
       <c r="C91" s="4">
-        <v>37194</v>
+        <v>36744</v>
       </c>
       <c r="D91" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="4" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="B92" s="4">
-        <v>37481</v>
+        <v>37194</v>
       </c>
       <c r="C92" s="4">
-        <v>37481</v>
+        <v>37194</v>
       </c>
       <c r="D92" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="4" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B93" s="4">
-        <v>37662</v>
+        <v>37481</v>
       </c>
       <c r="C93" s="4">
-        <v>37662</v>
+        <v>37481</v>
       </c>
       <c r="D93" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -1837,13 +1858,13 @@
         <v>6</v>
       </c>
       <c r="B94" s="4">
-        <v>37816</v>
+        <v>37662</v>
       </c>
       <c r="C94" s="4">
-        <v>37816</v>
+        <v>37662</v>
       </c>
       <c r="D94" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -1852,13 +1873,13 @@
         <v>6</v>
       </c>
       <c r="B95" s="4">
-        <v>37986</v>
+        <v>37816</v>
       </c>
       <c r="C95" s="4">
-        <v>37986</v>
+        <v>37816</v>
       </c>
       <c r="D95" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -1867,13 +1888,13 @@
         <v>6</v>
       </c>
       <c r="B96" s="4">
-        <v>38140</v>
+        <v>37986</v>
       </c>
       <c r="C96" s="4">
-        <v>38140</v>
+        <v>37986</v>
       </c>
       <c r="D96" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -1882,13 +1903,13 @@
         <v>6</v>
       </c>
       <c r="B97" s="4">
-        <v>38278</v>
+        <v>38140</v>
       </c>
       <c r="C97" s="4">
-        <v>38278</v>
+        <v>38140</v>
       </c>
       <c r="D97" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -1897,13 +1918,13 @@
         <v>6</v>
       </c>
       <c r="B98" s="4">
-        <v>38479</v>
+        <v>38278</v>
       </c>
       <c r="C98" s="4">
-        <v>38479</v>
+        <v>38278</v>
       </c>
       <c r="D98" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -1912,58 +1933,58 @@
         <v>6</v>
       </c>
       <c r="B99" s="4">
-        <v>38618</v>
+        <v>38479</v>
       </c>
       <c r="C99" s="4">
-        <v>38618</v>
+        <v>38479</v>
       </c>
       <c r="D99" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:5">
       <c r="A100" s="4" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="B100" s="4">
-        <v>40024</v>
+        <v>38618</v>
       </c>
       <c r="C100" s="4">
-        <v>40024</v>
+        <v>38618</v>
       </c>
       <c r="D100" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="4" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B101" s="4">
-        <v>40214</v>
+        <v>40024</v>
       </c>
       <c r="C101" s="4">
-        <v>40214</v>
+        <v>40024</v>
       </c>
       <c r="D101" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="4" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="B102" s="4">
-        <v>40388</v>
+        <v>40214</v>
       </c>
       <c r="C102" s="4">
-        <v>40388</v>
+        <v>40214</v>
       </c>
       <c r="D102" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -1972,81 +1993,81 @@
         <v>19</v>
       </c>
       <c r="B103" s="4">
-        <v>40726</v>
+        <v>40388</v>
       </c>
       <c r="C103" s="4">
-        <v>40726</v>
+        <v>40388</v>
       </c>
       <c r="D103" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="4" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B104" s="4">
-        <v>40827</v>
+        <v>40726</v>
       </c>
       <c r="C104" s="4">
-        <v>40827</v>
+        <v>40726</v>
       </c>
       <c r="D104" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B105" s="4">
+        <v>40827</v>
+      </c>
+      <c r="C105" s="4">
+        <v>40827</v>
+      </c>
+      <c r="D105" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
+      <c r="A106" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B105" s="4">
+      <c r="B106" s="4">
         <v>41030</v>
       </c>
-      <c r="C105" s="4">
+      <c r="C106" s="4">
         <v>41030</v>
       </c>
-      <c r="D105" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" ht="18.75">
-      <c r="A106" s="10" t="s">
+      <c r="D106" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="18.75">
+      <c r="A107" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="B106" s="10"/>
-      <c r="C106" s="10"/>
-      <c r="D106" s="10"/>
-    </row>
-    <row r="107" spans="1:5">
-      <c r="A107" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B107" s="4">
-        <v>41280</v>
-      </c>
-      <c r="C107" s="4">
-        <v>41280</v>
-      </c>
-      <c r="D107" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
+      <c r="B107" s="10"/>
+      <c r="C107" s="10"/>
+      <c r="D107" s="10"/>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="4" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="B108" s="4">
-        <v>42038</v>
+        <v>41280</v>
       </c>
       <c r="C108" s="4">
-        <v>42038</v>
+        <v>41280</v>
       </c>
       <c r="D108" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -2055,13 +2076,13 @@
         <v>19</v>
       </c>
       <c r="B109" s="4">
-        <v>42649</v>
+        <v>42038</v>
       </c>
       <c r="C109" s="4">
-        <v>42649</v>
+        <v>42038</v>
       </c>
       <c r="D109" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -2070,317 +2091,317 @@
         <v>19</v>
       </c>
       <c r="B110" s="4">
-        <v>43208</v>
+        <v>42649</v>
       </c>
       <c r="C110" s="4">
-        <v>43208</v>
+        <v>42649</v>
       </c>
       <c r="D110" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B111" s="4">
-        <v>43493</v>
+        <v>43208</v>
       </c>
       <c r="C111" s="4">
-        <v>43493</v>
+        <v>43208</v>
       </c>
       <c r="D111" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E111" t="s">
-        <v>50</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B112" s="4">
-        <v>43763</v>
+        <v>43493</v>
       </c>
       <c r="C112" s="4">
-        <v>43763</v>
+        <v>43493</v>
       </c>
       <c r="D112" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E112" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="4" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B113" s="4">
-        <v>44050</v>
+        <v>43763</v>
       </c>
       <c r="C113" s="4">
-        <v>44050</v>
+        <v>43763</v>
       </c>
       <c r="D113" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B114" s="4">
+        <v>44050</v>
+      </c>
+      <c r="C114" s="4">
+        <v>44050</v>
+      </c>
+      <c r="D114" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4">
+      <c r="A115" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B114" s="4">
+      <c r="B115" s="4">
         <v>44254</v>
       </c>
-      <c r="C114" s="4">
+      <c r="C115" s="4">
         <v>44254</v>
       </c>
-      <c r="D114" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" ht="18.75">
-      <c r="A115" s="12" t="s">
+      <c r="D115" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="18.75">
+      <c r="A116" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B115" s="12"/>
-      <c r="C115" s="12"/>
-      <c r="D115" s="12"/>
-    </row>
-    <row r="116" spans="1:4">
-      <c r="A116" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B116" s="4">
-        <v>44504</v>
-      </c>
-      <c r="C116" s="4">
-        <v>44504</v>
-      </c>
-      <c r="D116" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
+      <c r="B116" s="12"/>
+      <c r="C116" s="12"/>
+      <c r="D116" s="12"/>
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="4" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="B117" s="4">
-        <v>46191</v>
+        <v>44504</v>
       </c>
       <c r="C117" s="4">
-        <v>46191</v>
+        <v>44504</v>
       </c>
       <c r="D117" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="4" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="B118" s="4">
-        <v>48585</v>
+        <v>46191</v>
       </c>
       <c r="C118" s="4">
-        <v>48585</v>
+        <v>46191</v>
       </c>
       <c r="D118" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="4" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="B119" s="4">
-        <v>48941</v>
+        <v>48585</v>
       </c>
       <c r="C119" s="4">
-        <v>48941</v>
+        <v>48585</v>
       </c>
       <c r="D119" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B120" s="4">
+        <v>48941</v>
+      </c>
+      <c r="C120" s="4">
+        <v>48941</v>
+      </c>
+      <c r="D120" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
+      <c r="A121" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B120" s="4">
+      <c r="B121" s="4">
         <v>49144</v>
       </c>
-      <c r="C120" s="4">
+      <c r="C121" s="4">
         <v>49144</v>
       </c>
-      <c r="D120" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" ht="18.75">
-      <c r="A121" s="10" t="s">
+      <c r="D121" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" ht="18.75">
+      <c r="A122" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B121" s="10"/>
-      <c r="C121" s="10"/>
-      <c r="D121" s="10"/>
-    </row>
-    <row r="122" spans="1:4">
-      <c r="A122" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B122" s="4">
-        <v>49395</v>
-      </c>
-      <c r="C122" s="4">
-        <v>49395</v>
-      </c>
-      <c r="D122" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
+      <c r="B122" s="10"/>
+      <c r="C122" s="10"/>
+      <c r="D122" s="10"/>
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B123" s="4">
-        <v>49704</v>
+        <v>49395</v>
       </c>
       <c r="C123" s="4">
-        <v>49704</v>
+        <v>49395</v>
       </c>
       <c r="D123" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="4" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="B124" s="4">
-        <v>49883</v>
+        <v>49704</v>
       </c>
       <c r="C124" s="4">
-        <v>49883</v>
+        <v>49704</v>
       </c>
       <c r="D124" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B125" s="4">
-        <v>50088</v>
+        <v>49883</v>
       </c>
       <c r="C125" s="4">
-        <v>50088</v>
+        <v>49883</v>
       </c>
       <c r="D125" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="4" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="B126" s="4">
-        <v>50263</v>
+        <v>50088</v>
       </c>
       <c r="C126" s="4">
-        <v>50263</v>
+        <v>50088</v>
       </c>
       <c r="D126" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B127" s="4">
-        <v>50566</v>
+        <v>50263</v>
       </c>
       <c r="C127" s="4">
-        <v>50566</v>
+        <v>50263</v>
       </c>
       <c r="D127" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B128" s="4">
-        <v>50734</v>
+        <v>50566</v>
       </c>
       <c r="C128" s="4">
-        <v>50734</v>
+        <v>50566</v>
       </c>
       <c r="D128" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="4" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B129" s="4">
-        <v>50849</v>
+        <v>50734</v>
       </c>
       <c r="C129" s="4">
-        <v>50849</v>
+        <v>50734</v>
       </c>
       <c r="D129" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="4" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="B130" s="4">
-        <v>51176</v>
+        <v>50849</v>
       </c>
       <c r="C130" s="4">
-        <v>51176</v>
+        <v>50849</v>
       </c>
       <c r="D130" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="4" t="s">
-        <v>6</v>
+        <v>57</v>
       </c>
       <c r="B131" s="4">
-        <v>51327</v>
+        <v>51176</v>
       </c>
       <c r="C131" s="4">
-        <v>51327</v>
+        <v>51176</v>
       </c>
       <c r="D131" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -2389,181 +2410,196 @@
         <v>6</v>
       </c>
       <c r="B132" s="4">
-        <v>51577</v>
+        <v>51327</v>
       </c>
       <c r="C132" s="4">
-        <v>51577</v>
+        <v>51327</v>
       </c>
       <c r="D132" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="4" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="B133" s="4">
-        <v>51868</v>
+        <v>51577</v>
       </c>
       <c r="C133" s="4">
-        <v>51868</v>
+        <v>51577</v>
       </c>
       <c r="D133" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B134" s="4">
+        <v>51868</v>
+      </c>
+      <c r="C134" s="4">
+        <v>51868</v>
+      </c>
+      <c r="D134" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
+      <c r="A135" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B134" s="4">
+      <c r="B135" s="4">
         <v>52071</v>
       </c>
-      <c r="C134" s="4">
+      <c r="C135" s="4">
         <v>52071</v>
       </c>
-      <c r="D134" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" ht="18.75">
-      <c r="A135" s="12" t="s">
+      <c r="D135" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" ht="18.75">
+      <c r="A136" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="B135" s="12"/>
-      <c r="C135" s="12"/>
-      <c r="D135" s="12"/>
-    </row>
-    <row r="136" spans="1:4">
-      <c r="A136" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B136" s="4">
-        <v>52322</v>
-      </c>
-      <c r="C136" s="4">
-        <v>52322</v>
-      </c>
-      <c r="D136" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
+      <c r="B136" s="12"/>
+      <c r="C136" s="12"/>
+      <c r="D136" s="12"/>
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="4" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="B137" s="4">
-        <v>53245</v>
+        <v>52322</v>
       </c>
       <c r="C137" s="4">
-        <v>53245</v>
+        <v>52322</v>
       </c>
       <c r="D137" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="4" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="B138" s="4">
-        <v>55063</v>
+        <v>53245</v>
       </c>
       <c r="C138" s="4">
-        <v>55063</v>
+        <v>53245</v>
       </c>
       <c r="D138" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B139" s="4">
-        <v>55385</v>
+        <v>55063</v>
       </c>
       <c r="C139" s="4">
-        <v>55385</v>
+        <v>55063</v>
       </c>
       <c r="D139" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B140" s="4">
-        <v>55706</v>
+        <v>55385</v>
       </c>
       <c r="C140" s="4">
-        <v>55706</v>
+        <v>55385</v>
       </c>
       <c r="D140" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B141" s="4">
-        <v>56029</v>
+        <v>55706</v>
       </c>
       <c r="C141" s="4">
-        <v>56029</v>
+        <v>55706</v>
       </c>
       <c r="D141" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B142" s="4">
-        <v>58292</v>
+        <v>56029</v>
       </c>
       <c r="C142" s="4">
-        <v>58292</v>
+        <v>56029</v>
       </c>
       <c r="D142" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B143" s="4">
+        <v>58292</v>
+      </c>
+      <c r="C143" s="4">
+        <v>58292</v>
+      </c>
+      <c r="D143" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4">
+      <c r="A144" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B143" s="9">
+      <c r="B144" s="9">
         <v>0.71250000000000002</v>
       </c>
-      <c r="C143" s="9">
+      <c r="C144" s="9">
         <v>0.71250000000000002</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A115:D115"/>
-    <mergeCell ref="A121:D121"/>
-    <mergeCell ref="A135:D135"/>
-    <mergeCell ref="A50:D50"/>
-    <mergeCell ref="A63:D63"/>
-    <mergeCell ref="A74:D74"/>
-    <mergeCell ref="A79:D79"/>
-    <mergeCell ref="A84:D84"/>
-    <mergeCell ref="A106:D106"/>
+    <mergeCell ref="A116:D116"/>
+    <mergeCell ref="A122:D122"/>
+    <mergeCell ref="A136:D136"/>
+    <mergeCell ref="A51:D51"/>
+    <mergeCell ref="A64:D64"/>
+    <mergeCell ref="A75:D75"/>
+    <mergeCell ref="A80:D80"/>
+    <mergeCell ref="A85:D85"/>
+    <mergeCell ref="A107:D107"/>
     <mergeCell ref="A43:D43"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A7:D7"/>

</xml_diff>

<commit_message>
Wario - One more room done (copy/pasted from previous version)
</commit_message>
<xml_diff>
--- a/Wario/Wario.xlsx
+++ b/Wario/Wario.xlsx
@@ -329,9 +329,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -630,7 +630,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B53" sqref="B53"/>
+      <selection pane="bottomLeft" activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -654,12 +654,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -687,12 +687,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -726,12 +726,12 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
@@ -854,12 +854,12 @@
       </c>
     </row>
     <row r="19" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="4" t="s">
@@ -1027,12 +1027,12 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="18.75">
-      <c r="A31" s="12" t="s">
+      <c r="A31" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="4" t="s">
@@ -1200,12 +1200,12 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="18.75">
-      <c r="A43" s="10" t="s">
+      <c r="A43" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B43" s="10"/>
-      <c r="C43" s="10"/>
-      <c r="D43" s="10"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="4" t="s">
@@ -1313,12 +1313,12 @@
       </c>
     </row>
     <row r="51" spans="1:10" ht="18.75">
-      <c r="A51" s="12" t="s">
+      <c r="A51" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B51" s="12"/>
-      <c r="C51" s="12"/>
-      <c r="D51" s="12"/>
+      <c r="B51" s="10"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="4" t="s">
@@ -1339,12 +1339,15 @@
       <c r="A53" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="B53" s="4">
+        <v>18431</v>
+      </c>
       <c r="C53" s="4">
         <v>19925</v>
       </c>
       <c r="D53" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -1474,12 +1477,12 @@
       </c>
     </row>
     <row r="64" spans="1:10" ht="18.75">
-      <c r="A64" s="10" t="s">
+      <c r="A64" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B64" s="10"/>
-      <c r="C64" s="10"/>
-      <c r="D64" s="10"/>
+      <c r="B64" s="11"/>
+      <c r="C64" s="11"/>
+      <c r="D64" s="11"/>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="4" t="s">
@@ -1602,12 +1605,12 @@
       </c>
     </row>
     <row r="75" spans="1:4" ht="18.75">
-      <c r="A75" s="12" t="s">
+      <c r="A75" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B75" s="12"/>
-      <c r="C75" s="12"/>
-      <c r="D75" s="12"/>
+      <c r="B75" s="10"/>
+      <c r="C75" s="10"/>
+      <c r="D75" s="10"/>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="4" t="s">
@@ -1658,12 +1661,12 @@
       </c>
     </row>
     <row r="80" spans="1:4" ht="18.75">
-      <c r="A80" s="10" t="s">
+      <c r="A80" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B80" s="10"/>
-      <c r="C80" s="10"/>
-      <c r="D80" s="10"/>
+      <c r="B80" s="11"/>
+      <c r="C80" s="11"/>
+      <c r="D80" s="11"/>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="4" t="s">
@@ -1726,12 +1729,12 @@
       </c>
     </row>
     <row r="85" spans="1:4" ht="18.75">
-      <c r="A85" s="12" t="s">
+      <c r="A85" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B85" s="12"/>
-      <c r="C85" s="12"/>
-      <c r="D85" s="12"/>
+      <c r="B85" s="10"/>
+      <c r="C85" s="10"/>
+      <c r="D85" s="10"/>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="4" t="s">
@@ -2049,12 +2052,12 @@
       </c>
     </row>
     <row r="107" spans="1:5" ht="18.75">
-      <c r="A107" s="10" t="s">
+      <c r="A107" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B107" s="10"/>
-      <c r="C107" s="10"/>
-      <c r="D107" s="10"/>
+      <c r="B107" s="11"/>
+      <c r="C107" s="11"/>
+      <c r="D107" s="11"/>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="4" t="s">
@@ -2180,12 +2183,12 @@
       </c>
     </row>
     <row r="116" spans="1:4" ht="18.75">
-      <c r="A116" s="12" t="s">
+      <c r="A116" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B116" s="12"/>
-      <c r="C116" s="12"/>
-      <c r="D116" s="12"/>
+      <c r="B116" s="10"/>
+      <c r="C116" s="10"/>
+      <c r="D116" s="10"/>
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="4" t="s">
@@ -2263,12 +2266,12 @@
       </c>
     </row>
     <row r="122" spans="1:4" ht="18.75">
-      <c r="A122" s="10" t="s">
+      <c r="A122" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B122" s="10"/>
-      <c r="C122" s="10"/>
-      <c r="D122" s="10"/>
+      <c r="B122" s="11"/>
+      <c r="C122" s="11"/>
+      <c r="D122" s="11"/>
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="4" t="s">
@@ -2466,12 +2469,12 @@
       </c>
     </row>
     <row r="136" spans="1:4" ht="18.75">
-      <c r="A136" s="12" t="s">
+      <c r="A136" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B136" s="12"/>
-      <c r="C136" s="12"/>
-      <c r="D136" s="12"/>
+      <c r="B136" s="10"/>
+      <c r="C136" s="10"/>
+      <c r="D136" s="10"/>
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="4" t="s">
@@ -2591,6 +2594,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A31:D31"/>
     <mergeCell ref="A116:D116"/>
     <mergeCell ref="A122:D122"/>
     <mergeCell ref="A136:D136"/>
@@ -2600,12 +2609,6 @@
     <mergeCell ref="A80:D80"/>
     <mergeCell ref="A85:D85"/>
     <mergeCell ref="A107:D107"/>
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A31:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -2642,12 +2645,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -2675,12 +2678,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -2714,12 +2717,12 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
@@ -2803,12 +2806,12 @@
       </c>
     </row>
     <row r="17" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="4" t="s">
@@ -2976,12 +2979,12 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="18.75">
-      <c r="A29" s="12" t="s">
+      <c r="A29" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="4" t="s">
@@ -3059,12 +3062,12 @@
       </c>
     </row>
     <row r="35" spans="1:10" ht="18.75">
-      <c r="A35" s="10" t="s">
+      <c r="A35" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="4" t="s">
@@ -3157,12 +3160,12 @@
       </c>
     </row>
     <row r="42" spans="1:10" ht="18.75">
-      <c r="A42" s="12" t="s">
+      <c r="A42" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B42" s="12"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="4" t="s">
@@ -3351,12 +3354,12 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="18.75">
-      <c r="A55" s="10" t="s">
+      <c r="A55" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B55" s="10"/>
-      <c r="C55" s="10"/>
-      <c r="D55" s="10"/>
+      <c r="B55" s="11"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="11"/>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="4" t="s">
@@ -3509,12 +3512,12 @@
       </c>
     </row>
     <row r="66" spans="1:4" ht="18.75">
-      <c r="A66" s="12" t="s">
+      <c r="A66" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B66" s="12"/>
-      <c r="C66" s="12"/>
-      <c r="D66" s="12"/>
+      <c r="B66" s="10"/>
+      <c r="C66" s="10"/>
+      <c r="D66" s="10"/>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="4" t="s">
@@ -3577,12 +3580,12 @@
       </c>
     </row>
     <row r="71" spans="1:4" ht="18.75">
-      <c r="A71" s="10" t="s">
+      <c r="A71" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B71" s="10"/>
-      <c r="C71" s="10"/>
-      <c r="D71" s="10"/>
+      <c r="B71" s="11"/>
+      <c r="C71" s="11"/>
+      <c r="D71" s="11"/>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="4" t="s">
@@ -3645,12 +3648,12 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="18.75">
-      <c r="A76" s="12" t="s">
+      <c r="A76" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B76" s="12"/>
-      <c r="C76" s="12"/>
-      <c r="D76" s="12"/>
+      <c r="B76" s="10"/>
+      <c r="C76" s="10"/>
+      <c r="D76" s="10"/>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="4" t="s">
@@ -3968,12 +3971,12 @@
       </c>
     </row>
     <row r="98" spans="1:5" ht="18.75">
-      <c r="A98" s="10" t="s">
+      <c r="A98" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B98" s="10"/>
-      <c r="C98" s="10"/>
-      <c r="D98" s="10"/>
+      <c r="B98" s="11"/>
+      <c r="C98" s="11"/>
+      <c r="D98" s="11"/>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="4" t="s">
@@ -4099,12 +4102,12 @@
       </c>
     </row>
     <row r="107" spans="1:5" ht="18.75">
-      <c r="A107" s="12" t="s">
+      <c r="A107" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B107" s="12"/>
-      <c r="C107" s="12"/>
-      <c r="D107" s="12"/>
+      <c r="B107" s="10"/>
+      <c r="C107" s="10"/>
+      <c r="D107" s="10"/>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="4" t="s">
@@ -4182,12 +4185,12 @@
       </c>
     </row>
     <row r="113" spans="1:4" ht="18.75">
-      <c r="A113" s="10" t="s">
+      <c r="A113" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B113" s="10"/>
-      <c r="C113" s="10"/>
-      <c r="D113" s="10"/>
+      <c r="B113" s="11"/>
+      <c r="C113" s="11"/>
+      <c r="D113" s="11"/>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="4" t="s">
@@ -4385,12 +4388,12 @@
       </c>
     </row>
     <row r="127" spans="1:4" ht="18.75">
-      <c r="A127" s="12" t="s">
+      <c r="A127" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B127" s="12"/>
-      <c r="C127" s="12"/>
-      <c r="D127" s="12"/>
+      <c r="B127" s="10"/>
+      <c r="C127" s="10"/>
+      <c r="D127" s="10"/>
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="4" t="s">
@@ -4510,11 +4513,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A29:D29"/>
     <mergeCell ref="A127:D127"/>
     <mergeCell ref="A107:D107"/>
     <mergeCell ref="A113:D113"/>
@@ -4525,6 +4523,11 @@
     <mergeCell ref="A98:D98"/>
     <mergeCell ref="A66:D66"/>
     <mergeCell ref="A55:D55"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A29:D29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>

</xml_diff>

<commit_message>
Wario - Level 7 begin
</commit_message>
<xml_diff>
--- a/Wario/Wario.xlsx
+++ b/Wario/Wario.xlsx
@@ -329,9 +329,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -629,8 +629,8 @@
   <dimension ref="A1:J144"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B54" sqref="B54"/>
+      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -654,12 +654,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -687,12 +687,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -726,12 +726,12 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
@@ -854,12 +854,12 @@
       </c>
     </row>
     <row r="19" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="4" t="s">
@@ -1027,12 +1027,12 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="18.75">
-      <c r="A31" s="10" t="s">
+      <c r="A31" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="4" t="s">
@@ -1200,12 +1200,12 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="18.75">
-      <c r="A43" s="11" t="s">
+      <c r="A43" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B43" s="11"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="4" t="s">
@@ -1313,12 +1313,12 @@
       </c>
     </row>
     <row r="51" spans="1:10" ht="18.75">
-      <c r="A51" s="10" t="s">
+      <c r="A51" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B51" s="10"/>
-      <c r="C51" s="10"/>
-      <c r="D51" s="10"/>
+      <c r="B51" s="12"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="12"/>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="4" t="s">
@@ -1354,24 +1354,30 @@
       <c r="A54" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="B54" s="4">
+        <v>18823</v>
+      </c>
       <c r="C54" s="4">
         <v>20355</v>
       </c>
       <c r="D54" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1532</v>
       </c>
     </row>
     <row r="55" spans="1:10">
       <c r="A55" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="B55" s="4">
+        <v>19078</v>
+      </c>
       <c r="C55" s="4">
         <v>20623</v>
       </c>
       <c r="D55" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1545</v>
       </c>
       <c r="F55" s="6"/>
       <c r="H55" s="6"/>
@@ -1396,104 +1402,128 @@
       <c r="A57" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="B57" s="4">
+        <v>19425</v>
+      </c>
       <c r="C57" s="4">
         <v>20978</v>
       </c>
       <c r="D57" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1553</v>
       </c>
     </row>
     <row r="58" spans="1:10">
       <c r="A58" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="B58" s="4">
+        <v>19693</v>
+      </c>
       <c r="C58" s="4">
         <v>21288</v>
       </c>
       <c r="D58" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1595</v>
       </c>
     </row>
     <row r="59" spans="1:10">
       <c r="A59" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="B59" s="4">
+        <v>20164</v>
+      </c>
       <c r="C59" s="4">
         <v>21900</v>
       </c>
       <c r="D59" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1736</v>
       </c>
     </row>
     <row r="60" spans="1:10">
       <c r="A60" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="B60" s="4">
+        <v>20507</v>
+      </c>
       <c r="C60" s="4">
         <v>22268</v>
       </c>
       <c r="D60" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1761</v>
       </c>
     </row>
     <row r="61" spans="1:10">
       <c r="A61" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="B61" s="4">
+        <v>20719</v>
+      </c>
       <c r="C61" s="4">
         <v>22486</v>
       </c>
       <c r="D61" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1767</v>
       </c>
     </row>
     <row r="62" spans="1:10">
       <c r="A62" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="B62" s="4">
+        <v>20839</v>
+      </c>
       <c r="C62" s="4">
         <v>22606</v>
       </c>
       <c r="D62" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1767</v>
       </c>
     </row>
     <row r="63" spans="1:10">
       <c r="A63" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="B63" s="4">
+        <v>21043</v>
+      </c>
       <c r="C63" s="4">
         <v>22810</v>
       </c>
       <c r="D63" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1767</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="18.75">
-      <c r="A64" s="11" t="s">
+      <c r="A64" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B64" s="11"/>
-      <c r="C64" s="11"/>
-      <c r="D64" s="11"/>
+      <c r="B64" s="10"/>
+      <c r="C64" s="10"/>
+      <c r="D64" s="10"/>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="B65" s="4">
+        <v>21292</v>
+      </c>
       <c r="C65" s="4">
         <v>23060</v>
       </c>
       <c r="D65" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1768</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -1605,12 +1635,12 @@
       </c>
     </row>
     <row r="75" spans="1:4" ht="18.75">
-      <c r="A75" s="10" t="s">
+      <c r="A75" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B75" s="10"/>
-      <c r="C75" s="10"/>
-      <c r="D75" s="10"/>
+      <c r="B75" s="12"/>
+      <c r="C75" s="12"/>
+      <c r="D75" s="12"/>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="4" t="s">
@@ -1661,12 +1691,12 @@
       </c>
     </row>
     <row r="80" spans="1:4" ht="18.75">
-      <c r="A80" s="11" t="s">
+      <c r="A80" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B80" s="11"/>
-      <c r="C80" s="11"/>
-      <c r="D80" s="11"/>
+      <c r="B80" s="10"/>
+      <c r="C80" s="10"/>
+      <c r="D80" s="10"/>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="4" t="s">
@@ -1729,12 +1759,12 @@
       </c>
     </row>
     <row r="85" spans="1:4" ht="18.75">
-      <c r="A85" s="10" t="s">
+      <c r="A85" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B85" s="10"/>
-      <c r="C85" s="10"/>
-      <c r="D85" s="10"/>
+      <c r="B85" s="12"/>
+      <c r="C85" s="12"/>
+      <c r="D85" s="12"/>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="4" t="s">
@@ -2052,12 +2082,12 @@
       </c>
     </row>
     <row r="107" spans="1:5" ht="18.75">
-      <c r="A107" s="11" t="s">
+      <c r="A107" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="B107" s="11"/>
-      <c r="C107" s="11"/>
-      <c r="D107" s="11"/>
+      <c r="B107" s="10"/>
+      <c r="C107" s="10"/>
+      <c r="D107" s="10"/>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="4" t="s">
@@ -2183,12 +2213,12 @@
       </c>
     </row>
     <row r="116" spans="1:4" ht="18.75">
-      <c r="A116" s="10" t="s">
+      <c r="A116" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B116" s="10"/>
-      <c r="C116" s="10"/>
-      <c r="D116" s="10"/>
+      <c r="B116" s="12"/>
+      <c r="C116" s="12"/>
+      <c r="D116" s="12"/>
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="4" t="s">
@@ -2266,12 +2296,12 @@
       </c>
     </row>
     <row r="122" spans="1:4" ht="18.75">
-      <c r="A122" s="11" t="s">
+      <c r="A122" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B122" s="11"/>
-      <c r="C122" s="11"/>
-      <c r="D122" s="11"/>
+      <c r="B122" s="10"/>
+      <c r="C122" s="10"/>
+      <c r="D122" s="10"/>
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="4" t="s">
@@ -2469,12 +2499,12 @@
       </c>
     </row>
     <row r="136" spans="1:4" ht="18.75">
-      <c r="A136" s="10" t="s">
+      <c r="A136" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="B136" s="10"/>
-      <c r="C136" s="10"/>
-      <c r="D136" s="10"/>
+      <c r="B136" s="12"/>
+      <c r="C136" s="12"/>
+      <c r="D136" s="12"/>
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="4" t="s">
@@ -2594,12 +2624,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A31:D31"/>
     <mergeCell ref="A116:D116"/>
     <mergeCell ref="A122:D122"/>
     <mergeCell ref="A136:D136"/>
@@ -2609,6 +2633,12 @@
     <mergeCell ref="A80:D80"/>
     <mergeCell ref="A85:D85"/>
     <mergeCell ref="A107:D107"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A31:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -2645,12 +2675,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -2678,12 +2708,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -2717,12 +2747,12 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
@@ -2806,12 +2836,12 @@
       </c>
     </row>
     <row r="17" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="4" t="s">
@@ -2979,12 +3009,12 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="18.75">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="4" t="s">
@@ -3062,12 +3092,12 @@
       </c>
     </row>
     <row r="35" spans="1:10" ht="18.75">
-      <c r="A35" s="11" t="s">
+      <c r="A35" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="4" t="s">
@@ -3160,12 +3190,12 @@
       </c>
     </row>
     <row r="42" spans="1:10" ht="18.75">
-      <c r="A42" s="10" t="s">
+      <c r="A42" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B42" s="10"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="4" t="s">
@@ -3354,12 +3384,12 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="18.75">
-      <c r="A55" s="11" t="s">
+      <c r="A55" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B55" s="11"/>
-      <c r="C55" s="11"/>
-      <c r="D55" s="11"/>
+      <c r="B55" s="10"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="10"/>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="4" t="s">
@@ -3512,12 +3542,12 @@
       </c>
     </row>
     <row r="66" spans="1:4" ht="18.75">
-      <c r="A66" s="10" t="s">
+      <c r="A66" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B66" s="10"/>
-      <c r="C66" s="10"/>
-      <c r="D66" s="10"/>
+      <c r="B66" s="12"/>
+      <c r="C66" s="12"/>
+      <c r="D66" s="12"/>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="4" t="s">
@@ -3580,12 +3610,12 @@
       </c>
     </row>
     <row r="71" spans="1:4" ht="18.75">
-      <c r="A71" s="11" t="s">
+      <c r="A71" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B71" s="11"/>
-      <c r="C71" s="11"/>
-      <c r="D71" s="11"/>
+      <c r="B71" s="10"/>
+      <c r="C71" s="10"/>
+      <c r="D71" s="10"/>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="4" t="s">
@@ -3648,12 +3678,12 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="18.75">
-      <c r="A76" s="10" t="s">
+      <c r="A76" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B76" s="10"/>
-      <c r="C76" s="10"/>
-      <c r="D76" s="10"/>
+      <c r="B76" s="12"/>
+      <c r="C76" s="12"/>
+      <c r="D76" s="12"/>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="4" t="s">
@@ -3971,12 +4001,12 @@
       </c>
     </row>
     <row r="98" spans="1:5" ht="18.75">
-      <c r="A98" s="11" t="s">
+      <c r="A98" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="B98" s="11"/>
-      <c r="C98" s="11"/>
-      <c r="D98" s="11"/>
+      <c r="B98" s="10"/>
+      <c r="C98" s="10"/>
+      <c r="D98" s="10"/>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="4" t="s">
@@ -4102,12 +4132,12 @@
       </c>
     </row>
     <row r="107" spans="1:5" ht="18.75">
-      <c r="A107" s="10" t="s">
+      <c r="A107" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B107" s="10"/>
-      <c r="C107" s="10"/>
-      <c r="D107" s="10"/>
+      <c r="B107" s="12"/>
+      <c r="C107" s="12"/>
+      <c r="D107" s="12"/>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="4" t="s">
@@ -4185,12 +4215,12 @@
       </c>
     </row>
     <row r="113" spans="1:4" ht="18.75">
-      <c r="A113" s="11" t="s">
+      <c r="A113" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B113" s="11"/>
-      <c r="C113" s="11"/>
-      <c r="D113" s="11"/>
+      <c r="B113" s="10"/>
+      <c r="C113" s="10"/>
+      <c r="D113" s="10"/>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="4" t="s">
@@ -4388,12 +4418,12 @@
       </c>
     </row>
     <row r="127" spans="1:4" ht="18.75">
-      <c r="A127" s="10" t="s">
+      <c r="A127" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="B127" s="10"/>
-      <c r="C127" s="10"/>
-      <c r="D127" s="10"/>
+      <c r="B127" s="12"/>
+      <c r="C127" s="12"/>
+      <c r="D127" s="12"/>
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="4" t="s">
@@ -4513,6 +4543,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A29:D29"/>
     <mergeCell ref="A127:D127"/>
     <mergeCell ref="A107:D107"/>
     <mergeCell ref="A113:D113"/>
@@ -4523,11 +4558,6 @@
     <mergeCell ref="A98:D98"/>
     <mergeCell ref="A66:D66"/>
     <mergeCell ref="A55:D55"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A29:D29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>

</xml_diff>

<commit_message>
Wario - some of level 7 done.
</commit_message>
<xml_diff>
--- a/Wario/Wario.xlsx
+++ b/Wario/Wario.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="70">
   <si>
     <t>Enter pipe</t>
   </si>
@@ -222,6 +222,9 @@
   </si>
   <si>
     <t>Leave Level 5</t>
+  </si>
+  <si>
+    <t>Checkpoint</t>
   </si>
 </sst>
 </file>
@@ -329,9 +332,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -626,11 +629,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J144"/>
+  <dimension ref="A1:J145"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B66" sqref="B66"/>
+      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -654,12 +657,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -687,12 +690,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -726,12 +729,12 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
@@ -759,7 +762,7 @@
         <v>3962</v>
       </c>
       <c r="D12" s="4">
-        <f t="shared" ref="D12:D84" si="1">IF(B12 &gt;  0,C12-B12, 0)</f>
+        <f t="shared" ref="D12:D85" si="1">IF(B12 &gt;  0,C12-B12, 0)</f>
         <v>603</v>
       </c>
     </row>
@@ -854,12 +857,12 @@
       </c>
     </row>
     <row r="19" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="4" t="s">
@@ -1027,12 +1030,12 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="18.75">
-      <c r="A31" s="12" t="s">
+      <c r="A31" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="4" t="s">
@@ -1200,12 +1203,12 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="18.75">
-      <c r="A43" s="10" t="s">
+      <c r="A43" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B43" s="10"/>
-      <c r="C43" s="10"/>
-      <c r="D43" s="10"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="4" t="s">
@@ -1313,12 +1316,12 @@
       </c>
     </row>
     <row r="51" spans="1:10" ht="18.75">
-      <c r="A51" s="12" t="s">
+      <c r="A51" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B51" s="12"/>
-      <c r="C51" s="12"/>
-      <c r="D51" s="12"/>
+      <c r="B51" s="10"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="4" t="s">
@@ -1504,12 +1507,12 @@
       </c>
     </row>
     <row r="64" spans="1:10" ht="18.75">
-      <c r="A64" s="10" t="s">
+      <c r="A64" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B64" s="10"/>
-      <c r="C64" s="10"/>
-      <c r="D64" s="10"/>
+      <c r="B64" s="11"/>
+      <c r="C64" s="11"/>
+      <c r="D64" s="11"/>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="4" t="s">
@@ -1528,74 +1531,92 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="4" t="s">
-        <v>6</v>
+        <v>69</v>
+      </c>
+      <c r="B66" s="4">
+        <v>21654</v>
       </c>
       <c r="C66" s="4">
-        <v>24356</v>
+        <v>23438</v>
       </c>
       <c r="D66" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1784</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="B67" s="4">
+        <v>22525</v>
+      </c>
       <c r="C67" s="4">
-        <v>24520</v>
+        <v>24356</v>
       </c>
       <c r="D67" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1831</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="B68" s="4">
+        <v>22683</v>
       </c>
       <c r="C68" s="4">
-        <v>24693</v>
+        <v>24520</v>
       </c>
       <c r="D68" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1837</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="4" t="s">
-        <v>20</v>
+        <v>7</v>
+      </c>
+      <c r="B69" s="4">
+        <v>22853</v>
       </c>
       <c r="C69" s="4">
-        <v>25030</v>
+        <v>24693</v>
       </c>
       <c r="D69" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1840</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="4" t="s">
-        <v>7</v>
+        <v>20</v>
+      </c>
+      <c r="B70" s="4">
+        <v>23177</v>
       </c>
       <c r="C70" s="4">
-        <v>25625</v>
+        <v>25030</v>
       </c>
       <c r="D70" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1853</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="B71" s="4">
+        <v>23709</v>
+      </c>
       <c r="C71" s="4">
-        <v>26130</v>
+        <v>25625</v>
       </c>
       <c r="D71" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1916</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -1603,7 +1624,7 @@
         <v>7</v>
       </c>
       <c r="C72" s="4">
-        <v>26299</v>
+        <v>26130</v>
       </c>
       <c r="D72" s="4">
         <f t="shared" si="1"/>
@@ -1612,10 +1633,10 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="4" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="C73" s="4">
-        <v>26404</v>
+        <v>26299</v>
       </c>
       <c r="D73" s="4">
         <f t="shared" si="1"/>
@@ -1624,54 +1645,54 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C74" s="4">
+        <v>26404</v>
+      </c>
+      <c r="D74" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C74" s="4">
+      <c r="C75" s="4">
         <v>26607</v>
       </c>
-      <c r="D74" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" ht="18.75">
-      <c r="A75" s="12" t="s">
+      <c r="D75" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="18.75">
+      <c r="A76" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B75" s="12"/>
-      <c r="C75" s="12"/>
-      <c r="D75" s="12"/>
-    </row>
-    <row r="76" spans="1:4">
-      <c r="A76" s="4" t="s">
+      <c r="B76" s="10"/>
+      <c r="C76" s="10"/>
+      <c r="D76" s="10"/>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C76" s="4">
+      <c r="C77" s="4">
         <v>26858</v>
       </c>
-      <c r="D76" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4">
-      <c r="A77" s="8" t="s">
+      <c r="D77" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C77" s="4">
+      <c r="C78" s="4">
         <v>28167</v>
-      </c>
-      <c r="D77" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4">
-      <c r="A78" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C78" s="4">
-        <v>32142</v>
       </c>
       <c r="D78" s="4">
         <f t="shared" si="1"/>
@@ -1680,48 +1701,45 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C79" s="4">
+        <v>32142</v>
+      </c>
+      <c r="D79" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C79" s="4">
+      <c r="C80" s="4">
         <v>32671</v>
       </c>
-      <c r="D79" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" ht="18.75">
-      <c r="A80" s="10" t="s">
+      <c r="D80" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="18.75">
+      <c r="A81" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B80" s="10"/>
-      <c r="C80" s="10"/>
-      <c r="D80" s="10"/>
-    </row>
-    <row r="81" spans="1:4">
-      <c r="A81" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B81" s="4">
-        <v>32921</v>
-      </c>
-      <c r="C81" s="4">
-        <v>32921</v>
-      </c>
-      <c r="D81" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="B81" s="11"/>
+      <c r="C81" s="11"/>
+      <c r="D81" s="11"/>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="4" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="B82" s="4">
-        <v>34723</v>
+        <v>32921</v>
       </c>
       <c r="C82" s="4">
-        <v>34723</v>
+        <v>32921</v>
       </c>
       <c r="D82" s="4">
         <f t="shared" si="1"/>
@@ -1730,13 +1748,13 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="4" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B83" s="4">
-        <v>35373</v>
+        <v>34723</v>
       </c>
       <c r="C83" s="4">
-        <v>35373</v>
+        <v>34723</v>
       </c>
       <c r="D83" s="4">
         <f t="shared" si="1"/>
@@ -1745,54 +1763,54 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B84" s="4">
+        <v>35373</v>
+      </c>
+      <c r="C84" s="4">
+        <v>35373</v>
+      </c>
+      <c r="D84" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B84" s="4">
+      <c r="B85" s="4">
         <v>35577</v>
       </c>
-      <c r="C84" s="4">
+      <c r="C85" s="4">
         <v>35577</v>
       </c>
-      <c r="D84" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" ht="18.75">
-      <c r="A85" s="12" t="s">
+      <c r="D85" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="18.75">
+      <c r="A86" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B85" s="12"/>
-      <c r="C85" s="12"/>
-      <c r="D85" s="12"/>
-    </row>
-    <row r="86" spans="1:4">
-      <c r="A86" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B86" s="4">
-        <v>35826</v>
-      </c>
-      <c r="C86" s="4">
-        <v>35826</v>
-      </c>
-      <c r="D86" s="4">
-        <f t="shared" ref="D86:D143" si="3">IF(B86 &gt;  0,C86-B86, 0)</f>
-        <v>0</v>
-      </c>
+      <c r="B86" s="10"/>
+      <c r="C86" s="10"/>
+      <c r="D86" s="10"/>
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B87" s="4">
-        <v>36033</v>
+        <v>35826</v>
       </c>
       <c r="C87" s="4">
-        <v>36033</v>
+        <v>35826</v>
       </c>
       <c r="D87" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="D87:D144" si="3">IF(B87 &gt;  0,C87-B87, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1801,10 +1819,10 @@
         <v>45</v>
       </c>
       <c r="B88" s="4">
-        <v>36201</v>
+        <v>36033</v>
       </c>
       <c r="C88" s="4">
-        <v>36201</v>
+        <v>36033</v>
       </c>
       <c r="D88" s="4">
         <f t="shared" si="3"/>
@@ -1816,10 +1834,10 @@
         <v>45</v>
       </c>
       <c r="B89" s="4">
-        <v>36370</v>
+        <v>36201</v>
       </c>
       <c r="C89" s="4">
-        <v>36370</v>
+        <v>36201</v>
       </c>
       <c r="D89" s="4">
         <f t="shared" si="3"/>
@@ -1831,10 +1849,10 @@
         <v>45</v>
       </c>
       <c r="B90" s="4">
-        <v>36538</v>
+        <v>36370</v>
       </c>
       <c r="C90" s="4">
-        <v>36538</v>
+        <v>36370</v>
       </c>
       <c r="D90" s="4">
         <f t="shared" si="3"/>
@@ -1843,13 +1861,13 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B91" s="4">
-        <v>36744</v>
+        <v>36538</v>
       </c>
       <c r="C91" s="4">
-        <v>36744</v>
+        <v>36538</v>
       </c>
       <c r="D91" s="4">
         <f t="shared" si="3"/>
@@ -1858,13 +1876,13 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B92" s="4">
-        <v>37194</v>
+        <v>36744</v>
       </c>
       <c r="C92" s="4">
-        <v>37194</v>
+        <v>36744</v>
       </c>
       <c r="D92" s="4">
         <f t="shared" si="3"/>
@@ -1873,13 +1891,13 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="4" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="B93" s="4">
-        <v>37481</v>
+        <v>37194</v>
       </c>
       <c r="C93" s="4">
-        <v>37481</v>
+        <v>37194</v>
       </c>
       <c r="D93" s="4">
         <f t="shared" si="3"/>
@@ -1888,13 +1906,13 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="4" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B94" s="4">
-        <v>37662</v>
+        <v>37481</v>
       </c>
       <c r="C94" s="4">
-        <v>37662</v>
+        <v>37481</v>
       </c>
       <c r="D94" s="4">
         <f t="shared" si="3"/>
@@ -1906,10 +1924,10 @@
         <v>6</v>
       </c>
       <c r="B95" s="4">
-        <v>37816</v>
+        <v>37662</v>
       </c>
       <c r="C95" s="4">
-        <v>37816</v>
+        <v>37662</v>
       </c>
       <c r="D95" s="4">
         <f t="shared" si="3"/>
@@ -1921,472 +1939,472 @@
         <v>6</v>
       </c>
       <c r="B96" s="4">
-        <v>37986</v>
+        <v>37816</v>
       </c>
       <c r="C96" s="4">
-        <v>37986</v>
+        <v>37816</v>
       </c>
       <c r="D96" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:5">
+    <row r="97" spans="1:4">
       <c r="A97" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B97" s="4">
-        <v>38140</v>
+        <v>37986</v>
       </c>
       <c r="C97" s="4">
-        <v>38140</v>
+        <v>37986</v>
       </c>
       <c r="D97" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:5">
+    <row r="98" spans="1:4">
       <c r="A98" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B98" s="4">
-        <v>38278</v>
+        <v>38140</v>
       </c>
       <c r="C98" s="4">
-        <v>38278</v>
+        <v>38140</v>
       </c>
       <c r="D98" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:5">
+    <row r="99" spans="1:4">
       <c r="A99" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B99" s="4">
-        <v>38479</v>
+        <v>38278</v>
       </c>
       <c r="C99" s="4">
-        <v>38479</v>
+        <v>38278</v>
       </c>
       <c r="D99" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:5">
+    <row r="100" spans="1:4">
       <c r="A100" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B100" s="4">
+        <v>38479</v>
+      </c>
+      <c r="C100" s="4">
+        <v>38479</v>
+      </c>
+      <c r="D100" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B101" s="4">
         <v>38618</v>
       </c>
-      <c r="C100" s="4">
+      <c r="C101" s="4">
         <v>38618</v>
       </c>
-      <c r="D100" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5">
-      <c r="A101" s="4" t="s">
+      <c r="D101" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B101" s="4">
+      <c r="B102" s="4">
         <v>40024</v>
       </c>
-      <c r="C101" s="4">
+      <c r="C102" s="4">
         <v>40024</v>
       </c>
-      <c r="D101" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5">
-      <c r="A102" s="4" t="s">
+      <c r="D102" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B102" s="4">
+      <c r="B103" s="4">
         <v>40214</v>
       </c>
-      <c r="C102" s="4">
+      <c r="C103" s="4">
         <v>40214</v>
       </c>
-      <c r="D102" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5">
-      <c r="A103" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B103" s="4">
-        <v>40388</v>
-      </c>
-      <c r="C103" s="4">
-        <v>40388</v>
-      </c>
       <c r="D103" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:5">
+    <row r="104" spans="1:4">
       <c r="A104" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B104" s="4">
+        <v>40388</v>
+      </c>
+      <c r="C104" s="4">
+        <v>40388</v>
+      </c>
+      <c r="D104" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B105" s="4">
         <v>40726</v>
       </c>
-      <c r="C104" s="4">
+      <c r="C105" s="4">
         <v>40726</v>
       </c>
-      <c r="D104" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5">
-      <c r="A105" s="4" t="s">
+      <c r="D105" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B105" s="4">
+      <c r="B106" s="4">
         <v>40827</v>
       </c>
-      <c r="C105" s="4">
+      <c r="C106" s="4">
         <v>40827</v>
       </c>
-      <c r="D105" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5">
-      <c r="A106" s="4" t="s">
+      <c r="D106" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B106" s="4">
+      <c r="B107" s="4">
         <v>41030</v>
       </c>
-      <c r="C106" s="4">
+      <c r="C107" s="4">
         <v>41030</v>
       </c>
-      <c r="D106" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" ht="18.75">
-      <c r="A107" s="10" t="s">
+      <c r="D107" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="18.75">
+      <c r="A108" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B107" s="10"/>
-      <c r="C107" s="10"/>
-      <c r="D107" s="10"/>
-    </row>
-    <row r="108" spans="1:5">
-      <c r="A108" s="4" t="s">
+      <c r="B108" s="11"/>
+      <c r="C108" s="11"/>
+      <c r="D108" s="11"/>
+    </row>
+    <row r="109" spans="1:4">
+      <c r="A109" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B108" s="4">
+      <c r="B109" s="4">
         <v>41280</v>
       </c>
-      <c r="C108" s="4">
+      <c r="C109" s="4">
         <v>41280</v>
       </c>
-      <c r="D108" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5">
-      <c r="A109" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B109" s="4">
-        <v>42038</v>
-      </c>
-      <c r="C109" s="4">
-        <v>42038</v>
-      </c>
       <c r="D109" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:5">
+    <row r="110" spans="1:4">
       <c r="A110" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B110" s="4">
-        <v>42649</v>
+        <v>42038</v>
       </c>
       <c r="C110" s="4">
-        <v>42649</v>
+        <v>42038</v>
       </c>
       <c r="D110" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:5">
+    <row r="111" spans="1:4">
       <c r="A111" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B111" s="4">
+        <v>42649</v>
+      </c>
+      <c r="C111" s="4">
+        <v>42649</v>
+      </c>
+      <c r="D111" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4">
+      <c r="A112" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B112" s="4">
         <v>43208</v>
       </c>
-      <c r="C111" s="4">
+      <c r="C112" s="4">
         <v>43208</v>
       </c>
-      <c r="D111" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5">
-      <c r="A112" s="4" t="s">
+      <c r="D112" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5">
+      <c r="A113" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B112" s="4">
+      <c r="B113" s="4">
         <v>43493</v>
       </c>
-      <c r="C112" s="4">
+      <c r="C113" s="4">
         <v>43493</v>
       </c>
-      <c r="D112" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E112" t="s">
+      <c r="D113" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E113" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="113" spans="1:4">
-      <c r="A113" s="4" t="s">
+    <row r="114" spans="1:5">
+      <c r="A114" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B113" s="4">
+      <c r="B114" s="4">
         <v>43763</v>
       </c>
-      <c r="C113" s="4">
+      <c r="C114" s="4">
         <v>43763</v>
       </c>
-      <c r="D113" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4">
-      <c r="A114" s="4" t="s">
+      <c r="D114" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5">
+      <c r="A115" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B114" s="4">
+      <c r="B115" s="4">
         <v>44050</v>
       </c>
-      <c r="C114" s="4">
+      <c r="C115" s="4">
         <v>44050</v>
       </c>
-      <c r="D114" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4">
-      <c r="A115" s="4" t="s">
+      <c r="D115" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5">
+      <c r="A116" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B115" s="4">
+      <c r="B116" s="4">
         <v>44254</v>
       </c>
-      <c r="C115" s="4">
+      <c r="C116" s="4">
         <v>44254</v>
       </c>
-      <c r="D115" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" ht="18.75">
-      <c r="A116" s="12" t="s">
+      <c r="D116" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" ht="18.75">
+      <c r="A117" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B116" s="12"/>
-      <c r="C116" s="12"/>
-      <c r="D116" s="12"/>
-    </row>
-    <row r="117" spans="1:4">
-      <c r="A117" s="4" t="s">
+      <c r="B117" s="10"/>
+      <c r="C117" s="10"/>
+      <c r="D117" s="10"/>
+    </row>
+    <row r="118" spans="1:5">
+      <c r="A118" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B117" s="4">
+      <c r="B118" s="4">
         <v>44504</v>
       </c>
-      <c r="C117" s="4">
+      <c r="C118" s="4">
         <v>44504</v>
       </c>
-      <c r="D117" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4">
-      <c r="A118" s="4" t="s">
+      <c r="D118" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5">
+      <c r="A119" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B118" s="4">
+      <c r="B119" s="4">
         <v>46191</v>
       </c>
-      <c r="C118" s="4">
+      <c r="C119" s="4">
         <v>46191</v>
       </c>
-      <c r="D118" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4">
-      <c r="A119" s="4" t="s">
+      <c r="D119" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5">
+      <c r="A120" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B119" s="4">
+      <c r="B120" s="4">
         <v>48585</v>
       </c>
-      <c r="C119" s="4">
+      <c r="C120" s="4">
         <v>48585</v>
       </c>
-      <c r="D119" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4">
-      <c r="A120" s="4" t="s">
+      <c r="D120" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5">
+      <c r="A121" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B120" s="4">
+      <c r="B121" s="4">
         <v>48941</v>
       </c>
-      <c r="C120" s="4">
+      <c r="C121" s="4">
         <v>48941</v>
       </c>
-      <c r="D120" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4">
-      <c r="A121" s="4" t="s">
+      <c r="D121" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5">
+      <c r="A122" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B121" s="4">
+      <c r="B122" s="4">
         <v>49144</v>
       </c>
-      <c r="C121" s="4">
+      <c r="C122" s="4">
         <v>49144</v>
       </c>
-      <c r="D121" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" ht="18.75">
-      <c r="A122" s="10" t="s">
+      <c r="D122" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" ht="18.75">
+      <c r="A123" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B122" s="10"/>
-      <c r="C122" s="10"/>
-      <c r="D122" s="10"/>
-    </row>
-    <row r="123" spans="1:4">
-      <c r="A123" s="4" t="s">
+      <c r="B123" s="11"/>
+      <c r="C123" s="11"/>
+      <c r="D123" s="11"/>
+    </row>
+    <row r="124" spans="1:5">
+      <c r="A124" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B123" s="4">
+      <c r="B124" s="4">
         <v>49395</v>
       </c>
-      <c r="C123" s="4">
+      <c r="C124" s="4">
         <v>49395</v>
       </c>
-      <c r="D123" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4">
-      <c r="A124" s="4" t="s">
+      <c r="D124" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5">
+      <c r="A125" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B124" s="4">
+      <c r="B125" s="4">
         <v>49704</v>
       </c>
-      <c r="C124" s="4">
+      <c r="C125" s="4">
         <v>49704</v>
       </c>
-      <c r="D124" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4">
-      <c r="A125" s="4" t="s">
+      <c r="D125" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5">
+      <c r="A126" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B125" s="4">
+      <c r="B126" s="4">
         <v>49883</v>
       </c>
-      <c r="C125" s="4">
+      <c r="C126" s="4">
         <v>49883</v>
       </c>
-      <c r="D125" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4">
-      <c r="A126" s="4" t="s">
+      <c r="D126" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5">
+      <c r="A127" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B126" s="4">
+      <c r="B127" s="4">
         <v>50088</v>
       </c>
-      <c r="C126" s="4">
+      <c r="C127" s="4">
         <v>50088</v>
       </c>
-      <c r="D126" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4">
-      <c r="A127" s="4" t="s">
+      <c r="D127" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5">
+      <c r="A128" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B127" s="4">
+      <c r="B128" s="4">
         <v>50263</v>
       </c>
-      <c r="C127" s="4">
+      <c r="C128" s="4">
         <v>50263</v>
-      </c>
-      <c r="D127" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4">
-      <c r="A128" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B128" s="4">
-        <v>50566</v>
-      </c>
-      <c r="C128" s="4">
-        <v>50566</v>
       </c>
       <c r="D128" s="4">
         <f t="shared" si="3"/>
@@ -2395,13 +2413,13 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B129" s="4">
-        <v>50734</v>
+        <v>50566</v>
       </c>
       <c r="C129" s="4">
-        <v>50734</v>
+        <v>50566</v>
       </c>
       <c r="D129" s="4">
         <f t="shared" si="3"/>
@@ -2410,13 +2428,13 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="4" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B130" s="4">
-        <v>50849</v>
+        <v>50734</v>
       </c>
       <c r="C130" s="4">
-        <v>50849</v>
+        <v>50734</v>
       </c>
       <c r="D130" s="4">
         <f t="shared" si="3"/>
@@ -2425,13 +2443,13 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="4" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="B131" s="4">
-        <v>51176</v>
+        <v>50849</v>
       </c>
       <c r="C131" s="4">
-        <v>51176</v>
+        <v>50849</v>
       </c>
       <c r="D131" s="4">
         <f t="shared" si="3"/>
@@ -2440,13 +2458,13 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="4" t="s">
-        <v>6</v>
+        <v>57</v>
       </c>
       <c r="B132" s="4">
-        <v>51327</v>
+        <v>51176</v>
       </c>
       <c r="C132" s="4">
-        <v>51327</v>
+        <v>51176</v>
       </c>
       <c r="D132" s="4">
         <f t="shared" si="3"/>
@@ -2458,10 +2476,10 @@
         <v>6</v>
       </c>
       <c r="B133" s="4">
-        <v>51577</v>
+        <v>51327</v>
       </c>
       <c r="C133" s="4">
-        <v>51577</v>
+        <v>51327</v>
       </c>
       <c r="D133" s="4">
         <f t="shared" si="3"/>
@@ -2470,13 +2488,13 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="4" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="B134" s="4">
-        <v>51868</v>
+        <v>51577</v>
       </c>
       <c r="C134" s="4">
-        <v>51868</v>
+        <v>51577</v>
       </c>
       <c r="D134" s="4">
         <f t="shared" si="3"/>
@@ -2485,51 +2503,51 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B135" s="4">
+        <v>51868</v>
+      </c>
+      <c r="C135" s="4">
+        <v>51868</v>
+      </c>
+      <c r="D135" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
+      <c r="A136" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B135" s="4">
+      <c r="B136" s="4">
         <v>52071</v>
       </c>
-      <c r="C135" s="4">
+      <c r="C136" s="4">
         <v>52071</v>
       </c>
-      <c r="D135" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" ht="18.75">
-      <c r="A136" s="12" t="s">
+      <c r="D136" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" ht="18.75">
+      <c r="A137" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B136" s="12"/>
-      <c r="C136" s="12"/>
-      <c r="D136" s="12"/>
-    </row>
-    <row r="137" spans="1:4">
-      <c r="A137" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B137" s="4">
-        <v>52322</v>
-      </c>
-      <c r="C137" s="4">
-        <v>52322</v>
-      </c>
-      <c r="D137" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
+      <c r="B137" s="10"/>
+      <c r="C137" s="10"/>
+      <c r="D137" s="10"/>
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="4" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="B138" s="4">
-        <v>53245</v>
+        <v>52322</v>
       </c>
       <c r="C138" s="4">
-        <v>53245</v>
+        <v>52322</v>
       </c>
       <c r="D138" s="4">
         <f t="shared" si="3"/>
@@ -2538,13 +2556,13 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="4" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="B139" s="4">
-        <v>55063</v>
+        <v>53245</v>
       </c>
       <c r="C139" s="4">
-        <v>55063</v>
+        <v>53245</v>
       </c>
       <c r="D139" s="4">
         <f t="shared" si="3"/>
@@ -2553,13 +2571,13 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B140" s="4">
-        <v>55385</v>
+        <v>55063</v>
       </c>
       <c r="C140" s="4">
-        <v>55385</v>
+        <v>55063</v>
       </c>
       <c r="D140" s="4">
         <f t="shared" si="3"/>
@@ -2568,13 +2586,13 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B141" s="4">
-        <v>55706</v>
+        <v>55385</v>
       </c>
       <c r="C141" s="4">
-        <v>55706</v>
+        <v>55385</v>
       </c>
       <c r="D141" s="4">
         <f t="shared" si="3"/>
@@ -2583,13 +2601,13 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B142" s="4">
-        <v>56029</v>
+        <v>55706</v>
       </c>
       <c r="C142" s="4">
-        <v>56029</v>
+        <v>55706</v>
       </c>
       <c r="D142" s="4">
         <f t="shared" si="3"/>
@@ -2598,13 +2616,13 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B143" s="4">
-        <v>58292</v>
+        <v>56029</v>
       </c>
       <c r="C143" s="4">
-        <v>58292</v>
+        <v>56029</v>
       </c>
       <c r="D143" s="4">
         <f t="shared" si="3"/>
@@ -2613,32 +2631,47 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B144" s="4">
+        <v>58292</v>
+      </c>
+      <c r="C144" s="4">
+        <v>58292</v>
+      </c>
+      <c r="D144" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3">
+      <c r="A145" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B144" s="9">
+      <c r="B145" s="9">
         <v>0.71250000000000002</v>
       </c>
-      <c r="C144" s="9">
+      <c r="C145" s="9">
         <v>0.71250000000000002</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A116:D116"/>
-    <mergeCell ref="A122:D122"/>
-    <mergeCell ref="A136:D136"/>
-    <mergeCell ref="A51:D51"/>
-    <mergeCell ref="A64:D64"/>
-    <mergeCell ref="A75:D75"/>
-    <mergeCell ref="A80:D80"/>
-    <mergeCell ref="A85:D85"/>
-    <mergeCell ref="A107:D107"/>
     <mergeCell ref="A43:D43"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="A10:D10"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A117:D117"/>
+    <mergeCell ref="A123:D123"/>
+    <mergeCell ref="A137:D137"/>
+    <mergeCell ref="A51:D51"/>
+    <mergeCell ref="A64:D64"/>
+    <mergeCell ref="A76:D76"/>
+    <mergeCell ref="A81:D81"/>
+    <mergeCell ref="A86:D86"/>
+    <mergeCell ref="A108:D108"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -2675,12 +2708,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -2708,12 +2741,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -2747,12 +2780,12 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
@@ -2836,12 +2869,12 @@
       </c>
     </row>
     <row r="17" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="4" t="s">
@@ -3009,12 +3042,12 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="18.75">
-      <c r="A29" s="12" t="s">
+      <c r="A29" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="4" t="s">
@@ -3092,12 +3125,12 @@
       </c>
     </row>
     <row r="35" spans="1:10" ht="18.75">
-      <c r="A35" s="10" t="s">
+      <c r="A35" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="4" t="s">
@@ -3190,12 +3223,12 @@
       </c>
     </row>
     <row r="42" spans="1:10" ht="18.75">
-      <c r="A42" s="12" t="s">
+      <c r="A42" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B42" s="12"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="4" t="s">
@@ -3384,12 +3417,12 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="18.75">
-      <c r="A55" s="10" t="s">
+      <c r="A55" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B55" s="10"/>
-      <c r="C55" s="10"/>
-      <c r="D55" s="10"/>
+      <c r="B55" s="11"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="11"/>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="4" t="s">
@@ -3542,12 +3575,12 @@
       </c>
     </row>
     <row r="66" spans="1:4" ht="18.75">
-      <c r="A66" s="12" t="s">
+      <c r="A66" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B66" s="12"/>
-      <c r="C66" s="12"/>
-      <c r="D66" s="12"/>
+      <c r="B66" s="10"/>
+      <c r="C66" s="10"/>
+      <c r="D66" s="10"/>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="4" t="s">
@@ -3610,12 +3643,12 @@
       </c>
     </row>
     <row r="71" spans="1:4" ht="18.75">
-      <c r="A71" s="10" t="s">
+      <c r="A71" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B71" s="10"/>
-      <c r="C71" s="10"/>
-      <c r="D71" s="10"/>
+      <c r="B71" s="11"/>
+      <c r="C71" s="11"/>
+      <c r="D71" s="11"/>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="4" t="s">
@@ -3678,12 +3711,12 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="18.75">
-      <c r="A76" s="12" t="s">
+      <c r="A76" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B76" s="12"/>
-      <c r="C76" s="12"/>
-      <c r="D76" s="12"/>
+      <c r="B76" s="10"/>
+      <c r="C76" s="10"/>
+      <c r="D76" s="10"/>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="4" t="s">
@@ -4001,12 +4034,12 @@
       </c>
     </row>
     <row r="98" spans="1:5" ht="18.75">
-      <c r="A98" s="10" t="s">
+      <c r="A98" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B98" s="10"/>
-      <c r="C98" s="10"/>
-      <c r="D98" s="10"/>
+      <c r="B98" s="11"/>
+      <c r="C98" s="11"/>
+      <c r="D98" s="11"/>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="4" t="s">
@@ -4132,12 +4165,12 @@
       </c>
     </row>
     <row r="107" spans="1:5" ht="18.75">
-      <c r="A107" s="12" t="s">
+      <c r="A107" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B107" s="12"/>
-      <c r="C107" s="12"/>
-      <c r="D107" s="12"/>
+      <c r="B107" s="10"/>
+      <c r="C107" s="10"/>
+      <c r="D107" s="10"/>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="4" t="s">
@@ -4215,12 +4248,12 @@
       </c>
     </row>
     <row r="113" spans="1:4" ht="18.75">
-      <c r="A113" s="10" t="s">
+      <c r="A113" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B113" s="10"/>
-      <c r="C113" s="10"/>
-      <c r="D113" s="10"/>
+      <c r="B113" s="11"/>
+      <c r="C113" s="11"/>
+      <c r="D113" s="11"/>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="4" t="s">
@@ -4418,12 +4451,12 @@
       </c>
     </row>
     <row r="127" spans="1:4" ht="18.75">
-      <c r="A127" s="12" t="s">
+      <c r="A127" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B127" s="12"/>
-      <c r="C127" s="12"/>
-      <c r="D127" s="12"/>
+      <c r="B127" s="10"/>
+      <c r="C127" s="10"/>
+      <c r="D127" s="10"/>
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="4" t="s">
@@ -4543,11 +4576,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A29:D29"/>
     <mergeCell ref="A127:D127"/>
     <mergeCell ref="A107:D107"/>
     <mergeCell ref="A113:D113"/>
@@ -4558,6 +4586,11 @@
     <mergeCell ref="A98:D98"/>
     <mergeCell ref="A66:D66"/>
     <mergeCell ref="A55:D55"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A29:D29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>

</xml_diff>

<commit_message>
Wario - Level 8 done
</commit_message>
<xml_diff>
--- a/Wario/Wario.xlsx
+++ b/Wario/Wario.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="70">
   <si>
     <t>Enter pipe</t>
   </si>
@@ -332,9 +332,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -629,11 +629,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J145"/>
+  <dimension ref="A1:J149"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B72" sqref="B72"/>
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -657,12 +657,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -690,12 +690,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -729,12 +729,12 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
@@ -762,7 +762,7 @@
         <v>3962</v>
       </c>
       <c r="D12" s="4">
-        <f t="shared" ref="D12:D85" si="1">IF(B12 &gt;  0,C12-B12, 0)</f>
+        <f t="shared" ref="D12:D89" si="1">IF(B12 &gt;  0,C12-B12, 0)</f>
         <v>603</v>
       </c>
     </row>
@@ -857,12 +857,12 @@
       </c>
     </row>
     <row r="19" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="4" t="s">
@@ -1030,12 +1030,12 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="18.75">
-      <c r="A31" s="10" t="s">
+      <c r="A31" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="4" t="s">
@@ -1203,12 +1203,12 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="18.75">
-      <c r="A43" s="11" t="s">
+      <c r="A43" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B43" s="11"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="4" t="s">
@@ -1316,12 +1316,12 @@
       </c>
     </row>
     <row r="51" spans="1:10" ht="18.75">
-      <c r="A51" s="10" t="s">
+      <c r="A51" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B51" s="10"/>
-      <c r="C51" s="10"/>
-      <c r="D51" s="10"/>
+      <c r="B51" s="12"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="12"/>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="4" t="s">
@@ -1507,12 +1507,12 @@
       </c>
     </row>
     <row r="64" spans="1:10" ht="18.75">
-      <c r="A64" s="11" t="s">
+      <c r="A64" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B64" s="11"/>
-      <c r="C64" s="11"/>
-      <c r="D64" s="11"/>
+      <c r="B64" s="10"/>
+      <c r="C64" s="10"/>
+      <c r="D64" s="10"/>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="4" t="s">
@@ -1659,21 +1659,24 @@
       <c r="A75" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="B75" s="4">
+        <v>24691</v>
+      </c>
       <c r="C75" s="4">
         <v>26607</v>
       </c>
       <c r="D75" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1916</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="18.75">
-      <c r="A76" s="10" t="s">
+      <c r="A76" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B76" s="10"/>
-      <c r="C76" s="10"/>
-      <c r="D76" s="10"/>
+      <c r="B76" s="12"/>
+      <c r="C76" s="12"/>
+      <c r="D76" s="12"/>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="4" t="s">
@@ -1691,198 +1694,185 @@
       <c r="A78" s="8" t="s">
         <v>26</v>
       </c>
+      <c r="B78" s="4">
+        <v>26245</v>
+      </c>
       <c r="C78" s="4">
         <v>28167</v>
       </c>
       <c r="D78" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1922</v>
       </c>
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="4" t="s">
-        <v>39</v>
+        <v>66</v>
+      </c>
+      <c r="B79" s="4">
+        <v>27387</v>
       </c>
       <c r="C79" s="4">
-        <v>32142</v>
+        <v>29309</v>
       </c>
       <c r="D79" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1922</v>
       </c>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="4" t="s">
-        <v>40</v>
+        <v>60</v>
+      </c>
+      <c r="B80" s="4">
+        <v>28067</v>
       </c>
       <c r="C80" s="4">
-        <v>32671</v>
+        <v>29989</v>
       </c>
       <c r="D80" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" ht="18.75">
-      <c r="A81" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B81" s="11"/>
-      <c r="C81" s="11"/>
-      <c r="D81" s="11"/>
+        <v>1922</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B81" s="4">
+        <v>28747</v>
+      </c>
+      <c r="C81" s="4">
+        <v>30669</v>
+      </c>
+      <c r="D81" s="4">
+        <f t="shared" si="1"/>
+        <v>1922</v>
+      </c>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B82" s="4">
-        <v>32921</v>
+        <v>30220</v>
       </c>
       <c r="C82" s="4">
-        <v>32921</v>
+        <v>32142</v>
       </c>
       <c r="D82" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1922</v>
       </c>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B83" s="4">
-        <v>34723</v>
-      </c>
-      <c r="C83" s="4">
-        <v>34723</v>
-      </c>
-      <c r="D83" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>30546</v>
       </c>
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="4" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="B84" s="4">
-        <v>35373</v>
+        <v>30749</v>
       </c>
       <c r="C84" s="4">
-        <v>35373</v>
+        <v>32671</v>
       </c>
       <c r="D84" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4">
-      <c r="A85" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B85" s="4">
-        <v>35577</v>
-      </c>
-      <c r="C85" s="4">
-        <v>35577</v>
-      </c>
-      <c r="D85" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" ht="18.75">
-      <c r="A86" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B86" s="10"/>
-      <c r="C86" s="10"/>
-      <c r="D86" s="10"/>
+        <v>1922</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="18.75">
+      <c r="A85" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B85" s="10"/>
+      <c r="C85" s="10"/>
+      <c r="D85" s="10"/>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B86" s="4">
+        <v>30998</v>
+      </c>
+      <c r="C86" s="4">
+        <v>32921</v>
+      </c>
+      <c r="D86" s="4">
+        <f t="shared" si="1"/>
+        <v>1923</v>
+      </c>
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B87" s="4">
-        <v>35826</v>
+        <v>20</v>
       </c>
       <c r="C87" s="4">
-        <v>35826</v>
+        <v>34723</v>
       </c>
       <c r="D87" s="4">
-        <f t="shared" ref="D87:D144" si="3">IF(B87 &gt;  0,C87-B87, 0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B88" s="4">
-        <v>36033</v>
+        <v>27</v>
       </c>
       <c r="C88" s="4">
-        <v>36033</v>
+        <v>35373</v>
       </c>
       <c r="D88" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B89" s="4">
-        <v>36201</v>
+        <v>34</v>
       </c>
       <c r="C89" s="4">
-        <v>36201</v>
+        <v>35577</v>
       </c>
       <c r="D89" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4">
-      <c r="A90" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B90" s="4">
-        <v>36370</v>
-      </c>
-      <c r="C90" s="4">
-        <v>36370</v>
-      </c>
-      <c r="D90" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="18.75">
+      <c r="A90" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B90" s="12"/>
+      <c r="C90" s="12"/>
+      <c r="D90" s="12"/>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B91" s="4">
-        <v>36538</v>
+        <v>43</v>
       </c>
       <c r="C91" s="4">
-        <v>36538</v>
+        <v>35826</v>
       </c>
       <c r="D91" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="D91:D148" si="3">IF(B91 &gt;  0,C91-B91, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B92" s="4">
-        <v>36744</v>
+        <v>45</v>
       </c>
       <c r="C92" s="4">
-        <v>36744</v>
+        <v>36033</v>
       </c>
       <c r="D92" s="4">
         <f t="shared" si="3"/>
@@ -1891,13 +1881,10 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B93" s="4">
-        <v>37194</v>
+        <v>45</v>
       </c>
       <c r="C93" s="4">
-        <v>37194</v>
+        <v>36201</v>
       </c>
       <c r="D93" s="4">
         <f t="shared" si="3"/>
@@ -1906,13 +1893,10 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B94" s="4">
-        <v>37481</v>
+        <v>45</v>
       </c>
       <c r="C94" s="4">
-        <v>37481</v>
+        <v>36370</v>
       </c>
       <c r="D94" s="4">
         <f t="shared" si="3"/>
@@ -1921,13 +1905,10 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B95" s="4">
-        <v>37662</v>
+        <v>45</v>
       </c>
       <c r="C95" s="4">
-        <v>37662</v>
+        <v>36538</v>
       </c>
       <c r="D95" s="4">
         <f t="shared" si="3"/>
@@ -1936,13 +1917,10 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B96" s="4">
-        <v>37816</v>
+        <v>46</v>
       </c>
       <c r="C96" s="4">
-        <v>37816</v>
+        <v>36744</v>
       </c>
       <c r="D96" s="4">
         <f t="shared" si="3"/>
@@ -1951,13 +1929,10 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B97" s="4">
-        <v>37986</v>
+        <v>47</v>
       </c>
       <c r="C97" s="4">
-        <v>37986</v>
+        <v>37194</v>
       </c>
       <c r="D97" s="4">
         <f t="shared" si="3"/>
@@ -1966,13 +1941,10 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B98" s="4">
-        <v>38140</v>
+        <v>19</v>
       </c>
       <c r="C98" s="4">
-        <v>38140</v>
+        <v>37481</v>
       </c>
       <c r="D98" s="4">
         <f t="shared" si="3"/>
@@ -1983,11 +1955,8 @@
       <c r="A99" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B99" s="4">
-        <v>38278</v>
-      </c>
       <c r="C99" s="4">
-        <v>38278</v>
+        <v>37662</v>
       </c>
       <c r="D99" s="4">
         <f t="shared" si="3"/>
@@ -1998,11 +1967,8 @@
       <c r="A100" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B100" s="4">
-        <v>38479</v>
-      </c>
       <c r="C100" s="4">
-        <v>38479</v>
+        <v>37816</v>
       </c>
       <c r="D100" s="4">
         <f t="shared" si="3"/>
@@ -2013,11 +1979,8 @@
       <c r="A101" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B101" s="4">
-        <v>38618</v>
-      </c>
       <c r="C101" s="4">
-        <v>38618</v>
+        <v>37986</v>
       </c>
       <c r="D101" s="4">
         <f t="shared" si="3"/>
@@ -2026,13 +1989,10 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B102" s="4">
-        <v>40024</v>
+        <v>6</v>
       </c>
       <c r="C102" s="4">
-        <v>40024</v>
+        <v>38140</v>
       </c>
       <c r="D102" s="4">
         <f t="shared" si="3"/>
@@ -2043,11 +2003,8 @@
       <c r="A103" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B103" s="4">
-        <v>40214</v>
-      </c>
       <c r="C103" s="4">
-        <v>40214</v>
+        <v>38278</v>
       </c>
       <c r="D103" s="4">
         <f t="shared" si="3"/>
@@ -2056,13 +2013,10 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B104" s="4">
-        <v>40388</v>
+        <v>6</v>
       </c>
       <c r="C104" s="4">
-        <v>40388</v>
+        <v>38479</v>
       </c>
       <c r="D104" s="4">
         <f t="shared" si="3"/>
@@ -2071,13 +2025,10 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B105" s="4">
-        <v>40726</v>
+        <v>6</v>
       </c>
       <c r="C105" s="4">
-        <v>40726</v>
+        <v>38618</v>
       </c>
       <c r="D105" s="4">
         <f t="shared" si="3"/>
@@ -2086,13 +2037,10 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B106" s="4">
-        <v>40827</v>
+        <v>20</v>
       </c>
       <c r="C106" s="4">
-        <v>40827</v>
+        <v>40024</v>
       </c>
       <c r="D106" s="4">
         <f t="shared" si="3"/>
@@ -2101,36 +2049,34 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B107" s="4">
-        <v>41030</v>
+        <v>6</v>
       </c>
       <c r="C107" s="4">
-        <v>41030</v>
+        <v>40214</v>
       </c>
       <c r="D107" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="18.75">
-      <c r="A108" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B108" s="11"/>
-      <c r="C108" s="11"/>
-      <c r="D108" s="11"/>
+    <row r="108" spans="1:4">
+      <c r="A108" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C108" s="4">
+        <v>40388</v>
+      </c>
+      <c r="D108" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B109" s="4">
-        <v>41280</v>
+        <v>19</v>
       </c>
       <c r="C109" s="4">
-        <v>41280</v>
+        <v>40726</v>
       </c>
       <c r="D109" s="4">
         <f t="shared" si="3"/>
@@ -2139,13 +2085,10 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B110" s="4">
-        <v>42038</v>
+        <v>27</v>
       </c>
       <c r="C110" s="4">
-        <v>42038</v>
+        <v>40827</v>
       </c>
       <c r="D110" s="4">
         <f t="shared" si="3"/>
@@ -2154,61 +2097,42 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B111" s="4">
-        <v>42649</v>
+        <v>34</v>
       </c>
       <c r="C111" s="4">
-        <v>42649</v>
+        <v>41030</v>
       </c>
       <c r="D111" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:4">
-      <c r="A112" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B112" s="4">
-        <v>43208</v>
-      </c>
-      <c r="C112" s="4">
-        <v>43208</v>
-      </c>
-      <c r="D112" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
+    <row r="112" spans="1:4" ht="18.75">
+      <c r="A112" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B112" s="10"/>
+      <c r="C112" s="10"/>
+      <c r="D112" s="10"/>
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B113" s="4">
-        <v>43493</v>
+        <v>48</v>
       </c>
       <c r="C113" s="4">
-        <v>43493</v>
+        <v>41280</v>
       </c>
       <c r="D113" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
-      </c>
-      <c r="E113" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B114" s="4">
-        <v>43763</v>
-      </c>
       <c r="C114" s="4">
-        <v>43763</v>
+        <v>42038</v>
       </c>
       <c r="D114" s="4">
         <f t="shared" si="3"/>
@@ -2217,13 +2141,10 @@
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B115" s="4">
-        <v>44050</v>
+        <v>19</v>
       </c>
       <c r="C115" s="4">
-        <v>44050</v>
+        <v>42649</v>
       </c>
       <c r="D115" s="4">
         <f t="shared" si="3"/>
@@ -2232,36 +2153,37 @@
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B116" s="4">
-        <v>44254</v>
+        <v>19</v>
       </c>
       <c r="C116" s="4">
-        <v>44254</v>
+        <v>43208</v>
       </c>
       <c r="D116" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:5" ht="18.75">
-      <c r="A117" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B117" s="10"/>
-      <c r="C117" s="10"/>
-      <c r="D117" s="10"/>
+    <row r="117" spans="1:5">
+      <c r="A117" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C117" s="4">
+        <v>43493</v>
+      </c>
+      <c r="D117" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E117" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="118" spans="1:5">
       <c r="A118" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B118" s="4">
-        <v>44504</v>
+        <v>19</v>
       </c>
       <c r="C118" s="4">
-        <v>44504</v>
+        <v>43763</v>
       </c>
       <c r="D118" s="4">
         <f t="shared" si="3"/>
@@ -2270,13 +2192,10 @@
     </row>
     <row r="119" spans="1:5">
       <c r="A119" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B119" s="4">
-        <v>46191</v>
+        <v>27</v>
       </c>
       <c r="C119" s="4">
-        <v>46191</v>
+        <v>44050</v>
       </c>
       <c r="D119" s="4">
         <f t="shared" si="3"/>
@@ -2285,66 +2204,54 @@
     </row>
     <row r="120" spans="1:5">
       <c r="A120" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B120" s="4">
-        <v>48585</v>
+        <v>34</v>
       </c>
       <c r="C120" s="4">
-        <v>48585</v>
+        <v>44254</v>
       </c>
       <c r="D120" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:5">
-      <c r="A121" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B121" s="4">
-        <v>48941</v>
-      </c>
-      <c r="C121" s="4">
-        <v>48941</v>
-      </c>
-      <c r="D121" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
+    <row r="121" spans="1:5" ht="18.75">
+      <c r="A121" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B121" s="12"/>
+      <c r="C121" s="12"/>
+      <c r="D121" s="12"/>
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B122" s="4">
-        <v>49144</v>
+        <v>51</v>
       </c>
       <c r="C122" s="4">
-        <v>49144</v>
+        <v>44504</v>
       </c>
       <c r="D122" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:5" ht="18.75">
-      <c r="A123" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="B123" s="11"/>
-      <c r="C123" s="11"/>
-      <c r="D123" s="11"/>
+    <row r="123" spans="1:5">
+      <c r="A123" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C123" s="4">
+        <v>46191</v>
+      </c>
+      <c r="D123" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="124" spans="1:5">
       <c r="A124" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B124" s="4">
-        <v>49395</v>
+        <v>53</v>
       </c>
       <c r="C124" s="4">
-        <v>49395</v>
+        <v>48585</v>
       </c>
       <c r="D124" s="4">
         <f t="shared" si="3"/>
@@ -2353,13 +2260,10 @@
     </row>
     <row r="125" spans="1:5">
       <c r="A125" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B125" s="4">
-        <v>49704</v>
+        <v>27</v>
       </c>
       <c r="C125" s="4">
-        <v>49704</v>
+        <v>48941</v>
       </c>
       <c r="D125" s="4">
         <f t="shared" si="3"/>
@@ -2368,43 +2272,30 @@
     </row>
     <row r="126" spans="1:5">
       <c r="A126" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B126" s="4">
-        <v>49883</v>
+        <v>34</v>
       </c>
       <c r="C126" s="4">
-        <v>49883</v>
+        <v>49144</v>
       </c>
       <c r="D126" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:5">
-      <c r="A127" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B127" s="4">
-        <v>50088</v>
-      </c>
-      <c r="C127" s="4">
-        <v>50088</v>
-      </c>
-      <c r="D127" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
+    <row r="127" spans="1:5" ht="18.75">
+      <c r="A127" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B127" s="10"/>
+      <c r="C127" s="10"/>
+      <c r="D127" s="10"/>
     </row>
     <row r="128" spans="1:5">
       <c r="A128" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B128" s="4">
-        <v>50263</v>
+        <v>54</v>
       </c>
       <c r="C128" s="4">
-        <v>50263</v>
+        <v>49395</v>
       </c>
       <c r="D128" s="4">
         <f t="shared" si="3"/>
@@ -2413,13 +2304,10 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B129" s="4">
-        <v>50566</v>
+        <v>56</v>
       </c>
       <c r="C129" s="4">
-        <v>50566</v>
+        <v>49704</v>
       </c>
       <c r="D129" s="4">
         <f t="shared" si="3"/>
@@ -2428,13 +2316,10 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B130" s="4">
-        <v>50734</v>
+        <v>20</v>
       </c>
       <c r="C130" s="4">
-        <v>50734</v>
+        <v>49883</v>
       </c>
       <c r="D130" s="4">
         <f t="shared" si="3"/>
@@ -2445,11 +2330,8 @@
       <c r="A131" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B131" s="4">
-        <v>50849</v>
-      </c>
       <c r="C131" s="4">
-        <v>50849</v>
+        <v>50088</v>
       </c>
       <c r="D131" s="4">
         <f t="shared" si="3"/>
@@ -2458,13 +2340,10 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B132" s="4">
-        <v>51176</v>
+        <v>7</v>
       </c>
       <c r="C132" s="4">
-        <v>51176</v>
+        <v>50263</v>
       </c>
       <c r="D132" s="4">
         <f t="shared" si="3"/>
@@ -2475,11 +2354,8 @@
       <c r="A133" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B133" s="4">
-        <v>51327</v>
-      </c>
       <c r="C133" s="4">
-        <v>51327</v>
+        <v>50566</v>
       </c>
       <c r="D133" s="4">
         <f t="shared" si="3"/>
@@ -2488,13 +2364,10 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B134" s="4">
-        <v>51577</v>
+        <v>7</v>
       </c>
       <c r="C134" s="4">
-        <v>51577</v>
+        <v>50734</v>
       </c>
       <c r="D134" s="4">
         <f t="shared" si="3"/>
@@ -2503,13 +2376,10 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B135" s="4">
-        <v>51868</v>
+        <v>19</v>
       </c>
       <c r="C135" s="4">
-        <v>51868</v>
+        <v>50849</v>
       </c>
       <c r="D135" s="4">
         <f t="shared" si="3"/>
@@ -2518,36 +2388,34 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B136" s="4">
-        <v>52071</v>
+        <v>57</v>
       </c>
       <c r="C136" s="4">
-        <v>52071</v>
+        <v>51176</v>
       </c>
       <c r="D136" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="18.75">
-      <c r="A137" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="B137" s="10"/>
-      <c r="C137" s="10"/>
-      <c r="D137" s="10"/>
+    <row r="137" spans="1:4">
+      <c r="A137" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C137" s="4">
+        <v>51327</v>
+      </c>
+      <c r="D137" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B138" s="4">
-        <v>52322</v>
+        <v>6</v>
       </c>
       <c r="C138" s="4">
-        <v>52322</v>
+        <v>51577</v>
       </c>
       <c r="D138" s="4">
         <f t="shared" si="3"/>
@@ -2556,13 +2424,10 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B139" s="4">
-        <v>53245</v>
+        <v>27</v>
       </c>
       <c r="C139" s="4">
-        <v>53245</v>
+        <v>51868</v>
       </c>
       <c r="D139" s="4">
         <f t="shared" si="3"/>
@@ -2571,43 +2436,30 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B140" s="4">
-        <v>55063</v>
+        <v>34</v>
       </c>
       <c r="C140" s="4">
-        <v>55063</v>
+        <v>52071</v>
       </c>
       <c r="D140" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:4">
-      <c r="A141" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B141" s="4">
-        <v>55385</v>
-      </c>
-      <c r="C141" s="4">
-        <v>55385</v>
-      </c>
-      <c r="D141" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
+    <row r="141" spans="1:4" ht="18.75">
+      <c r="A141" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B141" s="12"/>
+      <c r="C141" s="12"/>
+      <c r="D141" s="12"/>
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B142" s="4">
-        <v>55706</v>
+        <v>58</v>
       </c>
       <c r="C142" s="4">
-        <v>55706</v>
+        <v>52322</v>
       </c>
       <c r="D142" s="4">
         <f t="shared" si="3"/>
@@ -2616,13 +2468,10 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B143" s="4">
-        <v>56029</v>
+        <v>26</v>
       </c>
       <c r="C143" s="4">
-        <v>56029</v>
+        <v>53245</v>
       </c>
       <c r="D143" s="4">
         <f t="shared" si="3"/>
@@ -2631,47 +2480,90 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C144" s="4">
+        <v>55063</v>
+      </c>
+      <c r="D144" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4">
+      <c r="A145" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C145" s="4">
+        <v>55385</v>
+      </c>
+      <c r="D145" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4">
+      <c r="A146" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C146" s="4">
+        <v>55706</v>
+      </c>
+      <c r="D146" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4">
+      <c r="A147" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C147" s="4">
+        <v>56029</v>
+      </c>
+      <c r="D147" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4">
+      <c r="A148" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B144" s="4">
+      <c r="C148" s="4">
         <v>58292</v>
       </c>
-      <c r="C144" s="4">
-        <v>58292</v>
-      </c>
-      <c r="D144" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3">
-      <c r="A145" s="4" t="s">
+      <c r="D148" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4">
+      <c r="A149" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B145" s="9">
-        <v>0.71250000000000002</v>
-      </c>
-      <c r="C145" s="9">
+      <c r="B149" s="9"/>
+      <c r="C149" s="9">
         <v>0.71250000000000002</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A121:D121"/>
+    <mergeCell ref="A127:D127"/>
+    <mergeCell ref="A141:D141"/>
+    <mergeCell ref="A51:D51"/>
+    <mergeCell ref="A64:D64"/>
+    <mergeCell ref="A76:D76"/>
+    <mergeCell ref="A85:D85"/>
+    <mergeCell ref="A90:D90"/>
+    <mergeCell ref="A112:D112"/>
     <mergeCell ref="A43:D43"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="A10:D10"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A31:D31"/>
-    <mergeCell ref="A117:D117"/>
-    <mergeCell ref="A123:D123"/>
-    <mergeCell ref="A137:D137"/>
-    <mergeCell ref="A51:D51"/>
-    <mergeCell ref="A64:D64"/>
-    <mergeCell ref="A76:D76"/>
-    <mergeCell ref="A81:D81"/>
-    <mergeCell ref="A86:D86"/>
-    <mergeCell ref="A108:D108"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -2708,12 +2600,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -2741,12 +2633,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -2780,12 +2672,12 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
@@ -2869,12 +2761,12 @@
       </c>
     </row>
     <row r="17" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="4" t="s">
@@ -3042,12 +2934,12 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="18.75">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="4" t="s">
@@ -3125,12 +3017,12 @@
       </c>
     </row>
     <row r="35" spans="1:10" ht="18.75">
-      <c r="A35" s="11" t="s">
+      <c r="A35" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="4" t="s">
@@ -3223,12 +3115,12 @@
       </c>
     </row>
     <row r="42" spans="1:10" ht="18.75">
-      <c r="A42" s="10" t="s">
+      <c r="A42" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B42" s="10"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="4" t="s">
@@ -3417,12 +3309,12 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="18.75">
-      <c r="A55" s="11" t="s">
+      <c r="A55" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B55" s="11"/>
-      <c r="C55" s="11"/>
-      <c r="D55" s="11"/>
+      <c r="B55" s="10"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="10"/>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="4" t="s">
@@ -3575,12 +3467,12 @@
       </c>
     </row>
     <row r="66" spans="1:4" ht="18.75">
-      <c r="A66" s="10" t="s">
+      <c r="A66" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B66" s="10"/>
-      <c r="C66" s="10"/>
-      <c r="D66" s="10"/>
+      <c r="B66" s="12"/>
+      <c r="C66" s="12"/>
+      <c r="D66" s="12"/>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="4" t="s">
@@ -3643,12 +3535,12 @@
       </c>
     </row>
     <row r="71" spans="1:4" ht="18.75">
-      <c r="A71" s="11" t="s">
+      <c r="A71" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B71" s="11"/>
-      <c r="C71" s="11"/>
-      <c r="D71" s="11"/>
+      <c r="B71" s="10"/>
+      <c r="C71" s="10"/>
+      <c r="D71" s="10"/>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="4" t="s">
@@ -3711,12 +3603,12 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="18.75">
-      <c r="A76" s="10" t="s">
+      <c r="A76" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B76" s="10"/>
-      <c r="C76" s="10"/>
-      <c r="D76" s="10"/>
+      <c r="B76" s="12"/>
+      <c r="C76" s="12"/>
+      <c r="D76" s="12"/>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="4" t="s">
@@ -4034,12 +3926,12 @@
       </c>
     </row>
     <row r="98" spans="1:5" ht="18.75">
-      <c r="A98" s="11" t="s">
+      <c r="A98" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="B98" s="11"/>
-      <c r="C98" s="11"/>
-      <c r="D98" s="11"/>
+      <c r="B98" s="10"/>
+      <c r="C98" s="10"/>
+      <c r="D98" s="10"/>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="4" t="s">
@@ -4165,12 +4057,12 @@
       </c>
     </row>
     <row r="107" spans="1:5" ht="18.75">
-      <c r="A107" s="10" t="s">
+      <c r="A107" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B107" s="10"/>
-      <c r="C107" s="10"/>
-      <c r="D107" s="10"/>
+      <c r="B107" s="12"/>
+      <c r="C107" s="12"/>
+      <c r="D107" s="12"/>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="4" t="s">
@@ -4248,12 +4140,12 @@
       </c>
     </row>
     <row r="113" spans="1:4" ht="18.75">
-      <c r="A113" s="11" t="s">
+      <c r="A113" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B113" s="11"/>
-      <c r="C113" s="11"/>
-      <c r="D113" s="11"/>
+      <c r="B113" s="10"/>
+      <c r="C113" s="10"/>
+      <c r="D113" s="10"/>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="4" t="s">
@@ -4451,12 +4343,12 @@
       </c>
     </row>
     <row r="127" spans="1:4" ht="18.75">
-      <c r="A127" s="10" t="s">
+      <c r="A127" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="B127" s="10"/>
-      <c r="C127" s="10"/>
-      <c r="D127" s="10"/>
+      <c r="B127" s="12"/>
+      <c r="C127" s="12"/>
+      <c r="D127" s="12"/>
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="4" t="s">
@@ -4576,6 +4468,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A29:D29"/>
     <mergeCell ref="A127:D127"/>
     <mergeCell ref="A107:D107"/>
     <mergeCell ref="A113:D113"/>
@@ -4586,11 +4483,6 @@
     <mergeCell ref="A98:D98"/>
     <mergeCell ref="A66:D66"/>
     <mergeCell ref="A55:D55"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A29:D29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>

</xml_diff>

<commit_message>
Wario - Level 10 begin.
</commit_message>
<xml_diff>
--- a/Wario/Wario.xlsx
+++ b/Wario/Wario.xlsx
@@ -332,9 +332,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -633,7 +633,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B87" sqref="B87"/>
+      <selection pane="bottomLeft" activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -657,12 +657,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -690,12 +690,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -729,12 +729,12 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
@@ -857,12 +857,12 @@
       </c>
     </row>
     <row r="19" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="4" t="s">
@@ -1030,12 +1030,12 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="18.75">
-      <c r="A31" s="12" t="s">
+      <c r="A31" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="4" t="s">
@@ -1203,12 +1203,12 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="18.75">
-      <c r="A43" s="10" t="s">
+      <c r="A43" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B43" s="10"/>
-      <c r="C43" s="10"/>
-      <c r="D43" s="10"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="4" t="s">
@@ -1316,12 +1316,12 @@
       </c>
     </row>
     <row r="51" spans="1:10" ht="18.75">
-      <c r="A51" s="12" t="s">
+      <c r="A51" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B51" s="12"/>
-      <c r="C51" s="12"/>
-      <c r="D51" s="12"/>
+      <c r="B51" s="10"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="4" t="s">
@@ -1507,12 +1507,12 @@
       </c>
     </row>
     <row r="64" spans="1:10" ht="18.75">
-      <c r="A64" s="10" t="s">
+      <c r="A64" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B64" s="10"/>
-      <c r="C64" s="10"/>
-      <c r="D64" s="10"/>
+      <c r="B64" s="11"/>
+      <c r="C64" s="11"/>
+      <c r="D64" s="11"/>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="4" t="s">
@@ -1671,12 +1671,12 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="18.75">
-      <c r="A76" s="12" t="s">
+      <c r="A76" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B76" s="12"/>
-      <c r="C76" s="12"/>
-      <c r="D76" s="12"/>
+      <c r="B76" s="10"/>
+      <c r="C76" s="10"/>
+      <c r="D76" s="10"/>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="4" t="s">
@@ -1789,12 +1789,12 @@
       </c>
     </row>
     <row r="85" spans="1:4" ht="18.75">
-      <c r="A85" s="10" t="s">
+      <c r="A85" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B85" s="10"/>
-      <c r="C85" s="10"/>
-      <c r="D85" s="10"/>
+      <c r="B85" s="11"/>
+      <c r="C85" s="11"/>
+      <c r="D85" s="11"/>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="4" t="s">
@@ -1827,44 +1827,53 @@
       <c r="A88" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="B88" s="4">
+        <v>33405</v>
+      </c>
       <c r="C88" s="4">
         <v>35373</v>
       </c>
       <c r="D88" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="B89" s="4">
+        <v>33609</v>
+      </c>
       <c r="C89" s="4">
         <v>35577</v>
       </c>
       <c r="D89" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="18.75">
-      <c r="A90" s="12" t="s">
+      <c r="A90" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B90" s="12"/>
-      <c r="C90" s="12"/>
-      <c r="D90" s="12"/>
+      <c r="B90" s="10"/>
+      <c r="C90" s="10"/>
+      <c r="D90" s="10"/>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="4" t="s">
         <v>43</v>
       </c>
+      <c r="B91" s="4">
+        <v>33858</v>
+      </c>
       <c r="C91" s="4">
         <v>35826</v>
       </c>
       <c r="D91" s="4">
         <f t="shared" ref="D91:D148" si="3">IF(B91 &gt;  0,C91-B91, 0)</f>
-        <v>0</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -2108,12 +2117,12 @@
       </c>
     </row>
     <row r="112" spans="1:4" ht="18.75">
-      <c r="A112" s="10" t="s">
+      <c r="A112" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B112" s="10"/>
-      <c r="C112" s="10"/>
-      <c r="D112" s="10"/>
+      <c r="B112" s="11"/>
+      <c r="C112" s="11"/>
+      <c r="D112" s="11"/>
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="4" t="s">
@@ -2215,12 +2224,12 @@
       </c>
     </row>
     <row r="121" spans="1:5" ht="18.75">
-      <c r="A121" s="12" t="s">
+      <c r="A121" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B121" s="12"/>
-      <c r="C121" s="12"/>
-      <c r="D121" s="12"/>
+      <c r="B121" s="10"/>
+      <c r="C121" s="10"/>
+      <c r="D121" s="10"/>
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="4" t="s">
@@ -2283,12 +2292,12 @@
       </c>
     </row>
     <row r="127" spans="1:5" ht="18.75">
-      <c r="A127" s="10" t="s">
+      <c r="A127" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B127" s="10"/>
-      <c r="C127" s="10"/>
-      <c r="D127" s="10"/>
+      <c r="B127" s="11"/>
+      <c r="C127" s="11"/>
+      <c r="D127" s="11"/>
     </row>
     <row r="128" spans="1:5">
       <c r="A128" s="4" t="s">
@@ -2447,12 +2456,12 @@
       </c>
     </row>
     <row r="141" spans="1:4" ht="18.75">
-      <c r="A141" s="12" t="s">
+      <c r="A141" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B141" s="12"/>
-      <c r="C141" s="12"/>
-      <c r="D141" s="12"/>
+      <c r="B141" s="10"/>
+      <c r="C141" s="10"/>
+      <c r="D141" s="10"/>
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="4" t="s">
@@ -2549,6 +2558,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A31:D31"/>
     <mergeCell ref="A121:D121"/>
     <mergeCell ref="A127:D127"/>
     <mergeCell ref="A141:D141"/>
@@ -2558,12 +2573,6 @@
     <mergeCell ref="A85:D85"/>
     <mergeCell ref="A90:D90"/>
     <mergeCell ref="A112:D112"/>
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A31:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -2600,12 +2609,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -2633,12 +2642,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -2672,12 +2681,12 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
@@ -2761,12 +2770,12 @@
       </c>
     </row>
     <row r="17" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="4" t="s">
@@ -2934,12 +2943,12 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="18.75">
-      <c r="A29" s="12" t="s">
+      <c r="A29" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="4" t="s">
@@ -3017,12 +3026,12 @@
       </c>
     </row>
     <row r="35" spans="1:10" ht="18.75">
-      <c r="A35" s="10" t="s">
+      <c r="A35" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="4" t="s">
@@ -3115,12 +3124,12 @@
       </c>
     </row>
     <row r="42" spans="1:10" ht="18.75">
-      <c r="A42" s="12" t="s">
+      <c r="A42" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B42" s="12"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="4" t="s">
@@ -3309,12 +3318,12 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="18.75">
-      <c r="A55" s="10" t="s">
+      <c r="A55" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B55" s="10"/>
-      <c r="C55" s="10"/>
-      <c r="D55" s="10"/>
+      <c r="B55" s="11"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="11"/>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="4" t="s">
@@ -3467,12 +3476,12 @@
       </c>
     </row>
     <row r="66" spans="1:4" ht="18.75">
-      <c r="A66" s="12" t="s">
+      <c r="A66" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B66" s="12"/>
-      <c r="C66" s="12"/>
-      <c r="D66" s="12"/>
+      <c r="B66" s="10"/>
+      <c r="C66" s="10"/>
+      <c r="D66" s="10"/>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="4" t="s">
@@ -3535,12 +3544,12 @@
       </c>
     </row>
     <row r="71" spans="1:4" ht="18.75">
-      <c r="A71" s="10" t="s">
+      <c r="A71" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B71" s="10"/>
-      <c r="C71" s="10"/>
-      <c r="D71" s="10"/>
+      <c r="B71" s="11"/>
+      <c r="C71" s="11"/>
+      <c r="D71" s="11"/>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="4" t="s">
@@ -3603,12 +3612,12 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="18.75">
-      <c r="A76" s="12" t="s">
+      <c r="A76" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B76" s="12"/>
-      <c r="C76" s="12"/>
-      <c r="D76" s="12"/>
+      <c r="B76" s="10"/>
+      <c r="C76" s="10"/>
+      <c r="D76" s="10"/>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="4" t="s">
@@ -3926,12 +3935,12 @@
       </c>
     </row>
     <row r="98" spans="1:5" ht="18.75">
-      <c r="A98" s="10" t="s">
+      <c r="A98" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B98" s="10"/>
-      <c r="C98" s="10"/>
-      <c r="D98" s="10"/>
+      <c r="B98" s="11"/>
+      <c r="C98" s="11"/>
+      <c r="D98" s="11"/>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="4" t="s">
@@ -4057,12 +4066,12 @@
       </c>
     </row>
     <row r="107" spans="1:5" ht="18.75">
-      <c r="A107" s="12" t="s">
+      <c r="A107" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B107" s="12"/>
-      <c r="C107" s="12"/>
-      <c r="D107" s="12"/>
+      <c r="B107" s="10"/>
+      <c r="C107" s="10"/>
+      <c r="D107" s="10"/>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="4" t="s">
@@ -4140,12 +4149,12 @@
       </c>
     </row>
     <row r="113" spans="1:4" ht="18.75">
-      <c r="A113" s="10" t="s">
+      <c r="A113" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B113" s="10"/>
-      <c r="C113" s="10"/>
-      <c r="D113" s="10"/>
+      <c r="B113" s="11"/>
+      <c r="C113" s="11"/>
+      <c r="D113" s="11"/>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="4" t="s">
@@ -4343,12 +4352,12 @@
       </c>
     </row>
     <row r="127" spans="1:4" ht="18.75">
-      <c r="A127" s="12" t="s">
+      <c r="A127" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B127" s="12"/>
-      <c r="C127" s="12"/>
-      <c r="D127" s="12"/>
+      <c r="B127" s="10"/>
+      <c r="C127" s="10"/>
+      <c r="D127" s="10"/>
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="4" t="s">
@@ -4468,11 +4477,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A29:D29"/>
     <mergeCell ref="A127:D127"/>
     <mergeCell ref="A107:D107"/>
     <mergeCell ref="A113:D113"/>
@@ -4483,6 +4487,11 @@
     <mergeCell ref="A98:D98"/>
     <mergeCell ref="A66:D66"/>
     <mergeCell ref="A55:D55"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A29:D29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>

</xml_diff>

<commit_message>
Wario - Level 10 and some of Level 11 done (mostly copy/pasting).
</commit_message>
<xml_diff>
--- a/Wario/Wario.xlsx
+++ b/Wario/Wario.xlsx
@@ -332,9 +332,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -632,8 +632,8 @@
   <dimension ref="A1:J149"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B92" sqref="B92"/>
+      <pane ySplit="1" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B116" sqref="B116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -657,12 +657,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -690,12 +690,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -729,12 +729,12 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
@@ -857,12 +857,12 @@
       </c>
     </row>
     <row r="19" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="4" t="s">
@@ -1030,12 +1030,12 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="18.75">
-      <c r="A31" s="10" t="s">
+      <c r="A31" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="4" t="s">
@@ -1203,12 +1203,12 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="18.75">
-      <c r="A43" s="11" t="s">
+      <c r="A43" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B43" s="11"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="4" t="s">
@@ -1316,12 +1316,12 @@
       </c>
     </row>
     <row r="51" spans="1:10" ht="18.75">
-      <c r="A51" s="10" t="s">
+      <c r="A51" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B51" s="10"/>
-      <c r="C51" s="10"/>
-      <c r="D51" s="10"/>
+      <c r="B51" s="12"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="12"/>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="4" t="s">
@@ -1507,12 +1507,12 @@
       </c>
     </row>
     <row r="64" spans="1:10" ht="18.75">
-      <c r="A64" s="11" t="s">
+      <c r="A64" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B64" s="11"/>
-      <c r="C64" s="11"/>
-      <c r="D64" s="11"/>
+      <c r="B64" s="10"/>
+      <c r="C64" s="10"/>
+      <c r="D64" s="10"/>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="4" t="s">
@@ -1671,12 +1671,12 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="18.75">
-      <c r="A76" s="10" t="s">
+      <c r="A76" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B76" s="10"/>
-      <c r="C76" s="10"/>
-      <c r="D76" s="10"/>
+      <c r="B76" s="12"/>
+      <c r="C76" s="12"/>
+      <c r="D76" s="12"/>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="4" t="s">
@@ -1789,12 +1789,12 @@
       </c>
     </row>
     <row r="85" spans="1:4" ht="18.75">
-      <c r="A85" s="11" t="s">
+      <c r="A85" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B85" s="11"/>
-      <c r="C85" s="11"/>
-      <c r="D85" s="11"/>
+      <c r="B85" s="10"/>
+      <c r="C85" s="10"/>
+      <c r="D85" s="10"/>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="4" t="s">
@@ -1854,12 +1854,12 @@
       </c>
     </row>
     <row r="90" spans="1:4" ht="18.75">
-      <c r="A90" s="10" t="s">
+      <c r="A90" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B90" s="10"/>
-      <c r="C90" s="10"/>
-      <c r="D90" s="10"/>
+      <c r="B90" s="12"/>
+      <c r="C90" s="12"/>
+      <c r="D90" s="12"/>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="4" t="s">
@@ -1916,12 +1916,15 @@
       <c r="A95" s="4" t="s">
         <v>45</v>
       </c>
+      <c r="B95" s="4">
+        <v>3</v>
+      </c>
       <c r="C95" s="4">
         <v>36538</v>
       </c>
       <c r="D95" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>36535</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -1952,48 +1955,60 @@
       <c r="A98" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="B98" s="4">
+        <v>35512</v>
+      </c>
       <c r="C98" s="4">
         <v>37481</v>
       </c>
       <c r="D98" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1969</v>
       </c>
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="B99" s="4">
+        <v>35693</v>
+      </c>
       <c r="C99" s="4">
         <v>37662</v>
       </c>
       <c r="D99" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1969</v>
       </c>
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="B100" s="4">
+        <v>35847</v>
+      </c>
       <c r="C100" s="4">
         <v>37816</v>
       </c>
       <c r="D100" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1969</v>
       </c>
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="B101" s="4">
+        <v>36020</v>
+      </c>
       <c r="C101" s="4">
         <v>37986</v>
       </c>
       <c r="D101" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1966</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -2048,116 +2063,143 @@
       <c r="A106" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="B106" s="4">
+        <v>38056</v>
+      </c>
       <c r="C106" s="4">
         <v>40024</v>
       </c>
       <c r="D106" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="B107" s="4">
+        <v>38245</v>
+      </c>
       <c r="C107" s="4">
         <v>40214</v>
       </c>
       <c r="D107" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1969</v>
       </c>
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="B108" s="4">
+        <v>38420</v>
+      </c>
       <c r="C108" s="4">
         <v>40388</v>
       </c>
       <c r="D108" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="B109" s="4">
+        <v>38758</v>
+      </c>
       <c r="C109" s="4">
         <v>40726</v>
       </c>
       <c r="D109" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="B110" s="4">
+        <v>38859</v>
+      </c>
       <c r="C110" s="4">
         <v>40827</v>
       </c>
       <c r="D110" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="B111" s="4">
+        <v>39062</v>
+      </c>
       <c r="C111" s="4">
         <v>41030</v>
       </c>
       <c r="D111" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="18.75">
-      <c r="A112" s="11" t="s">
+      <c r="A112" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="B112" s="11"/>
-      <c r="C112" s="11"/>
-      <c r="D112" s="11"/>
+      <c r="B112" s="10"/>
+      <c r="C112" s="10"/>
+      <c r="D112" s="10"/>
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="4" t="s">
         <v>48</v>
       </c>
+      <c r="B113" s="4">
+        <v>39312</v>
+      </c>
       <c r="C113" s="4">
         <v>41280</v>
       </c>
       <c r="D113" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="B114" s="4">
+        <v>40069</v>
+      </c>
       <c r="C114" s="4">
         <v>42038</v>
       </c>
       <c r="D114" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1969</v>
       </c>
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="B115" s="4">
+        <v>40681</v>
+      </c>
       <c r="C115" s="4">
         <v>42649</v>
       </c>
       <c r="D115" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="116" spans="1:5">
@@ -2224,12 +2266,12 @@
       </c>
     </row>
     <row r="121" spans="1:5" ht="18.75">
-      <c r="A121" s="10" t="s">
+      <c r="A121" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B121" s="10"/>
-      <c r="C121" s="10"/>
-      <c r="D121" s="10"/>
+      <c r="B121" s="12"/>
+      <c r="C121" s="12"/>
+      <c r="D121" s="12"/>
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="4" t="s">
@@ -2292,12 +2334,12 @@
       </c>
     </row>
     <row r="127" spans="1:5" ht="18.75">
-      <c r="A127" s="11" t="s">
+      <c r="A127" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B127" s="11"/>
-      <c r="C127" s="11"/>
-      <c r="D127" s="11"/>
+      <c r="B127" s="10"/>
+      <c r="C127" s="10"/>
+      <c r="D127" s="10"/>
     </row>
     <row r="128" spans="1:5">
       <c r="A128" s="4" t="s">
@@ -2456,12 +2498,12 @@
       </c>
     </row>
     <row r="141" spans="1:4" ht="18.75">
-      <c r="A141" s="10" t="s">
+      <c r="A141" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="B141" s="10"/>
-      <c r="C141" s="10"/>
-      <c r="D141" s="10"/>
+      <c r="B141" s="12"/>
+      <c r="C141" s="12"/>
+      <c r="D141" s="12"/>
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="4" t="s">
@@ -2558,12 +2600,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A31:D31"/>
     <mergeCell ref="A121:D121"/>
     <mergeCell ref="A127:D127"/>
     <mergeCell ref="A141:D141"/>
@@ -2573,6 +2609,12 @@
     <mergeCell ref="A85:D85"/>
     <mergeCell ref="A90:D90"/>
     <mergeCell ref="A112:D112"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A31:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -2609,12 +2651,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -2642,12 +2684,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -2681,12 +2723,12 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
@@ -2770,12 +2812,12 @@
       </c>
     </row>
     <row r="17" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="4" t="s">
@@ -2943,12 +2985,12 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="18.75">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="4" t="s">
@@ -3026,12 +3068,12 @@
       </c>
     </row>
     <row r="35" spans="1:10" ht="18.75">
-      <c r="A35" s="11" t="s">
+      <c r="A35" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="4" t="s">
@@ -3124,12 +3166,12 @@
       </c>
     </row>
     <row r="42" spans="1:10" ht="18.75">
-      <c r="A42" s="10" t="s">
+      <c r="A42" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B42" s="10"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="4" t="s">
@@ -3318,12 +3360,12 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="18.75">
-      <c r="A55" s="11" t="s">
+      <c r="A55" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B55" s="11"/>
-      <c r="C55" s="11"/>
-      <c r="D55" s="11"/>
+      <c r="B55" s="10"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="10"/>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="4" t="s">
@@ -3476,12 +3518,12 @@
       </c>
     </row>
     <row r="66" spans="1:4" ht="18.75">
-      <c r="A66" s="10" t="s">
+      <c r="A66" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B66" s="10"/>
-      <c r="C66" s="10"/>
-      <c r="D66" s="10"/>
+      <c r="B66" s="12"/>
+      <c r="C66" s="12"/>
+      <c r="D66" s="12"/>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="4" t="s">
@@ -3544,12 +3586,12 @@
       </c>
     </row>
     <row r="71" spans="1:4" ht="18.75">
-      <c r="A71" s="11" t="s">
+      <c r="A71" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B71" s="11"/>
-      <c r="C71" s="11"/>
-      <c r="D71" s="11"/>
+      <c r="B71" s="10"/>
+      <c r="C71" s="10"/>
+      <c r="D71" s="10"/>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="4" t="s">
@@ -3612,12 +3654,12 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="18.75">
-      <c r="A76" s="10" t="s">
+      <c r="A76" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B76" s="10"/>
-      <c r="C76" s="10"/>
-      <c r="D76" s="10"/>
+      <c r="B76" s="12"/>
+      <c r="C76" s="12"/>
+      <c r="D76" s="12"/>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="4" t="s">
@@ -3935,12 +3977,12 @@
       </c>
     </row>
     <row r="98" spans="1:5" ht="18.75">
-      <c r="A98" s="11" t="s">
+      <c r="A98" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="B98" s="11"/>
-      <c r="C98" s="11"/>
-      <c r="D98" s="11"/>
+      <c r="B98" s="10"/>
+      <c r="C98" s="10"/>
+      <c r="D98" s="10"/>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="4" t="s">
@@ -4066,12 +4108,12 @@
       </c>
     </row>
     <row r="107" spans="1:5" ht="18.75">
-      <c r="A107" s="10" t="s">
+      <c r="A107" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B107" s="10"/>
-      <c r="C107" s="10"/>
-      <c r="D107" s="10"/>
+      <c r="B107" s="12"/>
+      <c r="C107" s="12"/>
+      <c r="D107" s="12"/>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="4" t="s">
@@ -4149,12 +4191,12 @@
       </c>
     </row>
     <row r="113" spans="1:4" ht="18.75">
-      <c r="A113" s="11" t="s">
+      <c r="A113" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B113" s="11"/>
-      <c r="C113" s="11"/>
-      <c r="D113" s="11"/>
+      <c r="B113" s="10"/>
+      <c r="C113" s="10"/>
+      <c r="D113" s="10"/>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="4" t="s">
@@ -4352,12 +4394,12 @@
       </c>
     </row>
     <row r="127" spans="1:4" ht="18.75">
-      <c r="A127" s="10" t="s">
+      <c r="A127" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="B127" s="10"/>
-      <c r="C127" s="10"/>
-      <c r="D127" s="10"/>
+      <c r="B127" s="12"/>
+      <c r="C127" s="12"/>
+      <c r="D127" s="12"/>
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="4" t="s">
@@ -4477,6 +4519,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A29:D29"/>
     <mergeCell ref="A127:D127"/>
     <mergeCell ref="A107:D107"/>
     <mergeCell ref="A113:D113"/>
@@ -4487,11 +4534,6 @@
     <mergeCell ref="A98:D98"/>
     <mergeCell ref="A66:D66"/>
     <mergeCell ref="A55:D55"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A29:D29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>

</xml_diff>

<commit_message>
Wario - Level 12 begin
</commit_message>
<xml_diff>
--- a/Wario/Wario.xlsx
+++ b/Wario/Wario.xlsx
@@ -632,8 +632,8 @@
   <dimension ref="A1:J149"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B116" sqref="B116"/>
+      <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B123" sqref="B123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1872,7 +1872,7 @@
         <v>35826</v>
       </c>
       <c r="D91" s="4">
-        <f t="shared" ref="D91:D148" si="3">IF(B91 &gt;  0,C91-B91, 0)</f>
+        <f t="shared" ref="D91:D150" si="3">IF(B91 &gt;  0,C91-B91, 0)</f>
         <v>1968</v>
       </c>
     </row>
@@ -2206,24 +2206,30 @@
       <c r="A116" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="B116" s="4">
+        <v>41240</v>
+      </c>
       <c r="C116" s="4">
         <v>43208</v>
       </c>
       <c r="D116" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="B117" s="4">
+        <v>41469</v>
+      </c>
       <c r="C117" s="4">
         <v>43493</v>
       </c>
       <c r="D117" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2024</v>
       </c>
       <c r="E117" t="s">
         <v>50</v>
@@ -2233,36 +2239,45 @@
       <c r="A118" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="B118" s="4">
+        <v>41728</v>
+      </c>
       <c r="C118" s="4">
         <v>43763</v>
       </c>
       <c r="D118" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2035</v>
       </c>
     </row>
     <row r="119" spans="1:5">
       <c r="A119" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="B119" s="4">
+        <v>42015</v>
+      </c>
       <c r="C119" s="4">
         <v>44050</v>
       </c>
       <c r="D119" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2035</v>
       </c>
     </row>
     <row r="120" spans="1:5">
       <c r="A120" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="B120" s="4">
+        <v>42219</v>
+      </c>
       <c r="C120" s="4">
         <v>44254</v>
       </c>
       <c r="D120" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2035</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="18.75">
@@ -2277,12 +2292,15 @@
       <c r="A122" s="4" t="s">
         <v>51</v>
       </c>
+      <c r="B122" s="4">
+        <v>42469</v>
+      </c>
       <c r="C122" s="4">
         <v>44504</v>
       </c>
       <c r="D122" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2035</v>
       </c>
     </row>
     <row r="123" spans="1:5">

</xml_diff>

<commit_message>
Wario - Level 12 and some of 13 done.
</commit_message>
<xml_diff>
--- a/Wario/Wario.xlsx
+++ b/Wario/Wario.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="70">
   <si>
     <t>Enter pipe</t>
   </si>
@@ -332,9 +332,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -629,11 +629,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J149"/>
+  <dimension ref="A1:J151"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B123" sqref="B123"/>
+      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B134" sqref="B134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -657,12 +657,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -690,12 +690,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -729,12 +729,12 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
@@ -857,12 +857,12 @@
       </c>
     </row>
     <row r="19" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="4" t="s">
@@ -1030,12 +1030,12 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="18.75">
-      <c r="A31" s="12" t="s">
+      <c r="A31" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="4" t="s">
@@ -1203,12 +1203,12 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="18.75">
-      <c r="A43" s="10" t="s">
+      <c r="A43" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B43" s="10"/>
-      <c r="C43" s="10"/>
-      <c r="D43" s="10"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="4" t="s">
@@ -1316,12 +1316,12 @@
       </c>
     </row>
     <row r="51" spans="1:10" ht="18.75">
-      <c r="A51" s="12" t="s">
+      <c r="A51" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B51" s="12"/>
-      <c r="C51" s="12"/>
-      <c r="D51" s="12"/>
+      <c r="B51" s="10"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="4" t="s">
@@ -1507,12 +1507,12 @@
       </c>
     </row>
     <row r="64" spans="1:10" ht="18.75">
-      <c r="A64" s="10" t="s">
+      <c r="A64" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B64" s="10"/>
-      <c r="C64" s="10"/>
-      <c r="D64" s="10"/>
+      <c r="B64" s="11"/>
+      <c r="C64" s="11"/>
+      <c r="D64" s="11"/>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="4" t="s">
@@ -1671,12 +1671,12 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="18.75">
-      <c r="A76" s="12" t="s">
+      <c r="A76" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B76" s="12"/>
-      <c r="C76" s="12"/>
-      <c r="D76" s="12"/>
+      <c r="B76" s="10"/>
+      <c r="C76" s="10"/>
+      <c r="D76" s="10"/>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="4" t="s">
@@ -1789,12 +1789,12 @@
       </c>
     </row>
     <row r="85" spans="1:4" ht="18.75">
-      <c r="A85" s="10" t="s">
+      <c r="A85" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B85" s="10"/>
-      <c r="C85" s="10"/>
-      <c r="D85" s="10"/>
+      <c r="B85" s="11"/>
+      <c r="C85" s="11"/>
+      <c r="D85" s="11"/>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="4" t="s">
@@ -1854,12 +1854,12 @@
       </c>
     </row>
     <row r="90" spans="1:4" ht="18.75">
-      <c r="A90" s="12" t="s">
+      <c r="A90" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B90" s="12"/>
-      <c r="C90" s="12"/>
-      <c r="D90" s="12"/>
+      <c r="B90" s="10"/>
+      <c r="C90" s="10"/>
+      <c r="D90" s="10"/>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="4" t="s">
@@ -2150,12 +2150,12 @@
       </c>
     </row>
     <row r="112" spans="1:4" ht="18.75">
-      <c r="A112" s="10" t="s">
+      <c r="A112" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B112" s="10"/>
-      <c r="C112" s="10"/>
-      <c r="D112" s="10"/>
+      <c r="B112" s="11"/>
+      <c r="C112" s="11"/>
+      <c r="D112" s="11"/>
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="4" t="s">
@@ -2281,12 +2281,12 @@
       </c>
     </row>
     <row r="121" spans="1:5" ht="18.75">
-      <c r="A121" s="12" t="s">
+      <c r="A121" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B121" s="12"/>
-      <c r="C121" s="12"/>
-      <c r="D121" s="12"/>
+      <c r="B121" s="10"/>
+      <c r="C121" s="10"/>
+      <c r="D121" s="10"/>
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="4" t="s">
@@ -2305,130 +2305,160 @@
     </row>
     <row r="123" spans="1:5">
       <c r="A123" s="4" t="s">
-        <v>26</v>
+        <v>66</v>
+      </c>
+      <c r="B123" s="4">
+        <v>43196</v>
       </c>
       <c r="C123" s="4">
-        <v>46191</v>
+        <v>45232</v>
       </c>
       <c r="D123" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2036</v>
       </c>
     </row>
     <row r="124" spans="1:5">
       <c r="A124" s="4" t="s">
-        <v>53</v>
+        <v>60</v>
+      </c>
+      <c r="B124" s="4">
+        <v>43848</v>
       </c>
       <c r="C124" s="4">
-        <v>48585</v>
+        <v>45885</v>
       </c>
       <c r="D124" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2037</v>
       </c>
     </row>
     <row r="125" spans="1:5">
       <c r="A125" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="B125" s="4">
+        <v>44155</v>
       </c>
       <c r="C125" s="4">
-        <v>48941</v>
+        <v>46191</v>
       </c>
       <c r="D125" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2036</v>
       </c>
     </row>
     <row r="126" spans="1:5">
       <c r="A126" s="4" t="s">
-        <v>34</v>
+        <v>53</v>
+      </c>
+      <c r="B126" s="4">
+        <v>46549</v>
       </c>
       <c r="C126" s="4">
-        <v>49144</v>
+        <v>48585</v>
       </c>
       <c r="D126" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" ht="18.75">
-      <c r="A127" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="B127" s="10"/>
-      <c r="C127" s="10"/>
-      <c r="D127" s="10"/>
+        <v>2036</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5">
+      <c r="A127" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B127" s="4">
+        <v>46905</v>
+      </c>
+      <c r="C127" s="4">
+        <v>48941</v>
+      </c>
+      <c r="D127" s="4">
+        <f t="shared" si="3"/>
+        <v>2036</v>
+      </c>
     </row>
     <row r="128" spans="1:5">
       <c r="A128" s="4" t="s">
-        <v>54</v>
+        <v>34</v>
+      </c>
+      <c r="B128" s="4">
+        <v>47108</v>
       </c>
       <c r="C128" s="4">
-        <v>49395</v>
+        <v>49144</v>
       </c>
       <c r="D128" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4">
-      <c r="A129" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C129" s="4">
-        <v>49704</v>
-      </c>
-      <c r="D129" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
+        <v>2036</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" ht="18.75">
+      <c r="A129" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B129" s="11"/>
+      <c r="C129" s="11"/>
+      <c r="D129" s="11"/>
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="4" t="s">
-        <v>20</v>
+        <v>54</v>
+      </c>
+      <c r="B130" s="4">
+        <v>47359</v>
       </c>
       <c r="C130" s="4">
-        <v>49883</v>
+        <v>49395</v>
       </c>
       <c r="D130" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2036</v>
       </c>
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="4" t="s">
-        <v>19</v>
+        <v>56</v>
+      </c>
+      <c r="B131" s="4">
+        <v>47668</v>
       </c>
       <c r="C131" s="4">
-        <v>50088</v>
+        <v>49704</v>
       </c>
       <c r="D131" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2036</v>
       </c>
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="4" t="s">
-        <v>7</v>
+        <v>20</v>
+      </c>
+      <c r="B132" s="4">
+        <v>47847</v>
       </c>
       <c r="C132" s="4">
-        <v>50263</v>
+        <v>49883</v>
       </c>
       <c r="D132" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2036</v>
       </c>
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="4" t="s">
-        <v>6</v>
+        <v>19</v>
+      </c>
+      <c r="B133" s="4">
+        <v>48052</v>
       </c>
       <c r="C133" s="4">
-        <v>50566</v>
+        <v>50088</v>
       </c>
       <c r="D133" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2036</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -2436,7 +2466,7 @@
         <v>7</v>
       </c>
       <c r="C134" s="4">
-        <v>50734</v>
+        <v>50263</v>
       </c>
       <c r="D134" s="4">
         <f t="shared" si="3"/>
@@ -2445,10 +2475,10 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="4" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="C135" s="4">
-        <v>50849</v>
+        <v>50566</v>
       </c>
       <c r="D135" s="4">
         <f t="shared" si="3"/>
@@ -2457,10 +2487,10 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="4" t="s">
-        <v>57</v>
+        <v>7</v>
       </c>
       <c r="C136" s="4">
-        <v>51176</v>
+        <v>50734</v>
       </c>
       <c r="D136" s="4">
         <f t="shared" si="3"/>
@@ -2469,10 +2499,10 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="4" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="C137" s="4">
-        <v>51327</v>
+        <v>50849</v>
       </c>
       <c r="D137" s="4">
         <f t="shared" si="3"/>
@@ -2481,10 +2511,10 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="4" t="s">
-        <v>6</v>
+        <v>57</v>
       </c>
       <c r="C138" s="4">
-        <v>51577</v>
+        <v>51176</v>
       </c>
       <c r="D138" s="4">
         <f t="shared" si="3"/>
@@ -2493,10 +2523,10 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="4" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="C139" s="4">
-        <v>51868</v>
+        <v>51327</v>
       </c>
       <c r="D139" s="4">
         <f t="shared" si="3"/>
@@ -2505,54 +2535,54 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="4" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="C140" s="4">
-        <v>52071</v>
+        <v>51577</v>
       </c>
       <c r="D140" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:4" ht="18.75">
-      <c r="A141" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="B141" s="12"/>
-      <c r="C141" s="12"/>
-      <c r="D141" s="12"/>
+    <row r="141" spans="1:4">
+      <c r="A141" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C141" s="4">
+        <v>51868</v>
+      </c>
+      <c r="D141" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="4" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="C142" s="4">
-        <v>52322</v>
+        <v>52071</v>
       </c>
       <c r="D142" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:4">
-      <c r="A143" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C143" s="4">
-        <v>53245</v>
-      </c>
-      <c r="D143" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
+    <row r="143" spans="1:4" ht="18.75">
+      <c r="A143" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B143" s="10"/>
+      <c r="C143" s="10"/>
+      <c r="D143" s="10"/>
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C144" s="4">
-        <v>55063</v>
+        <v>52322</v>
       </c>
       <c r="D144" s="4">
         <f t="shared" si="3"/>
@@ -2561,10 +2591,10 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="4" t="s">
-        <v>62</v>
+        <v>26</v>
       </c>
       <c r="C145" s="4">
-        <v>55385</v>
+        <v>53245</v>
       </c>
       <c r="D145" s="4">
         <f t="shared" si="3"/>
@@ -2573,10 +2603,10 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C146" s="4">
-        <v>55706</v>
+        <v>55063</v>
       </c>
       <c r="D146" s="4">
         <f t="shared" si="3"/>
@@ -2585,10 +2615,10 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C147" s="4">
-        <v>56029</v>
+        <v>55385</v>
       </c>
       <c r="D147" s="4">
         <f t="shared" si="3"/>
@@ -2597,10 +2627,10 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C148" s="4">
-        <v>58292</v>
+        <v>55706</v>
       </c>
       <c r="D148" s="4">
         <f t="shared" si="3"/>
@@ -2609,30 +2639,54 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C149" s="4">
+        <v>56029</v>
+      </c>
+      <c r="D149" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4">
+      <c r="A150" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C150" s="4">
+        <v>58292</v>
+      </c>
+      <c r="D150" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4">
+      <c r="A151" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B149" s="9"/>
-      <c r="C149" s="9">
+      <c r="B151" s="9"/>
+      <c r="C151" s="9">
         <v>0.71250000000000002</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A31:D31"/>
     <mergeCell ref="A121:D121"/>
-    <mergeCell ref="A127:D127"/>
-    <mergeCell ref="A141:D141"/>
+    <mergeCell ref="A129:D129"/>
+    <mergeCell ref="A143:D143"/>
     <mergeCell ref="A51:D51"/>
     <mergeCell ref="A64:D64"/>
     <mergeCell ref="A76:D76"/>
     <mergeCell ref="A85:D85"/>
     <mergeCell ref="A90:D90"/>
     <mergeCell ref="A112:D112"/>
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A31:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -2669,12 +2723,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -2702,12 +2756,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -2741,12 +2795,12 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
@@ -2830,12 +2884,12 @@
       </c>
     </row>
     <row r="17" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="4" t="s">
@@ -3003,12 +3057,12 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="18.75">
-      <c r="A29" s="12" t="s">
+      <c r="A29" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="4" t="s">
@@ -3086,12 +3140,12 @@
       </c>
     </row>
     <row r="35" spans="1:10" ht="18.75">
-      <c r="A35" s="10" t="s">
+      <c r="A35" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="4" t="s">
@@ -3184,12 +3238,12 @@
       </c>
     </row>
     <row r="42" spans="1:10" ht="18.75">
-      <c r="A42" s="12" t="s">
+      <c r="A42" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B42" s="12"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="4" t="s">
@@ -3378,12 +3432,12 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="18.75">
-      <c r="A55" s="10" t="s">
+      <c r="A55" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B55" s="10"/>
-      <c r="C55" s="10"/>
-      <c r="D55" s="10"/>
+      <c r="B55" s="11"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="11"/>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="4" t="s">
@@ -3536,12 +3590,12 @@
       </c>
     </row>
     <row r="66" spans="1:4" ht="18.75">
-      <c r="A66" s="12" t="s">
+      <c r="A66" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B66" s="12"/>
-      <c r="C66" s="12"/>
-      <c r="D66" s="12"/>
+      <c r="B66" s="10"/>
+      <c r="C66" s="10"/>
+      <c r="D66" s="10"/>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="4" t="s">
@@ -3604,12 +3658,12 @@
       </c>
     </row>
     <row r="71" spans="1:4" ht="18.75">
-      <c r="A71" s="10" t="s">
+      <c r="A71" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B71" s="10"/>
-      <c r="C71" s="10"/>
-      <c r="D71" s="10"/>
+      <c r="B71" s="11"/>
+      <c r="C71" s="11"/>
+      <c r="D71" s="11"/>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="4" t="s">
@@ -3672,12 +3726,12 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="18.75">
-      <c r="A76" s="12" t="s">
+      <c r="A76" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B76" s="12"/>
-      <c r="C76" s="12"/>
-      <c r="D76" s="12"/>
+      <c r="B76" s="10"/>
+      <c r="C76" s="10"/>
+      <c r="D76" s="10"/>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="4" t="s">
@@ -3995,12 +4049,12 @@
       </c>
     </row>
     <row r="98" spans="1:5" ht="18.75">
-      <c r="A98" s="10" t="s">
+      <c r="A98" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B98" s="10"/>
-      <c r="C98" s="10"/>
-      <c r="D98" s="10"/>
+      <c r="B98" s="11"/>
+      <c r="C98" s="11"/>
+      <c r="D98" s="11"/>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="4" t="s">
@@ -4126,12 +4180,12 @@
       </c>
     </row>
     <row r="107" spans="1:5" ht="18.75">
-      <c r="A107" s="12" t="s">
+      <c r="A107" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B107" s="12"/>
-      <c r="C107" s="12"/>
-      <c r="D107" s="12"/>
+      <c r="B107" s="10"/>
+      <c r="C107" s="10"/>
+      <c r="D107" s="10"/>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="4" t="s">
@@ -4209,12 +4263,12 @@
       </c>
     </row>
     <row r="113" spans="1:4" ht="18.75">
-      <c r="A113" s="10" t="s">
+      <c r="A113" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B113" s="10"/>
-      <c r="C113" s="10"/>
-      <c r="D113" s="10"/>
+      <c r="B113" s="11"/>
+      <c r="C113" s="11"/>
+      <c r="D113" s="11"/>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="4" t="s">
@@ -4412,12 +4466,12 @@
       </c>
     </row>
     <row r="127" spans="1:4" ht="18.75">
-      <c r="A127" s="12" t="s">
+      <c r="A127" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B127" s="12"/>
-      <c r="C127" s="12"/>
-      <c r="D127" s="12"/>
+      <c r="B127" s="10"/>
+      <c r="C127" s="10"/>
+      <c r="D127" s="10"/>
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="4" t="s">
@@ -4537,11 +4591,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A29:D29"/>
     <mergeCell ref="A127:D127"/>
     <mergeCell ref="A107:D107"/>
     <mergeCell ref="A113:D113"/>
@@ -4552,6 +4601,11 @@
     <mergeCell ref="A98:D98"/>
     <mergeCell ref="A66:D66"/>
     <mergeCell ref="A55:D55"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A29:D29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>

</xml_diff>

<commit_message>
Wario - v2 done pending a few strat ideas for final boss.
</commit_message>
<xml_diff>
--- a/Wario/Wario.xlsx
+++ b/Wario/Wario.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="72">
   <si>
     <t>Enter pipe</t>
   </si>
@@ -225,6 +225,12 @@
   </si>
   <si>
     <t>Checkpoint</t>
+  </si>
+  <si>
+    <t>Bad enemy randomness</t>
+  </si>
+  <si>
+    <t>Bad randomness</t>
   </si>
 </sst>
 </file>
@@ -632,8 +638,8 @@
   <dimension ref="A1:J151"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B134" sqref="B134"/>
+      <pane ySplit="1" topLeftCell="A132" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B147" sqref="B147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2393,7 +2399,7 @@
         <v>2036</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="18.75">
+    <row r="129" spans="1:5" ht="18.75">
       <c r="A129" s="11" t="s">
         <v>55</v>
       </c>
@@ -2401,7 +2407,7 @@
       <c r="C129" s="11"/>
       <c r="D129" s="11"/>
     </row>
-    <row r="130" spans="1:4">
+    <row r="130" spans="1:5">
       <c r="A130" s="4" t="s">
         <v>54</v>
       </c>
@@ -2416,7 +2422,7 @@
         <v>2036</v>
       </c>
     </row>
-    <row r="131" spans="1:4">
+    <row r="131" spans="1:5">
       <c r="A131" s="4" t="s">
         <v>56</v>
       </c>
@@ -2431,7 +2437,7 @@
         <v>2036</v>
       </c>
     </row>
-    <row r="132" spans="1:4">
+    <row r="132" spans="1:5">
       <c r="A132" s="4" t="s">
         <v>20</v>
       </c>
@@ -2446,7 +2452,7 @@
         <v>2036</v>
       </c>
     </row>
-    <row r="133" spans="1:4">
+    <row r="133" spans="1:5">
       <c r="A133" s="4" t="s">
         <v>19</v>
       </c>
@@ -2461,115 +2467,148 @@
         <v>2036</v>
       </c>
     </row>
-    <row r="134" spans="1:4">
+    <row r="134" spans="1:5">
       <c r="A134" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="B134" s="4">
+        <v>48226</v>
+      </c>
       <c r="C134" s="4">
         <v>50263</v>
       </c>
       <c r="D134" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4">
+        <v>2037</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5">
       <c r="A135" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="B135" s="4">
+        <v>48530</v>
+      </c>
       <c r="C135" s="4">
         <v>50566</v>
       </c>
       <c r="D135" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4">
+        <v>2036</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5">
       <c r="A136" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="B136" s="4">
+        <v>48705</v>
+      </c>
       <c r="C136" s="4">
         <v>50734</v>
       </c>
       <c r="D136" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4">
+        <v>2029</v>
+      </c>
+      <c r="E136" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5">
       <c r="A137" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="B137" s="4">
+        <v>48820</v>
+      </c>
       <c r="C137" s="4">
         <v>50849</v>
       </c>
       <c r="D137" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4">
+        <v>2029</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5">
       <c r="A138" s="4" t="s">
         <v>57</v>
       </c>
+      <c r="B138" s="4">
+        <v>49147</v>
+      </c>
       <c r="C138" s="4">
         <v>51176</v>
       </c>
       <c r="D138" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4">
+        <v>2029</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5">
       <c r="A139" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="B139" s="4">
+        <v>49319</v>
+      </c>
       <c r="C139" s="4">
         <v>51327</v>
       </c>
       <c r="D139" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4">
+        <v>2008</v>
+      </c>
+      <c r="E139" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5">
       <c r="A140" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="B140" s="4">
+        <v>49569</v>
+      </c>
       <c r="C140" s="4">
         <v>51577</v>
       </c>
       <c r="D140" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5">
       <c r="A141" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="B141" s="4">
+        <v>49860</v>
+      </c>
       <c r="C141" s="4">
         <v>51868</v>
       </c>
       <c r="D141" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5">
       <c r="A142" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="B142" s="4">
+        <v>50063</v>
+      </c>
       <c r="C142" s="4">
         <v>52071</v>
       </c>
       <c r="D142" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" ht="18.75">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" ht="18.75">
       <c r="A143" s="10" t="s">
         <v>59</v>
       </c>
@@ -2577,7 +2616,7 @@
       <c r="C143" s="10"/>
       <c r="D143" s="10"/>
     </row>
-    <row r="144" spans="1:4">
+    <row r="144" spans="1:5">
       <c r="A144" s="4" t="s">
         <v>58</v>
       </c>
@@ -2593,12 +2632,15 @@
       <c r="A145" s="4" t="s">
         <v>26</v>
       </c>
+      <c r="B145" s="4">
+        <v>51237</v>
+      </c>
       <c r="C145" s="4">
         <v>53245</v>
       </c>
       <c r="D145" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="146" spans="1:4">

</xml_diff>

<commit_message>
Wario - nothing significant, some small changes I forgot to commit
</commit_message>
<xml_diff>
--- a/Wario/Wario.xlsx
+++ b/Wario/Wario.xlsx
@@ -338,9 +338,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -639,7 +639,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A132" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B147" sqref="B147"/>
+      <selection pane="bottomLeft" activeCell="D148" sqref="D148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -663,12 +663,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -696,12 +696,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -735,12 +735,12 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
@@ -863,12 +863,12 @@
       </c>
     </row>
     <row r="19" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="4" t="s">
@@ -1036,12 +1036,12 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="18.75">
-      <c r="A31" s="10" t="s">
+      <c r="A31" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="4" t="s">
@@ -1209,12 +1209,12 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="18.75">
-      <c r="A43" s="11" t="s">
+      <c r="A43" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B43" s="11"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="4" t="s">
@@ -1322,12 +1322,12 @@
       </c>
     </row>
     <row r="51" spans="1:10" ht="18.75">
-      <c r="A51" s="10" t="s">
+      <c r="A51" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B51" s="10"/>
-      <c r="C51" s="10"/>
-      <c r="D51" s="10"/>
+      <c r="B51" s="12"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="12"/>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="4" t="s">
@@ -1513,12 +1513,12 @@
       </c>
     </row>
     <row r="64" spans="1:10" ht="18.75">
-      <c r="A64" s="11" t="s">
+      <c r="A64" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B64" s="11"/>
-      <c r="C64" s="11"/>
-      <c r="D64" s="11"/>
+      <c r="B64" s="10"/>
+      <c r="C64" s="10"/>
+      <c r="D64" s="10"/>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="4" t="s">
@@ -1677,12 +1677,12 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="18.75">
-      <c r="A76" s="10" t="s">
+      <c r="A76" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B76" s="10"/>
-      <c r="C76" s="10"/>
-      <c r="D76" s="10"/>
+      <c r="B76" s="12"/>
+      <c r="C76" s="12"/>
+      <c r="D76" s="12"/>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="4" t="s">
@@ -1795,12 +1795,12 @@
       </c>
     </row>
     <row r="85" spans="1:4" ht="18.75">
-      <c r="A85" s="11" t="s">
+      <c r="A85" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B85" s="11"/>
-      <c r="C85" s="11"/>
-      <c r="D85" s="11"/>
+      <c r="B85" s="10"/>
+      <c r="C85" s="10"/>
+      <c r="D85" s="10"/>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="4" t="s">
@@ -1860,12 +1860,12 @@
       </c>
     </row>
     <row r="90" spans="1:4" ht="18.75">
-      <c r="A90" s="10" t="s">
+      <c r="A90" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B90" s="10"/>
-      <c r="C90" s="10"/>
-      <c r="D90" s="10"/>
+      <c r="B90" s="12"/>
+      <c r="C90" s="12"/>
+      <c r="D90" s="12"/>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="4" t="s">
@@ -2156,12 +2156,12 @@
       </c>
     </row>
     <row r="112" spans="1:4" ht="18.75">
-      <c r="A112" s="11" t="s">
+      <c r="A112" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="B112" s="11"/>
-      <c r="C112" s="11"/>
-      <c r="D112" s="11"/>
+      <c r="B112" s="10"/>
+      <c r="C112" s="10"/>
+      <c r="D112" s="10"/>
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="4" t="s">
@@ -2287,12 +2287,12 @@
       </c>
     </row>
     <row r="121" spans="1:5" ht="18.75">
-      <c r="A121" s="10" t="s">
+      <c r="A121" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B121" s="10"/>
-      <c r="C121" s="10"/>
-      <c r="D121" s="10"/>
+      <c r="B121" s="12"/>
+      <c r="C121" s="12"/>
+      <c r="D121" s="12"/>
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="4" t="s">
@@ -2400,12 +2400,12 @@
       </c>
     </row>
     <row r="129" spans="1:5" ht="18.75">
-      <c r="A129" s="11" t="s">
+      <c r="A129" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B129" s="11"/>
-      <c r="C129" s="11"/>
-      <c r="D129" s="11"/>
+      <c r="B129" s="10"/>
+      <c r="C129" s="10"/>
+      <c r="D129" s="10"/>
     </row>
     <row r="130" spans="1:5">
       <c r="A130" s="4" t="s">
@@ -2609,23 +2609,27 @@
       </c>
     </row>
     <row r="143" spans="1:5" ht="18.75">
-      <c r="A143" s="10" t="s">
+      <c r="A143" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="B143" s="10"/>
-      <c r="C143" s="10"/>
-      <c r="D143" s="10"/>
+      <c r="B143" s="12"/>
+      <c r="C143" s="12"/>
+      <c r="D143" s="12"/>
     </row>
     <row r="144" spans="1:5">
       <c r="A144" s="4" t="s">
         <v>58</v>
       </c>
+      <c r="B144" s="4">
+        <f>C144-2008</f>
+        <v>50314</v>
+      </c>
       <c r="C144" s="4">
         <v>52322</v>
       </c>
       <c r="D144" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="145" spans="1:4">
@@ -2647,79 +2651,98 @@
       <c r="A146" s="4" t="s">
         <v>60</v>
       </c>
+      <c r="B146" s="4">
+        <f>C146-2008</f>
+        <v>53055</v>
+      </c>
       <c r="C146" s="4">
         <v>55063</v>
       </c>
       <c r="D146" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="4" t="s">
         <v>62</v>
       </c>
+      <c r="B147" s="4">
+        <f>C147-2008</f>
+        <v>53377</v>
+      </c>
       <c r="C147" s="4">
         <v>55385</v>
       </c>
       <c r="D147" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="4" t="s">
         <v>61</v>
       </c>
+      <c r="B148" s="4">
+        <f>C148-2008</f>
+        <v>53698</v>
+      </c>
       <c r="C148" s="4">
         <v>55706</v>
       </c>
       <c r="D148" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="4" t="s">
         <v>63</v>
       </c>
+      <c r="B149" s="4">
+        <f>C149-2008</f>
+        <v>54021</v>
+      </c>
       <c r="C149" s="4">
         <v>56029</v>
       </c>
       <c r="D149" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="4" t="s">
         <v>64</v>
       </c>
+      <c r="B150" s="4">
+        <f>C150-2008</f>
+        <v>56284</v>
+      </c>
       <c r="C150" s="4">
         <v>58292</v>
       </c>
       <c r="D150" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B151" s="9"/>
+      <c r="B151" s="9">
+        <v>0.68541666666666667</v>
+      </c>
       <c r="C151" s="9">
         <v>0.71250000000000002</v>
       </c>
+      <c r="D151" s="9">
+        <v>2.7083333333333334E-2</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A31:D31"/>
     <mergeCell ref="A121:D121"/>
     <mergeCell ref="A129:D129"/>
     <mergeCell ref="A143:D143"/>
@@ -2729,6 +2752,12 @@
     <mergeCell ref="A85:D85"/>
     <mergeCell ref="A90:D90"/>
     <mergeCell ref="A112:D112"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A31:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -2765,12 +2794,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -2798,12 +2827,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -2837,12 +2866,12 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
@@ -2926,12 +2955,12 @@
       </c>
     </row>
     <row r="17" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="4" t="s">
@@ -3099,12 +3128,12 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="18.75">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="4" t="s">
@@ -3182,12 +3211,12 @@
       </c>
     </row>
     <row r="35" spans="1:10" ht="18.75">
-      <c r="A35" s="11" t="s">
+      <c r="A35" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="4" t="s">
@@ -3280,12 +3309,12 @@
       </c>
     </row>
     <row r="42" spans="1:10" ht="18.75">
-      <c r="A42" s="10" t="s">
+      <c r="A42" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B42" s="10"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="4" t="s">
@@ -3474,12 +3503,12 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="18.75">
-      <c r="A55" s="11" t="s">
+      <c r="A55" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B55" s="11"/>
-      <c r="C55" s="11"/>
-      <c r="D55" s="11"/>
+      <c r="B55" s="10"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="10"/>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="4" t="s">
@@ -3632,12 +3661,12 @@
       </c>
     </row>
     <row r="66" spans="1:4" ht="18.75">
-      <c r="A66" s="10" t="s">
+      <c r="A66" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B66" s="10"/>
-      <c r="C66" s="10"/>
-      <c r="D66" s="10"/>
+      <c r="B66" s="12"/>
+      <c r="C66" s="12"/>
+      <c r="D66" s="12"/>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="4" t="s">
@@ -3700,12 +3729,12 @@
       </c>
     </row>
     <row r="71" spans="1:4" ht="18.75">
-      <c r="A71" s="11" t="s">
+      <c r="A71" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B71" s="11"/>
-      <c r="C71" s="11"/>
-      <c r="D71" s="11"/>
+      <c r="B71" s="10"/>
+      <c r="C71" s="10"/>
+      <c r="D71" s="10"/>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="4" t="s">
@@ -3768,12 +3797,12 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="18.75">
-      <c r="A76" s="10" t="s">
+      <c r="A76" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B76" s="10"/>
-      <c r="C76" s="10"/>
-      <c r="D76" s="10"/>
+      <c r="B76" s="12"/>
+      <c r="C76" s="12"/>
+      <c r="D76" s="12"/>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="4" t="s">
@@ -4091,12 +4120,12 @@
       </c>
     </row>
     <row r="98" spans="1:5" ht="18.75">
-      <c r="A98" s="11" t="s">
+      <c r="A98" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="B98" s="11"/>
-      <c r="C98" s="11"/>
-      <c r="D98" s="11"/>
+      <c r="B98" s="10"/>
+      <c r="C98" s="10"/>
+      <c r="D98" s="10"/>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="4" t="s">
@@ -4222,12 +4251,12 @@
       </c>
     </row>
     <row r="107" spans="1:5" ht="18.75">
-      <c r="A107" s="10" t="s">
+      <c r="A107" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B107" s="10"/>
-      <c r="C107" s="10"/>
-      <c r="D107" s="10"/>
+      <c r="B107" s="12"/>
+      <c r="C107" s="12"/>
+      <c r="D107" s="12"/>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="4" t="s">
@@ -4305,12 +4334,12 @@
       </c>
     </row>
     <row r="113" spans="1:4" ht="18.75">
-      <c r="A113" s="11" t="s">
+      <c r="A113" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B113" s="11"/>
-      <c r="C113" s="11"/>
-      <c r="D113" s="11"/>
+      <c r="B113" s="10"/>
+      <c r="C113" s="10"/>
+      <c r="D113" s="10"/>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="4" t="s">
@@ -4508,12 +4537,12 @@
       </c>
     </row>
     <row r="127" spans="1:4" ht="18.75">
-      <c r="A127" s="10" t="s">
+      <c r="A127" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="B127" s="10"/>
-      <c r="C127" s="10"/>
-      <c r="D127" s="10"/>
+      <c r="B127" s="12"/>
+      <c r="C127" s="12"/>
+      <c r="D127" s="12"/>
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="4" t="s">
@@ -4633,6 +4662,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A29:D29"/>
     <mergeCell ref="A127:D127"/>
     <mergeCell ref="A107:D107"/>
     <mergeCell ref="A113:D113"/>
@@ -4643,11 +4677,6 @@
     <mergeCell ref="A98:D98"/>
     <mergeCell ref="A66:D66"/>
     <mergeCell ref="A55:D55"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A29:D29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>

</xml_diff>

<commit_message>
Wario - more restructuring
</commit_message>
<xml_diff>
--- a/Wario/Wario.xlsx
+++ b/Wario/Wario.xlsx
@@ -7,15 +7,16 @@
     <workbookView xWindow="0" yWindow="135" windowWidth="16080" windowHeight="7500"/>
   </bookViews>
   <sheets>
-    <sheet name="V2" sheetId="5" r:id="rId1"/>
-    <sheet name="V1" sheetId="4" r:id="rId2"/>
+    <sheet name="Full" sheetId="6" r:id="rId1"/>
+    <sheet name="V2" sheetId="5" r:id="rId2"/>
+    <sheet name="V1" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="72">
   <si>
     <t>Enter pipe</t>
   </si>
@@ -338,9 +339,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -638,7 +639,1743 @@
   <dimension ref="A1:J151"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A132" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="27.7109375" style="4" customWidth="1"/>
+    <col min="2" max="4" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="16.5" thickBot="1">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
+      <c r="A2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="3"/>
+      <c r="D3" s="4">
+        <f>IF(B3 &gt;  0,C3-B3, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="D4" s="4">
+        <f t="shared" ref="D4:D6" si="0">IF(B4 &gt;  0,C4-B4, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="D5" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="D6" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
+      <c r="A7" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="4">
+        <v>1113</v>
+      </c>
+      <c r="D8" s="4">
+        <f>IF(B8 &gt;  0,C8-B8, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="4">
+        <v>2596</v>
+      </c>
+      <c r="D9" s="4">
+        <f>IF(B9 &gt;  0,C9-B9, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="18.75">
+      <c r="A10" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="4">
+        <v>2845</v>
+      </c>
+      <c r="D11" s="4">
+        <f>IF(B11 &gt;  0,C11-B11, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="4">
+        <v>3359</v>
+      </c>
+      <c r="D12" s="4">
+        <f t="shared" ref="D12:D89" si="1">IF(B12 &gt;  0,C12-B12, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="4">
+        <v>3518</v>
+      </c>
+      <c r="D13" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="4">
+        <v>3675</v>
+      </c>
+      <c r="D14" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="4">
+        <v>3880</v>
+      </c>
+      <c r="D15" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="4">
+        <v>4470</v>
+      </c>
+      <c r="D16" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="4">
+        <v>4661</v>
+      </c>
+      <c r="D17" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="4">
+        <v>4865</v>
+      </c>
+      <c r="D18" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="1" customFormat="1" ht="18.75">
+      <c r="A19" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="4">
+        <v>5114</v>
+      </c>
+      <c r="D20" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="4">
+        <v>5680</v>
+      </c>
+      <c r="D21" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="4">
+        <v>6399</v>
+      </c>
+      <c r="D22" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="4">
+        <v>6767</v>
+      </c>
+      <c r="D23" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="4">
+        <v>7021</v>
+      </c>
+      <c r="D24" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="4">
+        <v>7303</v>
+      </c>
+      <c r="D25" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="4">
+        <v>7679</v>
+      </c>
+      <c r="D26" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="4">
+        <v>7889</v>
+      </c>
+      <c r="D27" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="4">
+        <v>8242</v>
+      </c>
+      <c r="D28" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="4">
+        <v>8601</v>
+      </c>
+      <c r="D29" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" s="4">
+        <v>8805</v>
+      </c>
+      <c r="D30" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="18.75">
+      <c r="A31" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="4">
+        <v>9054</v>
+      </c>
+      <c r="D32" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" s="4">
+        <v>9397</v>
+      </c>
+      <c r="D33" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="4">
+        <v>9633</v>
+      </c>
+      <c r="D34" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C35" s="4">
+        <v>9932</v>
+      </c>
+      <c r="D35" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C36" s="4">
+        <v>11304</v>
+      </c>
+      <c r="D36" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C37" s="4">
+        <v>12308</v>
+      </c>
+      <c r="D37" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C38" s="4">
+        <v>13312</v>
+      </c>
+      <c r="D38" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C39" s="4">
+        <v>14611</v>
+      </c>
+      <c r="D39" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C40" s="4">
+        <v>14800</v>
+      </c>
+      <c r="D40" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C41" s="4">
+        <v>14936</v>
+      </c>
+      <c r="D41" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C42" s="4">
+        <v>15140</v>
+      </c>
+      <c r="D42" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="18.75">
+      <c r="A43" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C44" s="4">
+        <v>15390</v>
+      </c>
+      <c r="D44" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" s="4">
+        <v>15841</v>
+      </c>
+      <c r="D45" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46" s="4">
+        <v>16245</v>
+      </c>
+      <c r="D46" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47" s="4">
+        <v>16760</v>
+      </c>
+      <c r="D47" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C48" s="4">
+        <v>16939</v>
+      </c>
+      <c r="D48" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C49" s="4">
+        <v>17105</v>
+      </c>
+      <c r="D49" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="A50" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C50" s="4">
+        <v>17309</v>
+      </c>
+      <c r="D50" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="18.75">
+      <c r="A51" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B51" s="10"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="A52" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C52" s="4">
+        <v>17558</v>
+      </c>
+      <c r="D52" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="A53" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C53" s="4">
+        <v>18431</v>
+      </c>
+      <c r="D53" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="A54" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54" s="4">
+        <v>18823</v>
+      </c>
+      <c r="D54" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="A55" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C55" s="4">
+        <v>19078</v>
+      </c>
+      <c r="D55" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F55" s="6"/>
+      <c r="H55" s="6"/>
+      <c r="J55" s="6"/>
+    </row>
+    <row r="56" spans="1:10">
+      <c r="A56" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D56" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F56" s="7"/>
+      <c r="H56" s="7"/>
+      <c r="J56" s="7"/>
+    </row>
+    <row r="57" spans="1:10">
+      <c r="A57" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C57" s="4">
+        <v>19425</v>
+      </c>
+      <c r="D57" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
+      <c r="A58" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C58" s="4">
+        <v>19693</v>
+      </c>
+      <c r="D58" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
+      <c r="A59" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C59" s="4">
+        <v>20164</v>
+      </c>
+      <c r="D59" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
+      <c r="A60" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C60" s="4">
+        <v>20507</v>
+      </c>
+      <c r="D60" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
+      <c r="A61" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C61" s="4">
+        <v>20719</v>
+      </c>
+      <c r="D61" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
+      <c r="A62" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C62" s="4">
+        <v>20839</v>
+      </c>
+      <c r="D62" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
+      <c r="A63" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C63" s="4">
+        <v>21043</v>
+      </c>
+      <c r="D63" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="18.75">
+      <c r="A64" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B64" s="11"/>
+      <c r="C64" s="11"/>
+      <c r="D64" s="11"/>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C65" s="4">
+        <v>21292</v>
+      </c>
+      <c r="D65" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C66" s="4">
+        <v>21654</v>
+      </c>
+      <c r="D66" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C67" s="4">
+        <v>22525</v>
+      </c>
+      <c r="D67" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C68" s="4">
+        <v>22683</v>
+      </c>
+      <c r="D68" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C69" s="4">
+        <v>22853</v>
+      </c>
+      <c r="D69" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C70" s="4">
+        <v>23177</v>
+      </c>
+      <c r="D70" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C71" s="4">
+        <v>23709</v>
+      </c>
+      <c r="D71" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D72" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D73" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D74" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C75" s="4">
+        <v>24691</v>
+      </c>
+      <c r="D75" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="18.75">
+      <c r="A76" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B76" s="10"/>
+      <c r="C76" s="10"/>
+      <c r="D76" s="10"/>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D77" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C78" s="4">
+        <v>26245</v>
+      </c>
+      <c r="D78" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C79" s="4">
+        <v>27387</v>
+      </c>
+      <c r="D79" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C80" s="4">
+        <v>28067</v>
+      </c>
+      <c r="D80" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C81" s="4">
+        <v>28747</v>
+      </c>
+      <c r="D81" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C82" s="4">
+        <v>30220</v>
+      </c>
+      <c r="D82" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C83" s="4">
+        <v>30546</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C84" s="4">
+        <v>30749</v>
+      </c>
+      <c r="D84" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="18.75">
+      <c r="A85" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B85" s="11"/>
+      <c r="C85" s="11"/>
+      <c r="D85" s="11"/>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C86" s="4">
+        <v>30998</v>
+      </c>
+      <c r="D86" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D87" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C88" s="4">
+        <v>33405</v>
+      </c>
+      <c r="D88" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C89" s="4">
+        <v>33609</v>
+      </c>
+      <c r="D89" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="18.75">
+      <c r="A90" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B90" s="10"/>
+      <c r="C90" s="10"/>
+      <c r="D90" s="10"/>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C91" s="4">
+        <v>33858</v>
+      </c>
+      <c r="D91" s="4">
+        <f t="shared" ref="D91:D150" si="2">IF(B91 &gt;  0,C91-B91, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D92" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D93" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D94" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C95" s="4">
+        <v>3</v>
+      </c>
+      <c r="D95" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D96" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D97" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C98" s="4">
+        <v>35512</v>
+      </c>
+      <c r="D98" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C99" s="4">
+        <v>35693</v>
+      </c>
+      <c r="D99" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C100" s="4">
+        <v>35847</v>
+      </c>
+      <c r="D100" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C101" s="4">
+        <v>36020</v>
+      </c>
+      <c r="D101" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D102" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D103" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D104" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D105" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C106" s="4">
+        <v>38056</v>
+      </c>
+      <c r="D106" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C107" s="4">
+        <v>38245</v>
+      </c>
+      <c r="D107" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="A108" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C108" s="4">
+        <v>38420</v>
+      </c>
+      <c r="D108" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4">
+      <c r="A109" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C109" s="4">
+        <v>38758</v>
+      </c>
+      <c r="D109" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
+      <c r="A110" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C110" s="4">
+        <v>38859</v>
+      </c>
+      <c r="D110" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C111" s="4">
+        <v>39062</v>
+      </c>
+      <c r="D111" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="18.75">
+      <c r="A112" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B112" s="11"/>
+      <c r="C112" s="11"/>
+      <c r="D112" s="11"/>
+    </row>
+    <row r="113" spans="1:5">
+      <c r="A113" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C113" s="4">
+        <v>39312</v>
+      </c>
+      <c r="D113" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5">
+      <c r="A114" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C114" s="4">
+        <v>40069</v>
+      </c>
+      <c r="D114" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5">
+      <c r="A115" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C115" s="4">
+        <v>40681</v>
+      </c>
+      <c r="D115" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5">
+      <c r="A116" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C116" s="4">
+        <v>41240</v>
+      </c>
+      <c r="D116" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5">
+      <c r="A117" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C117" s="4">
+        <v>41469</v>
+      </c>
+      <c r="D117" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E117" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5">
+      <c r="A118" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C118" s="4">
+        <v>41728</v>
+      </c>
+      <c r="D118" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5">
+      <c r="A119" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C119" s="4">
+        <v>42015</v>
+      </c>
+      <c r="D119" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5">
+      <c r="A120" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C120" s="4">
+        <v>42219</v>
+      </c>
+      <c r="D120" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" ht="18.75">
+      <c r="A121" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B121" s="10"/>
+      <c r="C121" s="10"/>
+      <c r="D121" s="10"/>
+    </row>
+    <row r="122" spans="1:5">
+      <c r="A122" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C122" s="4">
+        <v>42469</v>
+      </c>
+      <c r="D122" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5">
+      <c r="A123" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C123" s="4">
+        <v>43196</v>
+      </c>
+      <c r="D123" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5">
+      <c r="A124" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C124" s="4">
+        <v>43848</v>
+      </c>
+      <c r="D124" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5">
+      <c r="A125" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C125" s="4">
+        <v>44155</v>
+      </c>
+      <c r="D125" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5">
+      <c r="A126" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C126" s="4">
+        <v>46549</v>
+      </c>
+      <c r="D126" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5">
+      <c r="A127" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C127" s="4">
+        <v>46905</v>
+      </c>
+      <c r="D127" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5">
+      <c r="A128" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C128" s="4">
+        <v>47108</v>
+      </c>
+      <c r="D128" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" ht="18.75">
+      <c r="A129" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B129" s="11"/>
+      <c r="C129" s="11"/>
+      <c r="D129" s="11"/>
+    </row>
+    <row r="130" spans="1:5">
+      <c r="A130" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C130" s="4">
+        <v>47359</v>
+      </c>
+      <c r="D130" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5">
+      <c r="A131" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C131" s="4">
+        <v>47668</v>
+      </c>
+      <c r="D131" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5">
+      <c r="A132" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C132" s="4">
+        <v>47847</v>
+      </c>
+      <c r="D132" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5">
+      <c r="A133" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C133" s="4">
+        <v>48052</v>
+      </c>
+      <c r="D133" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5">
+      <c r="A134" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C134" s="4">
+        <v>48226</v>
+      </c>
+      <c r="D134" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5">
+      <c r="A135" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C135" s="4">
+        <v>48530</v>
+      </c>
+      <c r="D135" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5">
+      <c r="A136" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C136" s="4">
+        <v>48705</v>
+      </c>
+      <c r="D136" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E136" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5">
+      <c r="A137" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C137" s="4">
+        <v>48820</v>
+      </c>
+      <c r="D137" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5">
+      <c r="A138" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C138" s="4">
+        <v>49147</v>
+      </c>
+      <c r="D138" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5">
+      <c r="A139" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C139" s="4">
+        <v>49319</v>
+      </c>
+      <c r="D139" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E139" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5">
+      <c r="A140" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C140" s="4">
+        <v>49569</v>
+      </c>
+      <c r="D140" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5">
+      <c r="A141" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C141" s="4">
+        <v>49860</v>
+      </c>
+      <c r="D141" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5">
+      <c r="A142" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C142" s="4">
+        <v>50063</v>
+      </c>
+      <c r="D142" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" ht="18.75">
+      <c r="A143" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B143" s="10"/>
+      <c r="C143" s="10"/>
+      <c r="D143" s="10"/>
+    </row>
+    <row r="144" spans="1:5">
+      <c r="A144" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C144" s="4">
+        <v>50314</v>
+      </c>
+      <c r="D144" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4">
+      <c r="A145" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C145" s="4">
+        <v>51237</v>
+      </c>
+      <c r="D145" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4">
+      <c r="A146" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C146" s="4">
+        <v>53055</v>
+      </c>
+      <c r="D146" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4">
+      <c r="A147" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C147" s="4">
+        <v>53377</v>
+      </c>
+      <c r="D147" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4">
+      <c r="A148" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C148" s="4">
+        <v>53698</v>
+      </c>
+      <c r="D148" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4">
+      <c r="A149" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C149" s="4">
+        <v>54021</v>
+      </c>
+      <c r="D149" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4">
+      <c r="A150" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C150" s="4">
+        <v>56284</v>
+      </c>
+      <c r="D150" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4">
+      <c r="A151" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B151" s="9"/>
+      <c r="C151" s="9">
+        <v>0.68541666666666667</v>
+      </c>
+      <c r="D151" s="9">
+        <v>2.7083333333333334E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="A121:D121"/>
+    <mergeCell ref="A129:D129"/>
+    <mergeCell ref="A143:D143"/>
+    <mergeCell ref="A51:D51"/>
+    <mergeCell ref="A64:D64"/>
+    <mergeCell ref="A76:D76"/>
+    <mergeCell ref="A85:D85"/>
+    <mergeCell ref="A90:D90"/>
+    <mergeCell ref="A112:D112"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A43:D43"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J151"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D148" sqref="D148"/>
     </sheetView>
   </sheetViews>
@@ -663,12 +2400,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -696,12 +2433,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -735,12 +2472,12 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
@@ -863,12 +2600,12 @@
       </c>
     </row>
     <row r="19" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="4" t="s">
@@ -1036,12 +2773,12 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="18.75">
-      <c r="A31" s="12" t="s">
+      <c r="A31" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="4" t="s">
@@ -1209,12 +2946,12 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="18.75">
-      <c r="A43" s="10" t="s">
+      <c r="A43" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B43" s="10"/>
-      <c r="C43" s="10"/>
-      <c r="D43" s="10"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="4" t="s">
@@ -1322,12 +3059,12 @@
       </c>
     </row>
     <row r="51" spans="1:10" ht="18.75">
-      <c r="A51" s="12" t="s">
+      <c r="A51" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B51" s="12"/>
-      <c r="C51" s="12"/>
-      <c r="D51" s="12"/>
+      <c r="B51" s="10"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="4" t="s">
@@ -1513,12 +3250,12 @@
       </c>
     </row>
     <row r="64" spans="1:10" ht="18.75">
-      <c r="A64" s="10" t="s">
+      <c r="A64" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B64" s="10"/>
-      <c r="C64" s="10"/>
-      <c r="D64" s="10"/>
+      <c r="B64" s="11"/>
+      <c r="C64" s="11"/>
+      <c r="D64" s="11"/>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="4" t="s">
@@ -1677,12 +3414,12 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="18.75">
-      <c r="A76" s="12" t="s">
+      <c r="A76" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B76" s="12"/>
-      <c r="C76" s="12"/>
-      <c r="D76" s="12"/>
+      <c r="B76" s="10"/>
+      <c r="C76" s="10"/>
+      <c r="D76" s="10"/>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="4" t="s">
@@ -1795,12 +3532,12 @@
       </c>
     </row>
     <row r="85" spans="1:4" ht="18.75">
-      <c r="A85" s="10" t="s">
+      <c r="A85" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B85" s="10"/>
-      <c r="C85" s="10"/>
-      <c r="D85" s="10"/>
+      <c r="B85" s="11"/>
+      <c r="C85" s="11"/>
+      <c r="D85" s="11"/>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="4" t="s">
@@ -1860,12 +3597,12 @@
       </c>
     </row>
     <row r="90" spans="1:4" ht="18.75">
-      <c r="A90" s="12" t="s">
+      <c r="A90" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B90" s="12"/>
-      <c r="C90" s="12"/>
-      <c r="D90" s="12"/>
+      <c r="B90" s="10"/>
+      <c r="C90" s="10"/>
+      <c r="D90" s="10"/>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="4" t="s">
@@ -2156,12 +3893,12 @@
       </c>
     </row>
     <row r="112" spans="1:4" ht="18.75">
-      <c r="A112" s="10" t="s">
+      <c r="A112" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B112" s="10"/>
-      <c r="C112" s="10"/>
-      <c r="D112" s="10"/>
+      <c r="B112" s="11"/>
+      <c r="C112" s="11"/>
+      <c r="D112" s="11"/>
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="4" t="s">
@@ -2287,12 +4024,12 @@
       </c>
     </row>
     <row r="121" spans="1:5" ht="18.75">
-      <c r="A121" s="12" t="s">
+      <c r="A121" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B121" s="12"/>
-      <c r="C121" s="12"/>
-      <c r="D121" s="12"/>
+      <c r="B121" s="10"/>
+      <c r="C121" s="10"/>
+      <c r="D121" s="10"/>
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="4" t="s">
@@ -2400,12 +4137,12 @@
       </c>
     </row>
     <row r="129" spans="1:5" ht="18.75">
-      <c r="A129" s="10" t="s">
+      <c r="A129" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B129" s="10"/>
-      <c r="C129" s="10"/>
-      <c r="D129" s="10"/>
+      <c r="B129" s="11"/>
+      <c r="C129" s="11"/>
+      <c r="D129" s="11"/>
     </row>
     <row r="130" spans="1:5">
       <c r="A130" s="4" t="s">
@@ -2609,12 +4346,12 @@
       </c>
     </row>
     <row r="143" spans="1:5" ht="18.75">
-      <c r="A143" s="12" t="s">
+      <c r="A143" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B143" s="12"/>
-      <c r="C143" s="12"/>
-      <c r="D143" s="12"/>
+      <c r="B143" s="10"/>
+      <c r="C143" s="10"/>
+      <c r="D143" s="10"/>
     </row>
     <row r="144" spans="1:5">
       <c r="A144" s="4" t="s">
@@ -2743,6 +4480,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A31:D31"/>
     <mergeCell ref="A121:D121"/>
     <mergeCell ref="A129:D129"/>
     <mergeCell ref="A143:D143"/>
@@ -2752,25 +4495,19 @@
     <mergeCell ref="A85:D85"/>
     <mergeCell ref="A90:D90"/>
     <mergeCell ref="A112:D112"/>
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A31:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J135"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A114" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B135" sqref="B135"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2794,12 +4531,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -2827,12 +4564,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -2866,12 +4603,12 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
@@ -2955,12 +4692,12 @@
       </c>
     </row>
     <row r="17" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="4" t="s">
@@ -3128,12 +4865,12 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="18.75">
-      <c r="A29" s="12" t="s">
+      <c r="A29" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="4" t="s">
@@ -3211,12 +4948,12 @@
       </c>
     </row>
     <row r="35" spans="1:10" ht="18.75">
-      <c r="A35" s="10" t="s">
+      <c r="A35" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="4" t="s">
@@ -3309,12 +5046,12 @@
       </c>
     </row>
     <row r="42" spans="1:10" ht="18.75">
-      <c r="A42" s="12" t="s">
+      <c r="A42" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B42" s="12"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="4" t="s">
@@ -3503,12 +5240,12 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="18.75">
-      <c r="A55" s="10" t="s">
+      <c r="A55" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B55" s="10"/>
-      <c r="C55" s="10"/>
-      <c r="D55" s="10"/>
+      <c r="B55" s="11"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="11"/>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="4" t="s">
@@ -3661,12 +5398,12 @@
       </c>
     </row>
     <row r="66" spans="1:4" ht="18.75">
-      <c r="A66" s="12" t="s">
+      <c r="A66" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B66" s="12"/>
-      <c r="C66" s="12"/>
-      <c r="D66" s="12"/>
+      <c r="B66" s="10"/>
+      <c r="C66" s="10"/>
+      <c r="D66" s="10"/>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="4" t="s">
@@ -3729,12 +5466,12 @@
       </c>
     </row>
     <row r="71" spans="1:4" ht="18.75">
-      <c r="A71" s="10" t="s">
+      <c r="A71" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B71" s="10"/>
-      <c r="C71" s="10"/>
-      <c r="D71" s="10"/>
+      <c r="B71" s="11"/>
+      <c r="C71" s="11"/>
+      <c r="D71" s="11"/>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="4" t="s">
@@ -3797,12 +5534,12 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="18.75">
-      <c r="A76" s="12" t="s">
+      <c r="A76" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B76" s="12"/>
-      <c r="C76" s="12"/>
-      <c r="D76" s="12"/>
+      <c r="B76" s="10"/>
+      <c r="C76" s="10"/>
+      <c r="D76" s="10"/>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="4" t="s">
@@ -4120,12 +5857,12 @@
       </c>
     </row>
     <row r="98" spans="1:5" ht="18.75">
-      <c r="A98" s="10" t="s">
+      <c r="A98" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B98" s="10"/>
-      <c r="C98" s="10"/>
-      <c r="D98" s="10"/>
+      <c r="B98" s="11"/>
+      <c r="C98" s="11"/>
+      <c r="D98" s="11"/>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="4" t="s">
@@ -4251,12 +5988,12 @@
       </c>
     </row>
     <row r="107" spans="1:5" ht="18.75">
-      <c r="A107" s="12" t="s">
+      <c r="A107" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B107" s="12"/>
-      <c r="C107" s="12"/>
-      <c r="D107" s="12"/>
+      <c r="B107" s="10"/>
+      <c r="C107" s="10"/>
+      <c r="D107" s="10"/>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="4" t="s">
@@ -4334,12 +6071,12 @@
       </c>
     </row>
     <row r="113" spans="1:4" ht="18.75">
-      <c r="A113" s="10" t="s">
+      <c r="A113" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B113" s="10"/>
-      <c r="C113" s="10"/>
-      <c r="D113" s="10"/>
+      <c r="B113" s="11"/>
+      <c r="C113" s="11"/>
+      <c r="D113" s="11"/>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="4" t="s">
@@ -4537,12 +6274,12 @@
       </c>
     </row>
     <row r="127" spans="1:4" ht="18.75">
-      <c r="A127" s="12" t="s">
+      <c r="A127" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B127" s="12"/>
-      <c r="C127" s="12"/>
-      <c r="D127" s="12"/>
+      <c r="B127" s="10"/>
+      <c r="C127" s="10"/>
+      <c r="D127" s="10"/>
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="4" t="s">
@@ -4662,11 +6399,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A29:D29"/>
     <mergeCell ref="A127:D127"/>
     <mergeCell ref="A107:D107"/>
     <mergeCell ref="A113:D113"/>
@@ -4677,6 +6409,11 @@
     <mergeCell ref="A98:D98"/>
     <mergeCell ref="A66:D66"/>
     <mergeCell ref="A55:D55"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A29:D29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>

</xml_diff>

<commit_message>
Wario 100% - Level 1 done
</commit_message>
<xml_diff>
--- a/Wario/Wario.xlsx
+++ b/Wario/Wario.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="74">
   <si>
     <t>Enter pipe</t>
   </si>
@@ -232,6 +232,12 @@
   </si>
   <si>
     <t>Bad randomness</t>
+  </si>
+  <si>
+    <t>Get Treasure</t>
+  </si>
+  <si>
+    <t>Exit Room</t>
   </si>
 </sst>
 </file>
@@ -636,11 +642,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J151"/>
+  <dimension ref="A1:J155"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -708,6 +714,9 @@
       <c r="A8" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="B8" s="4">
+        <v>1113</v>
+      </c>
       <c r="C8" s="4">
         <v>1113</v>
       </c>
@@ -719,102 +728,96 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="4">
-        <v>2596</v>
-      </c>
-      <c r="D9" s="4">
-        <f>IF(B9 &gt;  0,C9-B9, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="18.75">
-      <c r="A10" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
+        <v>6</v>
+      </c>
+      <c r="B9" s="4">
+        <v>2158</v>
+      </c>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="4">
+        <v>2232</v>
+      </c>
+      <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="4">
-        <v>2845</v>
-      </c>
-      <c r="D11" s="4">
-        <f>IF(B11 &gt;  0,C11-B11, 0)</f>
-        <v>0</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="B11" s="4">
+        <v>2415</v>
+      </c>
+      <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="4">
-        <v>3359</v>
-      </c>
-      <c r="D12" s="4">
-        <f t="shared" ref="D12:D89" si="1">IF(B12 &gt;  0,C12-B12, 0)</f>
-        <v>0</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="B12" s="4">
+        <v>2859</v>
+      </c>
+      <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="4" t="s">
-        <v>6</v>
+        <v>12</v>
+      </c>
+      <c r="B13" s="4">
+        <v>3062</v>
       </c>
       <c r="C13" s="4">
-        <v>3518</v>
+        <v>2596</v>
       </c>
       <c r="D13" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="4">
-        <v>3675</v>
-      </c>
-      <c r="D14" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+        <f>IF(B13 &gt;  0,C13-B13, 0)</f>
+        <v>-466</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="18.75">
+      <c r="A14" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="4" t="s">
-        <v>20</v>
+        <v>13</v>
+      </c>
+      <c r="B15" s="4">
+        <v>3311</v>
       </c>
       <c r="C15" s="4">
-        <v>3880</v>
+        <v>2845</v>
       </c>
       <c r="D15" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>IF(B15 &gt;  0,C15-B15, 0)</f>
+        <v>-466</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="4" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C16" s="4">
-        <v>4470</v>
+        <v>3359</v>
       </c>
       <c r="D16" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="D16:D93" si="1">IF(B16 &gt;  0,C16-B16, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="4" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="C17" s="4">
-        <v>4661</v>
+        <v>3518</v>
       </c>
       <c r="D17" s="4">
         <f t="shared" si="1"/>
@@ -823,30 +826,34 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="4" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C18" s="4">
-        <v>4865</v>
+        <v>3675</v>
       </c>
       <c r="D18" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A19" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
+    <row r="19" spans="1:4">
+      <c r="A19" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="4">
+        <v>3880</v>
+      </c>
+      <c r="D19" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C20" s="4">
-        <v>5114</v>
+        <v>4470</v>
       </c>
       <c r="D20" s="4">
         <f t="shared" si="1"/>
@@ -854,11 +861,11 @@
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="5" t="s">
-        <v>0</v>
+      <c r="A21" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="C21" s="4">
-        <v>5680</v>
+        <v>4661</v>
       </c>
       <c r="D21" s="4">
         <f t="shared" si="1"/>
@@ -867,34 +874,30 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="4" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C22" s="4">
-        <v>6399</v>
+        <v>4865</v>
       </c>
       <c r="D22" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C23" s="4">
-        <v>6767</v>
-      </c>
-      <c r="D23" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+    <row r="23" spans="1:4" s="1" customFormat="1" ht="18.75">
+      <c r="A23" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C24" s="4">
-        <v>7021</v>
+        <v>5114</v>
       </c>
       <c r="D24" s="4">
         <f t="shared" si="1"/>
@@ -902,11 +905,11 @@
       </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="4" t="s">
-        <v>20</v>
+      <c r="A25" s="5" t="s">
+        <v>0</v>
       </c>
       <c r="C25" s="4">
-        <v>7303</v>
+        <v>5680</v>
       </c>
       <c r="D25" s="4">
         <f t="shared" si="1"/>
@@ -915,10 +918,10 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="4" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="C26" s="4">
-        <v>7679</v>
+        <v>6399</v>
       </c>
       <c r="D26" s="4">
         <f t="shared" si="1"/>
@@ -930,7 +933,7 @@
         <v>0</v>
       </c>
       <c r="C27" s="4">
-        <v>7889</v>
+        <v>6767</v>
       </c>
       <c r="D27" s="4">
         <f t="shared" si="1"/>
@@ -939,10 +942,10 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="4" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C28" s="4">
-        <v>8242</v>
+        <v>7021</v>
       </c>
       <c r="D28" s="4">
         <f t="shared" si="1"/>
@@ -951,10 +954,10 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C29" s="4">
-        <v>8601</v>
+        <v>7303</v>
       </c>
       <c r="D29" s="4">
         <f t="shared" si="1"/>
@@ -963,30 +966,34 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C30" s="4">
-        <v>8805</v>
+        <v>7679</v>
       </c>
       <c r="D30" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="18.75">
-      <c r="A31" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
+    <row r="31" spans="1:4">
+      <c r="A31" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="4">
+        <v>7889</v>
+      </c>
+      <c r="D31" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="4" t="s">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="C32" s="4">
-        <v>9054</v>
+        <v>8242</v>
       </c>
       <c r="D32" s="4">
         <f t="shared" si="1"/>
@@ -995,10 +1002,10 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="4" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="C33" s="4">
-        <v>9397</v>
+        <v>8601</v>
       </c>
       <c r="D33" s="4">
         <f t="shared" si="1"/>
@@ -1007,34 +1014,30 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="4" t="s">
-        <v>60</v>
+        <v>23</v>
       </c>
       <c r="C34" s="4">
-        <v>9633</v>
+        <v>8805</v>
       </c>
       <c r="D34" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C35" s="4">
-        <v>9932</v>
-      </c>
-      <c r="D35" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+    <row r="35" spans="1:4" ht="18.75">
+      <c r="A35" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="4" t="s">
-        <v>66</v>
+        <v>25</v>
       </c>
       <c r="C36" s="4">
-        <v>11304</v>
+        <v>9054</v>
       </c>
       <c r="D36" s="4">
         <f t="shared" si="1"/>
@@ -1043,10 +1046,10 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="4" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="C37" s="4">
-        <v>12308</v>
+        <v>9397</v>
       </c>
       <c r="D37" s="4">
         <f t="shared" si="1"/>
@@ -1055,10 +1058,10 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C38" s="4">
-        <v>13312</v>
+        <v>9633</v>
       </c>
       <c r="D38" s="4">
         <f t="shared" si="1"/>
@@ -1067,10 +1070,10 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="4" t="s">
-        <v>67</v>
+        <v>26</v>
       </c>
       <c r="C39" s="4">
-        <v>14611</v>
+        <v>9932</v>
       </c>
       <c r="D39" s="4">
         <f t="shared" si="1"/>
@@ -1079,10 +1082,10 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="4" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="C40" s="4">
-        <v>14800</v>
+        <v>11304</v>
       </c>
       <c r="D40" s="4">
         <f t="shared" si="1"/>
@@ -1091,10 +1094,10 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="4" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="C41" s="4">
-        <v>14936</v>
+        <v>12308</v>
       </c>
       <c r="D41" s="4">
         <f t="shared" si="1"/>
@@ -1103,30 +1106,34 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="4" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="C42" s="4">
-        <v>15140</v>
+        <v>13312</v>
       </c>
       <c r="D42" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="18.75">
-      <c r="A43" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B43" s="11"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
+    <row r="43" spans="1:4">
+      <c r="A43" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C43" s="4">
+        <v>14611</v>
+      </c>
+      <c r="D43" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="4" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C44" s="4">
-        <v>15390</v>
+        <v>14800</v>
       </c>
       <c r="D44" s="4">
         <f t="shared" si="1"/>
@@ -1135,10 +1142,10 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="4" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="C45" s="4">
-        <v>15841</v>
+        <v>14936</v>
       </c>
       <c r="D45" s="4">
         <f t="shared" si="1"/>
@@ -1147,34 +1154,30 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="4" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="C46" s="4">
-        <v>16245</v>
+        <v>15140</v>
       </c>
       <c r="D46" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
-      <c r="A47" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C47" s="4">
-        <v>16760</v>
-      </c>
-      <c r="D47" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+    <row r="47" spans="1:4" ht="18.75">
+      <c r="A47" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="4" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C48" s="4">
-        <v>16939</v>
+        <v>15390</v>
       </c>
       <c r="D48" s="4">
         <f t="shared" si="1"/>
@@ -1183,10 +1186,10 @@
     </row>
     <row r="49" spans="1:10">
       <c r="A49" s="4" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="C49" s="4">
-        <v>17105</v>
+        <v>15841</v>
       </c>
       <c r="D49" s="4">
         <f t="shared" si="1"/>
@@ -1195,30 +1198,34 @@
     </row>
     <row r="50" spans="1:10">
       <c r="A50" s="4" t="s">
-        <v>68</v>
+        <v>7</v>
       </c>
       <c r="C50" s="4">
-        <v>17309</v>
+        <v>16245</v>
       </c>
       <c r="D50" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="18.75">
-      <c r="A51" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B51" s="10"/>
-      <c r="C51" s="10"/>
-      <c r="D51" s="10"/>
+    <row r="51" spans="1:10">
+      <c r="A51" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C51" s="4">
+        <v>16760</v>
+      </c>
+      <c r="D51" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="4" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C52" s="4">
-        <v>17558</v>
+        <v>16939</v>
       </c>
       <c r="D52" s="4">
         <f t="shared" si="1"/>
@@ -1227,10 +1234,10 @@
     </row>
     <row r="53" spans="1:10">
       <c r="A53" s="4" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C53" s="4">
-        <v>18431</v>
+        <v>17105</v>
       </c>
       <c r="D53" s="4">
         <f t="shared" si="1"/>
@@ -1239,49 +1246,42 @@
     </row>
     <row r="54" spans="1:10">
       <c r="A54" s="4" t="s">
-        <v>7</v>
+        <v>68</v>
       </c>
       <c r="C54" s="4">
-        <v>18823</v>
+        <v>17309</v>
       </c>
       <c r="D54" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
-      <c r="A55" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C55" s="4">
-        <v>19078</v>
-      </c>
-      <c r="D55" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F55" s="6"/>
-      <c r="H55" s="6"/>
-      <c r="J55" s="6"/>
+    <row r="55" spans="1:10" ht="18.75">
+      <c r="A55" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B55" s="10"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="10"/>
     </row>
     <row r="56" spans="1:10">
       <c r="A56" s="4" t="s">
-        <v>20</v>
+        <v>31</v>
+      </c>
+      <c r="C56" s="4">
+        <v>17558</v>
       </c>
       <c r="D56" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F56" s="7"/>
-      <c r="H56" s="7"/>
-      <c r="J56" s="7"/>
     </row>
     <row r="57" spans="1:10">
       <c r="A57" s="4" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="C57" s="4">
-        <v>19425</v>
+        <v>18431</v>
       </c>
       <c r="D57" s="4">
         <f t="shared" si="1"/>
@@ -1293,7 +1293,7 @@
         <v>7</v>
       </c>
       <c r="C58" s="4">
-        <v>19693</v>
+        <v>18823</v>
       </c>
       <c r="D58" s="4">
         <f t="shared" si="1"/>
@@ -1302,34 +1302,37 @@
     </row>
     <row r="59" spans="1:10">
       <c r="A59" s="4" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C59" s="4">
-        <v>20164</v>
+        <v>19078</v>
       </c>
       <c r="D59" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="F59" s="6"/>
+      <c r="H59" s="6"/>
+      <c r="J59" s="6"/>
     </row>
     <row r="60" spans="1:10">
       <c r="A60" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C60" s="4">
-        <v>20507</v>
+        <v>20</v>
       </c>
       <c r="D60" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="F60" s="7"/>
+      <c r="H60" s="7"/>
+      <c r="J60" s="7"/>
     </row>
     <row r="61" spans="1:10">
       <c r="A61" s="4" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="C61" s="4">
-        <v>20719</v>
+        <v>19425</v>
       </c>
       <c r="D61" s="4">
         <f t="shared" si="1"/>
@@ -1338,10 +1341,10 @@
     </row>
     <row r="62" spans="1:10">
       <c r="A62" s="4" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="C62" s="4">
-        <v>20839</v>
+        <v>19693</v>
       </c>
       <c r="D62" s="4">
         <f t="shared" si="1"/>
@@ -1350,30 +1353,34 @@
     </row>
     <row r="63" spans="1:10">
       <c r="A63" s="4" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="C63" s="4">
-        <v>21043</v>
+        <v>20164</v>
       </c>
       <c r="D63" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="18.75">
-      <c r="A64" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B64" s="11"/>
-      <c r="C64" s="11"/>
-      <c r="D64" s="11"/>
+    <row r="64" spans="1:10">
+      <c r="A64" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C64" s="4">
+        <v>20507</v>
+      </c>
+      <c r="D64" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="4" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="C65" s="4">
-        <v>21292</v>
+        <v>20719</v>
       </c>
       <c r="D65" s="4">
         <f t="shared" si="1"/>
@@ -1382,10 +1389,10 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="4" t="s">
-        <v>69</v>
+        <v>27</v>
       </c>
       <c r="C66" s="4">
-        <v>21654</v>
+        <v>20839</v>
       </c>
       <c r="D66" s="4">
         <f t="shared" si="1"/>
@@ -1394,34 +1401,30 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="4" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="C67" s="4">
-        <v>22525</v>
+        <v>21043</v>
       </c>
       <c r="D67" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
-      <c r="A68" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C68" s="4">
-        <v>22683</v>
-      </c>
-      <c r="D68" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+    <row r="68" spans="1:4" ht="18.75">
+      <c r="A68" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B68" s="11"/>
+      <c r="C68" s="11"/>
+      <c r="D68" s="11"/>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="4" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="C69" s="4">
-        <v>22853</v>
+        <v>21292</v>
       </c>
       <c r="D69" s="4">
         <f t="shared" si="1"/>
@@ -1430,10 +1433,10 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="4" t="s">
-        <v>20</v>
+        <v>69</v>
       </c>
       <c r="C70" s="4">
-        <v>23177</v>
+        <v>21654</v>
       </c>
       <c r="D70" s="4">
         <f t="shared" si="1"/>
@@ -1442,10 +1445,10 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C71" s="4">
-        <v>23709</v>
+        <v>22525</v>
       </c>
       <c r="D71" s="4">
         <f t="shared" si="1"/>
@@ -1454,7 +1457,10 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="C72" s="4">
+        <v>22683</v>
       </c>
       <c r="D72" s="4">
         <f t="shared" si="1"/>
@@ -1465,6 +1471,9 @@
       <c r="A73" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="C73" s="4">
+        <v>22853</v>
+      </c>
       <c r="D73" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -1472,7 +1481,10 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="4" t="s">
-        <v>27</v>
+        <v>20</v>
+      </c>
+      <c r="C74" s="4">
+        <v>23177</v>
       </c>
       <c r="D74" s="4">
         <f t="shared" si="1"/>
@@ -1481,27 +1493,28 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="4" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="C75" s="4">
-        <v>24691</v>
+        <v>23709</v>
       </c>
       <c r="D75" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="18.75">
-      <c r="A76" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B76" s="10"/>
-      <c r="C76" s="10"/>
-      <c r="D76" s="10"/>
+    <row r="76" spans="1:4">
+      <c r="A76" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D76" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="4" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="D77" s="4">
         <f t="shared" si="1"/>
@@ -1509,11 +1522,8 @@
       </c>
     </row>
     <row r="78" spans="1:4">
-      <c r="A78" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C78" s="4">
-        <v>26245</v>
+      <c r="A78" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="D78" s="4">
         <f t="shared" si="1"/>
@@ -1522,34 +1532,27 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="4" t="s">
-        <v>66</v>
+        <v>34</v>
       </c>
       <c r="C79" s="4">
-        <v>27387</v>
+        <v>24691</v>
       </c>
       <c r="D79" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
-      <c r="A80" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C80" s="4">
-        <v>28067</v>
-      </c>
-      <c r="D80" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+    <row r="80" spans="1:4" ht="18.75">
+      <c r="A80" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B80" s="10"/>
+      <c r="C80" s="10"/>
+      <c r="D80" s="10"/>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C81" s="4">
-        <v>28747</v>
+        <v>37</v>
       </c>
       <c r="D81" s="4">
         <f t="shared" si="1"/>
@@ -1557,11 +1560,11 @@
       </c>
     </row>
     <row r="82" spans="1:4">
-      <c r="A82" s="4" t="s">
-        <v>39</v>
+      <c r="A82" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="C82" s="4">
-        <v>30220</v>
+        <v>26245</v>
       </c>
       <c r="D82" s="4">
         <f t="shared" si="1"/>
@@ -1570,38 +1573,46 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="4" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="C83" s="4">
-        <v>30546</v>
+        <v>27387</v>
+      </c>
+      <c r="D83" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="4" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="C84" s="4">
-        <v>30749</v>
+        <v>28067</v>
       </c>
       <c r="D84" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="18.75">
-      <c r="A85" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B85" s="11"/>
-      <c r="C85" s="11"/>
-      <c r="D85" s="11"/>
+    <row r="85" spans="1:4">
+      <c r="A85" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C85" s="4">
+        <v>28747</v>
+      </c>
+      <c r="D85" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C86" s="4">
-        <v>30998</v>
+        <v>30220</v>
       </c>
       <c r="D86" s="4">
         <f t="shared" si="1"/>
@@ -1610,99 +1621,100 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D87" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>27</v>
+      </c>
+      <c r="C87" s="4">
+        <v>30546</v>
       </c>
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="4" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="C88" s="4">
-        <v>33405</v>
+        <v>30749</v>
       </c>
       <c r="D88" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:4">
-      <c r="A89" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C89" s="4">
-        <v>33609</v>
-      </c>
-      <c r="D89" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" ht="18.75">
-      <c r="A90" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B90" s="10"/>
-      <c r="C90" s="10"/>
-      <c r="D90" s="10"/>
+    <row r="89" spans="1:4" ht="18.75">
+      <c r="A89" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B89" s="11"/>
+      <c r="C89" s="11"/>
+      <c r="D89" s="11"/>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C90" s="4">
+        <v>30998</v>
+      </c>
+      <c r="D90" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C91" s="4">
-        <v>33858</v>
+        <v>20</v>
       </c>
       <c r="D91" s="4">
-        <f t="shared" ref="D91:D150" si="2">IF(B91 &gt;  0,C91-B91, 0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="4" t="s">
-        <v>45</v>
+        <v>27</v>
+      </c>
+      <c r="C92" s="4">
+        <v>33405</v>
       </c>
       <c r="D92" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="4" t="s">
-        <v>45</v>
+        <v>34</v>
+      </c>
+      <c r="C93" s="4">
+        <v>33609</v>
       </c>
       <c r="D93" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4">
-      <c r="A94" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D94" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="18.75">
+      <c r="A94" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B94" s="10"/>
+      <c r="C94" s="10"/>
+      <c r="D94" s="10"/>
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C95" s="4">
-        <v>3</v>
+        <v>33858</v>
       </c>
       <c r="D95" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="D95:D154" si="2">IF(B95 &gt;  0,C95-B95, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D96" s="4">
         <f t="shared" si="2"/>
@@ -1711,7 +1723,7 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D97" s="4">
         <f t="shared" si="2"/>
@@ -1720,10 +1732,7 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C98" s="4">
-        <v>35512</v>
+        <v>45</v>
       </c>
       <c r="D98" s="4">
         <f t="shared" si="2"/>
@@ -1732,10 +1741,10 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="4" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="C99" s="4">
-        <v>35693</v>
+        <v>3</v>
       </c>
       <c r="D99" s="4">
         <f t="shared" si="2"/>
@@ -1744,10 +1753,7 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C100" s="4">
-        <v>35847</v>
+        <v>46</v>
       </c>
       <c r="D100" s="4">
         <f t="shared" si="2"/>
@@ -1756,10 +1762,7 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C101" s="4">
-        <v>36020</v>
+        <v>47</v>
       </c>
       <c r="D101" s="4">
         <f t="shared" si="2"/>
@@ -1768,7 +1771,10 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="4" t="s">
-        <v>6</v>
+        <v>19</v>
+      </c>
+      <c r="C102" s="4">
+        <v>35512</v>
       </c>
       <c r="D102" s="4">
         <f t="shared" si="2"/>
@@ -1779,6 +1785,9 @@
       <c r="A103" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="C103" s="4">
+        <v>35693</v>
+      </c>
       <c r="D103" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1788,6 +1797,9 @@
       <c r="A104" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="C104" s="4">
+        <v>35847</v>
+      </c>
       <c r="D104" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1797,6 +1809,9 @@
       <c r="A105" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="C105" s="4">
+        <v>36020</v>
+      </c>
       <c r="D105" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1804,10 +1819,7 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C106" s="4">
-        <v>38056</v>
+        <v>6</v>
       </c>
       <c r="D106" s="4">
         <f t="shared" si="2"/>
@@ -1818,9 +1830,6 @@
       <c r="A107" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C107" s="4">
-        <v>38245</v>
-      </c>
       <c r="D107" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1828,10 +1837,7 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C108" s="4">
-        <v>38420</v>
+        <v>6</v>
       </c>
       <c r="D108" s="4">
         <f t="shared" si="2"/>
@@ -1840,10 +1846,7 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C109" s="4">
-        <v>38758</v>
+        <v>6</v>
       </c>
       <c r="D109" s="4">
         <f t="shared" si="2"/>
@@ -1852,10 +1855,10 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="4" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C110" s="4">
-        <v>38859</v>
+        <v>38056</v>
       </c>
       <c r="D110" s="4">
         <f t="shared" si="2"/>
@@ -1864,30 +1867,34 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="4" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="C111" s="4">
-        <v>39062</v>
+        <v>38245</v>
       </c>
       <c r="D111" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="18.75">
-      <c r="A112" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B112" s="11"/>
-      <c r="C112" s="11"/>
-      <c r="D112" s="11"/>
+    <row r="112" spans="1:4">
+      <c r="A112" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C112" s="4">
+        <v>38420</v>
+      </c>
+      <c r="D112" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="4" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="C113" s="4">
-        <v>39312</v>
+        <v>38758</v>
       </c>
       <c r="D113" s="4">
         <f t="shared" si="2"/>
@@ -1896,10 +1903,10 @@
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="4" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C114" s="4">
-        <v>40069</v>
+        <v>38859</v>
       </c>
       <c r="D114" s="4">
         <f t="shared" si="2"/>
@@ -1908,41 +1915,34 @@
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="4" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="C115" s="4">
-        <v>40681</v>
+        <v>39062</v>
       </c>
       <c r="D115" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:5">
-      <c r="A116" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C116" s="4">
-        <v>41240</v>
-      </c>
-      <c r="D116" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
+    <row r="116" spans="1:5" ht="18.75">
+      <c r="A116" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B116" s="11"/>
+      <c r="C116" s="11"/>
+      <c r="D116" s="11"/>
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="4" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="C117" s="4">
-        <v>41469</v>
+        <v>39312</v>
       </c>
       <c r="D117" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
-      </c>
-      <c r="E117" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="118" spans="1:5">
@@ -1950,7 +1950,7 @@
         <v>19</v>
       </c>
       <c r="C118" s="4">
-        <v>41728</v>
+        <v>40069</v>
       </c>
       <c r="D118" s="4">
         <f t="shared" si="2"/>
@@ -1959,10 +1959,10 @@
     </row>
     <row r="119" spans="1:5">
       <c r="A119" s="4" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C119" s="4">
-        <v>42015</v>
+        <v>40681</v>
       </c>
       <c r="D119" s="4">
         <f t="shared" si="2"/>
@@ -1971,30 +1971,37 @@
     </row>
     <row r="120" spans="1:5">
       <c r="A120" s="4" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="C120" s="4">
-        <v>42219</v>
+        <v>41240</v>
       </c>
       <c r="D120" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:5" ht="18.75">
-      <c r="A121" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B121" s="10"/>
-      <c r="C121" s="10"/>
-      <c r="D121" s="10"/>
+    <row r="121" spans="1:5">
+      <c r="A121" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C121" s="4">
+        <v>41469</v>
+      </c>
+      <c r="D121" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E121" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="4" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="C122" s="4">
-        <v>42469</v>
+        <v>41728</v>
       </c>
       <c r="D122" s="4">
         <f t="shared" si="2"/>
@@ -2003,10 +2010,10 @@
     </row>
     <row r="123" spans="1:5">
       <c r="A123" s="4" t="s">
-        <v>66</v>
+        <v>27</v>
       </c>
       <c r="C123" s="4">
-        <v>43196</v>
+        <v>42015</v>
       </c>
       <c r="D123" s="4">
         <f t="shared" si="2"/>
@@ -2015,34 +2022,30 @@
     </row>
     <row r="124" spans="1:5">
       <c r="A124" s="4" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="C124" s="4">
-        <v>43848</v>
+        <v>42219</v>
       </c>
       <c r="D124" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:5">
-      <c r="A125" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C125" s="4">
-        <v>44155</v>
-      </c>
-      <c r="D125" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
+    <row r="125" spans="1:5" ht="18.75">
+      <c r="A125" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B125" s="10"/>
+      <c r="C125" s="10"/>
+      <c r="D125" s="10"/>
     </row>
     <row r="126" spans="1:5">
       <c r="A126" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C126" s="4">
-        <v>46549</v>
+        <v>42469</v>
       </c>
       <c r="D126" s="4">
         <f t="shared" si="2"/>
@@ -2051,10 +2054,10 @@
     </row>
     <row r="127" spans="1:5">
       <c r="A127" s="4" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="C127" s="4">
-        <v>46905</v>
+        <v>43196</v>
       </c>
       <c r="D127" s="4">
         <f t="shared" si="2"/>
@@ -2063,30 +2066,34 @@
     </row>
     <row r="128" spans="1:5">
       <c r="A128" s="4" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="C128" s="4">
-        <v>47108</v>
+        <v>43848</v>
       </c>
       <c r="D128" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:5" ht="18.75">
-      <c r="A129" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="B129" s="11"/>
-      <c r="C129" s="11"/>
-      <c r="D129" s="11"/>
+    <row r="129" spans="1:5">
+      <c r="A129" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C129" s="4">
+        <v>44155</v>
+      </c>
+      <c r="D129" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="130" spans="1:5">
       <c r="A130" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C130" s="4">
-        <v>47359</v>
+        <v>46549</v>
       </c>
       <c r="D130" s="4">
         <f t="shared" si="2"/>
@@ -2095,10 +2102,10 @@
     </row>
     <row r="131" spans="1:5">
       <c r="A131" s="4" t="s">
-        <v>56</v>
+        <v>27</v>
       </c>
       <c r="C131" s="4">
-        <v>47668</v>
+        <v>46905</v>
       </c>
       <c r="D131" s="4">
         <f t="shared" si="2"/>
@@ -2107,34 +2114,30 @@
     </row>
     <row r="132" spans="1:5">
       <c r="A132" s="4" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="C132" s="4">
-        <v>47847</v>
+        <v>47108</v>
       </c>
       <c r="D132" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:5">
-      <c r="A133" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C133" s="4">
-        <v>48052</v>
-      </c>
-      <c r="D133" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
+    <row r="133" spans="1:5" ht="18.75">
+      <c r="A133" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B133" s="11"/>
+      <c r="C133" s="11"/>
+      <c r="D133" s="11"/>
     </row>
     <row r="134" spans="1:5">
       <c r="A134" s="4" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="C134" s="4">
-        <v>48226</v>
+        <v>47359</v>
       </c>
       <c r="D134" s="4">
         <f t="shared" si="2"/>
@@ -2143,10 +2146,10 @@
     </row>
     <row r="135" spans="1:5">
       <c r="A135" s="4" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="C135" s="4">
-        <v>48530</v>
+        <v>47668</v>
       </c>
       <c r="D135" s="4">
         <f t="shared" si="2"/>
@@ -2155,17 +2158,14 @@
     </row>
     <row r="136" spans="1:5">
       <c r="A136" s="4" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C136" s="4">
-        <v>48705</v>
+        <v>47847</v>
       </c>
       <c r="D136" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
-      </c>
-      <c r="E136" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="137" spans="1:5">
@@ -2173,7 +2173,7 @@
         <v>19</v>
       </c>
       <c r="C137" s="4">
-        <v>48820</v>
+        <v>48052</v>
       </c>
       <c r="D137" s="4">
         <f t="shared" si="2"/>
@@ -2182,10 +2182,10 @@
     </row>
     <row r="138" spans="1:5">
       <c r="A138" s="4" t="s">
-        <v>57</v>
+        <v>7</v>
       </c>
       <c r="C138" s="4">
-        <v>49147</v>
+        <v>48226</v>
       </c>
       <c r="D138" s="4">
         <f t="shared" si="2"/>
@@ -2197,34 +2197,34 @@
         <v>6</v>
       </c>
       <c r="C139" s="4">
-        <v>49319</v>
+        <v>48530</v>
       </c>
       <c r="D139" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
-      </c>
-      <c r="E139" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="140" spans="1:5">
       <c r="A140" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C140" s="4">
-        <v>49569</v>
+        <v>48705</v>
       </c>
       <c r="D140" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
+      </c>
+      <c r="E140" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="141" spans="1:5">
       <c r="A141" s="4" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C141" s="4">
-        <v>49860</v>
+        <v>48820</v>
       </c>
       <c r="D141" s="4">
         <f t="shared" si="2"/>
@@ -2233,30 +2233,37 @@
     </row>
     <row r="142" spans="1:5">
       <c r="A142" s="4" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="C142" s="4">
-        <v>50063</v>
+        <v>49147</v>
       </c>
       <c r="D142" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:5" ht="18.75">
-      <c r="A143" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="B143" s="10"/>
-      <c r="C143" s="10"/>
-      <c r="D143" s="10"/>
+    <row r="143" spans="1:5">
+      <c r="A143" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C143" s="4">
+        <v>49319</v>
+      </c>
+      <c r="D143" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E143" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="144" spans="1:5">
       <c r="A144" s="4" t="s">
-        <v>58</v>
+        <v>6</v>
       </c>
       <c r="C144" s="4">
-        <v>50314</v>
+        <v>49569</v>
       </c>
       <c r="D144" s="4">
         <f t="shared" si="2"/>
@@ -2265,10 +2272,10 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C145" s="4">
-        <v>51237</v>
+        <v>49860</v>
       </c>
       <c r="D145" s="4">
         <f t="shared" si="2"/>
@@ -2277,34 +2284,30 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="4" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="C146" s="4">
-        <v>53055</v>
+        <v>50063</v>
       </c>
       <c r="D146" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:4">
-      <c r="A147" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C147" s="4">
-        <v>53377</v>
-      </c>
-      <c r="D147" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
+    <row r="147" spans="1:4" ht="18.75">
+      <c r="A147" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B147" s="10"/>
+      <c r="C147" s="10"/>
+      <c r="D147" s="10"/>
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C148" s="4">
-        <v>53698</v>
+        <v>50314</v>
       </c>
       <c r="D148" s="4">
         <f t="shared" si="2"/>
@@ -2313,10 +2316,10 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="4" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="C149" s="4">
-        <v>54021</v>
+        <v>51237</v>
       </c>
       <c r="D149" s="4">
         <f t="shared" si="2"/>
@@ -2325,10 +2328,10 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C150" s="4">
-        <v>56284</v>
+        <v>53055</v>
       </c>
       <c r="D150" s="4">
         <f t="shared" si="2"/>
@@ -2337,33 +2340,81 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C151" s="4">
+        <v>53377</v>
+      </c>
+      <c r="D151" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4">
+      <c r="A152" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C152" s="4">
+        <v>53698</v>
+      </c>
+      <c r="D152" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4">
+      <c r="A153" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C153" s="4">
+        <v>54021</v>
+      </c>
+      <c r="D153" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4">
+      <c r="A154" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C154" s="4">
+        <v>56284</v>
+      </c>
+      <c r="D154" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4">
+      <c r="A155" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B151" s="9"/>
-      <c r="C151" s="9">
+      <c r="B155" s="9"/>
+      <c r="C155" s="9">
         <v>0.68541666666666667</v>
       </c>
-      <c r="D151" s="9">
+      <c r="D155" s="9">
         <v>2.7083333333333334E-2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A121:D121"/>
-    <mergeCell ref="A129:D129"/>
-    <mergeCell ref="A143:D143"/>
-    <mergeCell ref="A51:D51"/>
-    <mergeCell ref="A64:D64"/>
-    <mergeCell ref="A76:D76"/>
-    <mergeCell ref="A85:D85"/>
-    <mergeCell ref="A90:D90"/>
-    <mergeCell ref="A112:D112"/>
+    <mergeCell ref="A47:D47"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="A125:D125"/>
+    <mergeCell ref="A133:D133"/>
+    <mergeCell ref="A147:D147"/>
+    <mergeCell ref="A55:D55"/>
+    <mergeCell ref="A68:D68"/>
+    <mergeCell ref="A80:D80"/>
+    <mergeCell ref="A89:D89"/>
+    <mergeCell ref="A94:D94"/>
+    <mergeCell ref="A116:D116"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -4480,12 +4531,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A31:D31"/>
     <mergeCell ref="A121:D121"/>
     <mergeCell ref="A129:D129"/>
     <mergeCell ref="A143:D143"/>
@@ -4495,6 +4540,12 @@
     <mergeCell ref="A85:D85"/>
     <mergeCell ref="A90:D90"/>
     <mergeCell ref="A112:D112"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A31:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -6399,6 +6450,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A29:D29"/>
     <mergeCell ref="A127:D127"/>
     <mergeCell ref="A107:D107"/>
     <mergeCell ref="A113:D113"/>
@@ -6409,11 +6465,6 @@
     <mergeCell ref="A98:D98"/>
     <mergeCell ref="A66:D66"/>
     <mergeCell ref="A55:D55"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A29:D29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>

</xml_diff>

<commit_message>
Wario 100% - about half of level 2 done.
</commit_message>
<xml_diff>
--- a/Wario/Wario.xlsx
+++ b/Wario/Wario.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="74">
   <si>
     <t>Enter pipe</t>
   </si>
@@ -276,7 +276,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -298,6 +298,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -334,7 +340,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -345,9 +351,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -642,11 +649,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J155"/>
+  <dimension ref="A1:J157"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -670,12 +677,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -703,12 +710,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -778,12 +785,12 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="18.75">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="4" t="s">
@@ -808,7 +815,7 @@
         <v>3359</v>
       </c>
       <c r="D16" s="4">
-        <f t="shared" ref="D16:D93" si="1">IF(B16 &gt;  0,C16-B16, 0)</f>
+        <f t="shared" ref="D16:D95" si="1">IF(B16 &gt;  0,C16-B16, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -840,88 +847,79 @@
       <c r="A19" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="B19" s="4">
+        <v>4346</v>
+      </c>
       <c r="C19" s="4">
         <v>3880</v>
       </c>
       <c r="D19" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-466</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="B20" s="4">
+        <v>4936</v>
+      </c>
       <c r="C20" s="4">
         <v>4470</v>
       </c>
       <c r="D20" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-466</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="4">
+        <v>5289</v>
+      </c>
+      <c r="C21" s="13"/>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C23" s="4">
         <v>4661</v>
       </c>
-      <c r="D21" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" s="4">
-        <v>4865</v>
-      </c>
-      <c r="D22" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A23" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
+      <c r="D23" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C24" s="4">
-        <v>5114</v>
+        <v>4865</v>
       </c>
       <c r="D24" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C25" s="4">
-        <v>5680</v>
-      </c>
-      <c r="D25" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+    <row r="25" spans="1:4" s="1" customFormat="1" ht="18.75">
+      <c r="A25" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="4" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C26" s="4">
-        <v>6399</v>
+        <v>5114</v>
       </c>
       <c r="D26" s="4">
         <f t="shared" si="1"/>
@@ -929,11 +927,11 @@
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C27" s="4">
-        <v>6767</v>
+        <v>5680</v>
       </c>
       <c r="D27" s="4">
         <f t="shared" si="1"/>
@@ -942,10 +940,10 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="4" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="C28" s="4">
-        <v>7021</v>
+        <v>6399</v>
       </c>
       <c r="D28" s="4">
         <f t="shared" si="1"/>
@@ -954,10 +952,10 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="4" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C29" s="4">
-        <v>7303</v>
+        <v>6767</v>
       </c>
       <c r="D29" s="4">
         <f t="shared" si="1"/>
@@ -966,10 +964,10 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C30" s="4">
-        <v>7679</v>
+        <v>7021</v>
       </c>
       <c r="D30" s="4">
         <f t="shared" si="1"/>
@@ -978,10 +976,10 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="4" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C31" s="4">
-        <v>7889</v>
+        <v>7303</v>
       </c>
       <c r="D31" s="4">
         <f t="shared" si="1"/>
@@ -990,10 +988,10 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="4" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="C32" s="4">
-        <v>8242</v>
+        <v>7679</v>
       </c>
       <c r="D32" s="4">
         <f t="shared" si="1"/>
@@ -1002,10 +1000,10 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="4" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C33" s="4">
-        <v>8601</v>
+        <v>7889</v>
       </c>
       <c r="D33" s="4">
         <f t="shared" si="1"/>
@@ -1014,54 +1012,54 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="4" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="C34" s="4">
-        <v>8805</v>
+        <v>8242</v>
       </c>
       <c r="D34" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="18.75">
-      <c r="A35" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
+    <row r="35" spans="1:4">
+      <c r="A35" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C35" s="4">
+        <v>8601</v>
+      </c>
+      <c r="D35" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C36" s="4">
-        <v>9054</v>
+        <v>8805</v>
       </c>
       <c r="D36" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C37" s="4">
-        <v>9397</v>
-      </c>
-      <c r="D37" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+    <row r="37" spans="1:4" ht="18.75">
+      <c r="A37" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37" s="12"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="4" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="C38" s="4">
-        <v>9633</v>
+        <v>9054</v>
       </c>
       <c r="D38" s="4">
         <f t="shared" si="1"/>
@@ -1070,10 +1068,10 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="4" t="s">
-        <v>26</v>
+        <v>66</v>
       </c>
       <c r="C39" s="4">
-        <v>9932</v>
+        <v>9397</v>
       </c>
       <c r="D39" s="4">
         <f t="shared" si="1"/>
@@ -1082,10 +1080,10 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="4" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C40" s="4">
-        <v>11304</v>
+        <v>9633</v>
       </c>
       <c r="D40" s="4">
         <f t="shared" si="1"/>
@@ -1094,10 +1092,10 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="4" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="C41" s="4">
-        <v>12308</v>
+        <v>9932</v>
       </c>
       <c r="D41" s="4">
         <f t="shared" si="1"/>
@@ -1106,10 +1104,10 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="4" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C42" s="4">
-        <v>13312</v>
+        <v>11304</v>
       </c>
       <c r="D42" s="4">
         <f t="shared" si="1"/>
@@ -1118,10 +1116,10 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="4" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C43" s="4">
-        <v>14611</v>
+        <v>12308</v>
       </c>
       <c r="D43" s="4">
         <f t="shared" si="1"/>
@@ -1130,10 +1128,10 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="4" t="s">
-        <v>20</v>
+        <v>62</v>
       </c>
       <c r="C44" s="4">
-        <v>14800</v>
+        <v>13312</v>
       </c>
       <c r="D44" s="4">
         <f t="shared" si="1"/>
@@ -1142,10 +1140,10 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="4" t="s">
-        <v>27</v>
+        <v>67</v>
       </c>
       <c r="C45" s="4">
-        <v>14936</v>
+        <v>14611</v>
       </c>
       <c r="D45" s="4">
         <f t="shared" si="1"/>
@@ -1154,54 +1152,54 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="4" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C46" s="4">
-        <v>15140</v>
+        <v>14800</v>
       </c>
       <c r="D46" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="18.75">
-      <c r="A47" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B47" s="11"/>
-      <c r="C47" s="11"/>
-      <c r="D47" s="11"/>
+    <row r="47" spans="1:4">
+      <c r="A47" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C47" s="4">
+        <v>14936</v>
+      </c>
+      <c r="D47" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C48" s="4">
-        <v>15390</v>
+        <v>15140</v>
       </c>
       <c r="D48" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
-      <c r="A49" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C49" s="4">
-        <v>15841</v>
-      </c>
-      <c r="D49" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+    <row r="49" spans="1:10" ht="18.75">
+      <c r="A49" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B49" s="10"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
     </row>
     <row r="50" spans="1:10">
       <c r="A50" s="4" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="C50" s="4">
-        <v>16245</v>
+        <v>15390</v>
       </c>
       <c r="D50" s="4">
         <f t="shared" si="1"/>
@@ -1213,7 +1211,7 @@
         <v>7</v>
       </c>
       <c r="C51" s="4">
-        <v>16760</v>
+        <v>15841</v>
       </c>
       <c r="D51" s="4">
         <f t="shared" si="1"/>
@@ -1222,10 +1220,10 @@
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="4" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C52" s="4">
-        <v>16939</v>
+        <v>16245</v>
       </c>
       <c r="D52" s="4">
         <f t="shared" si="1"/>
@@ -1234,10 +1232,10 @@
     </row>
     <row r="53" spans="1:10">
       <c r="A53" s="4" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="C53" s="4">
-        <v>17105</v>
+        <v>16760</v>
       </c>
       <c r="D53" s="4">
         <f t="shared" si="1"/>
@@ -1246,54 +1244,54 @@
     </row>
     <row r="54" spans="1:10">
       <c r="A54" s="4" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
       <c r="C54" s="4">
-        <v>17309</v>
+        <v>16939</v>
       </c>
       <c r="D54" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="18.75">
-      <c r="A55" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B55" s="10"/>
-      <c r="C55" s="10"/>
-      <c r="D55" s="10"/>
+    <row r="55" spans="1:10">
+      <c r="A55" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C55" s="4">
+        <v>17105</v>
+      </c>
+      <c r="D55" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="56" spans="1:10">
       <c r="A56" s="4" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
       <c r="C56" s="4">
-        <v>17558</v>
+        <v>17309</v>
       </c>
       <c r="D56" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
-      <c r="A57" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C57" s="4">
-        <v>18431</v>
-      </c>
-      <c r="D57" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+    <row r="57" spans="1:10" ht="18.75">
+      <c r="A57" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B57" s="12"/>
+      <c r="C57" s="12"/>
+      <c r="D57" s="12"/>
     </row>
     <row r="58" spans="1:10">
       <c r="A58" s="4" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="C58" s="4">
-        <v>18823</v>
+        <v>17558</v>
       </c>
       <c r="D58" s="4">
         <f t="shared" si="1"/>
@@ -1305,58 +1303,58 @@
         <v>19</v>
       </c>
       <c r="C59" s="4">
-        <v>19078</v>
+        <v>18431</v>
       </c>
       <c r="D59" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F59" s="6"/>
-      <c r="H59" s="6"/>
-      <c r="J59" s="6"/>
     </row>
     <row r="60" spans="1:10">
       <c r="A60" s="4" t="s">
-        <v>20</v>
+        <v>7</v>
+      </c>
+      <c r="C60" s="4">
+        <v>18823</v>
       </c>
       <c r="D60" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F60" s="7"/>
-      <c r="H60" s="7"/>
-      <c r="J60" s="7"/>
     </row>
     <row r="61" spans="1:10">
       <c r="A61" s="4" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="C61" s="4">
-        <v>19425</v>
+        <v>19078</v>
       </c>
       <c r="D61" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="F61" s="6"/>
+      <c r="H61" s="6"/>
+      <c r="J61" s="6"/>
     </row>
     <row r="62" spans="1:10">
       <c r="A62" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C62" s="4">
-        <v>19693</v>
+        <v>20</v>
       </c>
       <c r="D62" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="F62" s="7"/>
+      <c r="H62" s="7"/>
+      <c r="J62" s="7"/>
     </row>
     <row r="63" spans="1:10">
       <c r="A63" s="4" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="C63" s="4">
-        <v>20164</v>
+        <v>19425</v>
       </c>
       <c r="D63" s="4">
         <f t="shared" si="1"/>
@@ -1368,7 +1366,7 @@
         <v>7</v>
       </c>
       <c r="C64" s="4">
-        <v>20507</v>
+        <v>19693</v>
       </c>
       <c r="D64" s="4">
         <f t="shared" si="1"/>
@@ -1380,7 +1378,7 @@
         <v>7</v>
       </c>
       <c r="C65" s="4">
-        <v>20719</v>
+        <v>20164</v>
       </c>
       <c r="D65" s="4">
         <f t="shared" si="1"/>
@@ -1389,10 +1387,10 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="4" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="C66" s="4">
-        <v>20839</v>
+        <v>20507</v>
       </c>
       <c r="D66" s="4">
         <f t="shared" si="1"/>
@@ -1401,54 +1399,54 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="4" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="C67" s="4">
-        <v>21043</v>
+        <v>20719</v>
       </c>
       <c r="D67" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="18.75">
-      <c r="A68" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B68" s="11"/>
-      <c r="C68" s="11"/>
-      <c r="D68" s="11"/>
+    <row r="68" spans="1:4">
+      <c r="A68" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C68" s="4">
+        <v>20839</v>
+      </c>
+      <c r="D68" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C69" s="4">
-        <v>21292</v>
+        <v>21043</v>
       </c>
       <c r="D69" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
-      <c r="A70" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C70" s="4">
-        <v>21654</v>
-      </c>
-      <c r="D70" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+    <row r="70" spans="1:4" ht="18.75">
+      <c r="A70" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B70" s="10"/>
+      <c r="C70" s="10"/>
+      <c r="D70" s="10"/>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="4" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="C71" s="4">
-        <v>22525</v>
+        <v>21292</v>
       </c>
       <c r="D71" s="4">
         <f t="shared" si="1"/>
@@ -1457,10 +1455,10 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="4" t="s">
-        <v>6</v>
+        <v>69</v>
       </c>
       <c r="C72" s="4">
-        <v>22683</v>
+        <v>21654</v>
       </c>
       <c r="D72" s="4">
         <f t="shared" si="1"/>
@@ -1469,10 +1467,10 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C73" s="4">
-        <v>22853</v>
+        <v>22525</v>
       </c>
       <c r="D73" s="4">
         <f t="shared" si="1"/>
@@ -1481,10 +1479,10 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="4" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C74" s="4">
-        <v>23177</v>
+        <v>22683</v>
       </c>
       <c r="D74" s="4">
         <f t="shared" si="1"/>
@@ -1496,7 +1494,7 @@
         <v>7</v>
       </c>
       <c r="C75" s="4">
-        <v>23709</v>
+        <v>22853</v>
       </c>
       <c r="D75" s="4">
         <f t="shared" si="1"/>
@@ -1505,7 +1503,10 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="4" t="s">
-        <v>7</v>
+        <v>20</v>
+      </c>
+      <c r="C76" s="4">
+        <v>23177</v>
       </c>
       <c r="D76" s="4">
         <f t="shared" si="1"/>
@@ -1516,6 +1517,9 @@
       <c r="A77" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="C77" s="4">
+        <v>23709</v>
+      </c>
       <c r="D77" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -1523,7 +1527,7 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="4" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="D78" s="4">
         <f t="shared" si="1"/>
@@ -1532,51 +1536,45 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C79" s="4">
-        <v>24691</v>
+        <v>7</v>
       </c>
       <c r="D79" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="18.75">
-      <c r="A80" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B80" s="10"/>
-      <c r="C80" s="10"/>
-      <c r="D80" s="10"/>
+    <row r="80" spans="1:4">
+      <c r="A80" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D80" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
+      </c>
+      <c r="C81" s="4">
+        <v>24691</v>
       </c>
       <c r="D81" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:4">
-      <c r="A82" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C82" s="4">
-        <v>26245</v>
-      </c>
-      <c r="D82" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+    <row r="82" spans="1:4" ht="18.75">
+      <c r="A82" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B82" s="12"/>
+      <c r="C82" s="12"/>
+      <c r="D82" s="12"/>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C83" s="4">
-        <v>27387</v>
+        <v>37</v>
       </c>
       <c r="D83" s="4">
         <f t="shared" si="1"/>
@@ -1584,11 +1582,11 @@
       </c>
     </row>
     <row r="84" spans="1:4">
-      <c r="A84" s="4" t="s">
-        <v>60</v>
+      <c r="A84" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="C84" s="4">
-        <v>28067</v>
+        <v>26245</v>
       </c>
       <c r="D84" s="4">
         <f t="shared" si="1"/>
@@ -1597,10 +1595,10 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="4" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C85" s="4">
-        <v>28747</v>
+        <v>27387</v>
       </c>
       <c r="D85" s="4">
         <f t="shared" si="1"/>
@@ -1609,10 +1607,10 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="4" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="C86" s="4">
-        <v>30220</v>
+        <v>28067</v>
       </c>
       <c r="D86" s="4">
         <f t="shared" si="1"/>
@@ -1621,59 +1619,62 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="4" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="C87" s="4">
-        <v>30546</v>
+        <v>28747</v>
+      </c>
+      <c r="D87" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C88" s="4">
-        <v>30749</v>
+        <v>30220</v>
       </c>
       <c r="D88" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="18.75">
-      <c r="A89" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B89" s="11"/>
-      <c r="C89" s="11"/>
-      <c r="D89" s="11"/>
+    <row r="89" spans="1:4">
+      <c r="A89" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C89" s="4">
+        <v>30546</v>
+      </c>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C90" s="4">
-        <v>30998</v>
+        <v>30749</v>
       </c>
       <c r="D90" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:4">
-      <c r="A91" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D91" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+    <row r="91" spans="1:4" ht="18.75">
+      <c r="A91" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B91" s="10"/>
+      <c r="C91" s="10"/>
+      <c r="D91" s="10"/>
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="4" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="C92" s="4">
-        <v>33405</v>
+        <v>30998</v>
       </c>
       <c r="D92" s="4">
         <f t="shared" si="1"/>
@@ -1682,51 +1683,54 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C93" s="4">
-        <v>33609</v>
+        <v>20</v>
       </c>
       <c r="D93" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="18.75">
-      <c r="A94" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B94" s="10"/>
-      <c r="C94" s="10"/>
-      <c r="D94" s="10"/>
+    <row r="94" spans="1:4">
+      <c r="A94" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C94" s="4">
+        <v>33405</v>
+      </c>
+      <c r="D94" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="4" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C95" s="4">
-        <v>33858</v>
+        <v>33609</v>
       </c>
       <c r="D95" s="4">
-        <f t="shared" ref="D95:D154" si="2">IF(B95 &gt;  0,C95-B95, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4">
-      <c r="A96" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D96" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="18.75">
+      <c r="A96" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B96" s="12"/>
+      <c r="C96" s="12"/>
+      <c r="D96" s="12"/>
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="C97" s="4">
+        <v>33858</v>
       </c>
       <c r="D97" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="D97:D156" si="2">IF(B97 &gt;  0,C97-B97, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1743,9 +1747,6 @@
       <c r="A99" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C99" s="4">
-        <v>3</v>
-      </c>
       <c r="D99" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1753,7 +1754,7 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D100" s="4">
         <f t="shared" si="2"/>
@@ -1762,7 +1763,10 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
+      </c>
+      <c r="C101" s="4">
+        <v>3</v>
       </c>
       <c r="D101" s="4">
         <f t="shared" si="2"/>
@@ -1771,10 +1775,7 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C102" s="4">
-        <v>35512</v>
+        <v>46</v>
       </c>
       <c r="D102" s="4">
         <f t="shared" si="2"/>
@@ -1783,10 +1784,7 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C103" s="4">
-        <v>35693</v>
+        <v>47</v>
       </c>
       <c r="D103" s="4">
         <f t="shared" si="2"/>
@@ -1795,10 +1793,10 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="4" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="C104" s="4">
-        <v>35847</v>
+        <v>35512</v>
       </c>
       <c r="D104" s="4">
         <f t="shared" si="2"/>
@@ -1810,7 +1808,7 @@
         <v>6</v>
       </c>
       <c r="C105" s="4">
-        <v>36020</v>
+        <v>35693</v>
       </c>
       <c r="D105" s="4">
         <f t="shared" si="2"/>
@@ -1821,6 +1819,9 @@
       <c r="A106" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="C106" s="4">
+        <v>35847</v>
+      </c>
       <c r="D106" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1830,6 +1831,9 @@
       <c r="A107" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="C107" s="4">
+        <v>36020</v>
+      </c>
       <c r="D107" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1855,10 +1859,7 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C110" s="4">
-        <v>38056</v>
+        <v>6</v>
       </c>
       <c r="D110" s="4">
         <f t="shared" si="2"/>
@@ -1869,9 +1870,6 @@
       <c r="A111" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C111" s="4">
-        <v>38245</v>
-      </c>
       <c r="D111" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1879,10 +1877,10 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C112" s="4">
-        <v>38420</v>
+        <v>38056</v>
       </c>
       <c r="D112" s="4">
         <f t="shared" si="2"/>
@@ -1891,10 +1889,10 @@
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="4" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="C113" s="4">
-        <v>38758</v>
+        <v>38245</v>
       </c>
       <c r="D113" s="4">
         <f t="shared" si="2"/>
@@ -1903,10 +1901,10 @@
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="4" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C114" s="4">
-        <v>38859</v>
+        <v>38420</v>
       </c>
       <c r="D114" s="4">
         <f t="shared" si="2"/>
@@ -1915,54 +1913,54 @@
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="4" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="C115" s="4">
-        <v>39062</v>
+        <v>38758</v>
       </c>
       <c r="D115" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:5" ht="18.75">
-      <c r="A116" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B116" s="11"/>
-      <c r="C116" s="11"/>
-      <c r="D116" s="11"/>
+    <row r="116" spans="1:5">
+      <c r="A116" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C116" s="4">
+        <v>38859</v>
+      </c>
+      <c r="D116" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="4" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="C117" s="4">
-        <v>39312</v>
+        <v>39062</v>
       </c>
       <c r="D117" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:5">
-      <c r="A118" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C118" s="4">
-        <v>40069</v>
-      </c>
-      <c r="D118" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
+    <row r="118" spans="1:5" ht="18.75">
+      <c r="A118" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B118" s="10"/>
+      <c r="C118" s="10"/>
+      <c r="D118" s="10"/>
     </row>
     <row r="119" spans="1:5">
       <c r="A119" s="4" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="C119" s="4">
-        <v>40681</v>
+        <v>39312</v>
       </c>
       <c r="D119" s="4">
         <f t="shared" si="2"/>
@@ -1974,7 +1972,7 @@
         <v>19</v>
       </c>
       <c r="C120" s="4">
-        <v>41240</v>
+        <v>40069</v>
       </c>
       <c r="D120" s="4">
         <f t="shared" si="2"/>
@@ -1983,17 +1981,14 @@
     </row>
     <row r="121" spans="1:5">
       <c r="A121" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C121" s="4">
-        <v>41469</v>
+        <v>40681</v>
       </c>
       <c r="D121" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
-      </c>
-      <c r="E121" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="122" spans="1:5">
@@ -2001,7 +1996,7 @@
         <v>19</v>
       </c>
       <c r="C122" s="4">
-        <v>41728</v>
+        <v>41240</v>
       </c>
       <c r="D122" s="4">
         <f t="shared" si="2"/>
@@ -2010,66 +2005,69 @@
     </row>
     <row r="123" spans="1:5">
       <c r="A123" s="4" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C123" s="4">
-        <v>42015</v>
+        <v>41469</v>
       </c>
       <c r="D123" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
+      </c>
+      <c r="E123" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="124" spans="1:5">
       <c r="A124" s="4" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="C124" s="4">
-        <v>42219</v>
+        <v>41728</v>
       </c>
       <c r="D124" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:5" ht="18.75">
-      <c r="A125" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B125" s="10"/>
-      <c r="C125" s="10"/>
-      <c r="D125" s="10"/>
+    <row r="125" spans="1:5">
+      <c r="A125" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C125" s="4">
+        <v>42015</v>
+      </c>
+      <c r="D125" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="126" spans="1:5">
       <c r="A126" s="4" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="C126" s="4">
-        <v>42469</v>
+        <v>42219</v>
       </c>
       <c r="D126" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:5">
-      <c r="A127" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C127" s="4">
-        <v>43196</v>
-      </c>
-      <c r="D127" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
+    <row r="127" spans="1:5" ht="18.75">
+      <c r="A127" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B127" s="12"/>
+      <c r="C127" s="12"/>
+      <c r="D127" s="12"/>
     </row>
     <row r="128" spans="1:5">
       <c r="A128" s="4" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C128" s="4">
-        <v>43848</v>
+        <v>42469</v>
       </c>
       <c r="D128" s="4">
         <f t="shared" si="2"/>
@@ -2078,10 +2076,10 @@
     </row>
     <row r="129" spans="1:5">
       <c r="A129" s="4" t="s">
-        <v>26</v>
+        <v>66</v>
       </c>
       <c r="C129" s="4">
-        <v>44155</v>
+        <v>43196</v>
       </c>
       <c r="D129" s="4">
         <f t="shared" si="2"/>
@@ -2090,10 +2088,10 @@
     </row>
     <row r="130" spans="1:5">
       <c r="A130" s="4" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="C130" s="4">
-        <v>46549</v>
+        <v>43848</v>
       </c>
       <c r="D130" s="4">
         <f t="shared" si="2"/>
@@ -2102,10 +2100,10 @@
     </row>
     <row r="131" spans="1:5">
       <c r="A131" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C131" s="4">
-        <v>46905</v>
+        <v>44155</v>
       </c>
       <c r="D131" s="4">
         <f t="shared" si="2"/>
@@ -2114,54 +2112,54 @@
     </row>
     <row r="132" spans="1:5">
       <c r="A132" s="4" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="C132" s="4">
-        <v>47108</v>
+        <v>46549</v>
       </c>
       <c r="D132" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:5" ht="18.75">
-      <c r="A133" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="B133" s="11"/>
-      <c r="C133" s="11"/>
-      <c r="D133" s="11"/>
+    <row r="133" spans="1:5">
+      <c r="A133" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C133" s="4">
+        <v>46905</v>
+      </c>
+      <c r="D133" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="134" spans="1:5">
       <c r="A134" s="4" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="C134" s="4">
-        <v>47359</v>
+        <v>47108</v>
       </c>
       <c r="D134" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:5">
-      <c r="A135" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C135" s="4">
-        <v>47668</v>
-      </c>
-      <c r="D135" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
+    <row r="135" spans="1:5" ht="18.75">
+      <c r="A135" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B135" s="10"/>
+      <c r="C135" s="10"/>
+      <c r="D135" s="10"/>
     </row>
     <row r="136" spans="1:5">
       <c r="A136" s="4" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="C136" s="4">
-        <v>47847</v>
+        <v>47359</v>
       </c>
       <c r="D136" s="4">
         <f t="shared" si="2"/>
@@ -2170,10 +2168,10 @@
     </row>
     <row r="137" spans="1:5">
       <c r="A137" s="4" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="C137" s="4">
-        <v>48052</v>
+        <v>47668</v>
       </c>
       <c r="D137" s="4">
         <f t="shared" si="2"/>
@@ -2182,10 +2180,10 @@
     </row>
     <row r="138" spans="1:5">
       <c r="A138" s="4" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C138" s="4">
-        <v>48226</v>
+        <v>47847</v>
       </c>
       <c r="D138" s="4">
         <f t="shared" si="2"/>
@@ -2194,10 +2192,10 @@
     </row>
     <row r="139" spans="1:5">
       <c r="A139" s="4" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="C139" s="4">
-        <v>48530</v>
+        <v>48052</v>
       </c>
       <c r="D139" s="4">
         <f t="shared" si="2"/>
@@ -2209,22 +2207,19 @@
         <v>7</v>
       </c>
       <c r="C140" s="4">
-        <v>48705</v>
+        <v>48226</v>
       </c>
       <c r="D140" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
-      </c>
-      <c r="E140" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="141" spans="1:5">
       <c r="A141" s="4" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="C141" s="4">
-        <v>48820</v>
+        <v>48530</v>
       </c>
       <c r="D141" s="4">
         <f t="shared" si="2"/>
@@ -2233,188 +2228,215 @@
     </row>
     <row r="142" spans="1:5">
       <c r="A142" s="4" t="s">
-        <v>57</v>
+        <v>7</v>
       </c>
       <c r="C142" s="4">
-        <v>49147</v>
+        <v>48705</v>
       </c>
       <c r="D142" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
+      </c>
+      <c r="E142" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="143" spans="1:5">
       <c r="A143" s="4" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="C143" s="4">
-        <v>49319</v>
+        <v>48820</v>
       </c>
       <c r="D143" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
-      </c>
-      <c r="E143" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="144" spans="1:5">
       <c r="A144" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C144" s="4">
+        <v>49147</v>
+      </c>
+      <c r="D144" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5">
+      <c r="A145" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C144" s="4">
+      <c r="C145" s="4">
+        <v>49319</v>
+      </c>
+      <c r="D145" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E145" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5">
+      <c r="A146" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C146" s="4">
         <v>49569</v>
       </c>
-      <c r="D144" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4">
-      <c r="A145" s="4" t="s">
+      <c r="D146" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5">
+      <c r="A147" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C145" s="4">
+      <c r="C147" s="4">
         <v>49860</v>
       </c>
-      <c r="D145" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4">
-      <c r="A146" s="4" t="s">
+      <c r="D147" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5">
+      <c r="A148" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C146" s="4">
+      <c r="C148" s="4">
         <v>50063</v>
       </c>
-      <c r="D146" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" ht="18.75">
-      <c r="A147" s="10" t="s">
+      <c r="D148" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" ht="18.75">
+      <c r="A149" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="B147" s="10"/>
-      <c r="C147" s="10"/>
-      <c r="D147" s="10"/>
-    </row>
-    <row r="148" spans="1:4">
-      <c r="A148" s="4" t="s">
+      <c r="B149" s="12"/>
+      <c r="C149" s="12"/>
+      <c r="D149" s="12"/>
+    </row>
+    <row r="150" spans="1:5">
+      <c r="A150" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C148" s="4">
+      <c r="C150" s="4">
         <v>50314</v>
       </c>
-      <c r="D148" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4">
-      <c r="A149" s="4" t="s">
+      <c r="D150" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5">
+      <c r="A151" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C149" s="4">
+      <c r="C151" s="4">
         <v>51237</v>
       </c>
-      <c r="D149" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4">
-      <c r="A150" s="4" t="s">
+      <c r="D151" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5">
+      <c r="A152" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C150" s="4">
+      <c r="C152" s="4">
         <v>53055</v>
       </c>
-      <c r="D150" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4">
-      <c r="A151" s="4" t="s">
+      <c r="D152" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5">
+      <c r="A153" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C151" s="4">
+      <c r="C153" s="4">
         <v>53377</v>
       </c>
-      <c r="D151" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4">
-      <c r="A152" s="4" t="s">
+      <c r="D153" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5">
+      <c r="A154" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C152" s="4">
+      <c r="C154" s="4">
         <v>53698</v>
       </c>
-      <c r="D152" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4">
-      <c r="A153" s="4" t="s">
+      <c r="D154" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5">
+      <c r="A155" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C153" s="4">
+      <c r="C155" s="4">
         <v>54021</v>
       </c>
-      <c r="D153" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4">
-      <c r="A154" s="4" t="s">
+      <c r="D155" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5">
+      <c r="A156" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C154" s="4">
+      <c r="C156" s="4">
         <v>56284</v>
       </c>
-      <c r="D154" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4">
-      <c r="A155" s="4" t="s">
+      <c r="D156" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5">
+      <c r="A157" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B155" s="9"/>
-      <c r="C155" s="9">
+      <c r="B157" s="9"/>
+      <c r="C157" s="9">
         <v>0.68541666666666667</v>
       </c>
-      <c r="D155" s="9">
+      <c r="D157" s="9">
         <v>2.7083333333333334E-2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A47:D47"/>
+    <mergeCell ref="A127:D127"/>
+    <mergeCell ref="A135:D135"/>
+    <mergeCell ref="A149:D149"/>
+    <mergeCell ref="A57:D57"/>
+    <mergeCell ref="A70:D70"/>
+    <mergeCell ref="A82:D82"/>
+    <mergeCell ref="A91:D91"/>
+    <mergeCell ref="A96:D96"/>
+    <mergeCell ref="A118:D118"/>
+    <mergeCell ref="A49:D49"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="A14:D14"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="A125:D125"/>
-    <mergeCell ref="A133:D133"/>
-    <mergeCell ref="A147:D147"/>
-    <mergeCell ref="A55:D55"/>
-    <mergeCell ref="A68:D68"/>
-    <mergeCell ref="A80:D80"/>
-    <mergeCell ref="A89:D89"/>
-    <mergeCell ref="A94:D94"/>
-    <mergeCell ref="A116:D116"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A37:D37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -2451,12 +2473,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -2484,12 +2506,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -2523,12 +2545,12 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
@@ -2651,12 +2673,12 @@
       </c>
     </row>
     <row r="19" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="4" t="s">
@@ -2824,12 +2846,12 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="18.75">
-      <c r="A31" s="10" t="s">
+      <c r="A31" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="4" t="s">
@@ -2997,12 +3019,12 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="18.75">
-      <c r="A43" s="11" t="s">
+      <c r="A43" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B43" s="11"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="4" t="s">
@@ -3110,12 +3132,12 @@
       </c>
     </row>
     <row r="51" spans="1:10" ht="18.75">
-      <c r="A51" s="10" t="s">
+      <c r="A51" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B51" s="10"/>
-      <c r="C51" s="10"/>
-      <c r="D51" s="10"/>
+      <c r="B51" s="12"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="12"/>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="4" t="s">
@@ -3301,12 +3323,12 @@
       </c>
     </row>
     <row r="64" spans="1:10" ht="18.75">
-      <c r="A64" s="11" t="s">
+      <c r="A64" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B64" s="11"/>
-      <c r="C64" s="11"/>
-      <c r="D64" s="11"/>
+      <c r="B64" s="10"/>
+      <c r="C64" s="10"/>
+      <c r="D64" s="10"/>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="4" t="s">
@@ -3465,12 +3487,12 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="18.75">
-      <c r="A76" s="10" t="s">
+      <c r="A76" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B76" s="10"/>
-      <c r="C76" s="10"/>
-      <c r="D76" s="10"/>
+      <c r="B76" s="12"/>
+      <c r="C76" s="12"/>
+      <c r="D76" s="12"/>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="4" t="s">
@@ -3583,12 +3605,12 @@
       </c>
     </row>
     <row r="85" spans="1:4" ht="18.75">
-      <c r="A85" s="11" t="s">
+      <c r="A85" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B85" s="11"/>
-      <c r="C85" s="11"/>
-      <c r="D85" s="11"/>
+      <c r="B85" s="10"/>
+      <c r="C85" s="10"/>
+      <c r="D85" s="10"/>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="4" t="s">
@@ -3648,12 +3670,12 @@
       </c>
     </row>
     <row r="90" spans="1:4" ht="18.75">
-      <c r="A90" s="10" t="s">
+      <c r="A90" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B90" s="10"/>
-      <c r="C90" s="10"/>
-      <c r="D90" s="10"/>
+      <c r="B90" s="12"/>
+      <c r="C90" s="12"/>
+      <c r="D90" s="12"/>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="4" t="s">
@@ -3944,12 +3966,12 @@
       </c>
     </row>
     <row r="112" spans="1:4" ht="18.75">
-      <c r="A112" s="11" t="s">
+      <c r="A112" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="B112" s="11"/>
-      <c r="C112" s="11"/>
-      <c r="D112" s="11"/>
+      <c r="B112" s="10"/>
+      <c r="C112" s="10"/>
+      <c r="D112" s="10"/>
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="4" t="s">
@@ -4075,12 +4097,12 @@
       </c>
     </row>
     <row r="121" spans="1:5" ht="18.75">
-      <c r="A121" s="10" t="s">
+      <c r="A121" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B121" s="10"/>
-      <c r="C121" s="10"/>
-      <c r="D121" s="10"/>
+      <c r="B121" s="12"/>
+      <c r="C121" s="12"/>
+      <c r="D121" s="12"/>
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="4" t="s">
@@ -4188,12 +4210,12 @@
       </c>
     </row>
     <row r="129" spans="1:5" ht="18.75">
-      <c r="A129" s="11" t="s">
+      <c r="A129" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B129" s="11"/>
-      <c r="C129" s="11"/>
-      <c r="D129" s="11"/>
+      <c r="B129" s="10"/>
+      <c r="C129" s="10"/>
+      <c r="D129" s="10"/>
     </row>
     <row r="130" spans="1:5">
       <c r="A130" s="4" t="s">
@@ -4397,12 +4419,12 @@
       </c>
     </row>
     <row r="143" spans="1:5" ht="18.75">
-      <c r="A143" s="10" t="s">
+      <c r="A143" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="B143" s="10"/>
-      <c r="C143" s="10"/>
-      <c r="D143" s="10"/>
+      <c r="B143" s="12"/>
+      <c r="C143" s="12"/>
+      <c r="D143" s="12"/>
     </row>
     <row r="144" spans="1:5">
       <c r="A144" s="4" t="s">
@@ -4531,6 +4553,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A31:D31"/>
     <mergeCell ref="A121:D121"/>
     <mergeCell ref="A129:D129"/>
     <mergeCell ref="A143:D143"/>
@@ -4540,12 +4568,6 @@
     <mergeCell ref="A85:D85"/>
     <mergeCell ref="A90:D90"/>
     <mergeCell ref="A112:D112"/>
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A31:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -4582,12 +4604,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -4615,12 +4637,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -4654,12 +4676,12 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
@@ -4743,12 +4765,12 @@
       </c>
     </row>
     <row r="17" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="4" t="s">
@@ -4916,12 +4938,12 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="18.75">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="4" t="s">
@@ -4999,12 +5021,12 @@
       </c>
     </row>
     <row r="35" spans="1:10" ht="18.75">
-      <c r="A35" s="11" t="s">
+      <c r="A35" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="4" t="s">
@@ -5097,12 +5119,12 @@
       </c>
     </row>
     <row r="42" spans="1:10" ht="18.75">
-      <c r="A42" s="10" t="s">
+      <c r="A42" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B42" s="10"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="4" t="s">
@@ -5291,12 +5313,12 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="18.75">
-      <c r="A55" s="11" t="s">
+      <c r="A55" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B55" s="11"/>
-      <c r="C55" s="11"/>
-      <c r="D55" s="11"/>
+      <c r="B55" s="10"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="10"/>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="4" t="s">
@@ -5449,12 +5471,12 @@
       </c>
     </row>
     <row r="66" spans="1:4" ht="18.75">
-      <c r="A66" s="10" t="s">
+      <c r="A66" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B66" s="10"/>
-      <c r="C66" s="10"/>
-      <c r="D66" s="10"/>
+      <c r="B66" s="12"/>
+      <c r="C66" s="12"/>
+      <c r="D66" s="12"/>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="4" t="s">
@@ -5517,12 +5539,12 @@
       </c>
     </row>
     <row r="71" spans="1:4" ht="18.75">
-      <c r="A71" s="11" t="s">
+      <c r="A71" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B71" s="11"/>
-      <c r="C71" s="11"/>
-      <c r="D71" s="11"/>
+      <c r="B71" s="10"/>
+      <c r="C71" s="10"/>
+      <c r="D71" s="10"/>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="4" t="s">
@@ -5585,12 +5607,12 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="18.75">
-      <c r="A76" s="10" t="s">
+      <c r="A76" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B76" s="10"/>
-      <c r="C76" s="10"/>
-      <c r="D76" s="10"/>
+      <c r="B76" s="12"/>
+      <c r="C76" s="12"/>
+      <c r="D76" s="12"/>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="4" t="s">
@@ -5908,12 +5930,12 @@
       </c>
     </row>
     <row r="98" spans="1:5" ht="18.75">
-      <c r="A98" s="11" t="s">
+      <c r="A98" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="B98" s="11"/>
-      <c r="C98" s="11"/>
-      <c r="D98" s="11"/>
+      <c r="B98" s="10"/>
+      <c r="C98" s="10"/>
+      <c r="D98" s="10"/>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="4" t="s">
@@ -6039,12 +6061,12 @@
       </c>
     </row>
     <row r="107" spans="1:5" ht="18.75">
-      <c r="A107" s="10" t="s">
+      <c r="A107" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B107" s="10"/>
-      <c r="C107" s="10"/>
-      <c r="D107" s="10"/>
+      <c r="B107" s="12"/>
+      <c r="C107" s="12"/>
+      <c r="D107" s="12"/>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="4" t="s">
@@ -6122,12 +6144,12 @@
       </c>
     </row>
     <row r="113" spans="1:4" ht="18.75">
-      <c r="A113" s="11" t="s">
+      <c r="A113" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B113" s="11"/>
-      <c r="C113" s="11"/>
-      <c r="D113" s="11"/>
+      <c r="B113" s="10"/>
+      <c r="C113" s="10"/>
+      <c r="D113" s="10"/>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="4" t="s">
@@ -6325,12 +6347,12 @@
       </c>
     </row>
     <row r="127" spans="1:4" ht="18.75">
-      <c r="A127" s="10" t="s">
+      <c r="A127" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="B127" s="10"/>
-      <c r="C127" s="10"/>
-      <c r="D127" s="10"/>
+      <c r="B127" s="12"/>
+      <c r="C127" s="12"/>
+      <c r="D127" s="12"/>
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="4" t="s">
@@ -6450,11 +6472,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A29:D29"/>
     <mergeCell ref="A127:D127"/>
     <mergeCell ref="A107:D107"/>
     <mergeCell ref="A113:D113"/>
@@ -6465,6 +6482,11 @@
     <mergeCell ref="A98:D98"/>
     <mergeCell ref="A66:D66"/>
     <mergeCell ref="A55:D55"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A29:D29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>

</xml_diff>

<commit_message>
Wario 100% - all of level 2 done.
</commit_message>
<xml_diff>
--- a/Wario/Wario.xlsx
+++ b/Wario/Wario.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="75">
   <si>
     <t>Enter pipe</t>
   </si>
@@ -238,6 +238,9 @@
   </si>
   <si>
     <t>Exit Room</t>
+  </si>
+  <si>
+    <t>Up Pipe</t>
   </si>
 </sst>
 </file>
@@ -649,11 +652,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J157"/>
+  <dimension ref="A1:J162"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -815,7 +818,7 @@
         <v>3359</v>
       </c>
       <c r="D16" s="4">
-        <f t="shared" ref="D16:D95" si="1">IF(B16 &gt;  0,C16-B16, 0)</f>
+        <f t="shared" ref="D16:D100" si="1">IF(B16 &gt;  0,C16-B16, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -882,116 +885,113 @@
       </c>
       <c r="C21" s="13"/>
     </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="4">
+        <v>5477</v>
+      </c>
+      <c r="C22" s="13"/>
+    </row>
     <row r="23" spans="1:4">
       <c r="A23" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C23" s="4">
-        <v>4661</v>
-      </c>
-      <c r="D23" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="B23" s="4">
+        <v>5738</v>
+      </c>
+      <c r="C23" s="13"/>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C24" s="4">
-        <v>4865</v>
-      </c>
-      <c r="D24" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A25" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
+        <v>72</v>
+      </c>
+      <c r="C24" s="13"/>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="13"/>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C26" s="4">
-        <v>5114</v>
-      </c>
-      <c r="D26" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="B26" s="4">
+        <v>6255</v>
+      </c>
+      <c r="C26" s="13"/>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C27" s="4">
-        <v>5680</v>
-      </c>
-      <c r="D27" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="A27" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27" s="4">
+        <v>6442</v>
+      </c>
+      <c r="C27" s="13"/>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="4" t="s">
-        <v>0</v>
+        <v>27</v>
+      </c>
+      <c r="B28" s="4">
+        <v>6546</v>
       </c>
       <c r="C28" s="4">
-        <v>6399</v>
+        <v>4661</v>
       </c>
       <c r="D28" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-1885</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="4" t="s">
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="B29" s="4">
+        <v>6758</v>
       </c>
       <c r="C29" s="4">
-        <v>6767</v>
+        <v>4865</v>
       </c>
       <c r="D29" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C30" s="4">
-        <v>7021</v>
-      </c>
-      <c r="D30" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+        <v>-1893</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" s="1" customFormat="1" ht="18.75">
+      <c r="A30" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
+      </c>
+      <c r="B31" s="4">
+        <v>7007</v>
       </c>
       <c r="C31" s="4">
-        <v>7303</v>
+        <v>5114</v>
       </c>
       <c r="D31" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-1893</v>
       </c>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="4" t="s">
-        <v>21</v>
+      <c r="A32" s="5" t="s">
+        <v>0</v>
       </c>
       <c r="C32" s="4">
-        <v>7679</v>
+        <v>5680</v>
       </c>
       <c r="D32" s="4">
         <f t="shared" si="1"/>
@@ -1003,7 +1003,7 @@
         <v>0</v>
       </c>
       <c r="C33" s="4">
-        <v>7889</v>
+        <v>6399</v>
       </c>
       <c r="D33" s="4">
         <f t="shared" si="1"/>
@@ -1015,7 +1015,7 @@
         <v>0</v>
       </c>
       <c r="C34" s="4">
-        <v>8242</v>
+        <v>6767</v>
       </c>
       <c r="D34" s="4">
         <f t="shared" si="1"/>
@@ -1024,10 +1024,10 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C35" s="4">
-        <v>8601</v>
+        <v>7021</v>
       </c>
       <c r="D35" s="4">
         <f t="shared" si="1"/>
@@ -1036,30 +1036,34 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C36" s="4">
-        <v>8805</v>
+        <v>7303</v>
       </c>
       <c r="D36" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="18.75">
-      <c r="A37" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B37" s="12"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
+    <row r="37" spans="1:4">
+      <c r="A37" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37" s="4">
+        <v>7679</v>
+      </c>
+      <c r="D37" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="4" t="s">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="C38" s="4">
-        <v>9054</v>
+        <v>7889</v>
       </c>
       <c r="D38" s="4">
         <f t="shared" si="1"/>
@@ -1068,10 +1072,10 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="4" t="s">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="C39" s="4">
-        <v>9397</v>
+        <v>8242</v>
       </c>
       <c r="D39" s="4">
         <f t="shared" si="1"/>
@@ -1080,10 +1084,10 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="4" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="C40" s="4">
-        <v>9633</v>
+        <v>8601</v>
       </c>
       <c r="D40" s="4">
         <f t="shared" si="1"/>
@@ -1092,34 +1096,30 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C41" s="4">
-        <v>9932</v>
+        <v>8805</v>
       </c>
       <c r="D41" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C42" s="4">
-        <v>11304</v>
-      </c>
-      <c r="D42" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+    <row r="42" spans="1:4" ht="18.75">
+      <c r="A42" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="4" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="C43" s="4">
-        <v>12308</v>
+        <v>9054</v>
       </c>
       <c r="D43" s="4">
         <f t="shared" si="1"/>
@@ -1128,10 +1128,10 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="4" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C44" s="4">
-        <v>13312</v>
+        <v>9397</v>
       </c>
       <c r="D44" s="4">
         <f t="shared" si="1"/>
@@ -1140,10 +1140,10 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="4" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C45" s="4">
-        <v>14611</v>
+        <v>9633</v>
       </c>
       <c r="D45" s="4">
         <f t="shared" si="1"/>
@@ -1152,10 +1152,10 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="4" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C46" s="4">
-        <v>14800</v>
+        <v>9932</v>
       </c>
       <c r="D46" s="4">
         <f t="shared" si="1"/>
@@ -1164,10 +1164,10 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="4" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="C47" s="4">
-        <v>14936</v>
+        <v>11304</v>
       </c>
       <c r="D47" s="4">
         <f t="shared" si="1"/>
@@ -1176,376 +1176,385 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C48" s="4">
+        <v>12308</v>
+      </c>
+      <c r="D48" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C49" s="4">
+        <v>13312</v>
+      </c>
+      <c r="D49" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C50" s="4">
+        <v>14611</v>
+      </c>
+      <c r="D50" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C51" s="4">
+        <v>14800</v>
+      </c>
+      <c r="D51" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C52" s="4">
+        <v>14936</v>
+      </c>
+      <c r="D52" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C48" s="4">
+      <c r="C53" s="4">
         <v>15140</v>
       </c>
-      <c r="D48" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" ht="18.75">
-      <c r="A49" s="10" t="s">
+      <c r="D53" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="18.75">
+      <c r="A54" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B49" s="10"/>
-      <c r="C49" s="10"/>
-      <c r="D49" s="10"/>
-    </row>
-    <row r="50" spans="1:10">
-      <c r="A50" s="4" t="s">
+      <c r="B54" s="10"/>
+      <c r="C54" s="10"/>
+      <c r="D54" s="10"/>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C50" s="4">
+      <c r="C55" s="4">
         <v>15390</v>
       </c>
-      <c r="D50" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10">
-      <c r="A51" s="4" t="s">
+      <c r="D55" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C51" s="4">
+      <c r="C56" s="4">
         <v>15841</v>
       </c>
-      <c r="D51" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10">
-      <c r="A52" s="4" t="s">
+      <c r="D56" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C52" s="4">
+      <c r="C57" s="4">
         <v>16245</v>
       </c>
-      <c r="D52" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10">
-      <c r="A53" s="4" t="s">
+      <c r="D57" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C53" s="4">
+      <c r="C58" s="4">
         <v>16760</v>
       </c>
-      <c r="D53" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10">
-      <c r="A54" s="4" t="s">
+      <c r="D58" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C54" s="4">
+      <c r="C59" s="4">
         <v>16939</v>
       </c>
-      <c r="D54" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10">
-      <c r="A55" s="4" t="s">
+      <c r="D59" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C55" s="4">
+      <c r="C60" s="4">
         <v>17105</v>
       </c>
-      <c r="D55" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10">
-      <c r="A56" s="4" t="s">
+      <c r="D60" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C56" s="4">
+      <c r="C61" s="4">
         <v>17309</v>
       </c>
-      <c r="D56" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" ht="18.75">
-      <c r="A57" s="12" t="s">
+      <c r="D61" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="18.75">
+      <c r="A62" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B57" s="12"/>
-      <c r="C57" s="12"/>
-      <c r="D57" s="12"/>
-    </row>
-    <row r="58" spans="1:10">
-      <c r="A58" s="4" t="s">
+      <c r="B62" s="12"/>
+      <c r="C62" s="12"/>
+      <c r="D62" s="12"/>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C58" s="4">
+      <c r="C63" s="4">
         <v>17558</v>
       </c>
-      <c r="D58" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10">
-      <c r="A59" s="4" t="s">
+      <c r="D63" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C59" s="4">
+      <c r="C64" s="4">
         <v>18431</v>
       </c>
-      <c r="D59" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10">
-      <c r="A60" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C60" s="4">
-        <v>18823</v>
-      </c>
-      <c r="D60" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10">
-      <c r="A61" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C61" s="4">
-        <v>19078</v>
-      </c>
-      <c r="D61" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F61" s="6"/>
-      <c r="H61" s="6"/>
-      <c r="J61" s="6"/>
-    </row>
-    <row r="62" spans="1:10">
-      <c r="A62" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D62" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F62" s="7"/>
-      <c r="H62" s="7"/>
-      <c r="J62" s="7"/>
-    </row>
-    <row r="63" spans="1:10">
-      <c r="A63" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C63" s="4">
-        <v>19425</v>
-      </c>
-      <c r="D63" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10">
-      <c r="A64" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C64" s="4">
-        <v>19693</v>
-      </c>
       <c r="D64" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:10">
       <c r="A65" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C65" s="4">
+        <v>18823</v>
+      </c>
+      <c r="D65" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10">
+      <c r="A66" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C66" s="4">
+        <v>19078</v>
+      </c>
+      <c r="D66" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F66" s="6"/>
+      <c r="H66" s="6"/>
+      <c r="J66" s="6"/>
+    </row>
+    <row r="67" spans="1:10">
+      <c r="A67" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D67" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F67" s="7"/>
+      <c r="H67" s="7"/>
+      <c r="J67" s="7"/>
+    </row>
+    <row r="68" spans="1:10">
+      <c r="A68" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C68" s="4">
+        <v>19425</v>
+      </c>
+      <c r="D68" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10">
+      <c r="A69" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C69" s="4">
+        <v>19693</v>
+      </c>
+      <c r="D69" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10">
+      <c r="A70" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C70" s="4">
         <v>20164</v>
       </c>
-      <c r="D65" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4">
-      <c r="A66" s="4" t="s">
+      <c r="D70" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10">
+      <c r="A71" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C66" s="4">
+      <c r="C71" s="4">
         <v>20507</v>
       </c>
-      <c r="D66" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4">
-      <c r="A67" s="4" t="s">
+      <c r="D71" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10">
+      <c r="A72" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C67" s="4">
+      <c r="C72" s="4">
         <v>20719</v>
       </c>
-      <c r="D67" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4">
-      <c r="A68" s="4" t="s">
+      <c r="D72" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10">
+      <c r="A73" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C68" s="4">
+      <c r="C73" s="4">
         <v>20839</v>
       </c>
-      <c r="D68" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4">
-      <c r="A69" s="4" t="s">
+      <c r="D73" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10">
+      <c r="A74" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C69" s="4">
+      <c r="C74" s="4">
         <v>21043</v>
       </c>
-      <c r="D69" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="18.75">
-      <c r="A70" s="10" t="s">
+      <c r="D74" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" ht="18.75">
+      <c r="A75" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B70" s="10"/>
-      <c r="C70" s="10"/>
-      <c r="D70" s="10"/>
-    </row>
-    <row r="71" spans="1:4">
-      <c r="A71" s="4" t="s">
+      <c r="B75" s="10"/>
+      <c r="C75" s="10"/>
+      <c r="D75" s="10"/>
+    </row>
+    <row r="76" spans="1:10">
+      <c r="A76" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C71" s="4">
+      <c r="C76" s="4">
         <v>21292</v>
       </c>
-      <c r="D71" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4">
-      <c r="A72" s="4" t="s">
+      <c r="D76" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10">
+      <c r="A77" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C72" s="4">
+      <c r="C77" s="4">
         <v>21654</v>
       </c>
-      <c r="D72" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4">
-      <c r="A73" s="4" t="s">
+      <c r="D77" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10">
+      <c r="A78" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C73" s="4">
+      <c r="C78" s="4">
         <v>22525</v>
       </c>
-      <c r="D73" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4">
-      <c r="A74" s="4" t="s">
+      <c r="D78" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10">
+      <c r="A79" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C74" s="4">
+      <c r="C79" s="4">
         <v>22683</v>
       </c>
-      <c r="D74" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4">
-      <c r="A75" s="4" t="s">
+      <c r="D79" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10">
+      <c r="A80" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C75" s="4">
+      <c r="C80" s="4">
         <v>22853</v>
-      </c>
-      <c r="D75" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4">
-      <c r="A76" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C76" s="4">
-        <v>23177</v>
-      </c>
-      <c r="D76" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4">
-      <c r="A77" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C77" s="4">
-        <v>23709</v>
-      </c>
-      <c r="D77" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4">
-      <c r="A78" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D78" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4">
-      <c r="A79" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D79" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4">
-      <c r="A80" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="D80" s="4">
         <f t="shared" si="1"/>
@@ -1554,27 +1563,31 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="4" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="C81" s="4">
-        <v>24691</v>
+        <v>23177</v>
       </c>
       <c r="D81" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="18.75">
-      <c r="A82" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B82" s="12"/>
-      <c r="C82" s="12"/>
-      <c r="D82" s="12"/>
+    <row r="82" spans="1:4">
+      <c r="A82" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C82" s="4">
+        <v>23709</v>
+      </c>
+      <c r="D82" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="4" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="D83" s="4">
         <f t="shared" si="1"/>
@@ -1582,11 +1595,8 @@
       </c>
     </row>
     <row r="84" spans="1:4">
-      <c r="A84" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C84" s="4">
-        <v>26245</v>
+      <c r="A84" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="D84" s="4">
         <f t="shared" si="1"/>
@@ -1595,10 +1605,7 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C85" s="4">
-        <v>27387</v>
+        <v>27</v>
       </c>
       <c r="D85" s="4">
         <f t="shared" si="1"/>
@@ -1607,34 +1614,27 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="4" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="C86" s="4">
-        <v>28067</v>
+        <v>24691</v>
       </c>
       <c r="D86" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:4">
-      <c r="A87" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C87" s="4">
-        <v>28747</v>
-      </c>
-      <c r="D87" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+    <row r="87" spans="1:4" ht="18.75">
+      <c r="A87" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B87" s="12"/>
+      <c r="C87" s="12"/>
+      <c r="D87" s="12"/>
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C88" s="4">
-        <v>30220</v>
+        <v>37</v>
       </c>
       <c r="D88" s="4">
         <f t="shared" si="1"/>
@@ -1642,39 +1642,47 @@
       </c>
     </row>
     <row r="89" spans="1:4">
-      <c r="A89" s="4" t="s">
-        <v>27</v>
+      <c r="A89" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="C89" s="4">
-        <v>30546</v>
+        <v>26245</v>
+      </c>
+      <c r="D89" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="4" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="C90" s="4">
-        <v>30749</v>
+        <v>27387</v>
       </c>
       <c r="D90" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="18.75">
-      <c r="A91" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B91" s="10"/>
-      <c r="C91" s="10"/>
-      <c r="D91" s="10"/>
+    <row r="91" spans="1:4">
+      <c r="A91" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C91" s="4">
+        <v>28067</v>
+      </c>
+      <c r="D91" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="4" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="C92" s="4">
-        <v>30998</v>
+        <v>28747</v>
       </c>
       <c r="D92" s="4">
         <f t="shared" si="1"/>
@@ -1683,7 +1691,10 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="4" t="s">
-        <v>20</v>
+        <v>39</v>
+      </c>
+      <c r="C93" s="4">
+        <v>30220</v>
       </c>
       <c r="D93" s="4">
         <f t="shared" si="1"/>
@@ -1695,19 +1706,15 @@
         <v>27</v>
       </c>
       <c r="C94" s="4">
-        <v>33405</v>
-      </c>
-      <c r="D94" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>30546</v>
       </c>
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="4" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C95" s="4">
-        <v>33609</v>
+        <v>30749</v>
       </c>
       <c r="D95" s="4">
         <f t="shared" si="1"/>
@@ -1715,76 +1722,81 @@
       </c>
     </row>
     <row r="96" spans="1:4" ht="18.75">
-      <c r="A96" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B96" s="12"/>
-      <c r="C96" s="12"/>
-      <c r="D96" s="12"/>
+      <c r="A96" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B96" s="10"/>
+      <c r="C96" s="10"/>
+      <c r="D96" s="10"/>
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C97" s="4">
-        <v>33858</v>
+        <v>30998</v>
       </c>
       <c r="D97" s="4">
-        <f t="shared" ref="D97:D156" si="2">IF(B97 &gt;  0,C97-B97, 0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="4" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="D98" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="4" t="s">
-        <v>45</v>
+        <v>27</v>
+      </c>
+      <c r="C99" s="4">
+        <v>33405</v>
       </c>
       <c r="D99" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="4" t="s">
-        <v>45</v>
+        <v>34</v>
+      </c>
+      <c r="C100" s="4">
+        <v>33609</v>
       </c>
       <c r="D100" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4">
-      <c r="A101" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C101" s="4">
-        <v>3</v>
-      </c>
-      <c r="D101" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" ht="18.75">
+      <c r="A101" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B101" s="12"/>
+      <c r="C101" s="12"/>
+      <c r="D101" s="12"/>
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
+      </c>
+      <c r="C102" s="4">
+        <v>33858</v>
       </c>
       <c r="D102" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="D102:D161" si="2">IF(B102 &gt;  0,C102-B102, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D103" s="4">
         <f t="shared" si="2"/>
@@ -1793,10 +1805,7 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C104" s="4">
-        <v>35512</v>
+        <v>45</v>
       </c>
       <c r="D104" s="4">
         <f t="shared" si="2"/>
@@ -1805,10 +1814,7 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C105" s="4">
-        <v>35693</v>
+        <v>45</v>
       </c>
       <c r="D105" s="4">
         <f t="shared" si="2"/>
@@ -1817,10 +1823,10 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="4" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="C106" s="4">
-        <v>35847</v>
+        <v>3</v>
       </c>
       <c r="D106" s="4">
         <f t="shared" si="2"/>
@@ -1829,10 +1835,7 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C107" s="4">
-        <v>36020</v>
+        <v>46</v>
       </c>
       <c r="D107" s="4">
         <f t="shared" si="2"/>
@@ -1841,7 +1844,7 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="4" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="D108" s="4">
         <f t="shared" si="2"/>
@@ -1850,7 +1853,10 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="4" t="s">
-        <v>6</v>
+        <v>19</v>
+      </c>
+      <c r="C109" s="4">
+        <v>35512</v>
       </c>
       <c r="D109" s="4">
         <f t="shared" si="2"/>
@@ -1861,6 +1867,9 @@
       <c r="A110" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="C110" s="4">
+        <v>35693</v>
+      </c>
       <c r="D110" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1870,6 +1879,9 @@
       <c r="A111" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="C111" s="4">
+        <v>35847</v>
+      </c>
       <c r="D111" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1877,10 +1889,10 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="4" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C112" s="4">
-        <v>38056</v>
+        <v>36020</v>
       </c>
       <c r="D112" s="4">
         <f t="shared" si="2"/>
@@ -1891,9 +1903,6 @@
       <c r="A113" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C113" s="4">
-        <v>38245</v>
-      </c>
       <c r="D113" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1901,10 +1910,7 @@
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C114" s="4">
-        <v>38420</v>
+        <v>6</v>
       </c>
       <c r="D114" s="4">
         <f t="shared" si="2"/>
@@ -1913,10 +1919,7 @@
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C115" s="4">
-        <v>38758</v>
+        <v>6</v>
       </c>
       <c r="D115" s="4">
         <f t="shared" si="2"/>
@@ -1925,10 +1928,7 @@
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C116" s="4">
-        <v>38859</v>
+        <v>6</v>
       </c>
       <c r="D116" s="4">
         <f t="shared" si="2"/>
@@ -1937,30 +1937,34 @@
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="4" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="C117" s="4">
-        <v>39062</v>
+        <v>38056</v>
       </c>
       <c r="D117" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:5" ht="18.75">
-      <c r="A118" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="B118" s="10"/>
-      <c r="C118" s="10"/>
-      <c r="D118" s="10"/>
+    <row r="118" spans="1:5">
+      <c r="A118" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C118" s="4">
+        <v>38245</v>
+      </c>
+      <c r="D118" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="119" spans="1:5">
       <c r="A119" s="4" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="C119" s="4">
-        <v>39312</v>
+        <v>38420</v>
       </c>
       <c r="D119" s="4">
         <f t="shared" si="2"/>
@@ -1972,7 +1976,7 @@
         <v>19</v>
       </c>
       <c r="C120" s="4">
-        <v>40069</v>
+        <v>38758</v>
       </c>
       <c r="D120" s="4">
         <f t="shared" si="2"/>
@@ -1981,10 +1985,10 @@
     </row>
     <row r="121" spans="1:5">
       <c r="A121" s="4" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C121" s="4">
-        <v>40681</v>
+        <v>38859</v>
       </c>
       <c r="D121" s="4">
         <f t="shared" si="2"/>
@@ -1993,37 +1997,30 @@
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="4" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="C122" s="4">
-        <v>41240</v>
+        <v>39062</v>
       </c>
       <c r="D122" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:5">
-      <c r="A123" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C123" s="4">
-        <v>41469</v>
-      </c>
-      <c r="D123" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E123" t="s">
-        <v>50</v>
-      </c>
+    <row r="123" spans="1:5" ht="18.75">
+      <c r="A123" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B123" s="10"/>
+      <c r="C123" s="10"/>
+      <c r="D123" s="10"/>
     </row>
     <row r="124" spans="1:5">
       <c r="A124" s="4" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="C124" s="4">
-        <v>41728</v>
+        <v>39312</v>
       </c>
       <c r="D124" s="4">
         <f t="shared" si="2"/>
@@ -2032,10 +2029,10 @@
     </row>
     <row r="125" spans="1:5">
       <c r="A125" s="4" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C125" s="4">
-        <v>42015</v>
+        <v>40069</v>
       </c>
       <c r="D125" s="4">
         <f t="shared" si="2"/>
@@ -2044,221 +2041,221 @@
     </row>
     <row r="126" spans="1:5">
       <c r="A126" s="4" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="C126" s="4">
-        <v>42219</v>
+        <v>40681</v>
       </c>
       <c r="D126" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:5" ht="18.75">
-      <c r="A127" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="B127" s="12"/>
-      <c r="C127" s="12"/>
-      <c r="D127" s="12"/>
+    <row r="127" spans="1:5">
+      <c r="A127" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C127" s="4">
+        <v>41240</v>
+      </c>
+      <c r="D127" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="128" spans="1:5">
       <c r="A128" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C128" s="4">
+        <v>41469</v>
+      </c>
+      <c r="D128" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E128" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
+      <c r="A129" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C129" s="4">
+        <v>41728</v>
+      </c>
+      <c r="D129" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C130" s="4">
+        <v>42015</v>
+      </c>
+      <c r="D130" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4">
+      <c r="A131" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C131" s="4">
+        <v>42219</v>
+      </c>
+      <c r="D131" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" ht="18.75">
+      <c r="A132" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B132" s="12"/>
+      <c r="C132" s="12"/>
+      <c r="D132" s="12"/>
+    </row>
+    <row r="133" spans="1:4">
+      <c r="A133" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C128" s="4">
+      <c r="C133" s="4">
         <v>42469</v>
       </c>
-      <c r="D128" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5">
-      <c r="A129" s="4" t="s">
+      <c r="D133" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
+      <c r="A134" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C129" s="4">
+      <c r="C134" s="4">
         <v>43196</v>
       </c>
-      <c r="D129" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5">
-      <c r="A130" s="4" t="s">
+      <c r="D134" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
+      <c r="A135" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C130" s="4">
+      <c r="C135" s="4">
         <v>43848</v>
       </c>
-      <c r="D130" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5">
-      <c r="A131" s="4" t="s">
+      <c r="D135" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
+      <c r="A136" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C131" s="4">
+      <c r="C136" s="4">
         <v>44155</v>
       </c>
-      <c r="D131" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5">
-      <c r="A132" s="4" t="s">
+      <c r="D136" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4">
+      <c r="A137" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C132" s="4">
+      <c r="C137" s="4">
         <v>46549</v>
       </c>
-      <c r="D132" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5">
-      <c r="A133" s="4" t="s">
+      <c r="D137" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4">
+      <c r="A138" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C133" s="4">
+      <c r="C138" s="4">
         <v>46905</v>
       </c>
-      <c r="D133" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5">
-      <c r="A134" s="4" t="s">
+      <c r="D138" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4">
+      <c r="A139" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C134" s="4">
+      <c r="C139" s="4">
         <v>47108</v>
       </c>
-      <c r="D134" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" ht="18.75">
-      <c r="A135" s="10" t="s">
+      <c r="D139" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" ht="18.75">
+      <c r="A140" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B135" s="10"/>
-      <c r="C135" s="10"/>
-      <c r="D135" s="10"/>
-    </row>
-    <row r="136" spans="1:5">
-      <c r="A136" s="4" t="s">
+      <c r="B140" s="10"/>
+      <c r="C140" s="10"/>
+      <c r="D140" s="10"/>
+    </row>
+    <row r="141" spans="1:4">
+      <c r="A141" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C136" s="4">
+      <c r="C141" s="4">
         <v>47359</v>
       </c>
-      <c r="D136" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5">
-      <c r="A137" s="4" t="s">
+      <c r="D141" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4">
+      <c r="A142" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C137" s="4">
+      <c r="C142" s="4">
         <v>47668</v>
       </c>
-      <c r="D137" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5">
-      <c r="A138" s="4" t="s">
+      <c r="D142" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4">
+      <c r="A143" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C138" s="4">
+      <c r="C143" s="4">
         <v>47847</v>
       </c>
-      <c r="D138" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5">
-      <c r="A139" s="4" t="s">
+      <c r="D143" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4">
+      <c r="A144" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C139" s="4">
+      <c r="C144" s="4">
         <v>48052</v>
-      </c>
-      <c r="D139" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5">
-      <c r="A140" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C140" s="4">
-        <v>48226</v>
-      </c>
-      <c r="D140" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5">
-      <c r="A141" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C141" s="4">
-        <v>48530</v>
-      </c>
-      <c r="D141" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5">
-      <c r="A142" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C142" s="4">
-        <v>48705</v>
-      </c>
-      <c r="D142" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E142" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5">
-      <c r="A143" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C143" s="4">
-        <v>48820</v>
-      </c>
-      <c r="D143" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5">
-      <c r="A144" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C144" s="4">
-        <v>49147</v>
       </c>
       <c r="D144" s="4">
         <f t="shared" si="2"/>
@@ -2267,17 +2264,14 @@
     </row>
     <row r="145" spans="1:5">
       <c r="A145" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C145" s="4">
-        <v>49319</v>
+        <v>48226</v>
       </c>
       <c r="D145" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
-      </c>
-      <c r="E145" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="146" spans="1:5">
@@ -2285,7 +2279,7 @@
         <v>6</v>
       </c>
       <c r="C146" s="4">
-        <v>49569</v>
+        <v>48530</v>
       </c>
       <c r="D146" s="4">
         <f t="shared" si="2"/>
@@ -2294,54 +2288,64 @@
     </row>
     <row r="147" spans="1:5">
       <c r="A147" s="4" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="C147" s="4">
-        <v>49860</v>
+        <v>48705</v>
       </c>
       <c r="D147" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
+      </c>
+      <c r="E147" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="148" spans="1:5">
       <c r="A148" s="4" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="C148" s="4">
-        <v>50063</v>
+        <v>48820</v>
       </c>
       <c r="D148" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:5" ht="18.75">
-      <c r="A149" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="B149" s="12"/>
-      <c r="C149" s="12"/>
-      <c r="D149" s="12"/>
+    <row r="149" spans="1:5">
+      <c r="A149" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C149" s="4">
+        <v>49147</v>
+      </c>
+      <c r="D149" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="150" spans="1:5">
       <c r="A150" s="4" t="s">
-        <v>58</v>
+        <v>6</v>
       </c>
       <c r="C150" s="4">
-        <v>50314</v>
+        <v>49319</v>
       </c>
       <c r="D150" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
+      </c>
+      <c r="E150" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="151" spans="1:5">
       <c r="A151" s="4" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="C151" s="4">
-        <v>51237</v>
+        <v>49569</v>
       </c>
       <c r="D151" s="4">
         <f t="shared" si="2"/>
@@ -2350,10 +2354,10 @@
     </row>
     <row r="152" spans="1:5">
       <c r="A152" s="4" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="C152" s="4">
-        <v>53055</v>
+        <v>49860</v>
       </c>
       <c r="D152" s="4">
         <f t="shared" si="2"/>
@@ -2362,34 +2366,30 @@
     </row>
     <row r="153" spans="1:5">
       <c r="A153" s="4" t="s">
-        <v>62</v>
+        <v>34</v>
       </c>
       <c r="C153" s="4">
-        <v>53377</v>
+        <v>50063</v>
       </c>
       <c r="D153" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:5">
-      <c r="A154" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C154" s="4">
-        <v>53698</v>
-      </c>
-      <c r="D154" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
+    <row r="154" spans="1:5" ht="18.75">
+      <c r="A154" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B154" s="12"/>
+      <c r="C154" s="12"/>
+      <c r="D154" s="12"/>
     </row>
     <row r="155" spans="1:5">
       <c r="A155" s="4" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C155" s="4">
-        <v>54021</v>
+        <v>50314</v>
       </c>
       <c r="D155" s="4">
         <f t="shared" si="2"/>
@@ -2398,10 +2398,10 @@
     </row>
     <row r="156" spans="1:5">
       <c r="A156" s="4" t="s">
-        <v>64</v>
+        <v>26</v>
       </c>
       <c r="C156" s="4">
-        <v>56284</v>
+        <v>51237</v>
       </c>
       <c r="D156" s="4">
         <f t="shared" si="2"/>
@@ -2410,33 +2410,93 @@
     </row>
     <row r="157" spans="1:5">
       <c r="A157" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C157" s="4">
+        <v>53055</v>
+      </c>
+      <c r="D157" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5">
+      <c r="A158" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C158" s="4">
+        <v>53377</v>
+      </c>
+      <c r="D158" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5">
+      <c r="A159" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C159" s="4">
+        <v>53698</v>
+      </c>
+      <c r="D159" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5">
+      <c r="A160" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C160" s="4">
+        <v>54021</v>
+      </c>
+      <c r="D160" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4">
+      <c r="A161" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C161" s="4">
+        <v>56284</v>
+      </c>
+      <c r="D161" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4">
+      <c r="A162" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B157" s="9"/>
-      <c r="C157" s="9">
+      <c r="B162" s="9"/>
+      <c r="C162" s="9">
         <v>0.68541666666666667</v>
       </c>
-      <c r="D157" s="9">
+      <c r="D162" s="9">
         <v>2.7083333333333334E-2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A127:D127"/>
-    <mergeCell ref="A135:D135"/>
-    <mergeCell ref="A149:D149"/>
-    <mergeCell ref="A57:D57"/>
-    <mergeCell ref="A70:D70"/>
-    <mergeCell ref="A82:D82"/>
-    <mergeCell ref="A91:D91"/>
+    <mergeCell ref="A132:D132"/>
+    <mergeCell ref="A140:D140"/>
+    <mergeCell ref="A154:D154"/>
+    <mergeCell ref="A62:D62"/>
+    <mergeCell ref="A75:D75"/>
+    <mergeCell ref="A87:D87"/>
     <mergeCell ref="A96:D96"/>
-    <mergeCell ref="A118:D118"/>
-    <mergeCell ref="A49:D49"/>
+    <mergeCell ref="A101:D101"/>
+    <mergeCell ref="A123:D123"/>
+    <mergeCell ref="A54:D54"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="A14:D14"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A42:D42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>

</xml_diff>

<commit_message>
Wario 100% - Level 3 done
</commit_message>
<xml_diff>
--- a/Wario/Wario.xlsx
+++ b/Wario/Wario.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="76">
   <si>
     <t>Enter pipe</t>
   </si>
@@ -241,6 +241,9 @@
   </si>
   <si>
     <t>Up Pipe</t>
+  </si>
+  <si>
+    <t>Exit door</t>
   </si>
 </sst>
 </file>
@@ -354,10 +357,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -652,11 +655,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J162"/>
+  <dimension ref="A1:J163"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -680,12 +683,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -713,12 +716,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -788,12 +791,12 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="18.75">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="4" t="s">
@@ -818,7 +821,7 @@
         <v>3359</v>
       </c>
       <c r="D16" s="4">
-        <f t="shared" ref="D16:D100" si="1">IF(B16 &gt;  0,C16-B16, 0)</f>
+        <f t="shared" ref="D16:D101" si="1">IF(B16 &gt;  0,C16-B16, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -883,7 +886,7 @@
       <c r="B21" s="4">
         <v>5289</v>
       </c>
-      <c r="C21" s="13"/>
+      <c r="C21" s="10"/>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="4" t="s">
@@ -892,7 +895,7 @@
       <c r="B22" s="4">
         <v>5477</v>
       </c>
-      <c r="C22" s="13"/>
+      <c r="C22" s="10"/>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="4" t="s">
@@ -901,19 +904,19 @@
       <c r="B23" s="4">
         <v>5738</v>
       </c>
-      <c r="C23" s="13"/>
+      <c r="C23" s="10"/>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="13"/>
+      <c r="C24" s="10"/>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="13"/>
+      <c r="C25" s="10"/>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="4" t="s">
@@ -922,7 +925,7 @@
       <c r="B26" s="4">
         <v>6255</v>
       </c>
-      <c r="C26" s="13"/>
+      <c r="C26" s="10"/>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="4" t="s">
@@ -931,7 +934,7 @@
       <c r="B27" s="4">
         <v>6442</v>
       </c>
-      <c r="C27" s="13"/>
+      <c r="C27" s="10"/>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="4" t="s">
@@ -964,12 +967,12 @@
       </c>
     </row>
     <row r="30" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A30" s="10" t="s">
+      <c r="A30" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="4" t="s">
@@ -990,160 +993,189 @@
       <c r="A32" s="5" t="s">
         <v>0</v>
       </c>
+      <c r="B32" s="4">
+        <v>7556</v>
+      </c>
       <c r="C32" s="4">
         <v>5680</v>
       </c>
       <c r="D32" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-1876</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="4" t="s">
         <v>0</v>
       </c>
+      <c r="B33" s="4">
+        <v>8275</v>
+      </c>
       <c r="C33" s="4">
         <v>6399</v>
       </c>
       <c r="D33" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-1876</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="4" t="s">
         <v>0</v>
       </c>
+      <c r="B34" s="4">
+        <v>8632</v>
+      </c>
       <c r="C34" s="4">
         <v>6767</v>
       </c>
       <c r="D34" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-1865</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="B35" s="4">
+        <v>8887</v>
+      </c>
       <c r="C35" s="4">
         <v>7021</v>
       </c>
       <c r="D35" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-1866</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="B36" s="4">
+        <v>9160</v>
+      </c>
       <c r="C36" s="4">
         <v>7303</v>
       </c>
       <c r="D36" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-1857</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="4" t="s">
         <v>21</v>
       </c>
+      <c r="B37" s="4">
+        <v>9545</v>
+      </c>
       <c r="C37" s="4">
         <v>7679</v>
       </c>
       <c r="D37" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-1866</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="4" t="s">
         <v>0</v>
       </c>
+      <c r="B38" s="4">
+        <v>9749</v>
+      </c>
       <c r="C38" s="4">
         <v>7889</v>
       </c>
       <c r="D38" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-1860</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="4" t="s">
         <v>0</v>
       </c>
+      <c r="B39" s="4">
+        <v>10102</v>
+      </c>
       <c r="C39" s="4">
         <v>8242</v>
       </c>
       <c r="D39" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-1860</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C40" s="4">
-        <v>8601</v>
-      </c>
-      <c r="D40" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>75</v>
+      </c>
+      <c r="B40" s="4">
+        <v>11070</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B41" s="4">
+        <v>11261</v>
+      </c>
+      <c r="C41" s="4">
+        <v>8601</v>
+      </c>
+      <c r="D41" s="4">
+        <f t="shared" si="1"/>
+        <v>-2660</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C41" s="4">
+      <c r="B42" s="4">
+        <v>11465</v>
+      </c>
+      <c r="C42" s="4">
         <v>8805</v>
       </c>
-      <c r="D41" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="18.75">
-      <c r="A42" s="12" t="s">
+      <c r="D42" s="4">
+        <f t="shared" si="1"/>
+        <v>-2660</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="18.75">
+      <c r="A43" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B42" s="12"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C43" s="4">
-        <v>9054</v>
-      </c>
-      <c r="D43" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="4" t="s">
-        <v>66</v>
+        <v>25</v>
+      </c>
+      <c r="B44" s="4">
+        <v>11714</v>
       </c>
       <c r="C44" s="4">
-        <v>9397</v>
+        <v>9054</v>
       </c>
       <c r="D44" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-2660</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="4" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="C45" s="4">
-        <v>9633</v>
+        <v>9397</v>
       </c>
       <c r="D45" s="4">
         <f t="shared" si="1"/>
@@ -1152,10 +1184,10 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="4" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="C46" s="4">
-        <v>9932</v>
+        <v>9633</v>
       </c>
       <c r="D46" s="4">
         <f t="shared" si="1"/>
@@ -1164,10 +1196,10 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="4" t="s">
-        <v>66</v>
+        <v>26</v>
       </c>
       <c r="C47" s="4">
-        <v>11304</v>
+        <v>9932</v>
       </c>
       <c r="D47" s="4">
         <f t="shared" si="1"/>
@@ -1176,10 +1208,10 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="4" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="C48" s="4">
-        <v>12308</v>
+        <v>11304</v>
       </c>
       <c r="D48" s="4">
         <f t="shared" si="1"/>
@@ -1188,10 +1220,10 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C49" s="4">
-        <v>13312</v>
+        <v>12308</v>
       </c>
       <c r="D49" s="4">
         <f t="shared" si="1"/>
@@ -1200,10 +1232,10 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C50" s="4">
-        <v>14611</v>
+        <v>13312</v>
       </c>
       <c r="D50" s="4">
         <f t="shared" si="1"/>
@@ -1212,10 +1244,10 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="4" t="s">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="C51" s="4">
-        <v>14800</v>
+        <v>14611</v>
       </c>
       <c r="D51" s="4">
         <f t="shared" si="1"/>
@@ -1224,10 +1256,10 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="4" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C52" s="4">
-        <v>14936</v>
+        <v>14800</v>
       </c>
       <c r="D52" s="4">
         <f t="shared" si="1"/>
@@ -1236,42 +1268,42 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C53" s="4">
+        <v>14936</v>
+      </c>
+      <c r="D53" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C53" s="4">
+      <c r="C54" s="4">
         <v>15140</v>
       </c>
-      <c r="D53" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="18.75">
-      <c r="A54" s="10" t="s">
+      <c r="D54" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="18.75">
+      <c r="A55" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B54" s="10"/>
-      <c r="C54" s="10"/>
-      <c r="D54" s="10"/>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C55" s="4">
-        <v>15390</v>
-      </c>
-      <c r="D55" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="B55" s="12"/>
+      <c r="C55" s="12"/>
+      <c r="D55" s="12"/>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="4" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="C56" s="4">
-        <v>15841</v>
+        <v>15390</v>
       </c>
       <c r="D56" s="4">
         <f t="shared" si="1"/>
@@ -1283,7 +1315,7 @@
         <v>7</v>
       </c>
       <c r="C57" s="4">
-        <v>16245</v>
+        <v>15841</v>
       </c>
       <c r="D57" s="4">
         <f t="shared" si="1"/>
@@ -1295,7 +1327,7 @@
         <v>7</v>
       </c>
       <c r="C58" s="4">
-        <v>16760</v>
+        <v>16245</v>
       </c>
       <c r="D58" s="4">
         <f t="shared" si="1"/>
@@ -1304,10 +1336,10 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="4" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C59" s="4">
-        <v>16939</v>
+        <v>16760</v>
       </c>
       <c r="D59" s="4">
         <f t="shared" si="1"/>
@@ -1316,10 +1348,10 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="4" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C60" s="4">
-        <v>17105</v>
+        <v>16939</v>
       </c>
       <c r="D60" s="4">
         <f t="shared" si="1"/>
@@ -1328,42 +1360,42 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C61" s="4">
+        <v>17105</v>
+      </c>
+      <c r="D61" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C61" s="4">
+      <c r="C62" s="4">
         <v>17309</v>
       </c>
-      <c r="D61" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="18.75">
-      <c r="A62" s="12" t="s">
+      <c r="D62" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="18.75">
+      <c r="A63" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B62" s="12"/>
-      <c r="C62" s="12"/>
-      <c r="D62" s="12"/>
-    </row>
-    <row r="63" spans="1:4">
-      <c r="A63" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C63" s="4">
-        <v>17558</v>
-      </c>
-      <c r="D63" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="B63" s="11"/>
+      <c r="C63" s="11"/>
+      <c r="D63" s="11"/>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="4" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C64" s="4">
-        <v>18431</v>
+        <v>17558</v>
       </c>
       <c r="D64" s="4">
         <f t="shared" si="1"/>
@@ -1372,10 +1404,10 @@
     </row>
     <row r="65" spans="1:10">
       <c r="A65" s="4" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C65" s="4">
-        <v>18823</v>
+        <v>18431</v>
       </c>
       <c r="D65" s="4">
         <f t="shared" si="1"/>
@@ -1384,49 +1416,49 @@
     </row>
     <row r="66" spans="1:10">
       <c r="A66" s="4" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C66" s="4">
-        <v>19078</v>
+        <v>18823</v>
       </c>
       <c r="D66" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F66" s="6"/>
-      <c r="H66" s="6"/>
-      <c r="J66" s="6"/>
     </row>
     <row r="67" spans="1:10">
       <c r="A67" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="C67" s="4">
+        <v>19078</v>
       </c>
       <c r="D67" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F67" s="7"/>
-      <c r="H67" s="7"/>
-      <c r="J67" s="7"/>
+      <c r="F67" s="6"/>
+      <c r="H67" s="6"/>
+      <c r="J67" s="6"/>
     </row>
     <row r="68" spans="1:10">
       <c r="A68" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C68" s="4">
-        <v>19425</v>
+        <v>20</v>
       </c>
       <c r="D68" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="F68" s="7"/>
+      <c r="H68" s="7"/>
+      <c r="J68" s="7"/>
     </row>
     <row r="69" spans="1:10">
       <c r="A69" s="4" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="C69" s="4">
-        <v>19693</v>
+        <v>19425</v>
       </c>
       <c r="D69" s="4">
         <f t="shared" si="1"/>
@@ -1438,7 +1470,7 @@
         <v>7</v>
       </c>
       <c r="C70" s="4">
-        <v>20164</v>
+        <v>19693</v>
       </c>
       <c r="D70" s="4">
         <f t="shared" si="1"/>
@@ -1450,7 +1482,7 @@
         <v>7</v>
       </c>
       <c r="C71" s="4">
-        <v>20507</v>
+        <v>20164</v>
       </c>
       <c r="D71" s="4">
         <f t="shared" si="1"/>
@@ -1462,7 +1494,7 @@
         <v>7</v>
       </c>
       <c r="C72" s="4">
-        <v>20719</v>
+        <v>20507</v>
       </c>
       <c r="D72" s="4">
         <f t="shared" si="1"/>
@@ -1471,10 +1503,10 @@
     </row>
     <row r="73" spans="1:10">
       <c r="A73" s="4" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="C73" s="4">
-        <v>20839</v>
+        <v>20719</v>
       </c>
       <c r="D73" s="4">
         <f t="shared" si="1"/>
@@ -1483,42 +1515,42 @@
     </row>
     <row r="74" spans="1:10">
       <c r="A74" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C74" s="4">
+        <v>20839</v>
+      </c>
+      <c r="D74" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10">
+      <c r="A75" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C74" s="4">
+      <c r="C75" s="4">
         <v>21043</v>
       </c>
-      <c r="D74" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" ht="18.75">
-      <c r="A75" s="10" t="s">
+      <c r="D75" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" ht="18.75">
+      <c r="A76" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B75" s="10"/>
-      <c r="C75" s="10"/>
-      <c r="D75" s="10"/>
-    </row>
-    <row r="76" spans="1:10">
-      <c r="A76" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C76" s="4">
-        <v>21292</v>
-      </c>
-      <c r="D76" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="B76" s="12"/>
+      <c r="C76" s="12"/>
+      <c r="D76" s="12"/>
     </row>
     <row r="77" spans="1:10">
       <c r="A77" s="4" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
       <c r="C77" s="4">
-        <v>21654</v>
+        <v>21292</v>
       </c>
       <c r="D77" s="4">
         <f t="shared" si="1"/>
@@ -1527,10 +1559,10 @@
     </row>
     <row r="78" spans="1:10">
       <c r="A78" s="4" t="s">
-        <v>6</v>
+        <v>69</v>
       </c>
       <c r="C78" s="4">
-        <v>22525</v>
+        <v>21654</v>
       </c>
       <c r="D78" s="4">
         <f t="shared" si="1"/>
@@ -1542,7 +1574,7 @@
         <v>6</v>
       </c>
       <c r="C79" s="4">
-        <v>22683</v>
+        <v>22525</v>
       </c>
       <c r="D79" s="4">
         <f t="shared" si="1"/>
@@ -1551,10 +1583,10 @@
     </row>
     <row r="80" spans="1:10">
       <c r="A80" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C80" s="4">
-        <v>22853</v>
+        <v>22683</v>
       </c>
       <c r="D80" s="4">
         <f t="shared" si="1"/>
@@ -1563,10 +1595,10 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="4" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C81" s="4">
-        <v>23177</v>
+        <v>22853</v>
       </c>
       <c r="D81" s="4">
         <f t="shared" si="1"/>
@@ -1575,10 +1607,10 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="4" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C82" s="4">
-        <v>23709</v>
+        <v>23177</v>
       </c>
       <c r="D82" s="4">
         <f t="shared" si="1"/>
@@ -1589,6 +1621,9 @@
       <c r="A83" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="C83" s="4">
+        <v>23709</v>
+      </c>
       <c r="D83" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -1605,7 +1640,7 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="4" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="D85" s="4">
         <f t="shared" si="1"/>
@@ -1614,51 +1649,48 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D86" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C86" s="4">
+      <c r="C87" s="4">
         <v>24691</v>
       </c>
-      <c r="D86" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" ht="18.75">
-      <c r="A87" s="12" t="s">
+      <c r="D87" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="18.75">
+      <c r="A88" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B87" s="12"/>
-      <c r="C87" s="12"/>
-      <c r="D87" s="12"/>
-    </row>
-    <row r="88" spans="1:4">
-      <c r="A88" s="4" t="s">
+      <c r="B88" s="11"/>
+      <c r="C88" s="11"/>
+      <c r="D88" s="11"/>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D88" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4">
-      <c r="A89" s="8" t="s">
+      <c r="D89" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C89" s="4">
+      <c r="C90" s="4">
         <v>26245</v>
-      </c>
-      <c r="D89" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4">
-      <c r="A90" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C90" s="4">
-        <v>27387</v>
       </c>
       <c r="D90" s="4">
         <f t="shared" si="1"/>
@@ -1667,10 +1699,10 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="4" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="C91" s="4">
-        <v>28067</v>
+        <v>27387</v>
       </c>
       <c r="D91" s="4">
         <f t="shared" si="1"/>
@@ -1679,10 +1711,10 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C92" s="4">
-        <v>28747</v>
+        <v>28067</v>
       </c>
       <c r="D92" s="4">
         <f t="shared" si="1"/>
@@ -1691,10 +1723,10 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="4" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="C93" s="4">
-        <v>30220</v>
+        <v>28747</v>
       </c>
       <c r="D93" s="4">
         <f t="shared" si="1"/>
@@ -1703,47 +1735,50 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="4" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="C94" s="4">
-        <v>30546</v>
+        <v>30220</v>
+      </c>
+      <c r="D94" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C95" s="4">
+        <v>30546</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C95" s="4">
+      <c r="C96" s="4">
         <v>30749</v>
       </c>
-      <c r="D95" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" ht="18.75">
-      <c r="A96" s="10" t="s">
+      <c r="D96" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="18.75">
+      <c r="A97" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B96" s="10"/>
-      <c r="C96" s="10"/>
-      <c r="D96" s="10"/>
-    </row>
-    <row r="97" spans="1:4">
-      <c r="A97" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C97" s="4">
-        <v>30998</v>
-      </c>
-      <c r="D97" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="B97" s="12"/>
+      <c r="C97" s="12"/>
+      <c r="D97" s="12"/>
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="4" t="s">
-        <v>20</v>
+        <v>41</v>
+      </c>
+      <c r="C98" s="4">
+        <v>30998</v>
       </c>
       <c r="D98" s="4">
         <f t="shared" si="1"/>
@@ -1752,10 +1787,7 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C99" s="4">
-        <v>33405</v>
+        <v>20</v>
       </c>
       <c r="D99" s="4">
         <f t="shared" si="1"/>
@@ -1764,42 +1796,45 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C100" s="4">
+        <v>33405</v>
+      </c>
+      <c r="D100" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C100" s="4">
+      <c r="C101" s="4">
         <v>33609</v>
       </c>
-      <c r="D100" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" ht="18.75">
-      <c r="A101" s="12" t="s">
+      <c r="D101" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="18.75">
+      <c r="A102" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B101" s="12"/>
-      <c r="C101" s="12"/>
-      <c r="D101" s="12"/>
-    </row>
-    <row r="102" spans="1:4">
-      <c r="A102" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C102" s="4">
-        <v>33858</v>
-      </c>
-      <c r="D102" s="4">
-        <f t="shared" ref="D102:D161" si="2">IF(B102 &gt;  0,C102-B102, 0)</f>
-        <v>0</v>
-      </c>
+      <c r="B102" s="11"/>
+      <c r="C102" s="11"/>
+      <c r="D102" s="11"/>
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="C103" s="4">
+        <v>33858</v>
       </c>
       <c r="D103" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="D103:D162" si="2">IF(B103 &gt;  0,C103-B103, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1825,9 +1860,6 @@
       <c r="A106" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C106" s="4">
-        <v>3</v>
-      </c>
       <c r="D106" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1835,7 +1867,10 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="C107" s="4">
+        <v>3</v>
       </c>
       <c r="D107" s="4">
         <f t="shared" si="2"/>
@@ -1844,7 +1879,7 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D108" s="4">
         <f t="shared" si="2"/>
@@ -1853,10 +1888,7 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C109" s="4">
-        <v>35512</v>
+        <v>47</v>
       </c>
       <c r="D109" s="4">
         <f t="shared" si="2"/>
@@ -1865,10 +1897,10 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="4" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="C110" s="4">
-        <v>35693</v>
+        <v>35512</v>
       </c>
       <c r="D110" s="4">
         <f t="shared" si="2"/>
@@ -1880,7 +1912,7 @@
         <v>6</v>
       </c>
       <c r="C111" s="4">
-        <v>35847</v>
+        <v>35693</v>
       </c>
       <c r="D111" s="4">
         <f t="shared" si="2"/>
@@ -1892,23 +1924,26 @@
         <v>6</v>
       </c>
       <c r="C112" s="4">
-        <v>36020</v>
+        <v>35847</v>
       </c>
       <c r="D112" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:5">
+    <row r="113" spans="1:4">
       <c r="A113" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="C113" s="4">
+        <v>36020</v>
+      </c>
       <c r="D113" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:5">
+    <row r="114" spans="1:4">
       <c r="A114" s="4" t="s">
         <v>6</v>
       </c>
@@ -1917,7 +1952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:5">
+    <row r="115" spans="1:4">
       <c r="A115" s="4" t="s">
         <v>6</v>
       </c>
@@ -1926,7 +1961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:5">
+    <row r="116" spans="1:4">
       <c r="A116" s="4" t="s">
         <v>6</v>
       </c>
@@ -1935,327 +1970,324 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:5">
+    <row r="117" spans="1:4">
       <c r="A117" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D117" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
+      <c r="A118" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C117" s="4">
+      <c r="C118" s="4">
         <v>38056</v>
       </c>
-      <c r="D117" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5">
-      <c r="A118" s="4" t="s">
+      <c r="D118" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
+      <c r="A119" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C118" s="4">
+      <c r="C119" s="4">
         <v>38245</v>
       </c>
-      <c r="D118" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5">
-      <c r="A119" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C119" s="4">
-        <v>38420</v>
-      </c>
       <c r="D119" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:5">
+    <row r="120" spans="1:4">
       <c r="A120" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C120" s="4">
+        <v>38420</v>
+      </c>
+      <c r="D120" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
+      <c r="A121" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C121" s="4">
         <v>38758</v>
       </c>
-      <c r="D120" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5">
-      <c r="A121" s="4" t="s">
+      <c r="D121" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
+      <c r="A122" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C121" s="4">
+      <c r="C122" s="4">
         <v>38859</v>
       </c>
-      <c r="D121" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5">
-      <c r="A122" s="4" t="s">
+      <c r="D122" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4">
+      <c r="A123" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C122" s="4">
+      <c r="C123" s="4">
         <v>39062</v>
       </c>
-      <c r="D122" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" ht="18.75">
-      <c r="A123" s="10" t="s">
+      <c r="D123" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" ht="18.75">
+      <c r="A124" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B123" s="10"/>
-      <c r="C123" s="10"/>
-      <c r="D123" s="10"/>
-    </row>
-    <row r="124" spans="1:5">
-      <c r="A124" s="4" t="s">
+      <c r="B124" s="12"/>
+      <c r="C124" s="12"/>
+      <c r="D124" s="12"/>
+    </row>
+    <row r="125" spans="1:4">
+      <c r="A125" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C124" s="4">
+      <c r="C125" s="4">
         <v>39312</v>
       </c>
-      <c r="D124" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5">
-      <c r="A125" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C125" s="4">
-        <v>40069</v>
-      </c>
       <c r="D125" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:5">
+    <row r="126" spans="1:4">
       <c r="A126" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C126" s="4">
-        <v>40681</v>
+        <v>40069</v>
       </c>
       <c r="D126" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:5">
+    <row r="127" spans="1:4">
       <c r="A127" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C127" s="4">
+        <v>40681</v>
+      </c>
+      <c r="D127" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
+      <c r="A128" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C128" s="4">
         <v>41240</v>
       </c>
-      <c r="D127" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5">
-      <c r="A128" s="4" t="s">
+      <c r="D128" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5">
+      <c r="A129" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C128" s="4">
+      <c r="C129" s="4">
         <v>41469</v>
       </c>
-      <c r="D128" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E128" t="s">
+      <c r="D129" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E129" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="129" spans="1:4">
-      <c r="A129" s="4" t="s">
+    <row r="130" spans="1:5">
+      <c r="A130" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C129" s="4">
+      <c r="C130" s="4">
         <v>41728</v>
       </c>
-      <c r="D129" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4">
-      <c r="A130" s="4" t="s">
+      <c r="D130" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5">
+      <c r="A131" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C130" s="4">
+      <c r="C131" s="4">
         <v>42015</v>
       </c>
-      <c r="D130" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4">
-      <c r="A131" s="4" t="s">
+      <c r="D131" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5">
+      <c r="A132" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C131" s="4">
+      <c r="C132" s="4">
         <v>42219</v>
       </c>
-      <c r="D131" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" ht="18.75">
-      <c r="A132" s="12" t="s">
+      <c r="D132" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" ht="18.75">
+      <c r="A133" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B132" s="12"/>
-      <c r="C132" s="12"/>
-      <c r="D132" s="12"/>
-    </row>
-    <row r="133" spans="1:4">
-      <c r="A133" s="4" t="s">
+      <c r="B133" s="11"/>
+      <c r="C133" s="11"/>
+      <c r="D133" s="11"/>
+    </row>
+    <row r="134" spans="1:5">
+      <c r="A134" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C133" s="4">
+      <c r="C134" s="4">
         <v>42469</v>
       </c>
-      <c r="D133" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4">
-      <c r="A134" s="4" t="s">
+      <c r="D134" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5">
+      <c r="A135" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C134" s="4">
+      <c r="C135" s="4">
         <v>43196</v>
       </c>
-      <c r="D134" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4">
-      <c r="A135" s="4" t="s">
+      <c r="D135" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5">
+      <c r="A136" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C135" s="4">
+      <c r="C136" s="4">
         <v>43848</v>
       </c>
-      <c r="D135" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4">
-      <c r="A136" s="4" t="s">
+      <c r="D136" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5">
+      <c r="A137" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C136" s="4">
+      <c r="C137" s="4">
         <v>44155</v>
       </c>
-      <c r="D136" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4">
-      <c r="A137" s="4" t="s">
+      <c r="D137" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5">
+      <c r="A138" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C137" s="4">
+      <c r="C138" s="4">
         <v>46549</v>
       </c>
-      <c r="D137" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4">
-      <c r="A138" s="4" t="s">
+      <c r="D138" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5">
+      <c r="A139" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C138" s="4">
+      <c r="C139" s="4">
         <v>46905</v>
       </c>
-      <c r="D138" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4">
-      <c r="A139" s="4" t="s">
+      <c r="D139" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5">
+      <c r="A140" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C139" s="4">
+      <c r="C140" s="4">
         <v>47108</v>
       </c>
-      <c r="D139" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" ht="18.75">
-      <c r="A140" s="10" t="s">
+      <c r="D140" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" ht="18.75">
+      <c r="A141" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B140" s="10"/>
-      <c r="C140" s="10"/>
-      <c r="D140" s="10"/>
-    </row>
-    <row r="141" spans="1:4">
-      <c r="A141" s="4" t="s">
+      <c r="B141" s="12"/>
+      <c r="C141" s="12"/>
+      <c r="D141" s="12"/>
+    </row>
+    <row r="142" spans="1:5">
+      <c r="A142" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C141" s="4">
+      <c r="C142" s="4">
         <v>47359</v>
       </c>
-      <c r="D141" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4">
-      <c r="A142" s="4" t="s">
+      <c r="D142" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5">
+      <c r="A143" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C142" s="4">
+      <c r="C143" s="4">
         <v>47668</v>
       </c>
-      <c r="D142" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4">
-      <c r="A143" s="4" t="s">
+      <c r="D143" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5">
+      <c r="A144" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C143" s="4">
+      <c r="C144" s="4">
         <v>47847</v>
-      </c>
-      <c r="D143" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4">
-      <c r="A144" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C144" s="4">
-        <v>48052</v>
       </c>
       <c r="D144" s="4">
         <f t="shared" si="2"/>
@@ -2264,10 +2296,10 @@
     </row>
     <row r="145" spans="1:5">
       <c r="A145" s="4" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C145" s="4">
-        <v>48226</v>
+        <v>48052</v>
       </c>
       <c r="D145" s="4">
         <f t="shared" si="2"/>
@@ -2276,10 +2308,10 @@
     </row>
     <row r="146" spans="1:5">
       <c r="A146" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C146" s="4">
-        <v>48530</v>
+        <v>48226</v>
       </c>
       <c r="D146" s="4">
         <f t="shared" si="2"/>
@@ -2288,37 +2320,37 @@
     </row>
     <row r="147" spans="1:5">
       <c r="A147" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C147" s="4">
-        <v>48705</v>
+        <v>48530</v>
       </c>
       <c r="D147" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
-      </c>
-      <c r="E147" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="148" spans="1:5">
       <c r="A148" s="4" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C148" s="4">
-        <v>48820</v>
+        <v>48705</v>
       </c>
       <c r="D148" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
+      </c>
+      <c r="E148" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="149" spans="1:5">
       <c r="A149" s="4" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="C149" s="4">
-        <v>49147</v>
+        <v>48820</v>
       </c>
       <c r="D149" s="4">
         <f t="shared" si="2"/>
@@ -2327,17 +2359,14 @@
     </row>
     <row r="150" spans="1:5">
       <c r="A150" s="4" t="s">
-        <v>6</v>
+        <v>57</v>
       </c>
       <c r="C150" s="4">
-        <v>49319</v>
+        <v>49147</v>
       </c>
       <c r="D150" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
-      </c>
-      <c r="E150" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="151" spans="1:5">
@@ -2345,19 +2374,22 @@
         <v>6</v>
       </c>
       <c r="C151" s="4">
-        <v>49569</v>
+        <v>49319</v>
       </c>
       <c r="D151" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
+      </c>
+      <c r="E151" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="152" spans="1:5">
       <c r="A152" s="4" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="C152" s="4">
-        <v>49860</v>
+        <v>49569</v>
       </c>
       <c r="D152" s="4">
         <f t="shared" si="2"/>
@@ -2366,42 +2398,42 @@
     </row>
     <row r="153" spans="1:5">
       <c r="A153" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C153" s="4">
+        <v>49860</v>
+      </c>
+      <c r="D153" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5">
+      <c r="A154" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C153" s="4">
+      <c r="C154" s="4">
         <v>50063</v>
       </c>
-      <c r="D153" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" ht="18.75">
-      <c r="A154" s="12" t="s">
+      <c r="D154" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" ht="18.75">
+      <c r="A155" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="B154" s="12"/>
-      <c r="C154" s="12"/>
-      <c r="D154" s="12"/>
-    </row>
-    <row r="155" spans="1:5">
-      <c r="A155" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C155" s="4">
-        <v>50314</v>
-      </c>
-      <c r="D155" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
+      <c r="B155" s="11"/>
+      <c r="C155" s="11"/>
+      <c r="D155" s="11"/>
     </row>
     <row r="156" spans="1:5">
       <c r="A156" s="4" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="C156" s="4">
-        <v>51237</v>
+        <v>50314</v>
       </c>
       <c r="D156" s="4">
         <f t="shared" si="2"/>
@@ -2410,10 +2442,10 @@
     </row>
     <row r="157" spans="1:5">
       <c r="A157" s="4" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="C157" s="4">
-        <v>53055</v>
+        <v>51237</v>
       </c>
       <c r="D157" s="4">
         <f t="shared" si="2"/>
@@ -2422,10 +2454,10 @@
     </row>
     <row r="158" spans="1:5">
       <c r="A158" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C158" s="4">
-        <v>53377</v>
+        <v>53055</v>
       </c>
       <c r="D158" s="4">
         <f t="shared" si="2"/>
@@ -2434,10 +2466,10 @@
     </row>
     <row r="159" spans="1:5">
       <c r="A159" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C159" s="4">
-        <v>53698</v>
+        <v>53377</v>
       </c>
       <c r="D159" s="4">
         <f t="shared" si="2"/>
@@ -2446,10 +2478,10 @@
     </row>
     <row r="160" spans="1:5">
       <c r="A160" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C160" s="4">
-        <v>54021</v>
+        <v>53698</v>
       </c>
       <c r="D160" s="4">
         <f t="shared" si="2"/>
@@ -2458,10 +2490,10 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C161" s="4">
-        <v>56284</v>
+        <v>54021</v>
       </c>
       <c r="D161" s="4">
         <f t="shared" si="2"/>
@@ -2470,33 +2502,45 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C162" s="4">
+        <v>56284</v>
+      </c>
+      <c r="D162" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4">
+      <c r="A163" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B162" s="9"/>
-      <c r="C162" s="9">
+      <c r="B163" s="9"/>
+      <c r="C163" s="9">
         <v>0.68541666666666667</v>
       </c>
-      <c r="D162" s="9">
+      <c r="D163" s="9">
         <v>2.7083333333333334E-2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A132:D132"/>
-    <mergeCell ref="A140:D140"/>
-    <mergeCell ref="A154:D154"/>
-    <mergeCell ref="A62:D62"/>
-    <mergeCell ref="A75:D75"/>
-    <mergeCell ref="A87:D87"/>
-    <mergeCell ref="A96:D96"/>
-    <mergeCell ref="A101:D101"/>
-    <mergeCell ref="A123:D123"/>
-    <mergeCell ref="A54:D54"/>
+    <mergeCell ref="A55:D55"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="A14:D14"/>
     <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A133:D133"/>
+    <mergeCell ref="A141:D141"/>
+    <mergeCell ref="A155:D155"/>
+    <mergeCell ref="A63:D63"/>
+    <mergeCell ref="A76:D76"/>
+    <mergeCell ref="A88:D88"/>
+    <mergeCell ref="A97:D97"/>
+    <mergeCell ref="A102:D102"/>
+    <mergeCell ref="A124:D124"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -2533,12 +2577,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -2566,12 +2610,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -2605,12 +2649,12 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
@@ -2733,12 +2777,12 @@
       </c>
     </row>
     <row r="19" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="4" t="s">
@@ -2906,12 +2950,12 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="18.75">
-      <c r="A31" s="12" t="s">
+      <c r="A31" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="4" t="s">
@@ -3079,12 +3123,12 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="18.75">
-      <c r="A43" s="10" t="s">
+      <c r="A43" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B43" s="10"/>
-      <c r="C43" s="10"/>
-      <c r="D43" s="10"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="4" t="s">
@@ -3192,12 +3236,12 @@
       </c>
     </row>
     <row r="51" spans="1:10" ht="18.75">
-      <c r="A51" s="12" t="s">
+      <c r="A51" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B51" s="12"/>
-      <c r="C51" s="12"/>
-      <c r="D51" s="12"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="4" t="s">
@@ -3383,12 +3427,12 @@
       </c>
     </row>
     <row r="64" spans="1:10" ht="18.75">
-      <c r="A64" s="10" t="s">
+      <c r="A64" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B64" s="10"/>
-      <c r="C64" s="10"/>
-      <c r="D64" s="10"/>
+      <c r="B64" s="12"/>
+      <c r="C64" s="12"/>
+      <c r="D64" s="12"/>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="4" t="s">
@@ -3547,12 +3591,12 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="18.75">
-      <c r="A76" s="12" t="s">
+      <c r="A76" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B76" s="12"/>
-      <c r="C76" s="12"/>
-      <c r="D76" s="12"/>
+      <c r="B76" s="11"/>
+      <c r="C76" s="11"/>
+      <c r="D76" s="11"/>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="4" t="s">
@@ -3665,12 +3709,12 @@
       </c>
     </row>
     <row r="85" spans="1:4" ht="18.75">
-      <c r="A85" s="10" t="s">
+      <c r="A85" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B85" s="10"/>
-      <c r="C85" s="10"/>
-      <c r="D85" s="10"/>
+      <c r="B85" s="12"/>
+      <c r="C85" s="12"/>
+      <c r="D85" s="12"/>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="4" t="s">
@@ -3730,12 +3774,12 @@
       </c>
     </row>
     <row r="90" spans="1:4" ht="18.75">
-      <c r="A90" s="12" t="s">
+      <c r="A90" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B90" s="12"/>
-      <c r="C90" s="12"/>
-      <c r="D90" s="12"/>
+      <c r="B90" s="11"/>
+      <c r="C90" s="11"/>
+      <c r="D90" s="11"/>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="4" t="s">
@@ -4026,12 +4070,12 @@
       </c>
     </row>
     <row r="112" spans="1:4" ht="18.75">
-      <c r="A112" s="10" t="s">
+      <c r="A112" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B112" s="10"/>
-      <c r="C112" s="10"/>
-      <c r="D112" s="10"/>
+      <c r="B112" s="12"/>
+      <c r="C112" s="12"/>
+      <c r="D112" s="12"/>
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="4" t="s">
@@ -4157,12 +4201,12 @@
       </c>
     </row>
     <row r="121" spans="1:5" ht="18.75">
-      <c r="A121" s="12" t="s">
+      <c r="A121" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B121" s="12"/>
-      <c r="C121" s="12"/>
-      <c r="D121" s="12"/>
+      <c r="B121" s="11"/>
+      <c r="C121" s="11"/>
+      <c r="D121" s="11"/>
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="4" t="s">
@@ -4270,12 +4314,12 @@
       </c>
     </row>
     <row r="129" spans="1:5" ht="18.75">
-      <c r="A129" s="10" t="s">
+      <c r="A129" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B129" s="10"/>
-      <c r="C129" s="10"/>
-      <c r="D129" s="10"/>
+      <c r="B129" s="12"/>
+      <c r="C129" s="12"/>
+      <c r="D129" s="12"/>
     </row>
     <row r="130" spans="1:5">
       <c r="A130" s="4" t="s">
@@ -4479,12 +4523,12 @@
       </c>
     </row>
     <row r="143" spans="1:5" ht="18.75">
-      <c r="A143" s="12" t="s">
+      <c r="A143" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="B143" s="12"/>
-      <c r="C143" s="12"/>
-      <c r="D143" s="12"/>
+      <c r="B143" s="11"/>
+      <c r="C143" s="11"/>
+      <c r="D143" s="11"/>
     </row>
     <row r="144" spans="1:5">
       <c r="A144" s="4" t="s">
@@ -4613,12 +4657,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A31:D31"/>
     <mergeCell ref="A121:D121"/>
     <mergeCell ref="A129:D129"/>
     <mergeCell ref="A143:D143"/>
@@ -4628,6 +4666,12 @@
     <mergeCell ref="A85:D85"/>
     <mergeCell ref="A90:D90"/>
     <mergeCell ref="A112:D112"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A31:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -4664,12 +4708,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -4697,12 +4741,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -4736,12 +4780,12 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
@@ -4825,12 +4869,12 @@
       </c>
     </row>
     <row r="17" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="4" t="s">
@@ -4998,12 +5042,12 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="18.75">
-      <c r="A29" s="12" t="s">
+      <c r="A29" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="4" t="s">
@@ -5081,12 +5125,12 @@
       </c>
     </row>
     <row r="35" spans="1:10" ht="18.75">
-      <c r="A35" s="10" t="s">
+      <c r="A35" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="4" t="s">
@@ -5179,12 +5223,12 @@
       </c>
     </row>
     <row r="42" spans="1:10" ht="18.75">
-      <c r="A42" s="12" t="s">
+      <c r="A42" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B42" s="12"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="4" t="s">
@@ -5373,12 +5417,12 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="18.75">
-      <c r="A55" s="10" t="s">
+      <c r="A55" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B55" s="10"/>
-      <c r="C55" s="10"/>
-      <c r="D55" s="10"/>
+      <c r="B55" s="12"/>
+      <c r="C55" s="12"/>
+      <c r="D55" s="12"/>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="4" t="s">
@@ -5531,12 +5575,12 @@
       </c>
     </row>
     <row r="66" spans="1:4" ht="18.75">
-      <c r="A66" s="12" t="s">
+      <c r="A66" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B66" s="12"/>
-      <c r="C66" s="12"/>
-      <c r="D66" s="12"/>
+      <c r="B66" s="11"/>
+      <c r="C66" s="11"/>
+      <c r="D66" s="11"/>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="4" t="s">
@@ -5599,12 +5643,12 @@
       </c>
     </row>
     <row r="71" spans="1:4" ht="18.75">
-      <c r="A71" s="10" t="s">
+      <c r="A71" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B71" s="10"/>
-      <c r="C71" s="10"/>
-      <c r="D71" s="10"/>
+      <c r="B71" s="12"/>
+      <c r="C71" s="12"/>
+      <c r="D71" s="12"/>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="4" t="s">
@@ -5667,12 +5711,12 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="18.75">
-      <c r="A76" s="12" t="s">
+      <c r="A76" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B76" s="12"/>
-      <c r="C76" s="12"/>
-      <c r="D76" s="12"/>
+      <c r="B76" s="11"/>
+      <c r="C76" s="11"/>
+      <c r="D76" s="11"/>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="4" t="s">
@@ -5990,12 +6034,12 @@
       </c>
     </row>
     <row r="98" spans="1:5" ht="18.75">
-      <c r="A98" s="10" t="s">
+      <c r="A98" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B98" s="10"/>
-      <c r="C98" s="10"/>
-      <c r="D98" s="10"/>
+      <c r="B98" s="12"/>
+      <c r="C98" s="12"/>
+      <c r="D98" s="12"/>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="4" t="s">
@@ -6121,12 +6165,12 @@
       </c>
     </row>
     <row r="107" spans="1:5" ht="18.75">
-      <c r="A107" s="12" t="s">
+      <c r="A107" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B107" s="12"/>
-      <c r="C107" s="12"/>
-      <c r="D107" s="12"/>
+      <c r="B107" s="11"/>
+      <c r="C107" s="11"/>
+      <c r="D107" s="11"/>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="4" t="s">
@@ -6204,12 +6248,12 @@
       </c>
     </row>
     <row r="113" spans="1:4" ht="18.75">
-      <c r="A113" s="10" t="s">
+      <c r="A113" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B113" s="10"/>
-      <c r="C113" s="10"/>
-      <c r="D113" s="10"/>
+      <c r="B113" s="12"/>
+      <c r="C113" s="12"/>
+      <c r="D113" s="12"/>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="4" t="s">
@@ -6407,12 +6451,12 @@
       </c>
     </row>
     <row r="127" spans="1:4" ht="18.75">
-      <c r="A127" s="12" t="s">
+      <c r="A127" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="B127" s="12"/>
-      <c r="C127" s="12"/>
-      <c r="D127" s="12"/>
+      <c r="B127" s="11"/>
+      <c r="C127" s="11"/>
+      <c r="D127" s="11"/>
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="4" t="s">
@@ -6532,6 +6576,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A29:D29"/>
     <mergeCell ref="A127:D127"/>
     <mergeCell ref="A107:D107"/>
     <mergeCell ref="A113:D113"/>
@@ -6542,11 +6591,6 @@
     <mergeCell ref="A98:D98"/>
     <mergeCell ref="A66:D66"/>
     <mergeCell ref="A55:D55"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A29:D29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>

</xml_diff>

<commit_message>
Wario - some of level 4, Level 3 & 4 savestates
</commit_message>
<xml_diff>
--- a/Wario/Wario.xlsx
+++ b/Wario/Wario.xlsx
@@ -658,8 +658,8 @@
   <dimension ref="A1:J163"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B45" sqref="B45"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1186,24 +1186,30 @@
       <c r="A46" s="4" t="s">
         <v>60</v>
       </c>
+      <c r="B46" s="4">
+        <v>12291</v>
+      </c>
       <c r="C46" s="4">
         <v>9633</v>
       </c>
       <c r="D46" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-2658</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="4" t="s">
         <v>26</v>
       </c>
+      <c r="B47" s="4">
+        <v>12592</v>
+      </c>
       <c r="C47" s="4">
         <v>9932</v>
       </c>
       <c r="D47" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-2660</v>
       </c>
     </row>
     <row r="48" spans="1:4">

</xml_diff>

<commit_message>
Level 4 done, Level 5 savestate.
</commit_message>
<xml_diff>
--- a/Wario/Wario.xlsx
+++ b/Wario/Wario.xlsx
@@ -658,8 +658,8 @@
   <dimension ref="A1:J163"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B48" sqref="B48"/>
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1276,12 +1276,15 @@
       <c r="A53" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="B53" s="4">
+        <v>17596</v>
+      </c>
       <c r="C53" s="4">
         <v>14936</v>
       </c>
       <c r="D53" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-2660</v>
       </c>
     </row>
     <row r="54" spans="1:4">

</xml_diff>

<commit_message>
Wario - Level 5 up to key
</commit_message>
<xml_diff>
--- a/Wario/Wario.xlsx
+++ b/Wario/Wario.xlsx
@@ -658,8 +658,8 @@
   <dimension ref="A1:J163"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B54" sqref="B54"/>
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1359,12 +1359,16 @@
       <c r="A60" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="B60" s="4">
+        <f>C60+2660</f>
+        <v>19599</v>
+      </c>
       <c r="C60" s="4">
         <v>16939</v>
       </c>
       <c r="D60" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-2660</v>
       </c>
     </row>
     <row r="61" spans="1:4">

</xml_diff>

<commit_message>
Wario 100% - first room of level 6 done
</commit_message>
<xml_diff>
--- a/Wario/Wario.xlsx
+++ b/Wario/Wario.xlsx
@@ -358,9 +358,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -658,8 +658,8 @@
   <dimension ref="A1:J163"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B61" sqref="B61"/>
+      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -683,12 +683,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -716,12 +716,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -791,12 +791,12 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="18.75">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="4" t="s">
@@ -967,12 +967,12 @@
       </c>
     </row>
     <row r="30" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A30" s="12" t="s">
+      <c r="A30" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="4" t="s">
@@ -1148,12 +1148,12 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="18.75">
-      <c r="A43" s="11" t="s">
+      <c r="A43" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B43" s="11"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="4" t="s">
@@ -1300,12 +1300,12 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="18.75">
-      <c r="A55" s="12" t="s">
+      <c r="A55" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B55" s="12"/>
-      <c r="C55" s="12"/>
-      <c r="D55" s="12"/>
+      <c r="B55" s="11"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="11"/>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="4" t="s">
@@ -1396,35 +1396,41 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="18.75">
-      <c r="A63" s="11" t="s">
+      <c r="A63" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B63" s="11"/>
-      <c r="C63" s="11"/>
-      <c r="D63" s="11"/>
+      <c r="B63" s="13"/>
+      <c r="C63" s="13"/>
+      <c r="D63" s="13"/>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="B64" s="4">
+        <v>21497</v>
+      </c>
       <c r="C64" s="4">
         <v>17558</v>
       </c>
       <c r="D64" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-3939</v>
       </c>
     </row>
     <row r="65" spans="1:10">
       <c r="A65" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="B65" s="4">
+        <v>22357</v>
+      </c>
       <c r="C65" s="4">
         <v>18431</v>
       </c>
       <c r="D65" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-3926</v>
       </c>
     </row>
     <row r="66" spans="1:10">
@@ -1551,12 +1557,12 @@
       </c>
     </row>
     <row r="76" spans="1:10" ht="18.75">
-      <c r="A76" s="12" t="s">
+      <c r="A76" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B76" s="12"/>
-      <c r="C76" s="12"/>
-      <c r="D76" s="12"/>
+      <c r="B76" s="11"/>
+      <c r="C76" s="11"/>
+      <c r="D76" s="11"/>
     </row>
     <row r="77" spans="1:10">
       <c r="A77" s="4" t="s">
@@ -1682,12 +1688,12 @@
       </c>
     </row>
     <row r="88" spans="1:4" ht="18.75">
-      <c r="A88" s="11" t="s">
+      <c r="A88" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B88" s="11"/>
-      <c r="C88" s="11"/>
-      <c r="D88" s="11"/>
+      <c r="B88" s="13"/>
+      <c r="C88" s="13"/>
+      <c r="D88" s="13"/>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="4" t="s">
@@ -1779,12 +1785,12 @@
       </c>
     </row>
     <row r="97" spans="1:4" ht="18.75">
-      <c r="A97" s="12" t="s">
+      <c r="A97" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B97" s="12"/>
-      <c r="C97" s="12"/>
-      <c r="D97" s="12"/>
+      <c r="B97" s="11"/>
+      <c r="C97" s="11"/>
+      <c r="D97" s="11"/>
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="4" t="s">
@@ -1832,12 +1838,12 @@
       </c>
     </row>
     <row r="102" spans="1:4" ht="18.75">
-      <c r="A102" s="11" t="s">
+      <c r="A102" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B102" s="11"/>
-      <c r="C102" s="11"/>
-      <c r="D102" s="11"/>
+      <c r="B102" s="13"/>
+      <c r="C102" s="13"/>
+      <c r="D102" s="13"/>
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="4" t="s">
@@ -2065,12 +2071,12 @@
       </c>
     </row>
     <row r="124" spans="1:4" ht="18.75">
-      <c r="A124" s="12" t="s">
+      <c r="A124" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B124" s="12"/>
-      <c r="C124" s="12"/>
-      <c r="D124" s="12"/>
+      <c r="B124" s="11"/>
+      <c r="C124" s="11"/>
+      <c r="D124" s="11"/>
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="4" t="s">
@@ -2172,12 +2178,12 @@
       </c>
     </row>
     <row r="133" spans="1:5" ht="18.75">
-      <c r="A133" s="11" t="s">
+      <c r="A133" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="B133" s="11"/>
-      <c r="C133" s="11"/>
-      <c r="D133" s="11"/>
+      <c r="B133" s="13"/>
+      <c r="C133" s="13"/>
+      <c r="D133" s="13"/>
     </row>
     <row r="134" spans="1:5">
       <c r="A134" s="4" t="s">
@@ -2264,12 +2270,12 @@
       </c>
     </row>
     <row r="141" spans="1:5" ht="18.75">
-      <c r="A141" s="12" t="s">
+      <c r="A141" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B141" s="12"/>
-      <c r="C141" s="12"/>
-      <c r="D141" s="12"/>
+      <c r="B141" s="11"/>
+      <c r="C141" s="11"/>
+      <c r="D141" s="11"/>
     </row>
     <row r="142" spans="1:5">
       <c r="A142" s="4" t="s">
@@ -2434,12 +2440,12 @@
       </c>
     </row>
     <row r="155" spans="1:5" ht="18.75">
-      <c r="A155" s="11" t="s">
+      <c r="A155" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="B155" s="11"/>
-      <c r="C155" s="11"/>
-      <c r="D155" s="11"/>
+      <c r="B155" s="13"/>
+      <c r="C155" s="13"/>
+      <c r="D155" s="13"/>
     </row>
     <row r="156" spans="1:5">
       <c r="A156" s="4" t="s">
@@ -2539,12 +2545,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A55:D55"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A43:D43"/>
     <mergeCell ref="A133:D133"/>
     <mergeCell ref="A141:D141"/>
     <mergeCell ref="A155:D155"/>
@@ -2554,6 +2554,12 @@
     <mergeCell ref="A97:D97"/>
     <mergeCell ref="A102:D102"/>
     <mergeCell ref="A124:D124"/>
+    <mergeCell ref="A55:D55"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A43:D43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -2590,12 +2596,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -2623,12 +2629,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -2662,12 +2668,12 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
@@ -2790,12 +2796,12 @@
       </c>
     </row>
     <row r="19" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="4" t="s">
@@ -2963,12 +2969,12 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="18.75">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="4" t="s">
@@ -3136,12 +3142,12 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="18.75">
-      <c r="A43" s="12" t="s">
+      <c r="A43" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B43" s="12"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="4" t="s">
@@ -3249,12 +3255,12 @@
       </c>
     </row>
     <row r="51" spans="1:10" ht="18.75">
-      <c r="A51" s="11" t="s">
+      <c r="A51" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B51" s="11"/>
-      <c r="C51" s="11"/>
-      <c r="D51" s="11"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="13"/>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="4" t="s">
@@ -3440,12 +3446,12 @@
       </c>
     </row>
     <row r="64" spans="1:10" ht="18.75">
-      <c r="A64" s="12" t="s">
+      <c r="A64" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B64" s="12"/>
-      <c r="C64" s="12"/>
-      <c r="D64" s="12"/>
+      <c r="B64" s="11"/>
+      <c r="C64" s="11"/>
+      <c r="D64" s="11"/>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="4" t="s">
@@ -3604,12 +3610,12 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="18.75">
-      <c r="A76" s="11" t="s">
+      <c r="A76" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B76" s="11"/>
-      <c r="C76" s="11"/>
-      <c r="D76" s="11"/>
+      <c r="B76" s="13"/>
+      <c r="C76" s="13"/>
+      <c r="D76" s="13"/>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="4" t="s">
@@ -3722,12 +3728,12 @@
       </c>
     </row>
     <row r="85" spans="1:4" ht="18.75">
-      <c r="A85" s="12" t="s">
+      <c r="A85" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B85" s="12"/>
-      <c r="C85" s="12"/>
-      <c r="D85" s="12"/>
+      <c r="B85" s="11"/>
+      <c r="C85" s="11"/>
+      <c r="D85" s="11"/>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="4" t="s">
@@ -3787,12 +3793,12 @@
       </c>
     </row>
     <row r="90" spans="1:4" ht="18.75">
-      <c r="A90" s="11" t="s">
+      <c r="A90" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B90" s="11"/>
-      <c r="C90" s="11"/>
-      <c r="D90" s="11"/>
+      <c r="B90" s="13"/>
+      <c r="C90" s="13"/>
+      <c r="D90" s="13"/>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="4" t="s">
@@ -4083,12 +4089,12 @@
       </c>
     </row>
     <row r="112" spans="1:4" ht="18.75">
-      <c r="A112" s="12" t="s">
+      <c r="A112" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B112" s="12"/>
-      <c r="C112" s="12"/>
-      <c r="D112" s="12"/>
+      <c r="B112" s="11"/>
+      <c r="C112" s="11"/>
+      <c r="D112" s="11"/>
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="4" t="s">
@@ -4214,12 +4220,12 @@
       </c>
     </row>
     <row r="121" spans="1:5" ht="18.75">
-      <c r="A121" s="11" t="s">
+      <c r="A121" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="B121" s="11"/>
-      <c r="C121" s="11"/>
-      <c r="D121" s="11"/>
+      <c r="B121" s="13"/>
+      <c r="C121" s="13"/>
+      <c r="D121" s="13"/>
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="4" t="s">
@@ -4327,12 +4333,12 @@
       </c>
     </row>
     <row r="129" spans="1:5" ht="18.75">
-      <c r="A129" s="12" t="s">
+      <c r="A129" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B129" s="12"/>
-      <c r="C129" s="12"/>
-      <c r="D129" s="12"/>
+      <c r="B129" s="11"/>
+      <c r="C129" s="11"/>
+      <c r="D129" s="11"/>
     </row>
     <row r="130" spans="1:5">
       <c r="A130" s="4" t="s">
@@ -4536,12 +4542,12 @@
       </c>
     </row>
     <row r="143" spans="1:5" ht="18.75">
-      <c r="A143" s="11" t="s">
+      <c r="A143" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="B143" s="11"/>
-      <c r="C143" s="11"/>
-      <c r="D143" s="11"/>
+      <c r="B143" s="13"/>
+      <c r="C143" s="13"/>
+      <c r="D143" s="13"/>
     </row>
     <row r="144" spans="1:5">
       <c r="A144" s="4" t="s">
@@ -4670,6 +4676,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A31:D31"/>
     <mergeCell ref="A121:D121"/>
     <mergeCell ref="A129:D129"/>
     <mergeCell ref="A143:D143"/>
@@ -4679,12 +4691,6 @@
     <mergeCell ref="A85:D85"/>
     <mergeCell ref="A90:D90"/>
     <mergeCell ref="A112:D112"/>
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A31:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -4721,12 +4727,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -4754,12 +4760,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -4793,12 +4799,12 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
@@ -4882,12 +4888,12 @@
       </c>
     </row>
     <row r="17" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="4" t="s">
@@ -5055,12 +5061,12 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="18.75">
-      <c r="A29" s="11" t="s">
+      <c r="A29" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="4" t="s">
@@ -5138,12 +5144,12 @@
       </c>
     </row>
     <row r="35" spans="1:10" ht="18.75">
-      <c r="A35" s="12" t="s">
+      <c r="A35" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="12"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="4" t="s">
@@ -5236,12 +5242,12 @@
       </c>
     </row>
     <row r="42" spans="1:10" ht="18.75">
-      <c r="A42" s="11" t="s">
+      <c r="A42" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B42" s="11"/>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="4" t="s">
@@ -5430,12 +5436,12 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="18.75">
-      <c r="A55" s="12" t="s">
+      <c r="A55" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B55" s="12"/>
-      <c r="C55" s="12"/>
-      <c r="D55" s="12"/>
+      <c r="B55" s="11"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="11"/>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="4" t="s">
@@ -5588,12 +5594,12 @@
       </c>
     </row>
     <row r="66" spans="1:4" ht="18.75">
-      <c r="A66" s="11" t="s">
+      <c r="A66" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B66" s="11"/>
-      <c r="C66" s="11"/>
-      <c r="D66" s="11"/>
+      <c r="B66" s="13"/>
+      <c r="C66" s="13"/>
+      <c r="D66" s="13"/>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="4" t="s">
@@ -5656,12 +5662,12 @@
       </c>
     </row>
     <row r="71" spans="1:4" ht="18.75">
-      <c r="A71" s="12" t="s">
+      <c r="A71" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B71" s="12"/>
-      <c r="C71" s="12"/>
-      <c r="D71" s="12"/>
+      <c r="B71" s="11"/>
+      <c r="C71" s="11"/>
+      <c r="D71" s="11"/>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="4" t="s">
@@ -5724,12 +5730,12 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="18.75">
-      <c r="A76" s="11" t="s">
+      <c r="A76" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B76" s="11"/>
-      <c r="C76" s="11"/>
-      <c r="D76" s="11"/>
+      <c r="B76" s="13"/>
+      <c r="C76" s="13"/>
+      <c r="D76" s="13"/>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="4" t="s">
@@ -6047,12 +6053,12 @@
       </c>
     </row>
     <row r="98" spans="1:5" ht="18.75">
-      <c r="A98" s="12" t="s">
+      <c r="A98" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B98" s="12"/>
-      <c r="C98" s="12"/>
-      <c r="D98" s="12"/>
+      <c r="B98" s="11"/>
+      <c r="C98" s="11"/>
+      <c r="D98" s="11"/>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="4" t="s">
@@ -6178,12 +6184,12 @@
       </c>
     </row>
     <row r="107" spans="1:5" ht="18.75">
-      <c r="A107" s="11" t="s">
+      <c r="A107" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="B107" s="11"/>
-      <c r="C107" s="11"/>
-      <c r="D107" s="11"/>
+      <c r="B107" s="13"/>
+      <c r="C107" s="13"/>
+      <c r="D107" s="13"/>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="4" t="s">
@@ -6261,12 +6267,12 @@
       </c>
     </row>
     <row r="113" spans="1:4" ht="18.75">
-      <c r="A113" s="12" t="s">
+      <c r="A113" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B113" s="12"/>
-      <c r="C113" s="12"/>
-      <c r="D113" s="12"/>
+      <c r="B113" s="11"/>
+      <c r="C113" s="11"/>
+      <c r="D113" s="11"/>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="4" t="s">
@@ -6464,12 +6470,12 @@
       </c>
     </row>
     <row r="127" spans="1:4" ht="18.75">
-      <c r="A127" s="11" t="s">
+      <c r="A127" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="B127" s="11"/>
-      <c r="C127" s="11"/>
-      <c r="D127" s="11"/>
+      <c r="B127" s="13"/>
+      <c r="C127" s="13"/>
+      <c r="D127" s="13"/>
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="4" t="s">
@@ -6589,11 +6595,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A29:D29"/>
     <mergeCell ref="A127:D127"/>
     <mergeCell ref="A107:D107"/>
     <mergeCell ref="A113:D113"/>
@@ -6604,6 +6605,11 @@
     <mergeCell ref="A98:D98"/>
     <mergeCell ref="A66:D66"/>
     <mergeCell ref="A55:D55"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A29:D29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>

</xml_diff>

<commit_message>
wario 100% - more level 6 done (activate plunger, go down pipe on way to key)
</commit_message>
<xml_diff>
--- a/Wario/Wario.xlsx
+++ b/Wario/Wario.xlsx
@@ -658,8 +658,8 @@
   <dimension ref="A1:J163"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B66" sqref="B66"/>
+      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1437,24 +1437,30 @@
       <c r="A66" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="B66" s="4">
+        <v>22749</v>
+      </c>
       <c r="C66" s="4">
         <v>18823</v>
       </c>
       <c r="D66" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-3926</v>
       </c>
     </row>
     <row r="67" spans="1:10">
       <c r="A67" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="B67" s="4">
+        <v>23004</v>
+      </c>
       <c r="C67" s="4">
         <v>19078</v>
       </c>
       <c r="D67" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-3926</v>
       </c>
       <c r="F67" s="6"/>
       <c r="H67" s="6"/>
@@ -1464,9 +1470,15 @@
       <c r="A68" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="B68" s="4">
+        <v>23146</v>
+      </c>
+      <c r="C68" s="4">
+        <v>19220</v>
+      </c>
       <c r="D68" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-3926</v>
       </c>
       <c r="F68" s="7"/>
       <c r="H68" s="7"/>
@@ -1476,24 +1488,30 @@
       <c r="A69" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="B69" s="4">
+        <v>23352</v>
+      </c>
       <c r="C69" s="4">
         <v>19425</v>
       </c>
       <c r="D69" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-3927</v>
       </c>
     </row>
     <row r="70" spans="1:10">
       <c r="A70" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="B70" s="4">
+        <v>23620</v>
+      </c>
       <c r="C70" s="4">
         <v>19693</v>
       </c>
       <c r="D70" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-3927</v>
       </c>
     </row>
     <row r="71" spans="1:10">

</xml_diff>

<commit_message>
Wario - Level 6 almost done
</commit_message>
<xml_diff>
--- a/Wario/Wario.xlsx
+++ b/Wario/Wario.xlsx
@@ -358,9 +358,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -657,9 +657,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J163"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B71" sqref="B71"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I66" sqref="I66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -683,12 +683,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -716,12 +716,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -791,12 +791,12 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="18.75">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="4" t="s">
@@ -967,12 +967,12 @@
       </c>
     </row>
     <row r="30" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A30" s="11" t="s">
+      <c r="A30" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="4" t="s">
@@ -1148,12 +1148,12 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="18.75">
-      <c r="A43" s="13" t="s">
+      <c r="A43" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B43" s="13"/>
-      <c r="C43" s="13"/>
-      <c r="D43" s="13"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="4" t="s">
@@ -1300,12 +1300,12 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="18.75">
-      <c r="A55" s="11" t="s">
+      <c r="A55" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B55" s="11"/>
-      <c r="C55" s="11"/>
-      <c r="D55" s="11"/>
+      <c r="B55" s="12"/>
+      <c r="C55" s="12"/>
+      <c r="D55" s="12"/>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="4" t="s">
@@ -1396,12 +1396,12 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="18.75">
-      <c r="A63" s="13" t="s">
+      <c r="A63" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B63" s="13"/>
-      <c r="C63" s="13"/>
-      <c r="D63" s="13"/>
+      <c r="B63" s="11"/>
+      <c r="C63" s="11"/>
+      <c r="D63" s="11"/>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="4" t="s">
@@ -1438,29 +1438,26 @@
         <v>7</v>
       </c>
       <c r="B66" s="4">
-        <v>22749</v>
+        <v>23752</v>
       </c>
       <c r="C66" s="4">
         <v>18823</v>
       </c>
       <c r="D66" s="4">
         <f t="shared" si="1"/>
-        <v>-3926</v>
+        <v>-4929</v>
       </c>
     </row>
     <row r="67" spans="1:10">
       <c r="A67" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B67" s="4">
-        <v>23004</v>
-      </c>
       <c r="C67" s="4">
         <v>19078</v>
       </c>
       <c r="D67" s="4">
         <f t="shared" si="1"/>
-        <v>-3926</v>
+        <v>0</v>
       </c>
       <c r="F67" s="6"/>
       <c r="H67" s="6"/>
@@ -1471,14 +1468,14 @@
         <v>20</v>
       </c>
       <c r="B68" s="4">
-        <v>23146</v>
+        <v>24413</v>
       </c>
       <c r="C68" s="4">
-        <v>19220</v>
+        <v>19485</v>
       </c>
       <c r="D68" s="4">
         <f t="shared" si="1"/>
-        <v>-3926</v>
+        <v>-4928</v>
       </c>
       <c r="F68" s="7"/>
       <c r="H68" s="7"/>
@@ -1489,14 +1486,14 @@
         <v>33</v>
       </c>
       <c r="B69" s="4">
-        <v>23352</v>
+        <v>24353</v>
       </c>
       <c r="C69" s="4">
         <v>19425</v>
       </c>
       <c r="D69" s="4">
         <f t="shared" si="1"/>
-        <v>-3927</v>
+        <v>-4928</v>
       </c>
     </row>
     <row r="70" spans="1:10">
@@ -1504,26 +1501,29 @@
         <v>7</v>
       </c>
       <c r="B70" s="4">
-        <v>23620</v>
+        <v>24625</v>
       </c>
       <c r="C70" s="4">
         <v>19693</v>
       </c>
       <c r="D70" s="4">
         <f t="shared" si="1"/>
-        <v>-3927</v>
+        <v>-4932</v>
       </c>
     </row>
     <row r="71" spans="1:10">
       <c r="A71" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="B71" s="4">
+        <v>25964</v>
+      </c>
       <c r="C71" s="4">
         <v>20164</v>
       </c>
       <c r="D71" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-5800</v>
       </c>
     </row>
     <row r="72" spans="1:10">
@@ -1575,12 +1575,12 @@
       </c>
     </row>
     <row r="76" spans="1:10" ht="18.75">
-      <c r="A76" s="11" t="s">
+      <c r="A76" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B76" s="11"/>
-      <c r="C76" s="11"/>
-      <c r="D76" s="11"/>
+      <c r="B76" s="12"/>
+      <c r="C76" s="12"/>
+      <c r="D76" s="12"/>
     </row>
     <row r="77" spans="1:10">
       <c r="A77" s="4" t="s">
@@ -1706,12 +1706,12 @@
       </c>
     </row>
     <row r="88" spans="1:4" ht="18.75">
-      <c r="A88" s="13" t="s">
+      <c r="A88" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B88" s="13"/>
-      <c r="C88" s="13"/>
-      <c r="D88" s="13"/>
+      <c r="B88" s="11"/>
+      <c r="C88" s="11"/>
+      <c r="D88" s="11"/>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="4" t="s">
@@ -1803,12 +1803,12 @@
       </c>
     </row>
     <row r="97" spans="1:4" ht="18.75">
-      <c r="A97" s="11" t="s">
+      <c r="A97" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B97" s="11"/>
-      <c r="C97" s="11"/>
-      <c r="D97" s="11"/>
+      <c r="B97" s="12"/>
+      <c r="C97" s="12"/>
+      <c r="D97" s="12"/>
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="4" t="s">
@@ -1856,12 +1856,12 @@
       </c>
     </row>
     <row r="102" spans="1:4" ht="18.75">
-      <c r="A102" s="13" t="s">
+      <c r="A102" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B102" s="13"/>
-      <c r="C102" s="13"/>
-      <c r="D102" s="13"/>
+      <c r="B102" s="11"/>
+      <c r="C102" s="11"/>
+      <c r="D102" s="11"/>
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="4" t="s">
@@ -2089,12 +2089,12 @@
       </c>
     </row>
     <row r="124" spans="1:4" ht="18.75">
-      <c r="A124" s="11" t="s">
+      <c r="A124" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B124" s="11"/>
-      <c r="C124" s="11"/>
-      <c r="D124" s="11"/>
+      <c r="B124" s="12"/>
+      <c r="C124" s="12"/>
+      <c r="D124" s="12"/>
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="4" t="s">
@@ -2196,12 +2196,12 @@
       </c>
     </row>
     <row r="133" spans="1:5" ht="18.75">
-      <c r="A133" s="13" t="s">
+      <c r="A133" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B133" s="13"/>
-      <c r="C133" s="13"/>
-      <c r="D133" s="13"/>
+      <c r="B133" s="11"/>
+      <c r="C133" s="11"/>
+      <c r="D133" s="11"/>
     </row>
     <row r="134" spans="1:5">
       <c r="A134" s="4" t="s">
@@ -2288,12 +2288,12 @@
       </c>
     </row>
     <row r="141" spans="1:5" ht="18.75">
-      <c r="A141" s="11" t="s">
+      <c r="A141" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B141" s="11"/>
-      <c r="C141" s="11"/>
-      <c r="D141" s="11"/>
+      <c r="B141" s="12"/>
+      <c r="C141" s="12"/>
+      <c r="D141" s="12"/>
     </row>
     <row r="142" spans="1:5">
       <c r="A142" s="4" t="s">
@@ -2458,12 +2458,12 @@
       </c>
     </row>
     <row r="155" spans="1:5" ht="18.75">
-      <c r="A155" s="13" t="s">
+      <c r="A155" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="B155" s="13"/>
-      <c r="C155" s="13"/>
-      <c r="D155" s="13"/>
+      <c r="B155" s="11"/>
+      <c r="C155" s="11"/>
+      <c r="D155" s="11"/>
     </row>
     <row r="156" spans="1:5">
       <c r="A156" s="4" t="s">
@@ -2563,6 +2563,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A55:D55"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A43:D43"/>
     <mergeCell ref="A133:D133"/>
     <mergeCell ref="A141:D141"/>
     <mergeCell ref="A155:D155"/>
@@ -2572,12 +2578,6 @@
     <mergeCell ref="A97:D97"/>
     <mergeCell ref="A102:D102"/>
     <mergeCell ref="A124:D124"/>
-    <mergeCell ref="A55:D55"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A43:D43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -2614,12 +2614,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -2647,12 +2647,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -2686,12 +2686,12 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
@@ -2814,12 +2814,12 @@
       </c>
     </row>
     <row r="19" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="4" t="s">
@@ -2987,12 +2987,12 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="18.75">
-      <c r="A31" s="13" t="s">
+      <c r="A31" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="4" t="s">
@@ -3160,12 +3160,12 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="18.75">
-      <c r="A43" s="11" t="s">
+      <c r="A43" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B43" s="11"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="4" t="s">
@@ -3273,12 +3273,12 @@
       </c>
     </row>
     <row r="51" spans="1:10" ht="18.75">
-      <c r="A51" s="13" t="s">
+      <c r="A51" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B51" s="13"/>
-      <c r="C51" s="13"/>
-      <c r="D51" s="13"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="4" t="s">
@@ -3464,12 +3464,12 @@
       </c>
     </row>
     <row r="64" spans="1:10" ht="18.75">
-      <c r="A64" s="11" t="s">
+      <c r="A64" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B64" s="11"/>
-      <c r="C64" s="11"/>
-      <c r="D64" s="11"/>
+      <c r="B64" s="12"/>
+      <c r="C64" s="12"/>
+      <c r="D64" s="12"/>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="4" t="s">
@@ -3628,12 +3628,12 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="18.75">
-      <c r="A76" s="13" t="s">
+      <c r="A76" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B76" s="13"/>
-      <c r="C76" s="13"/>
-      <c r="D76" s="13"/>
+      <c r="B76" s="11"/>
+      <c r="C76" s="11"/>
+      <c r="D76" s="11"/>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="4" t="s">
@@ -3746,12 +3746,12 @@
       </c>
     </row>
     <row r="85" spans="1:4" ht="18.75">
-      <c r="A85" s="11" t="s">
+      <c r="A85" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B85" s="11"/>
-      <c r="C85" s="11"/>
-      <c r="D85" s="11"/>
+      <c r="B85" s="12"/>
+      <c r="C85" s="12"/>
+      <c r="D85" s="12"/>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="4" t="s">
@@ -3811,12 +3811,12 @@
       </c>
     </row>
     <row r="90" spans="1:4" ht="18.75">
-      <c r="A90" s="13" t="s">
+      <c r="A90" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B90" s="13"/>
-      <c r="C90" s="13"/>
-      <c r="D90" s="13"/>
+      <c r="B90" s="11"/>
+      <c r="C90" s="11"/>
+      <c r="D90" s="11"/>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="4" t="s">
@@ -4107,12 +4107,12 @@
       </c>
     </row>
     <row r="112" spans="1:4" ht="18.75">
-      <c r="A112" s="11" t="s">
+      <c r="A112" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B112" s="11"/>
-      <c r="C112" s="11"/>
-      <c r="D112" s="11"/>
+      <c r="B112" s="12"/>
+      <c r="C112" s="12"/>
+      <c r="D112" s="12"/>
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="4" t="s">
@@ -4238,12 +4238,12 @@
       </c>
     </row>
     <row r="121" spans="1:5" ht="18.75">
-      <c r="A121" s="13" t="s">
+      <c r="A121" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B121" s="13"/>
-      <c r="C121" s="13"/>
-      <c r="D121" s="13"/>
+      <c r="B121" s="11"/>
+      <c r="C121" s="11"/>
+      <c r="D121" s="11"/>
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="4" t="s">
@@ -4351,12 +4351,12 @@
       </c>
     </row>
     <row r="129" spans="1:5" ht="18.75">
-      <c r="A129" s="11" t="s">
+      <c r="A129" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B129" s="11"/>
-      <c r="C129" s="11"/>
-      <c r="D129" s="11"/>
+      <c r="B129" s="12"/>
+      <c r="C129" s="12"/>
+      <c r="D129" s="12"/>
     </row>
     <row r="130" spans="1:5">
       <c r="A130" s="4" t="s">
@@ -4560,12 +4560,12 @@
       </c>
     </row>
     <row r="143" spans="1:5" ht="18.75">
-      <c r="A143" s="13" t="s">
+      <c r="A143" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="B143" s="13"/>
-      <c r="C143" s="13"/>
-      <c r="D143" s="13"/>
+      <c r="B143" s="11"/>
+      <c r="C143" s="11"/>
+      <c r="D143" s="11"/>
     </row>
     <row r="144" spans="1:5">
       <c r="A144" s="4" t="s">
@@ -4694,12 +4694,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A31:D31"/>
     <mergeCell ref="A121:D121"/>
     <mergeCell ref="A129:D129"/>
     <mergeCell ref="A143:D143"/>
@@ -4709,6 +4703,12 @@
     <mergeCell ref="A85:D85"/>
     <mergeCell ref="A90:D90"/>
     <mergeCell ref="A112:D112"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A31:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -4745,12 +4745,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -4778,12 +4778,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -4817,12 +4817,12 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
@@ -4906,12 +4906,12 @@
       </c>
     </row>
     <row r="17" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="4" t="s">
@@ -5079,12 +5079,12 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="18.75">
-      <c r="A29" s="13" t="s">
+      <c r="A29" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="4" t="s">
@@ -5162,12 +5162,12 @@
       </c>
     </row>
     <row r="35" spans="1:10" ht="18.75">
-      <c r="A35" s="11" t="s">
+      <c r="A35" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="4" t="s">
@@ -5260,12 +5260,12 @@
       </c>
     </row>
     <row r="42" spans="1:10" ht="18.75">
-      <c r="A42" s="13" t="s">
+      <c r="A42" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B42" s="13"/>
-      <c r="C42" s="13"/>
-      <c r="D42" s="13"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="4" t="s">
@@ -5454,12 +5454,12 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="18.75">
-      <c r="A55" s="11" t="s">
+      <c r="A55" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B55" s="11"/>
-      <c r="C55" s="11"/>
-      <c r="D55" s="11"/>
+      <c r="B55" s="12"/>
+      <c r="C55" s="12"/>
+      <c r="D55" s="12"/>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="4" t="s">
@@ -5612,12 +5612,12 @@
       </c>
     </row>
     <row r="66" spans="1:4" ht="18.75">
-      <c r="A66" s="13" t="s">
+      <c r="A66" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B66" s="13"/>
-      <c r="C66" s="13"/>
-      <c r="D66" s="13"/>
+      <c r="B66" s="11"/>
+      <c r="C66" s="11"/>
+      <c r="D66" s="11"/>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="4" t="s">
@@ -5680,12 +5680,12 @@
       </c>
     </row>
     <row r="71" spans="1:4" ht="18.75">
-      <c r="A71" s="11" t="s">
+      <c r="A71" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B71" s="11"/>
-      <c r="C71" s="11"/>
-      <c r="D71" s="11"/>
+      <c r="B71" s="12"/>
+      <c r="C71" s="12"/>
+      <c r="D71" s="12"/>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="4" t="s">
@@ -5748,12 +5748,12 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="18.75">
-      <c r="A76" s="13" t="s">
+      <c r="A76" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B76" s="13"/>
-      <c r="C76" s="13"/>
-      <c r="D76" s="13"/>
+      <c r="B76" s="11"/>
+      <c r="C76" s="11"/>
+      <c r="D76" s="11"/>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="4" t="s">
@@ -6071,12 +6071,12 @@
       </c>
     </row>
     <row r="98" spans="1:5" ht="18.75">
-      <c r="A98" s="11" t="s">
+      <c r="A98" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B98" s="11"/>
-      <c r="C98" s="11"/>
-      <c r="D98" s="11"/>
+      <c r="B98" s="12"/>
+      <c r="C98" s="12"/>
+      <c r="D98" s="12"/>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="4" t="s">
@@ -6202,12 +6202,12 @@
       </c>
     </row>
     <row r="107" spans="1:5" ht="18.75">
-      <c r="A107" s="13" t="s">
+      <c r="A107" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B107" s="13"/>
-      <c r="C107" s="13"/>
-      <c r="D107" s="13"/>
+      <c r="B107" s="11"/>
+      <c r="C107" s="11"/>
+      <c r="D107" s="11"/>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="4" t="s">
@@ -6285,12 +6285,12 @@
       </c>
     </row>
     <row r="113" spans="1:4" ht="18.75">
-      <c r="A113" s="11" t="s">
+      <c r="A113" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B113" s="11"/>
-      <c r="C113" s="11"/>
-      <c r="D113" s="11"/>
+      <c r="B113" s="12"/>
+      <c r="C113" s="12"/>
+      <c r="D113" s="12"/>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="4" t="s">
@@ -6488,12 +6488,12 @@
       </c>
     </row>
     <row r="127" spans="1:4" ht="18.75">
-      <c r="A127" s="13" t="s">
+      <c r="A127" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="B127" s="13"/>
-      <c r="C127" s="13"/>
-      <c r="D127" s="13"/>
+      <c r="B127" s="11"/>
+      <c r="C127" s="11"/>
+      <c r="D127" s="11"/>
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="4" t="s">
@@ -6613,6 +6613,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A29:D29"/>
     <mergeCell ref="A127:D127"/>
     <mergeCell ref="A107:D107"/>
     <mergeCell ref="A113:D113"/>
@@ -6623,11 +6628,6 @@
     <mergeCell ref="A98:D98"/>
     <mergeCell ref="A66:D66"/>
     <mergeCell ref="A55:D55"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A29:D29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>

</xml_diff>

<commit_message>
Wario - Level 6 done
</commit_message>
<xml_diff>
--- a/Wario/Wario.xlsx
+++ b/Wario/Wario.xlsx
@@ -358,9 +358,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -658,8 +658,8 @@
   <dimension ref="A1:J163"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I66" sqref="I66"/>
+      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -683,12 +683,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -716,12 +716,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -791,12 +791,12 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="18.75">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="4" t="s">
@@ -967,12 +967,12 @@
       </c>
     </row>
     <row r="30" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A30" s="12" t="s">
+      <c r="A30" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="4" t="s">
@@ -1148,12 +1148,12 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="18.75">
-      <c r="A43" s="11" t="s">
+      <c r="A43" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B43" s="11"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="4" t="s">
@@ -1300,12 +1300,12 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="18.75">
-      <c r="A55" s="12" t="s">
+      <c r="A55" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B55" s="12"/>
-      <c r="C55" s="12"/>
-      <c r="D55" s="12"/>
+      <c r="B55" s="11"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="11"/>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="4" t="s">
@@ -1396,12 +1396,12 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="18.75">
-      <c r="A63" s="11" t="s">
+      <c r="A63" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B63" s="11"/>
-      <c r="C63" s="11"/>
-      <c r="D63" s="11"/>
+      <c r="B63" s="13"/>
+      <c r="C63" s="13"/>
+      <c r="D63" s="13"/>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="4" t="s">
@@ -1516,82 +1516,97 @@
         <v>7</v>
       </c>
       <c r="B71" s="4">
-        <v>25964</v>
+        <v>25938</v>
       </c>
       <c r="C71" s="4">
         <v>20164</v>
       </c>
       <c r="D71" s="4">
         <f t="shared" si="1"/>
-        <v>-5800</v>
+        <v>-5774</v>
       </c>
     </row>
     <row r="72" spans="1:10">
       <c r="A72" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="B72" s="4">
+        <v>26289</v>
+      </c>
       <c r="C72" s="4">
         <v>20507</v>
       </c>
       <c r="D72" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-5782</v>
       </c>
     </row>
     <row r="73" spans="1:10">
       <c r="A73" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="B73" s="4">
+        <v>26503</v>
+      </c>
       <c r="C73" s="4">
         <v>20719</v>
       </c>
       <c r="D73" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-5784</v>
       </c>
     </row>
     <row r="74" spans="1:10">
       <c r="A74" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="B74" s="4">
+        <v>26632</v>
+      </c>
       <c r="C74" s="4">
         <v>20839</v>
       </c>
       <c r="D74" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-5793</v>
       </c>
     </row>
     <row r="75" spans="1:10">
       <c r="A75" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="B75" s="4">
+        <v>26836</v>
+      </c>
       <c r="C75" s="4">
         <v>21043</v>
       </c>
       <c r="D75" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-5793</v>
       </c>
     </row>
     <row r="76" spans="1:10" ht="18.75">
-      <c r="A76" s="12" t="s">
+      <c r="A76" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B76" s="12"/>
-      <c r="C76" s="12"/>
-      <c r="D76" s="12"/>
+      <c r="B76" s="11"/>
+      <c r="C76" s="11"/>
+      <c r="D76" s="11"/>
     </row>
     <row r="77" spans="1:10">
       <c r="A77" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="B77" s="4">
+        <v>27085</v>
+      </c>
       <c r="C77" s="4">
         <v>21292</v>
       </c>
       <c r="D77" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-5793</v>
       </c>
     </row>
     <row r="78" spans="1:10">
@@ -1706,12 +1721,12 @@
       </c>
     </row>
     <row r="88" spans="1:4" ht="18.75">
-      <c r="A88" s="11" t="s">
+      <c r="A88" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B88" s="11"/>
-      <c r="C88" s="11"/>
-      <c r="D88" s="11"/>
+      <c r="B88" s="13"/>
+      <c r="C88" s="13"/>
+      <c r="D88" s="13"/>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="4" t="s">
@@ -1803,12 +1818,12 @@
       </c>
     </row>
     <row r="97" spans="1:4" ht="18.75">
-      <c r="A97" s="12" t="s">
+      <c r="A97" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B97" s="12"/>
-      <c r="C97" s="12"/>
-      <c r="D97" s="12"/>
+      <c r="B97" s="11"/>
+      <c r="C97" s="11"/>
+      <c r="D97" s="11"/>
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="4" t="s">
@@ -1856,12 +1871,12 @@
       </c>
     </row>
     <row r="102" spans="1:4" ht="18.75">
-      <c r="A102" s="11" t="s">
+      <c r="A102" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B102" s="11"/>
-      <c r="C102" s="11"/>
-      <c r="D102" s="11"/>
+      <c r="B102" s="13"/>
+      <c r="C102" s="13"/>
+      <c r="D102" s="13"/>
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="4" t="s">
@@ -2089,12 +2104,12 @@
       </c>
     </row>
     <row r="124" spans="1:4" ht="18.75">
-      <c r="A124" s="12" t="s">
+      <c r="A124" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B124" s="12"/>
-      <c r="C124" s="12"/>
-      <c r="D124" s="12"/>
+      <c r="B124" s="11"/>
+      <c r="C124" s="11"/>
+      <c r="D124" s="11"/>
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="4" t="s">
@@ -2196,12 +2211,12 @@
       </c>
     </row>
     <row r="133" spans="1:5" ht="18.75">
-      <c r="A133" s="11" t="s">
+      <c r="A133" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="B133" s="11"/>
-      <c r="C133" s="11"/>
-      <c r="D133" s="11"/>
+      <c r="B133" s="13"/>
+      <c r="C133" s="13"/>
+      <c r="D133" s="13"/>
     </row>
     <row r="134" spans="1:5">
       <c r="A134" s="4" t="s">
@@ -2288,12 +2303,12 @@
       </c>
     </row>
     <row r="141" spans="1:5" ht="18.75">
-      <c r="A141" s="12" t="s">
+      <c r="A141" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B141" s="12"/>
-      <c r="C141" s="12"/>
-      <c r="D141" s="12"/>
+      <c r="B141" s="11"/>
+      <c r="C141" s="11"/>
+      <c r="D141" s="11"/>
     </row>
     <row r="142" spans="1:5">
       <c r="A142" s="4" t="s">
@@ -2458,12 +2473,12 @@
       </c>
     </row>
     <row r="155" spans="1:5" ht="18.75">
-      <c r="A155" s="11" t="s">
+      <c r="A155" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="B155" s="11"/>
-      <c r="C155" s="11"/>
-      <c r="D155" s="11"/>
+      <c r="B155" s="13"/>
+      <c r="C155" s="13"/>
+      <c r="D155" s="13"/>
     </row>
     <row r="156" spans="1:5">
       <c r="A156" s="4" t="s">
@@ -2563,12 +2578,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A55:D55"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A43:D43"/>
     <mergeCell ref="A133:D133"/>
     <mergeCell ref="A141:D141"/>
     <mergeCell ref="A155:D155"/>
@@ -2578,6 +2587,12 @@
     <mergeCell ref="A97:D97"/>
     <mergeCell ref="A102:D102"/>
     <mergeCell ref="A124:D124"/>
+    <mergeCell ref="A55:D55"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A43:D43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -2614,12 +2629,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -2647,12 +2662,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -2686,12 +2701,12 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
@@ -2814,12 +2829,12 @@
       </c>
     </row>
     <row r="19" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="4" t="s">
@@ -2987,12 +3002,12 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="18.75">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="4" t="s">
@@ -3160,12 +3175,12 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="18.75">
-      <c r="A43" s="12" t="s">
+      <c r="A43" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B43" s="12"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="4" t="s">
@@ -3273,12 +3288,12 @@
       </c>
     </row>
     <row r="51" spans="1:10" ht="18.75">
-      <c r="A51" s="11" t="s">
+      <c r="A51" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B51" s="11"/>
-      <c r="C51" s="11"/>
-      <c r="D51" s="11"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="13"/>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="4" t="s">
@@ -3464,12 +3479,12 @@
       </c>
     </row>
     <row r="64" spans="1:10" ht="18.75">
-      <c r="A64" s="12" t="s">
+      <c r="A64" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B64" s="12"/>
-      <c r="C64" s="12"/>
-      <c r="D64" s="12"/>
+      <c r="B64" s="11"/>
+      <c r="C64" s="11"/>
+      <c r="D64" s="11"/>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="4" t="s">
@@ -3628,12 +3643,12 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="18.75">
-      <c r="A76" s="11" t="s">
+      <c r="A76" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B76" s="11"/>
-      <c r="C76" s="11"/>
-      <c r="D76" s="11"/>
+      <c r="B76" s="13"/>
+      <c r="C76" s="13"/>
+      <c r="D76" s="13"/>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="4" t="s">
@@ -3746,12 +3761,12 @@
       </c>
     </row>
     <row r="85" spans="1:4" ht="18.75">
-      <c r="A85" s="12" t="s">
+      <c r="A85" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B85" s="12"/>
-      <c r="C85" s="12"/>
-      <c r="D85" s="12"/>
+      <c r="B85" s="11"/>
+      <c r="C85" s="11"/>
+      <c r="D85" s="11"/>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="4" t="s">
@@ -3811,12 +3826,12 @@
       </c>
     </row>
     <row r="90" spans="1:4" ht="18.75">
-      <c r="A90" s="11" t="s">
+      <c r="A90" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B90" s="11"/>
-      <c r="C90" s="11"/>
-      <c r="D90" s="11"/>
+      <c r="B90" s="13"/>
+      <c r="C90" s="13"/>
+      <c r="D90" s="13"/>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="4" t="s">
@@ -4107,12 +4122,12 @@
       </c>
     </row>
     <row r="112" spans="1:4" ht="18.75">
-      <c r="A112" s="12" t="s">
+      <c r="A112" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B112" s="12"/>
-      <c r="C112" s="12"/>
-      <c r="D112" s="12"/>
+      <c r="B112" s="11"/>
+      <c r="C112" s="11"/>
+      <c r="D112" s="11"/>
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="4" t="s">
@@ -4238,12 +4253,12 @@
       </c>
     </row>
     <row r="121" spans="1:5" ht="18.75">
-      <c r="A121" s="11" t="s">
+      <c r="A121" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="B121" s="11"/>
-      <c r="C121" s="11"/>
-      <c r="D121" s="11"/>
+      <c r="B121" s="13"/>
+      <c r="C121" s="13"/>
+      <c r="D121" s="13"/>
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="4" t="s">
@@ -4351,12 +4366,12 @@
       </c>
     </row>
     <row r="129" spans="1:5" ht="18.75">
-      <c r="A129" s="12" t="s">
+      <c r="A129" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B129" s="12"/>
-      <c r="C129" s="12"/>
-      <c r="D129" s="12"/>
+      <c r="B129" s="11"/>
+      <c r="C129" s="11"/>
+      <c r="D129" s="11"/>
     </row>
     <row r="130" spans="1:5">
       <c r="A130" s="4" t="s">
@@ -4560,12 +4575,12 @@
       </c>
     </row>
     <row r="143" spans="1:5" ht="18.75">
-      <c r="A143" s="11" t="s">
+      <c r="A143" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="B143" s="11"/>
-      <c r="C143" s="11"/>
-      <c r="D143" s="11"/>
+      <c r="B143" s="13"/>
+      <c r="C143" s="13"/>
+      <c r="D143" s="13"/>
     </row>
     <row r="144" spans="1:5">
       <c r="A144" s="4" t="s">
@@ -4694,6 +4709,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A31:D31"/>
     <mergeCell ref="A121:D121"/>
     <mergeCell ref="A129:D129"/>
     <mergeCell ref="A143:D143"/>
@@ -4703,12 +4724,6 @@
     <mergeCell ref="A85:D85"/>
     <mergeCell ref="A90:D90"/>
     <mergeCell ref="A112:D112"/>
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A31:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -4745,12 +4760,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -4778,12 +4793,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -4817,12 +4832,12 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
@@ -4906,12 +4921,12 @@
       </c>
     </row>
     <row r="17" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="4" t="s">
@@ -5079,12 +5094,12 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="18.75">
-      <c r="A29" s="11" t="s">
+      <c r="A29" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="4" t="s">
@@ -5162,12 +5177,12 @@
       </c>
     </row>
     <row r="35" spans="1:10" ht="18.75">
-      <c r="A35" s="12" t="s">
+      <c r="A35" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="12"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="4" t="s">
@@ -5260,12 +5275,12 @@
       </c>
     </row>
     <row r="42" spans="1:10" ht="18.75">
-      <c r="A42" s="11" t="s">
+      <c r="A42" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B42" s="11"/>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="4" t="s">
@@ -5454,12 +5469,12 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="18.75">
-      <c r="A55" s="12" t="s">
+      <c r="A55" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B55" s="12"/>
-      <c r="C55" s="12"/>
-      <c r="D55" s="12"/>
+      <c r="B55" s="11"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="11"/>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="4" t="s">
@@ -5612,12 +5627,12 @@
       </c>
     </row>
     <row r="66" spans="1:4" ht="18.75">
-      <c r="A66" s="11" t="s">
+      <c r="A66" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B66" s="11"/>
-      <c r="C66" s="11"/>
-      <c r="D66" s="11"/>
+      <c r="B66" s="13"/>
+      <c r="C66" s="13"/>
+      <c r="D66" s="13"/>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="4" t="s">
@@ -5680,12 +5695,12 @@
       </c>
     </row>
     <row r="71" spans="1:4" ht="18.75">
-      <c r="A71" s="12" t="s">
+      <c r="A71" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B71" s="12"/>
-      <c r="C71" s="12"/>
-      <c r="D71" s="12"/>
+      <c r="B71" s="11"/>
+      <c r="C71" s="11"/>
+      <c r="D71" s="11"/>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="4" t="s">
@@ -5748,12 +5763,12 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="18.75">
-      <c r="A76" s="11" t="s">
+      <c r="A76" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B76" s="11"/>
-      <c r="C76" s="11"/>
-      <c r="D76" s="11"/>
+      <c r="B76" s="13"/>
+      <c r="C76" s="13"/>
+      <c r="D76" s="13"/>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="4" t="s">
@@ -6071,12 +6086,12 @@
       </c>
     </row>
     <row r="98" spans="1:5" ht="18.75">
-      <c r="A98" s="12" t="s">
+      <c r="A98" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B98" s="12"/>
-      <c r="C98" s="12"/>
-      <c r="D98" s="12"/>
+      <c r="B98" s="11"/>
+      <c r="C98" s="11"/>
+      <c r="D98" s="11"/>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="4" t="s">
@@ -6202,12 +6217,12 @@
       </c>
     </row>
     <row r="107" spans="1:5" ht="18.75">
-      <c r="A107" s="11" t="s">
+      <c r="A107" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="B107" s="11"/>
-      <c r="C107" s="11"/>
-      <c r="D107" s="11"/>
+      <c r="B107" s="13"/>
+      <c r="C107" s="13"/>
+      <c r="D107" s="13"/>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="4" t="s">
@@ -6285,12 +6300,12 @@
       </c>
     </row>
     <row r="113" spans="1:4" ht="18.75">
-      <c r="A113" s="12" t="s">
+      <c r="A113" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B113" s="12"/>
-      <c r="C113" s="12"/>
-      <c r="D113" s="12"/>
+      <c r="B113" s="11"/>
+      <c r="C113" s="11"/>
+      <c r="D113" s="11"/>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="4" t="s">
@@ -6488,12 +6503,12 @@
       </c>
     </row>
     <row r="127" spans="1:4" ht="18.75">
-      <c r="A127" s="11" t="s">
+      <c r="A127" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="B127" s="11"/>
-      <c r="C127" s="11"/>
-      <c r="D127" s="11"/>
+      <c r="B127" s="13"/>
+      <c r="C127" s="13"/>
+      <c r="D127" s="13"/>
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="4" t="s">
@@ -6613,11 +6628,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A29:D29"/>
     <mergeCell ref="A127:D127"/>
     <mergeCell ref="A107:D107"/>
     <mergeCell ref="A113:D113"/>
@@ -6628,6 +6638,11 @@
     <mergeCell ref="A98:D98"/>
     <mergeCell ref="A66:D66"/>
     <mergeCell ref="A55:D55"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A29:D29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>

</xml_diff>

<commit_message>
Wario - pasted some of level 7 from any%.  TODO: route plan this level.
</commit_message>
<xml_diff>
--- a/Wario/Wario.xlsx
+++ b/Wario/Wario.xlsx
@@ -659,7 +659,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B78" sqref="B78"/>
+      <selection pane="bottomLeft" activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1625,12 +1625,15 @@
       <c r="A79" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="B79" s="4">
+        <v>28318</v>
+      </c>
       <c r="C79" s="4">
         <v>22525</v>
       </c>
       <c r="D79" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-5793</v>
       </c>
     </row>
     <row r="80" spans="1:10">

</xml_diff>

<commit_message>
Wario 100% - Got treasure for level 7 up to the convergance point with the any% movie.
</commit_message>
<xml_diff>
--- a/Wario/Wario.xlsx
+++ b/Wario/Wario.xlsx
@@ -658,8 +658,8 @@
   <dimension ref="A1:J163"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B80" sqref="B80"/>
+      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B84" sqref="B84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1676,12 +1676,15 @@
       <c r="A83" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="B83" s="4">
+        <v>31131</v>
+      </c>
       <c r="C83" s="4">
         <v>23709</v>
       </c>
       <c r="D83" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-7422</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -1706,9 +1709,15 @@
       <c r="A86" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="B86" s="4">
+        <v>28980</v>
+      </c>
+      <c r="C86" s="4">
+        <v>23177</v>
+      </c>
       <c r="D86" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-5803</v>
       </c>
     </row>
     <row r="87" spans="1:4">

</xml_diff>

<commit_message>
Wario 100% - Level 7 done, first hit on mini boss of level 8 done.
</commit_message>
<xml_diff>
--- a/Wario/Wario.xlsx
+++ b/Wario/Wario.xlsx
@@ -658,8 +658,8 @@
   <dimension ref="A1:J163"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B84" sqref="B84"/>
+      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D90" sqref="D90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1664,12 +1664,15 @@
       <c r="A82" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="B82" s="4">
+        <v>28980</v>
+      </c>
       <c r="C82" s="4">
         <v>23177</v>
       </c>
       <c r="D82" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-5803</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -1700,9 +1703,12 @@
       <c r="A85" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="B85" s="4">
+        <v>31805</v>
+      </c>
       <c r="D85" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-31805</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -1710,26 +1716,26 @@
         <v>27</v>
       </c>
       <c r="B86" s="4">
-        <v>28980</v>
-      </c>
-      <c r="C86" s="4">
-        <v>23177</v>
+        <v>31910</v>
       </c>
       <c r="D86" s="4">
         <f t="shared" si="1"/>
-        <v>-5803</v>
+        <v>-31910</v>
       </c>
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="B87" s="4">
+        <v>32113</v>
+      </c>
       <c r="C87" s="4">
         <v>24691</v>
       </c>
       <c r="D87" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-7422</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="18.75">
@@ -1744,9 +1750,12 @@
       <c r="A89" s="4" t="s">
         <v>37</v>
       </c>
+      <c r="B89" s="4">
+        <v>32364</v>
+      </c>
       <c r="D89" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-32364</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -1765,12 +1774,16 @@
       <c r="A91" s="4" t="s">
         <v>66</v>
       </c>
+      <c r="B91" s="4">
+        <f>C91-D89</f>
+        <v>59751</v>
+      </c>
       <c r="C91" s="4">
         <v>27387</v>
       </c>
       <c r="D91" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-32364</v>
       </c>
     </row>
     <row r="92" spans="1:4">

</xml_diff>

<commit_message>
Wario 100% - Enter Level 8 boss room
</commit_message>
<xml_diff>
--- a/Wario/Wario.xlsx
+++ b/Wario/Wario.xlsx
@@ -358,9 +358,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -658,8 +658,8 @@
   <dimension ref="A1:J163"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D90" sqref="D90"/>
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B90" sqref="B90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -683,12 +683,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -716,12 +716,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -791,12 +791,12 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="18.75">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="4" t="s">
@@ -967,12 +967,12 @@
       </c>
     </row>
     <row r="30" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A30" s="11" t="s">
+      <c r="A30" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="4" t="s">
@@ -1148,12 +1148,12 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="18.75">
-      <c r="A43" s="13" t="s">
+      <c r="A43" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B43" s="13"/>
-      <c r="C43" s="13"/>
-      <c r="D43" s="13"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="4" t="s">
@@ -1300,12 +1300,12 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="18.75">
-      <c r="A55" s="11" t="s">
+      <c r="A55" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B55" s="11"/>
-      <c r="C55" s="11"/>
-      <c r="D55" s="11"/>
+      <c r="B55" s="12"/>
+      <c r="C55" s="12"/>
+      <c r="D55" s="12"/>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="4" t="s">
@@ -1396,12 +1396,12 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="18.75">
-      <c r="A63" s="13" t="s">
+      <c r="A63" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B63" s="13"/>
-      <c r="C63" s="13"/>
-      <c r="D63" s="13"/>
+      <c r="B63" s="11"/>
+      <c r="C63" s="11"/>
+      <c r="D63" s="11"/>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="4" t="s">
@@ -1587,12 +1587,12 @@
       </c>
     </row>
     <row r="76" spans="1:10" ht="18.75">
-      <c r="A76" s="11" t="s">
+      <c r="A76" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B76" s="11"/>
-      <c r="C76" s="11"/>
-      <c r="D76" s="11"/>
+      <c r="B76" s="12"/>
+      <c r="C76" s="12"/>
+      <c r="D76" s="12"/>
     </row>
     <row r="77" spans="1:10">
       <c r="A77" s="4" t="s">
@@ -1739,12 +1739,12 @@
       </c>
     </row>
     <row r="88" spans="1:4" ht="18.75">
-      <c r="A88" s="13" t="s">
+      <c r="A88" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B88" s="13"/>
-      <c r="C88" s="13"/>
-      <c r="D88" s="13"/>
+      <c r="B88" s="11"/>
+      <c r="C88" s="11"/>
+      <c r="D88" s="11"/>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="4" t="s">
@@ -1762,28 +1762,27 @@
       <c r="A90" s="8" t="s">
         <v>26</v>
       </c>
+      <c r="B90" s="4">
+        <v>33665</v>
+      </c>
       <c r="C90" s="4">
         <v>26245</v>
       </c>
       <c r="D90" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-7420</v>
       </c>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B91" s="4">
-        <f>C91-D89</f>
-        <v>59751</v>
-      </c>
       <c r="C91" s="4">
         <v>27387</v>
       </c>
       <c r="D91" s="4">
         <f t="shared" si="1"/>
-        <v>-32364</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -1843,12 +1842,12 @@
       </c>
     </row>
     <row r="97" spans="1:4" ht="18.75">
-      <c r="A97" s="11" t="s">
+      <c r="A97" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B97" s="11"/>
-      <c r="C97" s="11"/>
-      <c r="D97" s="11"/>
+      <c r="B97" s="12"/>
+      <c r="C97" s="12"/>
+      <c r="D97" s="12"/>
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="4" t="s">
@@ -1896,12 +1895,12 @@
       </c>
     </row>
     <row r="102" spans="1:4" ht="18.75">
-      <c r="A102" s="13" t="s">
+      <c r="A102" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B102" s="13"/>
-      <c r="C102" s="13"/>
-      <c r="D102" s="13"/>
+      <c r="B102" s="11"/>
+      <c r="C102" s="11"/>
+      <c r="D102" s="11"/>
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="4" t="s">
@@ -2129,12 +2128,12 @@
       </c>
     </row>
     <row r="124" spans="1:4" ht="18.75">
-      <c r="A124" s="11" t="s">
+      <c r="A124" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B124" s="11"/>
-      <c r="C124" s="11"/>
-      <c r="D124" s="11"/>
+      <c r="B124" s="12"/>
+      <c r="C124" s="12"/>
+      <c r="D124" s="12"/>
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="4" t="s">
@@ -2236,12 +2235,12 @@
       </c>
     </row>
     <row r="133" spans="1:5" ht="18.75">
-      <c r="A133" s="13" t="s">
+      <c r="A133" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B133" s="13"/>
-      <c r="C133" s="13"/>
-      <c r="D133" s="13"/>
+      <c r="B133" s="11"/>
+      <c r="C133" s="11"/>
+      <c r="D133" s="11"/>
     </row>
     <row r="134" spans="1:5">
       <c r="A134" s="4" t="s">
@@ -2328,12 +2327,12 @@
       </c>
     </row>
     <row r="141" spans="1:5" ht="18.75">
-      <c r="A141" s="11" t="s">
+      <c r="A141" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B141" s="11"/>
-      <c r="C141" s="11"/>
-      <c r="D141" s="11"/>
+      <c r="B141" s="12"/>
+      <c r="C141" s="12"/>
+      <c r="D141" s="12"/>
     </row>
     <row r="142" spans="1:5">
       <c r="A142" s="4" t="s">
@@ -2498,12 +2497,12 @@
       </c>
     </row>
     <row r="155" spans="1:5" ht="18.75">
-      <c r="A155" s="13" t="s">
+      <c r="A155" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="B155" s="13"/>
-      <c r="C155" s="13"/>
-      <c r="D155" s="13"/>
+      <c r="B155" s="11"/>
+      <c r="C155" s="11"/>
+      <c r="D155" s="11"/>
     </row>
     <row r="156" spans="1:5">
       <c r="A156" s="4" t="s">
@@ -2603,6 +2602,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A55:D55"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A43:D43"/>
     <mergeCell ref="A133:D133"/>
     <mergeCell ref="A141:D141"/>
     <mergeCell ref="A155:D155"/>
@@ -2612,12 +2617,6 @@
     <mergeCell ref="A97:D97"/>
     <mergeCell ref="A102:D102"/>
     <mergeCell ref="A124:D124"/>
-    <mergeCell ref="A55:D55"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A43:D43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -2654,12 +2653,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -2687,12 +2686,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -2726,12 +2725,12 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
@@ -2854,12 +2853,12 @@
       </c>
     </row>
     <row r="19" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="4" t="s">
@@ -3027,12 +3026,12 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="18.75">
-      <c r="A31" s="13" t="s">
+      <c r="A31" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="4" t="s">
@@ -3200,12 +3199,12 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="18.75">
-      <c r="A43" s="11" t="s">
+      <c r="A43" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B43" s="11"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="4" t="s">
@@ -3313,12 +3312,12 @@
       </c>
     </row>
     <row r="51" spans="1:10" ht="18.75">
-      <c r="A51" s="13" t="s">
+      <c r="A51" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B51" s="13"/>
-      <c r="C51" s="13"/>
-      <c r="D51" s="13"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="4" t="s">
@@ -3504,12 +3503,12 @@
       </c>
     </row>
     <row r="64" spans="1:10" ht="18.75">
-      <c r="A64" s="11" t="s">
+      <c r="A64" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B64" s="11"/>
-      <c r="C64" s="11"/>
-      <c r="D64" s="11"/>
+      <c r="B64" s="12"/>
+      <c r="C64" s="12"/>
+      <c r="D64" s="12"/>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="4" t="s">
@@ -3668,12 +3667,12 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="18.75">
-      <c r="A76" s="13" t="s">
+      <c r="A76" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B76" s="13"/>
-      <c r="C76" s="13"/>
-      <c r="D76" s="13"/>
+      <c r="B76" s="11"/>
+      <c r="C76" s="11"/>
+      <c r="D76" s="11"/>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="4" t="s">
@@ -3786,12 +3785,12 @@
       </c>
     </row>
     <row r="85" spans="1:4" ht="18.75">
-      <c r="A85" s="11" t="s">
+      <c r="A85" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B85" s="11"/>
-      <c r="C85" s="11"/>
-      <c r="D85" s="11"/>
+      <c r="B85" s="12"/>
+      <c r="C85" s="12"/>
+      <c r="D85" s="12"/>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="4" t="s">
@@ -3851,12 +3850,12 @@
       </c>
     </row>
     <row r="90" spans="1:4" ht="18.75">
-      <c r="A90" s="13" t="s">
+      <c r="A90" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B90" s="13"/>
-      <c r="C90" s="13"/>
-      <c r="D90" s="13"/>
+      <c r="B90" s="11"/>
+      <c r="C90" s="11"/>
+      <c r="D90" s="11"/>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="4" t="s">
@@ -4147,12 +4146,12 @@
       </c>
     </row>
     <row r="112" spans="1:4" ht="18.75">
-      <c r="A112" s="11" t="s">
+      <c r="A112" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B112" s="11"/>
-      <c r="C112" s="11"/>
-      <c r="D112" s="11"/>
+      <c r="B112" s="12"/>
+      <c r="C112" s="12"/>
+      <c r="D112" s="12"/>
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="4" t="s">
@@ -4278,12 +4277,12 @@
       </c>
     </row>
     <row r="121" spans="1:5" ht="18.75">
-      <c r="A121" s="13" t="s">
+      <c r="A121" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B121" s="13"/>
-      <c r="C121" s="13"/>
-      <c r="D121" s="13"/>
+      <c r="B121" s="11"/>
+      <c r="C121" s="11"/>
+      <c r="D121" s="11"/>
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="4" t="s">
@@ -4391,12 +4390,12 @@
       </c>
     </row>
     <row r="129" spans="1:5" ht="18.75">
-      <c r="A129" s="11" t="s">
+      <c r="A129" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B129" s="11"/>
-      <c r="C129" s="11"/>
-      <c r="D129" s="11"/>
+      <c r="B129" s="12"/>
+      <c r="C129" s="12"/>
+      <c r="D129" s="12"/>
     </row>
     <row r="130" spans="1:5">
       <c r="A130" s="4" t="s">
@@ -4600,12 +4599,12 @@
       </c>
     </row>
     <row r="143" spans="1:5" ht="18.75">
-      <c r="A143" s="13" t="s">
+      <c r="A143" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="B143" s="13"/>
-      <c r="C143" s="13"/>
-      <c r="D143" s="13"/>
+      <c r="B143" s="11"/>
+      <c r="C143" s="11"/>
+      <c r="D143" s="11"/>
     </row>
     <row r="144" spans="1:5">
       <c r="A144" s="4" t="s">
@@ -4734,12 +4733,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A31:D31"/>
     <mergeCell ref="A121:D121"/>
     <mergeCell ref="A129:D129"/>
     <mergeCell ref="A143:D143"/>
@@ -4749,6 +4742,12 @@
     <mergeCell ref="A85:D85"/>
     <mergeCell ref="A90:D90"/>
     <mergeCell ref="A112:D112"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A31:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -4785,12 +4784,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -4818,12 +4817,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -4857,12 +4856,12 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
@@ -4946,12 +4945,12 @@
       </c>
     </row>
     <row r="17" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="4" t="s">
@@ -5119,12 +5118,12 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="18.75">
-      <c r="A29" s="13" t="s">
+      <c r="A29" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="4" t="s">
@@ -5202,12 +5201,12 @@
       </c>
     </row>
     <row r="35" spans="1:10" ht="18.75">
-      <c r="A35" s="11" t="s">
+      <c r="A35" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="4" t="s">
@@ -5300,12 +5299,12 @@
       </c>
     </row>
     <row r="42" spans="1:10" ht="18.75">
-      <c r="A42" s="13" t="s">
+      <c r="A42" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B42" s="13"/>
-      <c r="C42" s="13"/>
-      <c r="D42" s="13"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="4" t="s">
@@ -5494,12 +5493,12 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="18.75">
-      <c r="A55" s="11" t="s">
+      <c r="A55" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B55" s="11"/>
-      <c r="C55" s="11"/>
-      <c r="D55" s="11"/>
+      <c r="B55" s="12"/>
+      <c r="C55" s="12"/>
+      <c r="D55" s="12"/>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="4" t="s">
@@ -5652,12 +5651,12 @@
       </c>
     </row>
     <row r="66" spans="1:4" ht="18.75">
-      <c r="A66" s="13" t="s">
+      <c r="A66" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B66" s="13"/>
-      <c r="C66" s="13"/>
-      <c r="D66" s="13"/>
+      <c r="B66" s="11"/>
+      <c r="C66" s="11"/>
+      <c r="D66" s="11"/>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="4" t="s">
@@ -5720,12 +5719,12 @@
       </c>
     </row>
     <row r="71" spans="1:4" ht="18.75">
-      <c r="A71" s="11" t="s">
+      <c r="A71" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B71" s="11"/>
-      <c r="C71" s="11"/>
-      <c r="D71" s="11"/>
+      <c r="B71" s="12"/>
+      <c r="C71" s="12"/>
+      <c r="D71" s="12"/>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="4" t="s">
@@ -5788,12 +5787,12 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="18.75">
-      <c r="A76" s="13" t="s">
+      <c r="A76" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B76" s="13"/>
-      <c r="C76" s="13"/>
-      <c r="D76" s="13"/>
+      <c r="B76" s="11"/>
+      <c r="C76" s="11"/>
+      <c r="D76" s="11"/>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="4" t="s">
@@ -6111,12 +6110,12 @@
       </c>
     </row>
     <row r="98" spans="1:5" ht="18.75">
-      <c r="A98" s="11" t="s">
+      <c r="A98" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B98" s="11"/>
-      <c r="C98" s="11"/>
-      <c r="D98" s="11"/>
+      <c r="B98" s="12"/>
+      <c r="C98" s="12"/>
+      <c r="D98" s="12"/>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="4" t="s">
@@ -6242,12 +6241,12 @@
       </c>
     </row>
     <row r="107" spans="1:5" ht="18.75">
-      <c r="A107" s="13" t="s">
+      <c r="A107" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B107" s="13"/>
-      <c r="C107" s="13"/>
-      <c r="D107" s="13"/>
+      <c r="B107" s="11"/>
+      <c r="C107" s="11"/>
+      <c r="D107" s="11"/>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="4" t="s">
@@ -6325,12 +6324,12 @@
       </c>
     </row>
     <row r="113" spans="1:4" ht="18.75">
-      <c r="A113" s="11" t="s">
+      <c r="A113" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B113" s="11"/>
-      <c r="C113" s="11"/>
-      <c r="D113" s="11"/>
+      <c r="B113" s="12"/>
+      <c r="C113" s="12"/>
+      <c r="D113" s="12"/>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="4" t="s">
@@ -6528,12 +6527,12 @@
       </c>
     </row>
     <row r="127" spans="1:4" ht="18.75">
-      <c r="A127" s="13" t="s">
+      <c r="A127" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="B127" s="13"/>
-      <c r="C127" s="13"/>
-      <c r="D127" s="13"/>
+      <c r="B127" s="11"/>
+      <c r="C127" s="11"/>
+      <c r="D127" s="11"/>
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="4" t="s">
@@ -6653,6 +6652,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A29:D29"/>
     <mergeCell ref="A127:D127"/>
     <mergeCell ref="A107:D107"/>
     <mergeCell ref="A113:D113"/>
@@ -6663,11 +6667,6 @@
     <mergeCell ref="A98:D98"/>
     <mergeCell ref="A66:D66"/>
     <mergeCell ref="A55:D55"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A29:D29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>

</xml_diff>

<commit_message>
Wario 100% - Level 8 done, Level 9 savestate, fix level 7 & 8 leel savestates
</commit_message>
<xml_diff>
--- a/Wario/Wario.xlsx
+++ b/Wario/Wario.xlsx
@@ -358,9 +358,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -658,8 +658,8 @@
   <dimension ref="A1:J163"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B90" sqref="B90"/>
+      <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B99" sqref="B99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -683,12 +683,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -716,12 +716,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -791,12 +791,12 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="18.75">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="4" t="s">
@@ -967,12 +967,12 @@
       </c>
     </row>
     <row r="30" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A30" s="12" t="s">
+      <c r="A30" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="4" t="s">
@@ -1148,12 +1148,12 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="18.75">
-      <c r="A43" s="11" t="s">
+      <c r="A43" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B43" s="11"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="4" t="s">
@@ -1300,12 +1300,12 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="18.75">
-      <c r="A55" s="12" t="s">
+      <c r="A55" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B55" s="12"/>
-      <c r="C55" s="12"/>
-      <c r="D55" s="12"/>
+      <c r="B55" s="11"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="11"/>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="4" t="s">
@@ -1396,12 +1396,12 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="18.75">
-      <c r="A63" s="11" t="s">
+      <c r="A63" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B63" s="11"/>
-      <c r="C63" s="11"/>
-      <c r="D63" s="11"/>
+      <c r="B63" s="13"/>
+      <c r="C63" s="13"/>
+      <c r="D63" s="13"/>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="4" t="s">
@@ -1587,12 +1587,12 @@
       </c>
     </row>
     <row r="76" spans="1:10" ht="18.75">
-      <c r="A76" s="12" t="s">
+      <c r="A76" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B76" s="12"/>
-      <c r="C76" s="12"/>
-      <c r="D76" s="12"/>
+      <c r="B76" s="11"/>
+      <c r="C76" s="11"/>
+      <c r="D76" s="11"/>
     </row>
     <row r="77" spans="1:10">
       <c r="A77" s="4" t="s">
@@ -1739,12 +1739,12 @@
       </c>
     </row>
     <row r="88" spans="1:4" ht="18.75">
-      <c r="A88" s="11" t="s">
+      <c r="A88" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B88" s="11"/>
-      <c r="C88" s="11"/>
-      <c r="D88" s="11"/>
+      <c r="B88" s="13"/>
+      <c r="C88" s="13"/>
+      <c r="D88" s="13"/>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="4" t="s">
@@ -1777,48 +1777,60 @@
       <c r="A91" s="4" t="s">
         <v>66</v>
       </c>
+      <c r="B91" s="4">
+        <v>34807</v>
+      </c>
       <c r="C91" s="4">
         <v>27387</v>
       </c>
       <c r="D91" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-7420</v>
       </c>
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="4" t="s">
         <v>60</v>
       </c>
+      <c r="B92" s="4">
+        <v>35487</v>
+      </c>
       <c r="C92" s="4">
         <v>28067</v>
       </c>
       <c r="D92" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-7420</v>
       </c>
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="4" t="s">
         <v>62</v>
       </c>
+      <c r="B93" s="4">
+        <v>36167</v>
+      </c>
       <c r="C93" s="4">
         <v>28747</v>
       </c>
       <c r="D93" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-7420</v>
       </c>
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="4" t="s">
         <v>39</v>
       </c>
+      <c r="B94" s="4">
+        <v>37639</v>
+      </c>
       <c r="C94" s="4">
         <v>30220</v>
       </c>
       <c r="D94" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-7419</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -1833,32 +1845,38 @@
       <c r="A96" s="4" t="s">
         <v>40</v>
       </c>
+      <c r="B96" s="4">
+        <v>38169</v>
+      </c>
       <c r="C96" s="4">
         <v>30749</v>
       </c>
       <c r="D96" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-7420</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="18.75">
-      <c r="A97" s="12" t="s">
+      <c r="A97" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B97" s="12"/>
-      <c r="C97" s="12"/>
-      <c r="D97" s="12"/>
+      <c r="B97" s="11"/>
+      <c r="C97" s="11"/>
+      <c r="D97" s="11"/>
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="4" t="s">
         <v>41</v>
       </c>
+      <c r="B98" s="4">
+        <v>38419</v>
+      </c>
       <c r="C98" s="4">
         <v>30998</v>
       </c>
       <c r="D98" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-7421</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -1895,12 +1913,12 @@
       </c>
     </row>
     <row r="102" spans="1:4" ht="18.75">
-      <c r="A102" s="11" t="s">
+      <c r="A102" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B102" s="11"/>
-      <c r="C102" s="11"/>
-      <c r="D102" s="11"/>
+      <c r="B102" s="13"/>
+      <c r="C102" s="13"/>
+      <c r="D102" s="13"/>
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="4" t="s">
@@ -2128,12 +2146,12 @@
       </c>
     </row>
     <row r="124" spans="1:4" ht="18.75">
-      <c r="A124" s="12" t="s">
+      <c r="A124" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B124" s="12"/>
-      <c r="C124" s="12"/>
-      <c r="D124" s="12"/>
+      <c r="B124" s="11"/>
+      <c r="C124" s="11"/>
+      <c r="D124" s="11"/>
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="4" t="s">
@@ -2235,12 +2253,12 @@
       </c>
     </row>
     <row r="133" spans="1:5" ht="18.75">
-      <c r="A133" s="11" t="s">
+      <c r="A133" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="B133" s="11"/>
-      <c r="C133" s="11"/>
-      <c r="D133" s="11"/>
+      <c r="B133" s="13"/>
+      <c r="C133" s="13"/>
+      <c r="D133" s="13"/>
     </row>
     <row r="134" spans="1:5">
       <c r="A134" s="4" t="s">
@@ -2327,12 +2345,12 @@
       </c>
     </row>
     <row r="141" spans="1:5" ht="18.75">
-      <c r="A141" s="12" t="s">
+      <c r="A141" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B141" s="12"/>
-      <c r="C141" s="12"/>
-      <c r="D141" s="12"/>
+      <c r="B141" s="11"/>
+      <c r="C141" s="11"/>
+      <c r="D141" s="11"/>
     </row>
     <row r="142" spans="1:5">
       <c r="A142" s="4" t="s">
@@ -2497,12 +2515,12 @@
       </c>
     </row>
     <row r="155" spans="1:5" ht="18.75">
-      <c r="A155" s="11" t="s">
+      <c r="A155" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="B155" s="11"/>
-      <c r="C155" s="11"/>
-      <c r="D155" s="11"/>
+      <c r="B155" s="13"/>
+      <c r="C155" s="13"/>
+      <c r="D155" s="13"/>
     </row>
     <row r="156" spans="1:5">
       <c r="A156" s="4" t="s">
@@ -2602,12 +2620,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A55:D55"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A43:D43"/>
     <mergeCell ref="A133:D133"/>
     <mergeCell ref="A141:D141"/>
     <mergeCell ref="A155:D155"/>
@@ -2617,6 +2629,12 @@
     <mergeCell ref="A97:D97"/>
     <mergeCell ref="A102:D102"/>
     <mergeCell ref="A124:D124"/>
+    <mergeCell ref="A55:D55"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A43:D43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -2653,12 +2671,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -2686,12 +2704,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -2725,12 +2743,12 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
@@ -2853,12 +2871,12 @@
       </c>
     </row>
     <row r="19" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="4" t="s">
@@ -3026,12 +3044,12 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="18.75">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="4" t="s">
@@ -3199,12 +3217,12 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="18.75">
-      <c r="A43" s="12" t="s">
+      <c r="A43" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B43" s="12"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="4" t="s">
@@ -3312,12 +3330,12 @@
       </c>
     </row>
     <row r="51" spans="1:10" ht="18.75">
-      <c r="A51" s="11" t="s">
+      <c r="A51" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B51" s="11"/>
-      <c r="C51" s="11"/>
-      <c r="D51" s="11"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="13"/>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="4" t="s">
@@ -3503,12 +3521,12 @@
       </c>
     </row>
     <row r="64" spans="1:10" ht="18.75">
-      <c r="A64" s="12" t="s">
+      <c r="A64" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B64" s="12"/>
-      <c r="C64" s="12"/>
-      <c r="D64" s="12"/>
+      <c r="B64" s="11"/>
+      <c r="C64" s="11"/>
+      <c r="D64" s="11"/>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="4" t="s">
@@ -3667,12 +3685,12 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="18.75">
-      <c r="A76" s="11" t="s">
+      <c r="A76" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B76" s="11"/>
-      <c r="C76" s="11"/>
-      <c r="D76" s="11"/>
+      <c r="B76" s="13"/>
+      <c r="C76" s="13"/>
+      <c r="D76" s="13"/>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="4" t="s">
@@ -3785,12 +3803,12 @@
       </c>
     </row>
     <row r="85" spans="1:4" ht="18.75">
-      <c r="A85" s="12" t="s">
+      <c r="A85" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B85" s="12"/>
-      <c r="C85" s="12"/>
-      <c r="D85" s="12"/>
+      <c r="B85" s="11"/>
+      <c r="C85" s="11"/>
+      <c r="D85" s="11"/>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="4" t="s">
@@ -3850,12 +3868,12 @@
       </c>
     </row>
     <row r="90" spans="1:4" ht="18.75">
-      <c r="A90" s="11" t="s">
+      <c r="A90" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B90" s="11"/>
-      <c r="C90" s="11"/>
-      <c r="D90" s="11"/>
+      <c r="B90" s="13"/>
+      <c r="C90" s="13"/>
+      <c r="D90" s="13"/>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="4" t="s">
@@ -4146,12 +4164,12 @@
       </c>
     </row>
     <row r="112" spans="1:4" ht="18.75">
-      <c r="A112" s="12" t="s">
+      <c r="A112" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B112" s="12"/>
-      <c r="C112" s="12"/>
-      <c r="D112" s="12"/>
+      <c r="B112" s="11"/>
+      <c r="C112" s="11"/>
+      <c r="D112" s="11"/>
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="4" t="s">
@@ -4277,12 +4295,12 @@
       </c>
     </row>
     <row r="121" spans="1:5" ht="18.75">
-      <c r="A121" s="11" t="s">
+      <c r="A121" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="B121" s="11"/>
-      <c r="C121" s="11"/>
-      <c r="D121" s="11"/>
+      <c r="B121" s="13"/>
+      <c r="C121" s="13"/>
+      <c r="D121" s="13"/>
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="4" t="s">
@@ -4390,12 +4408,12 @@
       </c>
     </row>
     <row r="129" spans="1:5" ht="18.75">
-      <c r="A129" s="12" t="s">
+      <c r="A129" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B129" s="12"/>
-      <c r="C129" s="12"/>
-      <c r="D129" s="12"/>
+      <c r="B129" s="11"/>
+      <c r="C129" s="11"/>
+      <c r="D129" s="11"/>
     </row>
     <row r="130" spans="1:5">
       <c r="A130" s="4" t="s">
@@ -4599,12 +4617,12 @@
       </c>
     </row>
     <row r="143" spans="1:5" ht="18.75">
-      <c r="A143" s="11" t="s">
+      <c r="A143" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="B143" s="11"/>
-      <c r="C143" s="11"/>
-      <c r="D143" s="11"/>
+      <c r="B143" s="13"/>
+      <c r="C143" s="13"/>
+      <c r="D143" s="13"/>
     </row>
     <row r="144" spans="1:5">
       <c r="A144" s="4" t="s">
@@ -4733,6 +4751,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A31:D31"/>
     <mergeCell ref="A121:D121"/>
     <mergeCell ref="A129:D129"/>
     <mergeCell ref="A143:D143"/>
@@ -4742,12 +4766,6 @@
     <mergeCell ref="A85:D85"/>
     <mergeCell ref="A90:D90"/>
     <mergeCell ref="A112:D112"/>
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A31:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -4784,12 +4802,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -4817,12 +4835,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -4856,12 +4874,12 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
@@ -4945,12 +4963,12 @@
       </c>
     </row>
     <row r="17" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="4" t="s">
@@ -5118,12 +5136,12 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="18.75">
-      <c r="A29" s="11" t="s">
+      <c r="A29" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="4" t="s">
@@ -5201,12 +5219,12 @@
       </c>
     </row>
     <row r="35" spans="1:10" ht="18.75">
-      <c r="A35" s="12" t="s">
+      <c r="A35" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="12"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="4" t="s">
@@ -5299,12 +5317,12 @@
       </c>
     </row>
     <row r="42" spans="1:10" ht="18.75">
-      <c r="A42" s="11" t="s">
+      <c r="A42" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B42" s="11"/>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="4" t="s">
@@ -5493,12 +5511,12 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="18.75">
-      <c r="A55" s="12" t="s">
+      <c r="A55" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B55" s="12"/>
-      <c r="C55" s="12"/>
-      <c r="D55" s="12"/>
+      <c r="B55" s="11"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="11"/>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="4" t="s">
@@ -5651,12 +5669,12 @@
       </c>
     </row>
     <row r="66" spans="1:4" ht="18.75">
-      <c r="A66" s="11" t="s">
+      <c r="A66" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B66" s="11"/>
-      <c r="C66" s="11"/>
-      <c r="D66" s="11"/>
+      <c r="B66" s="13"/>
+      <c r="C66" s="13"/>
+      <c r="D66" s="13"/>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="4" t="s">
@@ -5719,12 +5737,12 @@
       </c>
     </row>
     <row r="71" spans="1:4" ht="18.75">
-      <c r="A71" s="12" t="s">
+      <c r="A71" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B71" s="12"/>
-      <c r="C71" s="12"/>
-      <c r="D71" s="12"/>
+      <c r="B71" s="11"/>
+      <c r="C71" s="11"/>
+      <c r="D71" s="11"/>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="4" t="s">
@@ -5787,12 +5805,12 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="18.75">
-      <c r="A76" s="11" t="s">
+      <c r="A76" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B76" s="11"/>
-      <c r="C76" s="11"/>
-      <c r="D76" s="11"/>
+      <c r="B76" s="13"/>
+      <c r="C76" s="13"/>
+      <c r="D76" s="13"/>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="4" t="s">
@@ -6110,12 +6128,12 @@
       </c>
     </row>
     <row r="98" spans="1:5" ht="18.75">
-      <c r="A98" s="12" t="s">
+      <c r="A98" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B98" s="12"/>
-      <c r="C98" s="12"/>
-      <c r="D98" s="12"/>
+      <c r="B98" s="11"/>
+      <c r="C98" s="11"/>
+      <c r="D98" s="11"/>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="4" t="s">
@@ -6241,12 +6259,12 @@
       </c>
     </row>
     <row r="107" spans="1:5" ht="18.75">
-      <c r="A107" s="11" t="s">
+      <c r="A107" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="B107" s="11"/>
-      <c r="C107" s="11"/>
-      <c r="D107" s="11"/>
+      <c r="B107" s="13"/>
+      <c r="C107" s="13"/>
+      <c r="D107" s="13"/>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="4" t="s">
@@ -6324,12 +6342,12 @@
       </c>
     </row>
     <row r="113" spans="1:4" ht="18.75">
-      <c r="A113" s="12" t="s">
+      <c r="A113" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B113" s="12"/>
-      <c r="C113" s="12"/>
-      <c r="D113" s="12"/>
+      <c r="B113" s="11"/>
+      <c r="C113" s="11"/>
+      <c r="D113" s="11"/>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="4" t="s">
@@ -6527,12 +6545,12 @@
       </c>
     </row>
     <row r="127" spans="1:4" ht="18.75">
-      <c r="A127" s="11" t="s">
+      <c r="A127" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="B127" s="11"/>
-      <c r="C127" s="11"/>
-      <c r="D127" s="11"/>
+      <c r="B127" s="13"/>
+      <c r="C127" s="13"/>
+      <c r="D127" s="13"/>
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="4" t="s">
@@ -6652,11 +6670,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A29:D29"/>
     <mergeCell ref="A127:D127"/>
     <mergeCell ref="A107:D107"/>
     <mergeCell ref="A113:D113"/>
@@ -6667,6 +6680,11 @@
     <mergeCell ref="A98:D98"/>
     <mergeCell ref="A66:D66"/>
     <mergeCell ref="A55:D55"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A29:D29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>

</xml_diff>

<commit_message>
Wario 100% - Level 10 begin.
</commit_message>
<xml_diff>
--- a/Wario/Wario.xlsx
+++ b/Wario/Wario.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="76">
   <si>
     <t>Enter pipe</t>
   </si>
@@ -655,11 +655,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J163"/>
+  <dimension ref="A1:J164"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B99" sqref="B99"/>
+      <pane ySplit="1" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B105" sqref="B105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -821,7 +821,7 @@
         <v>3359</v>
       </c>
       <c r="D16" s="4">
-        <f t="shared" ref="D16:D101" si="1">IF(B16 &gt;  0,C16-B16, 0)</f>
+        <f t="shared" ref="D16:D102" si="1">IF(B16 &gt;  0,C16-B16, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1890,55 +1890,70 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="4" t="s">
-        <v>27</v>
+        <v>69</v>
+      </c>
+      <c r="B100" s="4">
+        <v>40410</v>
       </c>
       <c r="C100" s="4">
-        <v>33405</v>
+        <v>32946</v>
       </c>
       <c r="D100" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-7464</v>
       </c>
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B101" s="4">
+        <v>42018</v>
+      </c>
+      <c r="C101" s="4">
+        <v>33405</v>
+      </c>
+      <c r="D101" s="4">
+        <f t="shared" si="1"/>
+        <v>-8613</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C101" s="4">
+      <c r="B102" s="4">
+        <v>42221</v>
+      </c>
+      <c r="C102" s="4">
         <v>33609</v>
       </c>
-      <c r="D101" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" ht="18.75">
-      <c r="A102" s="13" t="s">
+      <c r="D102" s="4">
+        <f t="shared" si="1"/>
+        <v>-8612</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="18.75">
+      <c r="A103" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B102" s="13"/>
-      <c r="C102" s="13"/>
-      <c r="D102" s="13"/>
-    </row>
-    <row r="103" spans="1:4">
-      <c r="A103" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C103" s="4">
-        <v>33858</v>
-      </c>
-      <c r="D103" s="4">
-        <f t="shared" ref="D103:D162" si="2">IF(B103 &gt;  0,C103-B103, 0)</f>
-        <v>0</v>
-      </c>
+      <c r="B103" s="13"/>
+      <c r="C103" s="13"/>
+      <c r="D103" s="13"/>
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="B104" s="4">
+        <v>42470</v>
+      </c>
+      <c r="C104" s="4">
+        <v>33858</v>
       </c>
       <c r="D104" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" ref="D104:D163" si="2">IF(B104 &gt;  0,C104-B104, 0)</f>
+        <v>-8612</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -1963,9 +1978,6 @@
       <c r="A107" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C107" s="4">
-        <v>3</v>
-      </c>
       <c r="D107" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1973,7 +1985,10 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="C108" s="4">
+        <v>3</v>
       </c>
       <c r="D108" s="4">
         <f t="shared" si="2"/>
@@ -1982,7 +1997,7 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D109" s="4">
         <f t="shared" si="2"/>
@@ -1991,10 +2006,7 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C110" s="4">
-        <v>35512</v>
+        <v>47</v>
       </c>
       <c r="D110" s="4">
         <f t="shared" si="2"/>
@@ -2003,10 +2015,10 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="4" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="C111" s="4">
-        <v>35693</v>
+        <v>35512</v>
       </c>
       <c r="D111" s="4">
         <f t="shared" si="2"/>
@@ -2018,7 +2030,7 @@
         <v>6</v>
       </c>
       <c r="C112" s="4">
-        <v>35847</v>
+        <v>35693</v>
       </c>
       <c r="D112" s="4">
         <f t="shared" si="2"/>
@@ -2030,7 +2042,7 @@
         <v>6</v>
       </c>
       <c r="C113" s="4">
-        <v>36020</v>
+        <v>35847</v>
       </c>
       <c r="D113" s="4">
         <f t="shared" si="2"/>
@@ -2041,6 +2053,9 @@
       <c r="A114" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="C114" s="4">
+        <v>36020</v>
+      </c>
       <c r="D114" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2075,10 +2090,7 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C118" s="4">
-        <v>38056</v>
+        <v>6</v>
       </c>
       <c r="D118" s="4">
         <f t="shared" si="2"/>
@@ -2087,10 +2099,10 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="4" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C119" s="4">
-        <v>38245</v>
+        <v>38056</v>
       </c>
       <c r="D119" s="4">
         <f t="shared" si="2"/>
@@ -2099,10 +2111,10 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="4" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="C120" s="4">
-        <v>38420</v>
+        <v>38245</v>
       </c>
       <c r="D120" s="4">
         <f t="shared" si="2"/>
@@ -2114,7 +2126,7 @@
         <v>19</v>
       </c>
       <c r="C121" s="4">
-        <v>38758</v>
+        <v>38420</v>
       </c>
       <c r="D121" s="4">
         <f t="shared" si="2"/>
@@ -2123,10 +2135,10 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="4" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C122" s="4">
-        <v>38859</v>
+        <v>38758</v>
       </c>
       <c r="D122" s="4">
         <f t="shared" si="2"/>
@@ -2135,42 +2147,42 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C123" s="4">
+        <v>38859</v>
+      </c>
+      <c r="D123" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
+      <c r="A124" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C123" s="4">
+      <c r="C124" s="4">
         <v>39062</v>
       </c>
-      <c r="D123" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" ht="18.75">
-      <c r="A124" s="11" t="s">
+      <c r="D124" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" ht="18.75">
+      <c r="A125" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B124" s="11"/>
-      <c r="C124" s="11"/>
-      <c r="D124" s="11"/>
-    </row>
-    <row r="125" spans="1:4">
-      <c r="A125" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C125" s="4">
-        <v>39312</v>
-      </c>
-      <c r="D125" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
+      <c r="B125" s="11"/>
+      <c r="C125" s="11"/>
+      <c r="D125" s="11"/>
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="4" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="C126" s="4">
-        <v>40069</v>
+        <v>39312</v>
       </c>
       <c r="D126" s="4">
         <f t="shared" si="2"/>
@@ -2182,7 +2194,7 @@
         <v>19</v>
       </c>
       <c r="C127" s="4">
-        <v>40681</v>
+        <v>40069</v>
       </c>
       <c r="D127" s="4">
         <f t="shared" si="2"/>
@@ -2194,7 +2206,7 @@
         <v>19</v>
       </c>
       <c r="C128" s="4">
-        <v>41240</v>
+        <v>40681</v>
       </c>
       <c r="D128" s="4">
         <f t="shared" si="2"/>
@@ -2203,37 +2215,37 @@
     </row>
     <row r="129" spans="1:5">
       <c r="A129" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C129" s="4">
-        <v>41469</v>
+        <v>41240</v>
       </c>
       <c r="D129" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
-      </c>
-      <c r="E129" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="130" spans="1:5">
       <c r="A130" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C130" s="4">
-        <v>41728</v>
+        <v>41469</v>
       </c>
       <c r="D130" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
+      </c>
+      <c r="E130" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="131" spans="1:5">
       <c r="A131" s="4" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C131" s="4">
-        <v>42015</v>
+        <v>41728</v>
       </c>
       <c r="D131" s="4">
         <f t="shared" si="2"/>
@@ -2242,42 +2254,42 @@
     </row>
     <row r="132" spans="1:5">
       <c r="A132" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C132" s="4">
+        <v>42015</v>
+      </c>
+      <c r="D132" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5">
+      <c r="A133" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C132" s="4">
+      <c r="C133" s="4">
         <v>42219</v>
       </c>
-      <c r="D132" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" ht="18.75">
-      <c r="A133" s="13" t="s">
+      <c r="D133" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" ht="18.75">
+      <c r="A134" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="B133" s="13"/>
-      <c r="C133" s="13"/>
-      <c r="D133" s="13"/>
-    </row>
-    <row r="134" spans="1:5">
-      <c r="A134" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C134" s="4">
-        <v>42469</v>
-      </c>
-      <c r="D134" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
+      <c r="B134" s="13"/>
+      <c r="C134" s="13"/>
+      <c r="D134" s="13"/>
     </row>
     <row r="135" spans="1:5">
       <c r="A135" s="4" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="C135" s="4">
-        <v>43196</v>
+        <v>42469</v>
       </c>
       <c r="D135" s="4">
         <f t="shared" si="2"/>
@@ -2286,10 +2298,10 @@
     </row>
     <row r="136" spans="1:5">
       <c r="A136" s="4" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="C136" s="4">
-        <v>43848</v>
+        <v>43196</v>
       </c>
       <c r="D136" s="4">
         <f t="shared" si="2"/>
@@ -2298,10 +2310,10 @@
     </row>
     <row r="137" spans="1:5">
       <c r="A137" s="4" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="C137" s="4">
-        <v>44155</v>
+        <v>43848</v>
       </c>
       <c r="D137" s="4">
         <f t="shared" si="2"/>
@@ -2310,10 +2322,10 @@
     </row>
     <row r="138" spans="1:5">
       <c r="A138" s="4" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="C138" s="4">
-        <v>46549</v>
+        <v>44155</v>
       </c>
       <c r="D138" s="4">
         <f t="shared" si="2"/>
@@ -2322,10 +2334,10 @@
     </row>
     <row r="139" spans="1:5">
       <c r="A139" s="4" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="C139" s="4">
-        <v>46905</v>
+        <v>46549</v>
       </c>
       <c r="D139" s="4">
         <f t="shared" si="2"/>
@@ -2334,42 +2346,42 @@
     </row>
     <row r="140" spans="1:5">
       <c r="A140" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C140" s="4">
+        <v>46905</v>
+      </c>
+      <c r="D140" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5">
+      <c r="A141" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C140" s="4">
+      <c r="C141" s="4">
         <v>47108</v>
       </c>
-      <c r="D140" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" ht="18.75">
-      <c r="A141" s="11" t="s">
+      <c r="D141" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" ht="18.75">
+      <c r="A142" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B141" s="11"/>
-      <c r="C141" s="11"/>
-      <c r="D141" s="11"/>
-    </row>
-    <row r="142" spans="1:5">
-      <c r="A142" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C142" s="4">
-        <v>47359</v>
-      </c>
-      <c r="D142" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
+      <c r="B142" s="11"/>
+      <c r="C142" s="11"/>
+      <c r="D142" s="11"/>
     </row>
     <row r="143" spans="1:5">
       <c r="A143" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C143" s="4">
-        <v>47668</v>
+        <v>47359</v>
       </c>
       <c r="D143" s="4">
         <f t="shared" si="2"/>
@@ -2378,10 +2390,10 @@
     </row>
     <row r="144" spans="1:5">
       <c r="A144" s="4" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="C144" s="4">
-        <v>47847</v>
+        <v>47668</v>
       </c>
       <c r="D144" s="4">
         <f t="shared" si="2"/>
@@ -2390,10 +2402,10 @@
     </row>
     <row r="145" spans="1:5">
       <c r="A145" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C145" s="4">
-        <v>48052</v>
+        <v>47847</v>
       </c>
       <c r="D145" s="4">
         <f t="shared" si="2"/>
@@ -2402,10 +2414,10 @@
     </row>
     <row r="146" spans="1:5">
       <c r="A146" s="4" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C146" s="4">
-        <v>48226</v>
+        <v>48052</v>
       </c>
       <c r="D146" s="4">
         <f t="shared" si="2"/>
@@ -2414,10 +2426,10 @@
     </row>
     <row r="147" spans="1:5">
       <c r="A147" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C147" s="4">
-        <v>48530</v>
+        <v>48226</v>
       </c>
       <c r="D147" s="4">
         <f t="shared" si="2"/>
@@ -2426,37 +2438,37 @@
     </row>
     <row r="148" spans="1:5">
       <c r="A148" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C148" s="4">
-        <v>48705</v>
+        <v>48530</v>
       </c>
       <c r="D148" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
-      </c>
-      <c r="E148" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="149" spans="1:5">
       <c r="A149" s="4" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C149" s="4">
-        <v>48820</v>
+        <v>48705</v>
       </c>
       <c r="D149" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
+      </c>
+      <c r="E149" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="150" spans="1:5">
       <c r="A150" s="4" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="C150" s="4">
-        <v>49147</v>
+        <v>48820</v>
       </c>
       <c r="D150" s="4">
         <f t="shared" si="2"/>
@@ -2465,17 +2477,14 @@
     </row>
     <row r="151" spans="1:5">
       <c r="A151" s="4" t="s">
-        <v>6</v>
+        <v>57</v>
       </c>
       <c r="C151" s="4">
-        <v>49319</v>
+        <v>49147</v>
       </c>
       <c r="D151" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
-      </c>
-      <c r="E151" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="152" spans="1:5">
@@ -2483,19 +2492,22 @@
         <v>6</v>
       </c>
       <c r="C152" s="4">
-        <v>49569</v>
+        <v>49319</v>
       </c>
       <c r="D152" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
+      </c>
+      <c r="E152" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="153" spans="1:5">
       <c r="A153" s="4" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="C153" s="4">
-        <v>49860</v>
+        <v>49569</v>
       </c>
       <c r="D153" s="4">
         <f t="shared" si="2"/>
@@ -2504,42 +2516,42 @@
     </row>
     <row r="154" spans="1:5">
       <c r="A154" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C154" s="4">
+        <v>49860</v>
+      </c>
+      <c r="D154" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5">
+      <c r="A155" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C154" s="4">
+      <c r="C155" s="4">
         <v>50063</v>
       </c>
-      <c r="D154" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5" ht="18.75">
-      <c r="A155" s="13" t="s">
+      <c r="D155" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" ht="18.75">
+      <c r="A156" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="B155" s="13"/>
-      <c r="C155" s="13"/>
-      <c r="D155" s="13"/>
-    </row>
-    <row r="156" spans="1:5">
-      <c r="A156" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C156" s="4">
-        <v>50314</v>
-      </c>
-      <c r="D156" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
+      <c r="B156" s="13"/>
+      <c r="C156" s="13"/>
+      <c r="D156" s="13"/>
     </row>
     <row r="157" spans="1:5">
       <c r="A157" s="4" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="C157" s="4">
-        <v>51237</v>
+        <v>50314</v>
       </c>
       <c r="D157" s="4">
         <f t="shared" si="2"/>
@@ -2548,10 +2560,10 @@
     </row>
     <row r="158" spans="1:5">
       <c r="A158" s="4" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="C158" s="4">
-        <v>53055</v>
+        <v>51237</v>
       </c>
       <c r="D158" s="4">
         <f t="shared" si="2"/>
@@ -2560,10 +2572,10 @@
     </row>
     <row r="159" spans="1:5">
       <c r="A159" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C159" s="4">
-        <v>53377</v>
+        <v>53055</v>
       </c>
       <c r="D159" s="4">
         <f t="shared" si="2"/>
@@ -2572,10 +2584,10 @@
     </row>
     <row r="160" spans="1:5">
       <c r="A160" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C160" s="4">
-        <v>53698</v>
+        <v>53377</v>
       </c>
       <c r="D160" s="4">
         <f t="shared" si="2"/>
@@ -2584,10 +2596,10 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C161" s="4">
-        <v>54021</v>
+        <v>53698</v>
       </c>
       <c r="D161" s="4">
         <f t="shared" si="2"/>
@@ -2596,10 +2608,10 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C162" s="4">
-        <v>56284</v>
+        <v>54021</v>
       </c>
       <c r="D162" s="4">
         <f t="shared" si="2"/>
@@ -2608,27 +2620,39 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C163" s="4">
+        <v>56284</v>
+      </c>
+      <c r="D163" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4">
+      <c r="A164" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B163" s="9"/>
-      <c r="C163" s="9">
+      <c r="B164" s="9"/>
+      <c r="C164" s="9">
         <v>0.68541666666666667</v>
       </c>
-      <c r="D163" s="9">
+      <c r="D164" s="9">
         <v>2.7083333333333334E-2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A133:D133"/>
-    <mergeCell ref="A141:D141"/>
-    <mergeCell ref="A155:D155"/>
+    <mergeCell ref="A134:D134"/>
+    <mergeCell ref="A142:D142"/>
+    <mergeCell ref="A156:D156"/>
     <mergeCell ref="A63:D63"/>
     <mergeCell ref="A76:D76"/>
     <mergeCell ref="A88:D88"/>
     <mergeCell ref="A97:D97"/>
-    <mergeCell ref="A102:D102"/>
-    <mergeCell ref="A124:D124"/>
+    <mergeCell ref="A103:D103"/>
+    <mergeCell ref="A125:D125"/>
     <mergeCell ref="A55:D55"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A7:D7"/>

</xml_diff>

<commit_message>
Wario 100% - got treasure, about to get key, it must cost 1 900ish frame rule.
</commit_message>
<xml_diff>
--- a/Wario/Wario.xlsx
+++ b/Wario/Wario.xlsx
@@ -358,9 +358,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -658,8 +658,8 @@
   <dimension ref="A1:J164"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B105" sqref="B105"/>
+      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B119" sqref="B119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -683,12 +683,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -716,12 +716,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -791,12 +791,12 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="18.75">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="4" t="s">
@@ -967,12 +967,12 @@
       </c>
     </row>
     <row r="30" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A30" s="11" t="s">
+      <c r="A30" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="4" t="s">
@@ -1148,12 +1148,12 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="18.75">
-      <c r="A43" s="13" t="s">
+      <c r="A43" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B43" s="13"/>
-      <c r="C43" s="13"/>
-      <c r="D43" s="13"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="4" t="s">
@@ -1300,12 +1300,12 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="18.75">
-      <c r="A55" s="11" t="s">
+      <c r="A55" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B55" s="11"/>
-      <c r="C55" s="11"/>
-      <c r="D55" s="11"/>
+      <c r="B55" s="12"/>
+      <c r="C55" s="12"/>
+      <c r="D55" s="12"/>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="4" t="s">
@@ -1396,12 +1396,12 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="18.75">
-      <c r="A63" s="13" t="s">
+      <c r="A63" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B63" s="13"/>
-      <c r="C63" s="13"/>
-      <c r="D63" s="13"/>
+      <c r="B63" s="11"/>
+      <c r="C63" s="11"/>
+      <c r="D63" s="11"/>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="4" t="s">
@@ -1587,12 +1587,12 @@
       </c>
     </row>
     <row r="76" spans="1:10" ht="18.75">
-      <c r="A76" s="11" t="s">
+      <c r="A76" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B76" s="11"/>
-      <c r="C76" s="11"/>
-      <c r="D76" s="11"/>
+      <c r="B76" s="12"/>
+      <c r="C76" s="12"/>
+      <c r="D76" s="12"/>
     </row>
     <row r="77" spans="1:10">
       <c r="A77" s="4" t="s">
@@ -1739,12 +1739,12 @@
       </c>
     </row>
     <row r="88" spans="1:4" ht="18.75">
-      <c r="A88" s="13" t="s">
+      <c r="A88" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B88" s="13"/>
-      <c r="C88" s="13"/>
-      <c r="D88" s="13"/>
+      <c r="B88" s="11"/>
+      <c r="C88" s="11"/>
+      <c r="D88" s="11"/>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="4" t="s">
@@ -1857,12 +1857,12 @@
       </c>
     </row>
     <row r="97" spans="1:4" ht="18.75">
-      <c r="A97" s="11" t="s">
+      <c r="A97" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B97" s="11"/>
-      <c r="C97" s="11"/>
-      <c r="D97" s="11"/>
+      <c r="B97" s="12"/>
+      <c r="C97" s="12"/>
+      <c r="D97" s="12"/>
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="4" t="s">
@@ -1934,12 +1934,12 @@
       </c>
     </row>
     <row r="103" spans="1:4" ht="18.75">
-      <c r="A103" s="13" t="s">
+      <c r="A103" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B103" s="13"/>
-      <c r="C103" s="13"/>
-      <c r="D103" s="13"/>
+      <c r="B103" s="11"/>
+      <c r="C103" s="11"/>
+      <c r="D103" s="11"/>
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="4" t="s">
@@ -2083,30 +2083,39 @@
       <c r="A117" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="B117" s="4">
+        <v>46481</v>
+      </c>
       <c r="D117" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-46481</v>
       </c>
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="B118" s="4">
+        <v>46656</v>
+      </c>
       <c r="D118" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-46656</v>
       </c>
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="B119" s="4">
+        <v>47301</v>
+      </c>
       <c r="C119" s="4">
         <v>38056</v>
       </c>
       <c r="D119" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-9245</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -2170,12 +2179,12 @@
       </c>
     </row>
     <row r="125" spans="1:4" ht="18.75">
-      <c r="A125" s="11" t="s">
+      <c r="A125" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B125" s="11"/>
-      <c r="C125" s="11"/>
-      <c r="D125" s="11"/>
+      <c r="B125" s="12"/>
+      <c r="C125" s="12"/>
+      <c r="D125" s="12"/>
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="4" t="s">
@@ -2277,12 +2286,12 @@
       </c>
     </row>
     <row r="134" spans="1:5" ht="18.75">
-      <c r="A134" s="13" t="s">
+      <c r="A134" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B134" s="13"/>
-      <c r="C134" s="13"/>
-      <c r="D134" s="13"/>
+      <c r="B134" s="11"/>
+      <c r="C134" s="11"/>
+      <c r="D134" s="11"/>
     </row>
     <row r="135" spans="1:5">
       <c r="A135" s="4" t="s">
@@ -2369,12 +2378,12 @@
       </c>
     </row>
     <row r="142" spans="1:5" ht="18.75">
-      <c r="A142" s="11" t="s">
+      <c r="A142" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B142" s="11"/>
-      <c r="C142" s="11"/>
-      <c r="D142" s="11"/>
+      <c r="B142" s="12"/>
+      <c r="C142" s="12"/>
+      <c r="D142" s="12"/>
     </row>
     <row r="143" spans="1:5">
       <c r="A143" s="4" t="s">
@@ -2539,12 +2548,12 @@
       </c>
     </row>
     <row r="156" spans="1:5" ht="18.75">
-      <c r="A156" s="13" t="s">
+      <c r="A156" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="B156" s="13"/>
-      <c r="C156" s="13"/>
-      <c r="D156" s="13"/>
+      <c r="B156" s="11"/>
+      <c r="C156" s="11"/>
+      <c r="D156" s="11"/>
     </row>
     <row r="157" spans="1:5">
       <c r="A157" s="4" t="s">
@@ -2644,6 +2653,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A55:D55"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A43:D43"/>
     <mergeCell ref="A134:D134"/>
     <mergeCell ref="A142:D142"/>
     <mergeCell ref="A156:D156"/>
@@ -2653,12 +2668,6 @@
     <mergeCell ref="A97:D97"/>
     <mergeCell ref="A103:D103"/>
     <mergeCell ref="A125:D125"/>
-    <mergeCell ref="A55:D55"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A43:D43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -2695,12 +2704,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -2728,12 +2737,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -2767,12 +2776,12 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
@@ -2895,12 +2904,12 @@
       </c>
     </row>
     <row r="19" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="4" t="s">
@@ -3068,12 +3077,12 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="18.75">
-      <c r="A31" s="13" t="s">
+      <c r="A31" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="4" t="s">
@@ -3241,12 +3250,12 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="18.75">
-      <c r="A43" s="11" t="s">
+      <c r="A43" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B43" s="11"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="4" t="s">
@@ -3354,12 +3363,12 @@
       </c>
     </row>
     <row r="51" spans="1:10" ht="18.75">
-      <c r="A51" s="13" t="s">
+      <c r="A51" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B51" s="13"/>
-      <c r="C51" s="13"/>
-      <c r="D51" s="13"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="4" t="s">
@@ -3545,12 +3554,12 @@
       </c>
     </row>
     <row r="64" spans="1:10" ht="18.75">
-      <c r="A64" s="11" t="s">
+      <c r="A64" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B64" s="11"/>
-      <c r="C64" s="11"/>
-      <c r="D64" s="11"/>
+      <c r="B64" s="12"/>
+      <c r="C64" s="12"/>
+      <c r="D64" s="12"/>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="4" t="s">
@@ -3709,12 +3718,12 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="18.75">
-      <c r="A76" s="13" t="s">
+      <c r="A76" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B76" s="13"/>
-      <c r="C76" s="13"/>
-      <c r="D76" s="13"/>
+      <c r="B76" s="11"/>
+      <c r="C76" s="11"/>
+      <c r="D76" s="11"/>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="4" t="s">
@@ -3827,12 +3836,12 @@
       </c>
     </row>
     <row r="85" spans="1:4" ht="18.75">
-      <c r="A85" s="11" t="s">
+      <c r="A85" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B85" s="11"/>
-      <c r="C85" s="11"/>
-      <c r="D85" s="11"/>
+      <c r="B85" s="12"/>
+      <c r="C85" s="12"/>
+      <c r="D85" s="12"/>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="4" t="s">
@@ -3892,12 +3901,12 @@
       </c>
     </row>
     <row r="90" spans="1:4" ht="18.75">
-      <c r="A90" s="13" t="s">
+      <c r="A90" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B90" s="13"/>
-      <c r="C90" s="13"/>
-      <c r="D90" s="13"/>
+      <c r="B90" s="11"/>
+      <c r="C90" s="11"/>
+      <c r="D90" s="11"/>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="4" t="s">
@@ -4188,12 +4197,12 @@
       </c>
     </row>
     <row r="112" spans="1:4" ht="18.75">
-      <c r="A112" s="11" t="s">
+      <c r="A112" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B112" s="11"/>
-      <c r="C112" s="11"/>
-      <c r="D112" s="11"/>
+      <c r="B112" s="12"/>
+      <c r="C112" s="12"/>
+      <c r="D112" s="12"/>
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="4" t="s">
@@ -4319,12 +4328,12 @@
       </c>
     </row>
     <row r="121" spans="1:5" ht="18.75">
-      <c r="A121" s="13" t="s">
+      <c r="A121" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B121" s="13"/>
-      <c r="C121" s="13"/>
-      <c r="D121" s="13"/>
+      <c r="B121" s="11"/>
+      <c r="C121" s="11"/>
+      <c r="D121" s="11"/>
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="4" t="s">
@@ -4432,12 +4441,12 @@
       </c>
     </row>
     <row r="129" spans="1:5" ht="18.75">
-      <c r="A129" s="11" t="s">
+      <c r="A129" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B129" s="11"/>
-      <c r="C129" s="11"/>
-      <c r="D129" s="11"/>
+      <c r="B129" s="12"/>
+      <c r="C129" s="12"/>
+      <c r="D129" s="12"/>
     </row>
     <row r="130" spans="1:5">
       <c r="A130" s="4" t="s">
@@ -4641,12 +4650,12 @@
       </c>
     </row>
     <row r="143" spans="1:5" ht="18.75">
-      <c r="A143" s="13" t="s">
+      <c r="A143" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="B143" s="13"/>
-      <c r="C143" s="13"/>
-      <c r="D143" s="13"/>
+      <c r="B143" s="11"/>
+      <c r="C143" s="11"/>
+      <c r="D143" s="11"/>
     </row>
     <row r="144" spans="1:5">
       <c r="A144" s="4" t="s">
@@ -4775,12 +4784,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A31:D31"/>
     <mergeCell ref="A121:D121"/>
     <mergeCell ref="A129:D129"/>
     <mergeCell ref="A143:D143"/>
@@ -4790,6 +4793,12 @@
     <mergeCell ref="A85:D85"/>
     <mergeCell ref="A90:D90"/>
     <mergeCell ref="A112:D112"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A31:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -4826,12 +4835,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -4859,12 +4868,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -4898,12 +4907,12 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
@@ -4987,12 +4996,12 @@
       </c>
     </row>
     <row r="17" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="4" t="s">
@@ -5160,12 +5169,12 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="18.75">
-      <c r="A29" s="13" t="s">
+      <c r="A29" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="4" t="s">
@@ -5243,12 +5252,12 @@
       </c>
     </row>
     <row r="35" spans="1:10" ht="18.75">
-      <c r="A35" s="11" t="s">
+      <c r="A35" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="4" t="s">
@@ -5341,12 +5350,12 @@
       </c>
     </row>
     <row r="42" spans="1:10" ht="18.75">
-      <c r="A42" s="13" t="s">
+      <c r="A42" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B42" s="13"/>
-      <c r="C42" s="13"/>
-      <c r="D42" s="13"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="4" t="s">
@@ -5535,12 +5544,12 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="18.75">
-      <c r="A55" s="11" t="s">
+      <c r="A55" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B55" s="11"/>
-      <c r="C55" s="11"/>
-      <c r="D55" s="11"/>
+      <c r="B55" s="12"/>
+      <c r="C55" s="12"/>
+      <c r="D55" s="12"/>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="4" t="s">
@@ -5693,12 +5702,12 @@
       </c>
     </row>
     <row r="66" spans="1:4" ht="18.75">
-      <c r="A66" s="13" t="s">
+      <c r="A66" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B66" s="13"/>
-      <c r="C66" s="13"/>
-      <c r="D66" s="13"/>
+      <c r="B66" s="11"/>
+      <c r="C66" s="11"/>
+      <c r="D66" s="11"/>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="4" t="s">
@@ -5761,12 +5770,12 @@
       </c>
     </row>
     <row r="71" spans="1:4" ht="18.75">
-      <c r="A71" s="11" t="s">
+      <c r="A71" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B71" s="11"/>
-      <c r="C71" s="11"/>
-      <c r="D71" s="11"/>
+      <c r="B71" s="12"/>
+      <c r="C71" s="12"/>
+      <c r="D71" s="12"/>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="4" t="s">
@@ -5829,12 +5838,12 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="18.75">
-      <c r="A76" s="13" t="s">
+      <c r="A76" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B76" s="13"/>
-      <c r="C76" s="13"/>
-      <c r="D76" s="13"/>
+      <c r="B76" s="11"/>
+      <c r="C76" s="11"/>
+      <c r="D76" s="11"/>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="4" t="s">
@@ -6152,12 +6161,12 @@
       </c>
     </row>
     <row r="98" spans="1:5" ht="18.75">
-      <c r="A98" s="11" t="s">
+      <c r="A98" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B98" s="11"/>
-      <c r="C98" s="11"/>
-      <c r="D98" s="11"/>
+      <c r="B98" s="12"/>
+      <c r="C98" s="12"/>
+      <c r="D98" s="12"/>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="4" t="s">
@@ -6283,12 +6292,12 @@
       </c>
     </row>
     <row r="107" spans="1:5" ht="18.75">
-      <c r="A107" s="13" t="s">
+      <c r="A107" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B107" s="13"/>
-      <c r="C107" s="13"/>
-      <c r="D107" s="13"/>
+      <c r="B107" s="11"/>
+      <c r="C107" s="11"/>
+      <c r="D107" s="11"/>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="4" t="s">
@@ -6366,12 +6375,12 @@
       </c>
     </row>
     <row r="113" spans="1:4" ht="18.75">
-      <c r="A113" s="11" t="s">
+      <c r="A113" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B113" s="11"/>
-      <c r="C113" s="11"/>
-      <c r="D113" s="11"/>
+      <c r="B113" s="12"/>
+      <c r="C113" s="12"/>
+      <c r="D113" s="12"/>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="4" t="s">
@@ -6569,12 +6578,12 @@
       </c>
     </row>
     <row r="127" spans="1:4" ht="18.75">
-      <c r="A127" s="13" t="s">
+      <c r="A127" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="B127" s="13"/>
-      <c r="C127" s="13"/>
-      <c r="D127" s="13"/>
+      <c r="B127" s="11"/>
+      <c r="C127" s="11"/>
+      <c r="D127" s="11"/>
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="4" t="s">
@@ -6694,6 +6703,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A29:D29"/>
     <mergeCell ref="A127:D127"/>
     <mergeCell ref="A107:D107"/>
     <mergeCell ref="A113:D113"/>
@@ -6704,11 +6718,6 @@
     <mergeCell ref="A98:D98"/>
     <mergeCell ref="A66:D66"/>
     <mergeCell ref="A55:D55"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A29:D29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>

</xml_diff>

<commit_message>
Wario 100% - get key, restore eagle+bull wario
</commit_message>
<xml_diff>
--- a/Wario/Wario.xlsx
+++ b/Wario/Wario.xlsx
@@ -358,9 +358,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -658,8 +658,8 @@
   <dimension ref="A1:J164"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B119" sqref="B119"/>
+      <pane ySplit="1" topLeftCell="A102" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B122" sqref="B122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -683,12 +683,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -716,12 +716,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -791,12 +791,12 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="18.75">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="4" t="s">
@@ -967,12 +967,12 @@
       </c>
     </row>
     <row r="30" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A30" s="12" t="s">
+      <c r="A30" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="4" t="s">
@@ -1148,12 +1148,12 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="18.75">
-      <c r="A43" s="11" t="s">
+      <c r="A43" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B43" s="11"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="4" t="s">
@@ -1300,12 +1300,12 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="18.75">
-      <c r="A55" s="12" t="s">
+      <c r="A55" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B55" s="12"/>
-      <c r="C55" s="12"/>
-      <c r="D55" s="12"/>
+      <c r="B55" s="11"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="11"/>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="4" t="s">
@@ -1396,12 +1396,12 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="18.75">
-      <c r="A63" s="11" t="s">
+      <c r="A63" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B63" s="11"/>
-      <c r="C63" s="11"/>
-      <c r="D63" s="11"/>
+      <c r="B63" s="13"/>
+      <c r="C63" s="13"/>
+      <c r="D63" s="13"/>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="4" t="s">
@@ -1587,12 +1587,12 @@
       </c>
     </row>
     <row r="76" spans="1:10" ht="18.75">
-      <c r="A76" s="12" t="s">
+      <c r="A76" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B76" s="12"/>
-      <c r="C76" s="12"/>
-      <c r="D76" s="12"/>
+      <c r="B76" s="11"/>
+      <c r="C76" s="11"/>
+      <c r="D76" s="11"/>
     </row>
     <row r="77" spans="1:10">
       <c r="A77" s="4" t="s">
@@ -1739,12 +1739,12 @@
       </c>
     </row>
     <row r="88" spans="1:4" ht="18.75">
-      <c r="A88" s="11" t="s">
+      <c r="A88" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B88" s="11"/>
-      <c r="C88" s="11"/>
-      <c r="D88" s="11"/>
+      <c r="B88" s="13"/>
+      <c r="C88" s="13"/>
+      <c r="D88" s="13"/>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="4" t="s">
@@ -1857,12 +1857,12 @@
       </c>
     </row>
     <row r="97" spans="1:4" ht="18.75">
-      <c r="A97" s="12" t="s">
+      <c r="A97" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B97" s="12"/>
-      <c r="C97" s="12"/>
-      <c r="D97" s="12"/>
+      <c r="B97" s="11"/>
+      <c r="C97" s="11"/>
+      <c r="D97" s="11"/>
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="4" t="s">
@@ -1934,12 +1934,12 @@
       </c>
     </row>
     <row r="103" spans="1:4" ht="18.75">
-      <c r="A103" s="11" t="s">
+      <c r="A103" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B103" s="11"/>
-      <c r="C103" s="11"/>
-      <c r="D103" s="11"/>
+      <c r="B103" s="13"/>
+      <c r="C103" s="13"/>
+      <c r="D103" s="13"/>
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="4" t="s">
@@ -2108,38 +2108,44 @@
         <v>20</v>
       </c>
       <c r="B119" s="4">
-        <v>47301</v>
+        <v>47106</v>
       </c>
       <c r="C119" s="4">
         <v>38056</v>
       </c>
       <c r="D119" s="4">
         <f t="shared" si="2"/>
-        <v>-9245</v>
+        <v>-9050</v>
       </c>
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="B120" s="4">
+        <v>47306</v>
+      </c>
       <c r="C120" s="4">
         <v>38245</v>
       </c>
       <c r="D120" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-9061</v>
       </c>
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="B121" s="4">
+        <v>47968</v>
+      </c>
       <c r="C121" s="4">
         <v>38420</v>
       </c>
       <c r="D121" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-9548</v>
       </c>
     </row>
     <row r="122" spans="1:4">
@@ -2179,12 +2185,12 @@
       </c>
     </row>
     <row r="125" spans="1:4" ht="18.75">
-      <c r="A125" s="12" t="s">
+      <c r="A125" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B125" s="12"/>
-      <c r="C125" s="12"/>
-      <c r="D125" s="12"/>
+      <c r="B125" s="11"/>
+      <c r="C125" s="11"/>
+      <c r="D125" s="11"/>
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="4" t="s">
@@ -2286,12 +2292,12 @@
       </c>
     </row>
     <row r="134" spans="1:5" ht="18.75">
-      <c r="A134" s="11" t="s">
+      <c r="A134" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="B134" s="11"/>
-      <c r="C134" s="11"/>
-      <c r="D134" s="11"/>
+      <c r="B134" s="13"/>
+      <c r="C134" s="13"/>
+      <c r="D134" s="13"/>
     </row>
     <row r="135" spans="1:5">
       <c r="A135" s="4" t="s">
@@ -2378,12 +2384,12 @@
       </c>
     </row>
     <row r="142" spans="1:5" ht="18.75">
-      <c r="A142" s="12" t="s">
+      <c r="A142" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B142" s="12"/>
-      <c r="C142" s="12"/>
-      <c r="D142" s="12"/>
+      <c r="B142" s="11"/>
+      <c r="C142" s="11"/>
+      <c r="D142" s="11"/>
     </row>
     <row r="143" spans="1:5">
       <c r="A143" s="4" t="s">
@@ -2548,12 +2554,12 @@
       </c>
     </row>
     <row r="156" spans="1:5" ht="18.75">
-      <c r="A156" s="11" t="s">
+      <c r="A156" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="B156" s="11"/>
-      <c r="C156" s="11"/>
-      <c r="D156" s="11"/>
+      <c r="B156" s="13"/>
+      <c r="C156" s="13"/>
+      <c r="D156" s="13"/>
     </row>
     <row r="157" spans="1:5">
       <c r="A157" s="4" t="s">
@@ -2653,12 +2659,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A55:D55"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A43:D43"/>
     <mergeCell ref="A134:D134"/>
     <mergeCell ref="A142:D142"/>
     <mergeCell ref="A156:D156"/>
@@ -2668,6 +2668,12 @@
     <mergeCell ref="A97:D97"/>
     <mergeCell ref="A103:D103"/>
     <mergeCell ref="A125:D125"/>
+    <mergeCell ref="A55:D55"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A43:D43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -2704,12 +2710,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -2737,12 +2743,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -2776,12 +2782,12 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
@@ -2904,12 +2910,12 @@
       </c>
     </row>
     <row r="19" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="4" t="s">
@@ -3077,12 +3083,12 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="18.75">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="4" t="s">
@@ -3250,12 +3256,12 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="18.75">
-      <c r="A43" s="12" t="s">
+      <c r="A43" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B43" s="12"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="4" t="s">
@@ -3363,12 +3369,12 @@
       </c>
     </row>
     <row r="51" spans="1:10" ht="18.75">
-      <c r="A51" s="11" t="s">
+      <c r="A51" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B51" s="11"/>
-      <c r="C51" s="11"/>
-      <c r="D51" s="11"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="13"/>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="4" t="s">
@@ -3554,12 +3560,12 @@
       </c>
     </row>
     <row r="64" spans="1:10" ht="18.75">
-      <c r="A64" s="12" t="s">
+      <c r="A64" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B64" s="12"/>
-      <c r="C64" s="12"/>
-      <c r="D64" s="12"/>
+      <c r="B64" s="11"/>
+      <c r="C64" s="11"/>
+      <c r="D64" s="11"/>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="4" t="s">
@@ -3718,12 +3724,12 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="18.75">
-      <c r="A76" s="11" t="s">
+      <c r="A76" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B76" s="11"/>
-      <c r="C76" s="11"/>
-      <c r="D76" s="11"/>
+      <c r="B76" s="13"/>
+      <c r="C76" s="13"/>
+      <c r="D76" s="13"/>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="4" t="s">
@@ -3836,12 +3842,12 @@
       </c>
     </row>
     <row r="85" spans="1:4" ht="18.75">
-      <c r="A85" s="12" t="s">
+      <c r="A85" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B85" s="12"/>
-      <c r="C85" s="12"/>
-      <c r="D85" s="12"/>
+      <c r="B85" s="11"/>
+      <c r="C85" s="11"/>
+      <c r="D85" s="11"/>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="4" t="s">
@@ -3901,12 +3907,12 @@
       </c>
     </row>
     <row r="90" spans="1:4" ht="18.75">
-      <c r="A90" s="11" t="s">
+      <c r="A90" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B90" s="11"/>
-      <c r="C90" s="11"/>
-      <c r="D90" s="11"/>
+      <c r="B90" s="13"/>
+      <c r="C90" s="13"/>
+      <c r="D90" s="13"/>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="4" t="s">
@@ -4197,12 +4203,12 @@
       </c>
     </row>
     <row r="112" spans="1:4" ht="18.75">
-      <c r="A112" s="12" t="s">
+      <c r="A112" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B112" s="12"/>
-      <c r="C112" s="12"/>
-      <c r="D112" s="12"/>
+      <c r="B112" s="11"/>
+      <c r="C112" s="11"/>
+      <c r="D112" s="11"/>
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="4" t="s">
@@ -4328,12 +4334,12 @@
       </c>
     </row>
     <row r="121" spans="1:5" ht="18.75">
-      <c r="A121" s="11" t="s">
+      <c r="A121" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="B121" s="11"/>
-      <c r="C121" s="11"/>
-      <c r="D121" s="11"/>
+      <c r="B121" s="13"/>
+      <c r="C121" s="13"/>
+      <c r="D121" s="13"/>
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="4" t="s">
@@ -4441,12 +4447,12 @@
       </c>
     </row>
     <row r="129" spans="1:5" ht="18.75">
-      <c r="A129" s="12" t="s">
+      <c r="A129" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B129" s="12"/>
-      <c r="C129" s="12"/>
-      <c r="D129" s="12"/>
+      <c r="B129" s="11"/>
+      <c r="C129" s="11"/>
+      <c r="D129" s="11"/>
     </row>
     <row r="130" spans="1:5">
       <c r="A130" s="4" t="s">
@@ -4650,12 +4656,12 @@
       </c>
     </row>
     <row r="143" spans="1:5" ht="18.75">
-      <c r="A143" s="11" t="s">
+      <c r="A143" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="B143" s="11"/>
-      <c r="C143" s="11"/>
-      <c r="D143" s="11"/>
+      <c r="B143" s="13"/>
+      <c r="C143" s="13"/>
+      <c r="D143" s="13"/>
     </row>
     <row r="144" spans="1:5">
       <c r="A144" s="4" t="s">
@@ -4784,6 +4790,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A31:D31"/>
     <mergeCell ref="A121:D121"/>
     <mergeCell ref="A129:D129"/>
     <mergeCell ref="A143:D143"/>
@@ -4793,12 +4805,6 @@
     <mergeCell ref="A85:D85"/>
     <mergeCell ref="A90:D90"/>
     <mergeCell ref="A112:D112"/>
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A31:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -4835,12 +4841,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -4868,12 +4874,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -4907,12 +4913,12 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
@@ -4996,12 +5002,12 @@
       </c>
     </row>
     <row r="17" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="4" t="s">
@@ -5169,12 +5175,12 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="18.75">
-      <c r="A29" s="11" t="s">
+      <c r="A29" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="4" t="s">
@@ -5252,12 +5258,12 @@
       </c>
     </row>
     <row r="35" spans="1:10" ht="18.75">
-      <c r="A35" s="12" t="s">
+      <c r="A35" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="12"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="4" t="s">
@@ -5350,12 +5356,12 @@
       </c>
     </row>
     <row r="42" spans="1:10" ht="18.75">
-      <c r="A42" s="11" t="s">
+      <c r="A42" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B42" s="11"/>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="4" t="s">
@@ -5544,12 +5550,12 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="18.75">
-      <c r="A55" s="12" t="s">
+      <c r="A55" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B55" s="12"/>
-      <c r="C55" s="12"/>
-      <c r="D55" s="12"/>
+      <c r="B55" s="11"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="11"/>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="4" t="s">
@@ -5702,12 +5708,12 @@
       </c>
     </row>
     <row r="66" spans="1:4" ht="18.75">
-      <c r="A66" s="11" t="s">
+      <c r="A66" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B66" s="11"/>
-      <c r="C66" s="11"/>
-      <c r="D66" s="11"/>
+      <c r="B66" s="13"/>
+      <c r="C66" s="13"/>
+      <c r="D66" s="13"/>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="4" t="s">
@@ -5770,12 +5776,12 @@
       </c>
     </row>
     <row r="71" spans="1:4" ht="18.75">
-      <c r="A71" s="12" t="s">
+      <c r="A71" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B71" s="12"/>
-      <c r="C71" s="12"/>
-      <c r="D71" s="12"/>
+      <c r="B71" s="11"/>
+      <c r="C71" s="11"/>
+      <c r="D71" s="11"/>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="4" t="s">
@@ -5838,12 +5844,12 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="18.75">
-      <c r="A76" s="11" t="s">
+      <c r="A76" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B76" s="11"/>
-      <c r="C76" s="11"/>
-      <c r="D76" s="11"/>
+      <c r="B76" s="13"/>
+      <c r="C76" s="13"/>
+      <c r="D76" s="13"/>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="4" t="s">
@@ -6161,12 +6167,12 @@
       </c>
     </row>
     <row r="98" spans="1:5" ht="18.75">
-      <c r="A98" s="12" t="s">
+      <c r="A98" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B98" s="12"/>
-      <c r="C98" s="12"/>
-      <c r="D98" s="12"/>
+      <c r="B98" s="11"/>
+      <c r="C98" s="11"/>
+      <c r="D98" s="11"/>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="4" t="s">
@@ -6292,12 +6298,12 @@
       </c>
     </row>
     <row r="107" spans="1:5" ht="18.75">
-      <c r="A107" s="11" t="s">
+      <c r="A107" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="B107" s="11"/>
-      <c r="C107" s="11"/>
-      <c r="D107" s="11"/>
+      <c r="B107" s="13"/>
+      <c r="C107" s="13"/>
+      <c r="D107" s="13"/>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="4" t="s">
@@ -6375,12 +6381,12 @@
       </c>
     </row>
     <row r="113" spans="1:4" ht="18.75">
-      <c r="A113" s="12" t="s">
+      <c r="A113" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B113" s="12"/>
-      <c r="C113" s="12"/>
-      <c r="D113" s="12"/>
+      <c r="B113" s="11"/>
+      <c r="C113" s="11"/>
+      <c r="D113" s="11"/>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="4" t="s">
@@ -6578,12 +6584,12 @@
       </c>
     </row>
     <row r="127" spans="1:4" ht="18.75">
-      <c r="A127" s="11" t="s">
+      <c r="A127" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="B127" s="11"/>
-      <c r="C127" s="11"/>
-      <c r="D127" s="11"/>
+      <c r="B127" s="13"/>
+      <c r="C127" s="13"/>
+      <c r="D127" s="13"/>
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="4" t="s">
@@ -6703,11 +6709,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A29:D29"/>
     <mergeCell ref="A127:D127"/>
     <mergeCell ref="A107:D107"/>
     <mergeCell ref="A113:D113"/>
@@ -6718,6 +6719,11 @@
     <mergeCell ref="A98:D98"/>
     <mergeCell ref="A66:D66"/>
     <mergeCell ref="A55:D55"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A29:D29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>

</xml_diff>

<commit_message>
Wario 100% - Level 10 done, a chunk of level 11 done.  Don't know yet how much of it will survive as I haven't route planned yet.
</commit_message>
<xml_diff>
--- a/Wario/Wario.xlsx
+++ b/Wario/Wario.xlsx
@@ -658,8 +658,8 @@
   <dimension ref="A1:J164"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A102" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B122" sqref="B122"/>
+      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B127" sqref="B127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2164,24 +2164,30 @@
       <c r="A123" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="B123" s="4">
+        <v>48406</v>
+      </c>
       <c r="C123" s="4">
         <v>38859</v>
       </c>
       <c r="D123" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-9547</v>
       </c>
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="B124" s="4">
+        <v>48610</v>
+      </c>
       <c r="C124" s="4">
         <v>39062</v>
       </c>
       <c r="D124" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-9548</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="18.75">
@@ -2196,12 +2202,15 @@
       <c r="A126" s="4" t="s">
         <v>48</v>
       </c>
+      <c r="B126" s="4">
+        <v>48860</v>
+      </c>
       <c r="C126" s="4">
         <v>39312</v>
       </c>
       <c r="D126" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-9548</v>
       </c>
     </row>
     <row r="127" spans="1:4">

</xml_diff>

<commit_message>
Wario 100% - Level 11 done.
</commit_message>
<xml_diff>
--- a/Wario/Wario.xlsx
+++ b/Wario/Wario.xlsx
@@ -658,8 +658,8 @@
   <dimension ref="A1:J164"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B127" sqref="B127"/>
+      <pane ySplit="1" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B136" sqref="B136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2280,24 +2280,30 @@
       <c r="A132" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="B132" s="4">
+        <v>53138</v>
+      </c>
       <c r="C132" s="4">
         <v>42015</v>
       </c>
       <c r="D132" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-11123</v>
       </c>
     </row>
     <row r="133" spans="1:5">
       <c r="A133" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="B133" s="4">
+        <v>53349</v>
+      </c>
       <c r="C133" s="4">
         <v>42219</v>
       </c>
       <c r="D133" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-11130</v>
       </c>
     </row>
     <row r="134" spans="1:5" ht="18.75">
@@ -2312,12 +2318,15 @@
       <c r="A135" s="4" t="s">
         <v>51</v>
       </c>
+      <c r="B135" s="4">
+        <v>53598</v>
+      </c>
       <c r="C135" s="4">
         <v>42469</v>
       </c>
       <c r="D135" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-11129</v>
       </c>
     </row>
     <row r="136" spans="1:5">

</xml_diff>

<commit_message>
Wario 100% - Level 12 done.
</commit_message>
<xml_diff>
--- a/Wario/Wario.xlsx
+++ b/Wario/Wario.xlsx
@@ -358,9 +358,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -658,8 +658,8 @@
   <dimension ref="A1:J164"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B136" sqref="B136"/>
+      <pane ySplit="1" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B144" sqref="B144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -683,12 +683,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -716,12 +716,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -791,12 +791,12 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="18.75">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="4" t="s">
@@ -967,12 +967,12 @@
       </c>
     </row>
     <row r="30" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A30" s="11" t="s">
+      <c r="A30" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="4" t="s">
@@ -1148,12 +1148,12 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="18.75">
-      <c r="A43" s="13" t="s">
+      <c r="A43" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B43" s="13"/>
-      <c r="C43" s="13"/>
-      <c r="D43" s="13"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="4" t="s">
@@ -1300,12 +1300,12 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="18.75">
-      <c r="A55" s="11" t="s">
+      <c r="A55" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B55" s="11"/>
-      <c r="C55" s="11"/>
-      <c r="D55" s="11"/>
+      <c r="B55" s="12"/>
+      <c r="C55" s="12"/>
+      <c r="D55" s="12"/>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="4" t="s">
@@ -1396,12 +1396,12 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="18.75">
-      <c r="A63" s="13" t="s">
+      <c r="A63" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B63" s="13"/>
-      <c r="C63" s="13"/>
-      <c r="D63" s="13"/>
+      <c r="B63" s="11"/>
+      <c r="C63" s="11"/>
+      <c r="D63" s="11"/>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="4" t="s">
@@ -1587,12 +1587,12 @@
       </c>
     </row>
     <row r="76" spans="1:10" ht="18.75">
-      <c r="A76" s="11" t="s">
+      <c r="A76" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B76" s="11"/>
-      <c r="C76" s="11"/>
-      <c r="D76" s="11"/>
+      <c r="B76" s="12"/>
+      <c r="C76" s="12"/>
+      <c r="D76" s="12"/>
     </row>
     <row r="77" spans="1:10">
       <c r="A77" s="4" t="s">
@@ -1739,12 +1739,12 @@
       </c>
     </row>
     <row r="88" spans="1:4" ht="18.75">
-      <c r="A88" s="13" t="s">
+      <c r="A88" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B88" s="13"/>
-      <c r="C88" s="13"/>
-      <c r="D88" s="13"/>
+      <c r="B88" s="11"/>
+      <c r="C88" s="11"/>
+      <c r="D88" s="11"/>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="4" t="s">
@@ -1857,12 +1857,12 @@
       </c>
     </row>
     <row r="97" spans="1:4" ht="18.75">
-      <c r="A97" s="11" t="s">
+      <c r="A97" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B97" s="11"/>
-      <c r="C97" s="11"/>
-      <c r="D97" s="11"/>
+      <c r="B97" s="12"/>
+      <c r="C97" s="12"/>
+      <c r="D97" s="12"/>
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="4" t="s">
@@ -1934,12 +1934,12 @@
       </c>
     </row>
     <row r="103" spans="1:4" ht="18.75">
-      <c r="A103" s="13" t="s">
+      <c r="A103" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B103" s="13"/>
-      <c r="C103" s="13"/>
-      <c r="D103" s="13"/>
+      <c r="B103" s="11"/>
+      <c r="C103" s="11"/>
+      <c r="D103" s="11"/>
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="4" t="s">
@@ -2191,12 +2191,12 @@
       </c>
     </row>
     <row r="125" spans="1:4" ht="18.75">
-      <c r="A125" s="11" t="s">
+      <c r="A125" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B125" s="11"/>
-      <c r="C125" s="11"/>
-      <c r="D125" s="11"/>
+      <c r="B125" s="12"/>
+      <c r="C125" s="12"/>
+      <c r="D125" s="12"/>
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="4" t="s">
@@ -2307,12 +2307,12 @@
       </c>
     </row>
     <row r="134" spans="1:5" ht="18.75">
-      <c r="A134" s="13" t="s">
+      <c r="A134" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B134" s="13"/>
-      <c r="C134" s="13"/>
-      <c r="D134" s="13"/>
+      <c r="B134" s="11"/>
+      <c r="C134" s="11"/>
+      <c r="D134" s="11"/>
     </row>
     <row r="135" spans="1:5">
       <c r="A135" s="4" t="s">
@@ -2333,92 +2333,113 @@
       <c r="A136" s="4" t="s">
         <v>66</v>
       </c>
+      <c r="B136" s="4">
+        <v>54353</v>
+      </c>
       <c r="C136" s="4">
         <v>43196</v>
       </c>
       <c r="D136" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-11157</v>
       </c>
     </row>
     <row r="137" spans="1:5">
       <c r="A137" s="4" t="s">
         <v>60</v>
       </c>
+      <c r="B137" s="4">
+        <v>55005</v>
+      </c>
       <c r="C137" s="4">
         <v>43848</v>
       </c>
       <c r="D137" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-11157</v>
       </c>
     </row>
     <row r="138" spans="1:5">
       <c r="A138" s="4" t="s">
         <v>26</v>
       </c>
+      <c r="B138" s="4">
+        <v>55327</v>
+      </c>
       <c r="C138" s="4">
         <v>44155</v>
       </c>
       <c r="D138" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-11172</v>
       </c>
     </row>
     <row r="139" spans="1:5">
       <c r="A139" s="4" t="s">
         <v>53</v>
       </c>
+      <c r="B139" s="4">
+        <v>57741</v>
+      </c>
       <c r="C139" s="4">
         <v>46549</v>
       </c>
       <c r="D139" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-11192</v>
       </c>
     </row>
     <row r="140" spans="1:5">
       <c r="A140" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="B140" s="4">
+        <v>58132</v>
+      </c>
       <c r="C140" s="4">
         <v>46905</v>
       </c>
       <c r="D140" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-11227</v>
       </c>
     </row>
     <row r="141" spans="1:5">
       <c r="A141" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="B141" s="4">
+        <v>58344</v>
+      </c>
       <c r="C141" s="4">
         <v>47108</v>
       </c>
       <c r="D141" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-11236</v>
       </c>
     </row>
     <row r="142" spans="1:5" ht="18.75">
-      <c r="A142" s="11" t="s">
+      <c r="A142" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B142" s="11"/>
-      <c r="C142" s="11"/>
-      <c r="D142" s="11"/>
+      <c r="B142" s="12"/>
+      <c r="C142" s="12"/>
+      <c r="D142" s="12"/>
     </row>
     <row r="143" spans="1:5">
       <c r="A143" s="4" t="s">
         <v>54</v>
       </c>
+      <c r="B143" s="4">
+        <v>58593</v>
+      </c>
       <c r="C143" s="4">
         <v>47359</v>
       </c>
       <c r="D143" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-11234</v>
       </c>
     </row>
     <row r="144" spans="1:5">
@@ -2572,12 +2593,12 @@
       </c>
     </row>
     <row r="156" spans="1:5" ht="18.75">
-      <c r="A156" s="13" t="s">
+      <c r="A156" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="B156" s="13"/>
-      <c r="C156" s="13"/>
-      <c r="D156" s="13"/>
+      <c r="B156" s="11"/>
+      <c r="C156" s="11"/>
+      <c r="D156" s="11"/>
     </row>
     <row r="157" spans="1:5">
       <c r="A157" s="4" t="s">
@@ -2677,6 +2698,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A55:D55"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A43:D43"/>
     <mergeCell ref="A134:D134"/>
     <mergeCell ref="A142:D142"/>
     <mergeCell ref="A156:D156"/>
@@ -2686,12 +2713,6 @@
     <mergeCell ref="A97:D97"/>
     <mergeCell ref="A103:D103"/>
     <mergeCell ref="A125:D125"/>
-    <mergeCell ref="A55:D55"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A43:D43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -2728,12 +2749,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -2761,12 +2782,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -2800,12 +2821,12 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
@@ -2928,12 +2949,12 @@
       </c>
     </row>
     <row r="19" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="4" t="s">
@@ -3101,12 +3122,12 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="18.75">
-      <c r="A31" s="13" t="s">
+      <c r="A31" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="4" t="s">
@@ -3274,12 +3295,12 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="18.75">
-      <c r="A43" s="11" t="s">
+      <c r="A43" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B43" s="11"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="4" t="s">
@@ -3387,12 +3408,12 @@
       </c>
     </row>
     <row r="51" spans="1:10" ht="18.75">
-      <c r="A51" s="13" t="s">
+      <c r="A51" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B51" s="13"/>
-      <c r="C51" s="13"/>
-      <c r="D51" s="13"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="4" t="s">
@@ -3578,12 +3599,12 @@
       </c>
     </row>
     <row r="64" spans="1:10" ht="18.75">
-      <c r="A64" s="11" t="s">
+      <c r="A64" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B64" s="11"/>
-      <c r="C64" s="11"/>
-      <c r="D64" s="11"/>
+      <c r="B64" s="12"/>
+      <c r="C64" s="12"/>
+      <c r="D64" s="12"/>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="4" t="s">
@@ -3742,12 +3763,12 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="18.75">
-      <c r="A76" s="13" t="s">
+      <c r="A76" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B76" s="13"/>
-      <c r="C76" s="13"/>
-      <c r="D76" s="13"/>
+      <c r="B76" s="11"/>
+      <c r="C76" s="11"/>
+      <c r="D76" s="11"/>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="4" t="s">
@@ -3860,12 +3881,12 @@
       </c>
     </row>
     <row r="85" spans="1:4" ht="18.75">
-      <c r="A85" s="11" t="s">
+      <c r="A85" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B85" s="11"/>
-      <c r="C85" s="11"/>
-      <c r="D85" s="11"/>
+      <c r="B85" s="12"/>
+      <c r="C85" s="12"/>
+      <c r="D85" s="12"/>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="4" t="s">
@@ -3925,12 +3946,12 @@
       </c>
     </row>
     <row r="90" spans="1:4" ht="18.75">
-      <c r="A90" s="13" t="s">
+      <c r="A90" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B90" s="13"/>
-      <c r="C90" s="13"/>
-      <c r="D90" s="13"/>
+      <c r="B90" s="11"/>
+      <c r="C90" s="11"/>
+      <c r="D90" s="11"/>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="4" t="s">
@@ -4221,12 +4242,12 @@
       </c>
     </row>
     <row r="112" spans="1:4" ht="18.75">
-      <c r="A112" s="11" t="s">
+      <c r="A112" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B112" s="11"/>
-      <c r="C112" s="11"/>
-      <c r="D112" s="11"/>
+      <c r="B112" s="12"/>
+      <c r="C112" s="12"/>
+      <c r="D112" s="12"/>
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="4" t="s">
@@ -4352,12 +4373,12 @@
       </c>
     </row>
     <row r="121" spans="1:5" ht="18.75">
-      <c r="A121" s="13" t="s">
+      <c r="A121" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B121" s="13"/>
-      <c r="C121" s="13"/>
-      <c r="D121" s="13"/>
+      <c r="B121" s="11"/>
+      <c r="C121" s="11"/>
+      <c r="D121" s="11"/>
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="4" t="s">
@@ -4465,12 +4486,12 @@
       </c>
     </row>
     <row r="129" spans="1:5" ht="18.75">
-      <c r="A129" s="11" t="s">
+      <c r="A129" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B129" s="11"/>
-      <c r="C129" s="11"/>
-      <c r="D129" s="11"/>
+      <c r="B129" s="12"/>
+      <c r="C129" s="12"/>
+      <c r="D129" s="12"/>
     </row>
     <row r="130" spans="1:5">
       <c r="A130" s="4" t="s">
@@ -4674,12 +4695,12 @@
       </c>
     </row>
     <row r="143" spans="1:5" ht="18.75">
-      <c r="A143" s="13" t="s">
+      <c r="A143" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="B143" s="13"/>
-      <c r="C143" s="13"/>
-      <c r="D143" s="13"/>
+      <c r="B143" s="11"/>
+      <c r="C143" s="11"/>
+      <c r="D143" s="11"/>
     </row>
     <row r="144" spans="1:5">
       <c r="A144" s="4" t="s">
@@ -4808,12 +4829,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A31:D31"/>
     <mergeCell ref="A121:D121"/>
     <mergeCell ref="A129:D129"/>
     <mergeCell ref="A143:D143"/>
@@ -4823,6 +4838,12 @@
     <mergeCell ref="A85:D85"/>
     <mergeCell ref="A90:D90"/>
     <mergeCell ref="A112:D112"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A31:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -4859,12 +4880,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -4892,12 +4913,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -4931,12 +4952,12 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
@@ -5020,12 +5041,12 @@
       </c>
     </row>
     <row r="17" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="4" t="s">
@@ -5193,12 +5214,12 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="18.75">
-      <c r="A29" s="13" t="s">
+      <c r="A29" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="4" t="s">
@@ -5276,12 +5297,12 @@
       </c>
     </row>
     <row r="35" spans="1:10" ht="18.75">
-      <c r="A35" s="11" t="s">
+      <c r="A35" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="4" t="s">
@@ -5374,12 +5395,12 @@
       </c>
     </row>
     <row r="42" spans="1:10" ht="18.75">
-      <c r="A42" s="13" t="s">
+      <c r="A42" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B42" s="13"/>
-      <c r="C42" s="13"/>
-      <c r="D42" s="13"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="4" t="s">
@@ -5568,12 +5589,12 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="18.75">
-      <c r="A55" s="11" t="s">
+      <c r="A55" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B55" s="11"/>
-      <c r="C55" s="11"/>
-      <c r="D55" s="11"/>
+      <c r="B55" s="12"/>
+      <c r="C55" s="12"/>
+      <c r="D55" s="12"/>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="4" t="s">
@@ -5726,12 +5747,12 @@
       </c>
     </row>
     <row r="66" spans="1:4" ht="18.75">
-      <c r="A66" s="13" t="s">
+      <c r="A66" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B66" s="13"/>
-      <c r="C66" s="13"/>
-      <c r="D66" s="13"/>
+      <c r="B66" s="11"/>
+      <c r="C66" s="11"/>
+      <c r="D66" s="11"/>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="4" t="s">
@@ -5794,12 +5815,12 @@
       </c>
     </row>
     <row r="71" spans="1:4" ht="18.75">
-      <c r="A71" s="11" t="s">
+      <c r="A71" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B71" s="11"/>
-      <c r="C71" s="11"/>
-      <c r="D71" s="11"/>
+      <c r="B71" s="12"/>
+      <c r="C71" s="12"/>
+      <c r="D71" s="12"/>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="4" t="s">
@@ -5862,12 +5883,12 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="18.75">
-      <c r="A76" s="13" t="s">
+      <c r="A76" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B76" s="13"/>
-      <c r="C76" s="13"/>
-      <c r="D76" s="13"/>
+      <c r="B76" s="11"/>
+      <c r="C76" s="11"/>
+      <c r="D76" s="11"/>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="4" t="s">
@@ -6185,12 +6206,12 @@
       </c>
     </row>
     <row r="98" spans="1:5" ht="18.75">
-      <c r="A98" s="11" t="s">
+      <c r="A98" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B98" s="11"/>
-      <c r="C98" s="11"/>
-      <c r="D98" s="11"/>
+      <c r="B98" s="12"/>
+      <c r="C98" s="12"/>
+      <c r="D98" s="12"/>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="4" t="s">
@@ -6316,12 +6337,12 @@
       </c>
     </row>
     <row r="107" spans="1:5" ht="18.75">
-      <c r="A107" s="13" t="s">
+      <c r="A107" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B107" s="13"/>
-      <c r="C107" s="13"/>
-      <c r="D107" s="13"/>
+      <c r="B107" s="11"/>
+      <c r="C107" s="11"/>
+      <c r="D107" s="11"/>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="4" t="s">
@@ -6399,12 +6420,12 @@
       </c>
     </row>
     <row r="113" spans="1:4" ht="18.75">
-      <c r="A113" s="11" t="s">
+      <c r="A113" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B113" s="11"/>
-      <c r="C113" s="11"/>
-      <c r="D113" s="11"/>
+      <c r="B113" s="12"/>
+      <c r="C113" s="12"/>
+      <c r="D113" s="12"/>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="4" t="s">
@@ -6602,12 +6623,12 @@
       </c>
     </row>
     <row r="127" spans="1:4" ht="18.75">
-      <c r="A127" s="13" t="s">
+      <c r="A127" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="B127" s="13"/>
-      <c r="C127" s="13"/>
-      <c r="D127" s="13"/>
+      <c r="B127" s="11"/>
+      <c r="C127" s="11"/>
+      <c r="D127" s="11"/>
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="4" t="s">
@@ -6727,6 +6748,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A29:D29"/>
     <mergeCell ref="A127:D127"/>
     <mergeCell ref="A107:D107"/>
     <mergeCell ref="A113:D113"/>
@@ -6737,11 +6763,6 @@
     <mergeCell ref="A98:D98"/>
     <mergeCell ref="A66:D66"/>
     <mergeCell ref="A55:D55"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A29:D29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>

</xml_diff>

<commit_message>
Wario 100% - Level 13 up through getting treasure + key + more room
</commit_message>
<xml_diff>
--- a/Wario/Wario.xlsx
+++ b/Wario/Wario.xlsx
@@ -358,9 +358,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -658,8 +658,8 @@
   <dimension ref="A1:J164"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B144" sqref="B144"/>
+      <pane ySplit="1" topLeftCell="A137" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B148" sqref="B148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -683,12 +683,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -716,12 +716,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -791,12 +791,12 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="18.75">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="4" t="s">
@@ -967,12 +967,12 @@
       </c>
     </row>
     <row r="30" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A30" s="12" t="s">
+      <c r="A30" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="4" t="s">
@@ -1148,12 +1148,12 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="18.75">
-      <c r="A43" s="11" t="s">
+      <c r="A43" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B43" s="11"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="4" t="s">
@@ -1300,12 +1300,12 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="18.75">
-      <c r="A55" s="12" t="s">
+      <c r="A55" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B55" s="12"/>
-      <c r="C55" s="12"/>
-      <c r="D55" s="12"/>
+      <c r="B55" s="11"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="11"/>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="4" t="s">
@@ -1396,12 +1396,12 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="18.75">
-      <c r="A63" s="11" t="s">
+      <c r="A63" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B63" s="11"/>
-      <c r="C63" s="11"/>
-      <c r="D63" s="11"/>
+      <c r="B63" s="13"/>
+      <c r="C63" s="13"/>
+      <c r="D63" s="13"/>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="4" t="s">
@@ -1587,12 +1587,12 @@
       </c>
     </row>
     <row r="76" spans="1:10" ht="18.75">
-      <c r="A76" s="12" t="s">
+      <c r="A76" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B76" s="12"/>
-      <c r="C76" s="12"/>
-      <c r="D76" s="12"/>
+      <c r="B76" s="11"/>
+      <c r="C76" s="11"/>
+      <c r="D76" s="11"/>
     </row>
     <row r="77" spans="1:10">
       <c r="A77" s="4" t="s">
@@ -1739,12 +1739,12 @@
       </c>
     </row>
     <row r="88" spans="1:4" ht="18.75">
-      <c r="A88" s="11" t="s">
+      <c r="A88" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B88" s="11"/>
-      <c r="C88" s="11"/>
-      <c r="D88" s="11"/>
+      <c r="B88" s="13"/>
+      <c r="C88" s="13"/>
+      <c r="D88" s="13"/>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="4" t="s">
@@ -1857,12 +1857,12 @@
       </c>
     </row>
     <row r="97" spans="1:4" ht="18.75">
-      <c r="A97" s="12" t="s">
+      <c r="A97" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B97" s="12"/>
-      <c r="C97" s="12"/>
-      <c r="D97" s="12"/>
+      <c r="B97" s="11"/>
+      <c r="C97" s="11"/>
+      <c r="D97" s="11"/>
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="4" t="s">
@@ -1934,12 +1934,12 @@
       </c>
     </row>
     <row r="103" spans="1:4" ht="18.75">
-      <c r="A103" s="11" t="s">
+      <c r="A103" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B103" s="11"/>
-      <c r="C103" s="11"/>
-      <c r="D103" s="11"/>
+      <c r="B103" s="13"/>
+      <c r="C103" s="13"/>
+      <c r="D103" s="13"/>
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="4" t="s">
@@ -2191,12 +2191,12 @@
       </c>
     </row>
     <row r="125" spans="1:4" ht="18.75">
-      <c r="A125" s="12" t="s">
+      <c r="A125" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B125" s="12"/>
-      <c r="C125" s="12"/>
-      <c r="D125" s="12"/>
+      <c r="B125" s="11"/>
+      <c r="C125" s="11"/>
+      <c r="D125" s="11"/>
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="4" t="s">
@@ -2307,12 +2307,12 @@
       </c>
     </row>
     <row r="134" spans="1:5" ht="18.75">
-      <c r="A134" s="11" t="s">
+      <c r="A134" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="B134" s="11"/>
-      <c r="C134" s="11"/>
-      <c r="D134" s="11"/>
+      <c r="B134" s="13"/>
+      <c r="C134" s="13"/>
+      <c r="D134" s="13"/>
     </row>
     <row r="135" spans="1:5">
       <c r="A135" s="4" t="s">
@@ -2420,12 +2420,12 @@
       </c>
     </row>
     <row r="142" spans="1:5" ht="18.75">
-      <c r="A142" s="12" t="s">
+      <c r="A142" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B142" s="12"/>
-      <c r="C142" s="12"/>
-      <c r="D142" s="12"/>
+      <c r="B142" s="11"/>
+      <c r="C142" s="11"/>
+      <c r="D142" s="11"/>
     </row>
     <row r="143" spans="1:5">
       <c r="A143" s="4" t="s">
@@ -2458,36 +2458,45 @@
       <c r="A145" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="B145" s="4">
+        <v>59844</v>
+      </c>
       <c r="C145" s="4">
         <v>47847</v>
       </c>
       <c r="D145" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-11997</v>
       </c>
     </row>
     <row r="146" spans="1:5">
       <c r="A146" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="B146" s="4">
+        <v>60054</v>
+      </c>
       <c r="C146" s="4">
         <v>48052</v>
       </c>
       <c r="D146" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-12002</v>
       </c>
     </row>
     <row r="147" spans="1:5">
       <c r="A147" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="B147" s="4">
+        <v>60228</v>
+      </c>
       <c r="C147" s="4">
         <v>48226</v>
       </c>
       <c r="D147" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-12002</v>
       </c>
     </row>
     <row r="148" spans="1:5">
@@ -2593,12 +2602,12 @@
       </c>
     </row>
     <row r="156" spans="1:5" ht="18.75">
-      <c r="A156" s="11" t="s">
+      <c r="A156" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="B156" s="11"/>
-      <c r="C156" s="11"/>
-      <c r="D156" s="11"/>
+      <c r="B156" s="13"/>
+      <c r="C156" s="13"/>
+      <c r="D156" s="13"/>
     </row>
     <row r="157" spans="1:5">
       <c r="A157" s="4" t="s">
@@ -2698,12 +2707,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A55:D55"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A43:D43"/>
     <mergeCell ref="A134:D134"/>
     <mergeCell ref="A142:D142"/>
     <mergeCell ref="A156:D156"/>
@@ -2713,6 +2716,12 @@
     <mergeCell ref="A97:D97"/>
     <mergeCell ref="A103:D103"/>
     <mergeCell ref="A125:D125"/>
+    <mergeCell ref="A55:D55"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A43:D43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -2749,12 +2758,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -2782,12 +2791,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -2821,12 +2830,12 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
@@ -2949,12 +2958,12 @@
       </c>
     </row>
     <row r="19" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="4" t="s">
@@ -3122,12 +3131,12 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="18.75">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="4" t="s">
@@ -3295,12 +3304,12 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="18.75">
-      <c r="A43" s="12" t="s">
+      <c r="A43" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B43" s="12"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="4" t="s">
@@ -3408,12 +3417,12 @@
       </c>
     </row>
     <row r="51" spans="1:10" ht="18.75">
-      <c r="A51" s="11" t="s">
+      <c r="A51" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B51" s="11"/>
-      <c r="C51" s="11"/>
-      <c r="D51" s="11"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="13"/>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="4" t="s">
@@ -3599,12 +3608,12 @@
       </c>
     </row>
     <row r="64" spans="1:10" ht="18.75">
-      <c r="A64" s="12" t="s">
+      <c r="A64" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B64" s="12"/>
-      <c r="C64" s="12"/>
-      <c r="D64" s="12"/>
+      <c r="B64" s="11"/>
+      <c r="C64" s="11"/>
+      <c r="D64" s="11"/>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="4" t="s">
@@ -3763,12 +3772,12 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="18.75">
-      <c r="A76" s="11" t="s">
+      <c r="A76" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B76" s="11"/>
-      <c r="C76" s="11"/>
-      <c r="D76" s="11"/>
+      <c r="B76" s="13"/>
+      <c r="C76" s="13"/>
+      <c r="D76" s="13"/>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="4" t="s">
@@ -3881,12 +3890,12 @@
       </c>
     </row>
     <row r="85" spans="1:4" ht="18.75">
-      <c r="A85" s="12" t="s">
+      <c r="A85" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B85" s="12"/>
-      <c r="C85" s="12"/>
-      <c r="D85" s="12"/>
+      <c r="B85" s="11"/>
+      <c r="C85" s="11"/>
+      <c r="D85" s="11"/>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="4" t="s">
@@ -3946,12 +3955,12 @@
       </c>
     </row>
     <row r="90" spans="1:4" ht="18.75">
-      <c r="A90" s="11" t="s">
+      <c r="A90" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B90" s="11"/>
-      <c r="C90" s="11"/>
-      <c r="D90" s="11"/>
+      <c r="B90" s="13"/>
+      <c r="C90" s="13"/>
+      <c r="D90" s="13"/>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="4" t="s">
@@ -4242,12 +4251,12 @@
       </c>
     </row>
     <row r="112" spans="1:4" ht="18.75">
-      <c r="A112" s="12" t="s">
+      <c r="A112" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B112" s="12"/>
-      <c r="C112" s="12"/>
-      <c r="D112" s="12"/>
+      <c r="B112" s="11"/>
+      <c r="C112" s="11"/>
+      <c r="D112" s="11"/>
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="4" t="s">
@@ -4373,12 +4382,12 @@
       </c>
     </row>
     <row r="121" spans="1:5" ht="18.75">
-      <c r="A121" s="11" t="s">
+      <c r="A121" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="B121" s="11"/>
-      <c r="C121" s="11"/>
-      <c r="D121" s="11"/>
+      <c r="B121" s="13"/>
+      <c r="C121" s="13"/>
+      <c r="D121" s="13"/>
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="4" t="s">
@@ -4486,12 +4495,12 @@
       </c>
     </row>
     <row r="129" spans="1:5" ht="18.75">
-      <c r="A129" s="12" t="s">
+      <c r="A129" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B129" s="12"/>
-      <c r="C129" s="12"/>
-      <c r="D129" s="12"/>
+      <c r="B129" s="11"/>
+      <c r="C129" s="11"/>
+      <c r="D129" s="11"/>
     </row>
     <row r="130" spans="1:5">
       <c r="A130" s="4" t="s">
@@ -4695,12 +4704,12 @@
       </c>
     </row>
     <row r="143" spans="1:5" ht="18.75">
-      <c r="A143" s="11" t="s">
+      <c r="A143" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="B143" s="11"/>
-      <c r="C143" s="11"/>
-      <c r="D143" s="11"/>
+      <c r="B143" s="13"/>
+      <c r="C143" s="13"/>
+      <c r="D143" s="13"/>
     </row>
     <row r="144" spans="1:5">
       <c r="A144" s="4" t="s">
@@ -4829,6 +4838,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A31:D31"/>
     <mergeCell ref="A121:D121"/>
     <mergeCell ref="A129:D129"/>
     <mergeCell ref="A143:D143"/>
@@ -4838,12 +4853,6 @@
     <mergeCell ref="A85:D85"/>
     <mergeCell ref="A90:D90"/>
     <mergeCell ref="A112:D112"/>
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A31:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -4880,12 +4889,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3"/>
@@ -4913,12 +4922,12 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -4952,12 +4961,12 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
@@ -5041,12 +5050,12 @@
       </c>
     </row>
     <row r="17" spans="1:4" s="1" customFormat="1" ht="18.75">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="4" t="s">
@@ -5214,12 +5223,12 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="18.75">
-      <c r="A29" s="11" t="s">
+      <c r="A29" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="4" t="s">
@@ -5297,12 +5306,12 @@
       </c>
     </row>
     <row r="35" spans="1:10" ht="18.75">
-      <c r="A35" s="12" t="s">
+      <c r="A35" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="12"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="4" t="s">
@@ -5395,12 +5404,12 @@
       </c>
     </row>
     <row r="42" spans="1:10" ht="18.75">
-      <c r="A42" s="11" t="s">
+      <c r="A42" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B42" s="11"/>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="4" t="s">
@@ -5589,12 +5598,12 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="18.75">
-      <c r="A55" s="12" t="s">
+      <c r="A55" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B55" s="12"/>
-      <c r="C55" s="12"/>
-      <c r="D55" s="12"/>
+      <c r="B55" s="11"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="11"/>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="4" t="s">
@@ -5747,12 +5756,12 @@
       </c>
     </row>
     <row r="66" spans="1:4" ht="18.75">
-      <c r="A66" s="11" t="s">
+      <c r="A66" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B66" s="11"/>
-      <c r="C66" s="11"/>
-      <c r="D66" s="11"/>
+      <c r="B66" s="13"/>
+      <c r="C66" s="13"/>
+      <c r="D66" s="13"/>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="4" t="s">
@@ -5815,12 +5824,12 @@
       </c>
     </row>
     <row r="71" spans="1:4" ht="18.75">
-      <c r="A71" s="12" t="s">
+      <c r="A71" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B71" s="12"/>
-      <c r="C71" s="12"/>
-      <c r="D71" s="12"/>
+      <c r="B71" s="11"/>
+      <c r="C71" s="11"/>
+      <c r="D71" s="11"/>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="4" t="s">
@@ -5883,12 +5892,12 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="18.75">
-      <c r="A76" s="11" t="s">
+      <c r="A76" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B76" s="11"/>
-      <c r="C76" s="11"/>
-      <c r="D76" s="11"/>
+      <c r="B76" s="13"/>
+      <c r="C76" s="13"/>
+      <c r="D76" s="13"/>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="4" t="s">
@@ -6206,12 +6215,12 @@
       </c>
     </row>
     <row r="98" spans="1:5" ht="18.75">
-      <c r="A98" s="12" t="s">
+      <c r="A98" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B98" s="12"/>
-      <c r="C98" s="12"/>
-      <c r="D98" s="12"/>
+      <c r="B98" s="11"/>
+      <c r="C98" s="11"/>
+      <c r="D98" s="11"/>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="4" t="s">
@@ -6337,12 +6346,12 @@
       </c>
     </row>
     <row r="107" spans="1:5" ht="18.75">
-      <c r="A107" s="11" t="s">
+      <c r="A107" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="B107" s="11"/>
-      <c r="C107" s="11"/>
-      <c r="D107" s="11"/>
+      <c r="B107" s="13"/>
+      <c r="C107" s="13"/>
+      <c r="D107" s="13"/>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="4" t="s">
@@ -6420,12 +6429,12 @@
       </c>
     </row>
     <row r="113" spans="1:4" ht="18.75">
-      <c r="A113" s="12" t="s">
+      <c r="A113" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B113" s="12"/>
-      <c r="C113" s="12"/>
-      <c r="D113" s="12"/>
+      <c r="B113" s="11"/>
+      <c r="C113" s="11"/>
+      <c r="D113" s="11"/>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="4" t="s">
@@ -6623,12 +6632,12 @@
       </c>
     </row>
     <row r="127" spans="1:4" ht="18.75">
-      <c r="A127" s="11" t="s">
+      <c r="A127" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="B127" s="11"/>
-      <c r="C127" s="11"/>
-      <c r="D127" s="11"/>
+      <c r="B127" s="13"/>
+      <c r="C127" s="13"/>
+      <c r="D127" s="13"/>
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="4" t="s">
@@ -6748,11 +6757,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A29:D29"/>
     <mergeCell ref="A127:D127"/>
     <mergeCell ref="A107:D107"/>
     <mergeCell ref="A113:D113"/>
@@ -6763,6 +6767,11 @@
     <mergeCell ref="A98:D98"/>
     <mergeCell ref="A66:D66"/>
     <mergeCell ref="A55:D55"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A29:D29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>

</xml_diff>

<commit_message>
Wario 100% - Most of level 13
</commit_message>
<xml_diff>
--- a/Wario/Wario.xlsx
+++ b/Wario/Wario.xlsx
@@ -659,7 +659,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A137" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B148" sqref="B148"/>
+      <selection pane="bottomLeft" activeCell="B154" sqref="B154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2503,24 +2503,30 @@
       <c r="A148" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="B148" s="4">
+        <v>60532</v>
+      </c>
       <c r="C148" s="4">
         <v>48530</v>
       </c>
       <c r="D148" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-12002</v>
       </c>
     </row>
     <row r="149" spans="1:5">
       <c r="A149" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="B149" s="4">
+        <v>60714</v>
+      </c>
       <c r="C149" s="4">
         <v>48705</v>
       </c>
       <c r="D149" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-12009</v>
       </c>
       <c r="E149" t="s">
         <v>70</v>
@@ -2530,36 +2536,45 @@
       <c r="A150" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="B150" s="4">
+        <v>60829</v>
+      </c>
       <c r="C150" s="4">
         <v>48820</v>
       </c>
       <c r="D150" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-12009</v>
       </c>
     </row>
     <row r="151" spans="1:5">
       <c r="A151" s="4" t="s">
         <v>57</v>
       </c>
+      <c r="B151" s="4">
+        <v>61156</v>
+      </c>
       <c r="C151" s="4">
         <v>49147</v>
       </c>
       <c r="D151" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-12009</v>
       </c>
     </row>
     <row r="152" spans="1:5">
       <c r="A152" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="B152" s="4">
+        <v>61330</v>
+      </c>
       <c r="C152" s="4">
         <v>49319</v>
       </c>
       <c r="D152" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-12011</v>
       </c>
       <c r="E152" t="s">
         <v>71</v>
@@ -2569,12 +2584,15 @@
       <c r="A153" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="B153" s="4">
+        <v>61576</v>
+      </c>
       <c r="C153" s="4">
         <v>49569</v>
       </c>
       <c r="D153" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-12007</v>
       </c>
     </row>
     <row r="154" spans="1:5">

</xml_diff>

<commit_message>
Wario 100% - Level 13 done.
</commit_message>
<xml_diff>
--- a/Wario/Wario.xlsx
+++ b/Wario/Wario.xlsx
@@ -658,8 +658,8 @@
   <dimension ref="A1:J164"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A137" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B154" sqref="B154"/>
+      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B158" sqref="B158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2611,12 +2611,15 @@
       <c r="A155" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="B155" s="4">
+        <v>62070</v>
+      </c>
       <c r="C155" s="4">
         <v>50063</v>
       </c>
       <c r="D155" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-12007</v>
       </c>
     </row>
     <row r="156" spans="1:5" ht="18.75">
@@ -2631,12 +2634,15 @@
       <c r="A157" s="4" t="s">
         <v>58</v>
       </c>
+      <c r="B157" s="4">
+        <v>62321</v>
+      </c>
       <c r="C157" s="4">
         <v>50314</v>
       </c>
       <c r="D157" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-12007</v>
       </c>
     </row>
     <row r="158" spans="1:5">

</xml_diff>

<commit_message>
Wario 100% - enter final boss room
</commit_message>
<xml_diff>
--- a/Wario/Wario.xlsx
+++ b/Wario/Wario.xlsx
@@ -659,7 +659,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B158" sqref="B158"/>
+      <selection pane="bottomLeft" activeCell="G156" sqref="G156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2649,12 +2649,15 @@
       <c r="A158" s="4" t="s">
         <v>26</v>
       </c>
+      <c r="B158" s="4">
+        <v>63273</v>
+      </c>
       <c r="C158" s="4">
         <v>51237</v>
       </c>
       <c r="D158" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-12036</v>
       </c>
     </row>
     <row r="159" spans="1:5">

</xml_diff>